<commit_message>
Runs. WIP on visit_screening1_p1
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -166,23 +166,83 @@
     <t>Person_1 Triples</t>
   </si>
   <si>
-    <t>Complete through the code.ttl file for country codes</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
     <t>Minor label discrepancy</t>
   </si>
   <si>
-    <t>request to AO for minor label correction within AgeOutcome_1 : 63 YEARS not 63YRS</t>
+    <t>Issues</t>
+  </si>
+  <si>
+    <t>Ont</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Should be interval 1 with corrected label?</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_RI1  rdfs:label  Interval 10</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_RI1  time:hasEnd  cdiscpilot01:Date_29</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_LS1  rdfs:label  Interval 4</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_RI1  rdfs:label  Reference Interval 1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_RI1  time:hasEnd  cdiscpilot01:Date_30</t>
+  </si>
+  <si>
+    <t>Should be fixed after AO aligns dates</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_LS1  rdfs:label  Lifespan Interval 1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_LS1  rdfs:label  Study Participation Interval 1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:InformedConsent_1  study:hasOutcome  code:informedconsent_1</t>
+  </si>
+  <si>
+    <t>ProposedFix</t>
+  </si>
+  <si>
+    <t>Change label in ontology</t>
+  </si>
+  <si>
+    <t>Date assignment change in ontology (previously identified with list of date reassignments)</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:InformedConsent_1  code:hasOutcome  code:InformedConsent_1</t>
+  </si>
+  <si>
+    <t>Case change in ontology</t>
+  </si>
+  <si>
+    <t>Lower case in code.ttl (ontology version)</t>
+  </si>
+  <si>
+    <t>.. Unable to compare informedconsent_&lt;n&gt;/InformedConsent_&lt;n&gt; in code.ttl/code-R.ttl due to case discrepancy</t>
+  </si>
+  <si>
+    <t>(and children)</t>
+  </si>
+  <si>
+    <t>Changes made. Awaiting new file from AO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,8 +383,23 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,6 +588,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -677,7 +764,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -685,6 +772,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1042,10 +1147,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1054,218 +1159,268 @@
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.08984375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="65.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67" style="5" customWidth="1"/>
+    <col min="7" max="7" width="51.36328125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="57.08984375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="9"/>
+      <c r="G1" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="E2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="G11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D16" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="E16" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>0</v>
       </c>
@@ -1273,10 +1428,10 @@
         <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>0</v>
       </c>
@@ -1284,10 +1439,10 @@
         <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>0</v>
       </c>
@@ -1295,10 +1450,10 @@
         <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -1306,10 +1461,10 @@
         <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>0</v>
       </c>
@@ -1317,10 +1472,10 @@
         <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -1328,10 +1483,46 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
DM processing complete. Outstanding issues identified and pending. Next: VS processing
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -14,13 +14,14 @@
   <sheets>
     <sheet name="person_1" sheetId="1" r:id="rId1"/>
     <sheet name="Issues" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -236,6 +237,30 @@
   </si>
   <si>
     <t>Changes made. Awaiting new file from AO</t>
+  </si>
+  <si>
+    <t>Reported</t>
+  </si>
+  <si>
+    <t>Child: cdiscpilot01:Interval_PA1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_PA1  rdfs:label  Interval 7</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_PA1  rdfs:label  Product administration interval 1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_PA1  time:hasEnd  cdiscpilot01:Date_29</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_PA1  time:hasEnd  cdiscpilot01:Date_30</t>
+  </si>
+  <si>
+    <t>Should be fixed when date alignment occurs</t>
+  </si>
+  <si>
+    <t>Questions out to AO 5 May 17</t>
   </si>
 </sst>
 </file>
@@ -399,7 +424,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -600,6 +625,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -764,7 +801,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -792,6 +829,9 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1147,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1161,11 +1201,11 @@
     <col min="4" max="4" width="36.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="65.1796875" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="67" style="5" customWidth="1"/>
-    <col min="7" max="7" width="51.36328125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="57.08984375" style="4" customWidth="1"/>
+    <col min="7" max="8" width="51.36328125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="57.08984375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="E1" s="8" t="s">
         <v>50</v>
       </c>
@@ -1173,8 +1213,11 @@
       <c r="G1" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H1" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>44</v>
       </c>
@@ -1190,11 +1233,11 @@
       <c r="F2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1208,7 +1251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -1222,7 +1265,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1233,7 +1276,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1244,7 +1287,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1255,7 +1298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1274,8 +1317,9 @@
       <c r="G8" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1294,11 +1338,14 @@
       <c r="G9" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="13">
+        <v>42860</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -1311,11 +1358,14 @@
       <c r="G10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="13">
+        <v>42860</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1328,8 +1378,11 @@
       <c r="G11" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H11" s="13">
+        <v>42860</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1348,11 +1401,14 @@
       <c r="G12" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="13">
+        <v>42860</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1363,7 +1419,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1374,7 +1430,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1385,7 +1441,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>0</v>
       </c>
@@ -1404,11 +1460,14 @@
       <c r="G16" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="13">
+        <v>42860</v>
+      </c>
+      <c r="I16" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -1419,8 +1478,11 @@
       <c r="G17" s="12" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H17" s="13">
+        <v>42860</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>0</v>
       </c>
@@ -1431,40 +1493,46 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" t="s">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D19" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D20" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D21" s="14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="E21" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>0</v>
       </c>
@@ -1472,10 +1540,11 @@
         <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -1483,10 +1552,11 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>0</v>
       </c>
@@ -1494,10 +1564,10 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>0</v>
       </c>
@@ -1505,10 +1575,10 @@
         <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>0</v>
       </c>
@@ -1516,7 +1586,29 @@
         <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1600,4 +1692,63 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="51.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
prep for merge back to main. Work continues on VS conversion.
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="107">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -170,9 +170,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Minor label discrepancy</t>
-  </si>
-  <si>
     <t>Issues</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
     <t>R</t>
   </si>
   <si>
-    <t>Should be interval 1 with corrected label?</t>
-  </si>
-  <si>
     <t>cdiscpilot01:Interval_RI1  rdfs:label  Interval 10</t>
   </si>
   <si>
@@ -200,66 +194,33 @@
     <t>cdiscpilot01:Interval_RI1  time:hasEnd  cdiscpilot01:Date_30</t>
   </si>
   <si>
-    <t>Should be fixed after AO aligns dates</t>
-  </si>
-  <si>
     <t>cdiscpilot01:Interval_LS1  rdfs:label  Lifespan Interval 1</t>
   </si>
   <si>
     <t>cdiscpilot01:Interval_LS1  rdfs:label  Study Participation Interval 1</t>
   </si>
   <si>
-    <t>cdiscpilot01:InformedConsent_1  study:hasOutcome  code:informedconsent_1</t>
-  </si>
-  <si>
     <t>ProposedFix</t>
   </si>
   <si>
     <t>Change label in ontology</t>
   </si>
   <si>
-    <t>Date assignment change in ontology (previously identified with list of date reassignments)</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:InformedConsent_1  code:hasOutcome  code:InformedConsent_1</t>
-  </si>
-  <si>
-    <t>Case change in ontology</t>
-  </si>
-  <si>
-    <t>Lower case in code.ttl (ontology version)</t>
-  </si>
-  <si>
-    <t>.. Unable to compare informedconsent_&lt;n&gt;/InformedConsent_&lt;n&gt; in code.ttl/code-R.ttl due to case discrepancy</t>
-  </si>
-  <si>
     <t>(and children)</t>
   </si>
   <si>
-    <t>Changes made. Awaiting new file from AO</t>
-  </si>
-  <si>
     <t>Reported</t>
   </si>
   <si>
     <t>Child: cdiscpilot01:Interval_PA1</t>
   </si>
   <si>
-    <t>cdiscpilot01:Interval_PA1  rdfs:label  Interval 7</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Interval_PA1  rdfs:label  Product administration interval 1</t>
-  </si>
-  <si>
     <t>cdiscpilot01:Interval_PA1  time:hasEnd  cdiscpilot01:Date_29</t>
   </si>
   <si>
     <t>cdiscpilot01:Interval_PA1  time:hasEnd  cdiscpilot01:Date_30</t>
   </si>
   <si>
-    <t>Should be fixed when date alignment occurs</t>
-  </si>
-  <si>
     <t>cdiscpilot01:Randomization_1rdf:typecode:RandomizationBAL3</t>
   </si>
   <si>
@@ -267,13 +228,151 @@
   </si>
   <si>
     <t>Ont to be changed to match R's "BAL3" after 05May email to AO</t>
+  </si>
+  <si>
+    <t>Child: custom:visit_1</t>
+  </si>
+  <si>
+    <t>custom:visit_1  rdfs:label  SCREENING1</t>
+  </si>
+  <si>
+    <t>custom:visit_1  rdfs:label  SCREENING 1</t>
+  </si>
+  <si>
+    <t>Change ont to match R</t>
+  </si>
+  <si>
+    <t>custom:visit_1  skos:prefLabel  SCREENING 1</t>
+  </si>
+  <si>
+    <t>MISSING in ONT</t>
+  </si>
+  <si>
+    <t>Add to on. Other visits have pref_label but not visit_1</t>
+  </si>
+  <si>
+    <t>Ontology</t>
+  </si>
+  <si>
+    <t>DBP_1</t>
+  </si>
+  <si>
+    <t>links to</t>
+  </si>
+  <si>
+    <t>bpoutcome_2</t>
+  </si>
+  <si>
+    <t>bpoutcome_3</t>
+  </si>
+  <si>
+    <t>bpoutcome_1</t>
+  </si>
+  <si>
+    <t>DBP_2</t>
+  </si>
+  <si>
+    <t>DBP_3</t>
+  </si>
+  <si>
+    <t>Then in the custom terminlogy:</t>
+  </si>
+  <si>
+    <t>links to value:</t>
+  </si>
+  <si>
+    <t>(systolic)</t>
+  </si>
+  <si>
+    <t>bpoutcome_4</t>
+  </si>
+  <si>
+    <t>bpoutcome_5</t>
+  </si>
+  <si>
+    <t>bpoutcome_6</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_RI1  time:hasBeginning  cdiscpilot01:Date_21</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_RI1  time:hasBeginning  cdiscpilot01:Date_20</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_SP1  time:hasEnd  cdiscpilot01:Date_31</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_SP1  time:hasEnd  cdiscpilot01:Date_30</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_PA1  time:hasBeginning  cdiscpilot01:Date_21</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_PA1  time:hasBeginning  cdiscpilot01:Date_20</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:visit_SCREENING1_P1  study:hasSubActivity  cdiscpilot01:vspos_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:visit_SCREENING1_P1  study:hasSubActivity  cdiscpilot01:vspos_2</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:visit_SCREENING1_P1  rdfs:label  SCREENING1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:visit_SCREENING1_P1  study:laterality  https://github.com/phuse-org/SDTMasRDF/blob/master/data/rdf/sdtm-terminology#C99073.C25228</t>
+  </si>
+  <si>
+    <t>NOT IN R?</t>
+  </si>
+  <si>
+    <t>SEE LATERALITY!</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:visit_SCREENING1_P1  study:laterality  https://github.com/phuse-org/SDTMasRDF/blob/master/data/rdf/sdtm-terminology#C99073.C25229</t>
+  </si>
+  <si>
+    <t>See VPOS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">cdiscpilot01:visit_SCREENING1_P1  rdfs:label  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SCREENING1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">cdiscpilot01:visit_SCREENING1_P1  rdfs:label  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Person 1 Visit 1</t>
+    </r>
+  </si>
+  <si>
+    <t>Ont to match R. Is "Visit 1" proper, or show as Screening type of visit?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,8 +528,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -619,12 +725,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -801,7 +901,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -815,21 +915,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1186,10 +1290,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1197,23 +1302,24 @@
     <col min="1" max="1" width="14.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="65.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67" style="5" customWidth="1"/>
-    <col min="7" max="8" width="51.36328125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="49.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70" style="5" customWidth="1"/>
+    <col min="6" max="6" width="67" style="6" customWidth="1"/>
+    <col min="7" max="7" width="61.08984375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="57.08984375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E1" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>72</v>
+      <c r="E1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="13"/>
+      <c r="G1" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1227,10 +1333,10 @@
         <v>46</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>48</v>
@@ -1252,7 +1358,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -1304,17 +1410,17 @@
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="G8" t="s">
-        <v>64</v>
       </c>
       <c r="H8"/>
     </row>
@@ -1329,39 +1435,30 @@
         <v>13</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" t="s">
-        <v>64</v>
-      </c>
-      <c r="H9" s="11">
-        <v>42860</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>49</v>
+        <v>56</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="9">
+        <v>42870</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="E10" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="11">
-        <v>42860</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>59</v>
+        <v>90</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="9">
+        <v>42870</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1374,12 +1471,8 @@
       <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G11" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="11">
-        <v>42860</v>
-      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
@@ -1392,19 +1485,14 @@
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="11">
-        <v>42860</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>53</v>
+        <v>92</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="9">
+        <v>42870</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1441,182 +1529,272 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H16" s="11">
-        <v>42860</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>71</v>
-      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="6"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H17" s="11">
-        <v>42860</v>
+      <c r="B17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B18" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>25</v>
+        <v>63</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="14">
+        <v>42870</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="14">
+        <v>42870</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="E24" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="E25" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D26" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H26" s="14">
+        <v>42870</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D33" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D34" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" s="5" t="s">
+      <c r="G34" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B21" s="3" t="s">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C36" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" t="s">
-        <v>80</v>
-      </c>
-      <c r="F21" t="s">
-        <v>79</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
+      <c r="D36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
         <v>0</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C37" t="s">
         <v>22</v>
       </c>
-      <c r="D22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="12"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B23" t="s">
+      <c r="D37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
         <v>0</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C38" t="s">
         <v>22</v>
       </c>
-      <c r="D23" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="12"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
+      <c r="D38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
         <v>0</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C39" t="s">
         <v>22</v>
       </c>
-      <c r="D24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B25" t="s">
+      <c r="D39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
         <v>0</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C40" t="s">
         <v>22</v>
       </c>
-      <c r="D25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B26" t="s">
+      <c r="D40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
         <v>0</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C41" t="s">
         <v>22</v>
       </c>
-      <c r="D26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="D41" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1705,59 +1883,243 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="5">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" t="s">
-        <v>61</v>
-      </c>
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="5">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="6">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19">
+        <v>129</v>
+      </c>
+      <c r="E19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20">
+        <v>131</v>
+      </c>
+      <c r="E20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21">
+        <v>147</v>
+      </c>
+      <c r="E21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="10"/>
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="10"/>
+      <c r="B23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
code tidy. Vis scripting.
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="96">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -203,9 +203,6 @@
     <t>ProposedFix</t>
   </si>
   <si>
-    <t>Change label in ontology</t>
-  </si>
-  <si>
     <t>(and children)</t>
   </si>
   <si>
@@ -215,21 +212,6 @@
     <t>Child: cdiscpilot01:Interval_PA1</t>
   </si>
   <si>
-    <t>cdiscpilot01:Interval_PA1  time:hasEnd  cdiscpilot01:Date_29</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Interval_PA1  time:hasEnd  cdiscpilot01:Date_30</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Randomization_1rdf:typecode:RandomizationBAL3</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Randomization_1rdf:typecode:Randomization_3</t>
-  </si>
-  <si>
-    <t>Ont to be changed to match R's "BAL3" after 05May email to AO</t>
-  </si>
-  <si>
     <t>Child: custom:visit_1</t>
   </si>
   <si>
@@ -291,24 +273,6 @@
   </si>
   <si>
     <t>bpoutcome_6</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Interval_RI1  time:hasBeginning  cdiscpilot01:Date_21</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Interval_RI1  time:hasBeginning  cdiscpilot01:Date_20</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Interval_SP1  time:hasEnd  cdiscpilot01:Date_31</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Interval_SP1  time:hasEnd  cdiscpilot01:Date_30</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Interval_PA1  time:hasBeginning  cdiscpilot01:Date_21</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Interval_PA1  time:hasBeginning  cdiscpilot01:Date_20</t>
   </si>
   <si>
     <t>cdiscpilot01:visit_SCREENING1_P1  study:hasSubActivity  cdiscpilot01:vspos_1</t>
@@ -367,12 +331,15 @@
   <si>
     <t>Ont to match R. Is "Visit 1" proper, or show as Screening type of visit?</t>
   </si>
+  <si>
+    <t>DateLatestQC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -514,13 +481,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
@@ -536,7 +496,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -725,12 +685,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -901,7 +855,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -915,25 +869,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1290,517 +1243,475 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="70" style="5" customWidth="1"/>
-    <col min="6" max="6" width="67" style="6" customWidth="1"/>
-    <col min="7" max="7" width="61.08984375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="57.08984375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70" style="5" customWidth="1"/>
+    <col min="7" max="7" width="67" style="6" customWidth="1"/>
+    <col min="8" max="8" width="61.08984375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="57.08984375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E1" s="12" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F1" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="15"/>
+      <c r="H1" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="8">
+        <v>42872</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="8">
+        <v>42873</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="8">
+        <v>42872</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="8">
+        <v>42872</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="8"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="8">
+        <v>42873</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="8">
+        <v>42873</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="9">
+      <c r="I17" s="11"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="8">
+        <v>42872</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="F22" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="F23" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="11">
         <v>42870</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H10" s="9">
-        <v>42870</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="9">
-        <v>42870</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="E34" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="E35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18" s="14">
-        <v>42870</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H19" s="14">
-        <v>42870</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="E36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="E37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D22" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D23" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="E24" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="E25" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D26" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="H26" s="14">
-        <v>42870</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="D33" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="D34" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="E35" s="10"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B36" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="E38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
         <v>22</v>
       </c>
-      <c r="D36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E36" s="10"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B40" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B41" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" t="s">
-        <v>22</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="E39" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1938,7 +1849,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
         <v>51</v>
@@ -1949,69 +1860,69 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
         <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
         <v>51</v>
@@ -2022,24 +1933,24 @@
         <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B16" s="5">
         <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D16">
         <v>57</v>
@@ -2047,13 +1958,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B17" s="5">
         <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D17">
         <v>64</v>
@@ -2061,13 +1972,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B18" s="6">
         <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D18">
         <v>83</v>
@@ -2077,45 +1988,45 @@
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D19">
         <v>129</v>
       </c>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D20">
         <v>131</v>
       </c>
       <c r="E20" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D21">
         <v>147</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="10"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="10"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DM and SUPPDM triples in cdiscpilot01 namespace all correct (1st level triples off Person_1 validated).  Next: VS
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="111">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -207,9 +207,6 @@
   </si>
   <si>
     <t>Reported</t>
-  </si>
-  <si>
-    <t>Child: cdiscpilot01:Interval_PA1</t>
   </si>
   <si>
     <t>Child: custom:visit_1</t>
@@ -334,12 +331,60 @@
   <si>
     <t>DateLatestQC</t>
   </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>SUPPDM</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Date_6</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Date_20</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Date_29</t>
+  </si>
+  <si>
+    <t>In R not Ont</t>
+  </si>
+  <si>
+    <t>In Ont not R</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Investigator_123</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Date_30</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_IC1</t>
+  </si>
+  <si>
+    <t>CHILD</t>
+  </si>
+  <si>
+    <t>CHILD-CHILD</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_PA1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Date_20rdf:typestudy:StudyParticipationBegin</t>
+  </si>
+  <si>
+    <t>Checking does not extend past the cdiscpilot01 namespace. No checking of code:, custom:, study: etc.</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:sponsor_STUDYSPONSOR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,8 +540,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -694,8 +753,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -810,6 +881,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -855,7 +935,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -887,6 +967,14 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1243,11 +1331,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1257,28 +1345,32 @@
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70" style="5" customWidth="1"/>
-    <col min="7" max="7" width="67" style="6" customWidth="1"/>
-    <col min="8" max="8" width="61.08984375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="57.08984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="7.81640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="70" style="5" customWidth="1"/>
+    <col min="8" max="8" width="67" style="6" customWidth="1"/>
+    <col min="9" max="9" width="61.08984375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="57.08984375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F1" s="14" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="15"/>
+      <c r="I1" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -1290,16 +1382,19 @@
         <v>46</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>47</v>
       </c>
@@ -1313,7 +1408,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>60</v>
       </c>
@@ -1327,7 +1422,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1338,7 +1433,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1349,7 +1444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1360,7 +1455,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <v>42872</v>
       </c>
@@ -1373,345 +1468,581 @@
       <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F8"/>
-      <c r="G8" s="4"/>
+      <c r="G8"/>
       <c r="H8" s="4"/>
-      <c r="I8"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="8">
+      <c r="I8" s="4"/>
+      <c r="J8"/>
+    </row>
+    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11"/>
+      <c r="D9" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11"/>
+      <c r="D10" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10"/>
+      <c r="I10" s="6"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="8">
         <v>42873</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C11" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="8">
+      <c r="I11" s="4"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="8">
         <v>42872</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C14" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="8">
+      <c r="I14" s="4"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="8">
         <v>42872</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C16" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D16" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F11"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C12" s="1" t="s">
+      <c r="G16"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C19" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D19" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C13" s="1" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C20" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C14" s="1" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C21" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D21" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C15" s="1" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C22" s="9"/>
+      <c r="D22" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C23" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D23" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="8"/>
-      <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="8">
+      <c r="J23" s="8"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C24" s="9"/>
+      <c r="D24" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H24" s="5"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C25" s="9"/>
+      <c r="D25" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" s="5"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" s="8">
         <v>42873</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C26" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D26" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="8">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" s="8">
         <v>42873</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
+      <c r="C27" s="9"/>
+      <c r="D27" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H28" t="s">
+        <v>108</v>
+      </c>
+      <c r="J28" s="11"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" s="8"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J29" s="11"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" s="8">
+        <v>42872</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E32" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="E33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="G34" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="G35" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="E36" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="J36" s="11">
+        <v>42870</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="E37" s="9"/>
+      <c r="G37" s="9"/>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="E38" s="9"/>
+      <c r="G38" s="9"/>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="E39" s="9"/>
+      <c r="G39" s="9"/>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="E40" s="9"/>
+      <c r="G40" s="9"/>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="E41" s="9"/>
+      <c r="G41" s="9"/>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="E42" s="9"/>
+      <c r="G42" s="9"/>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="E43" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I17" s="11"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="8">
-        <v>42872</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="G43" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="E44" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="G45" s="9"/>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C46" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D46" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18"/>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C19" t="s">
+      <c r="E46" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G46" s="9"/>
+    </row>
+    <row r="47" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="D47" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G47" s="9"/>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C48" t="s">
         <v>0</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D48" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E20" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="F22" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="F23" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E24" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="I24" s="11">
-        <v>42870</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E32" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C34" t="s">
+      <c r="E48" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="D49" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C50" t="s">
         <v>0</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D50" t="s">
         <v>22</v>
       </c>
-      <c r="E34" t="s">
-        <v>29</v>
-      </c>
-      <c r="F34" s="9"/>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C35" t="s">
+      <c r="E50" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="D51" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C52" t="s">
         <v>0</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D52" t="s">
         <v>22</v>
       </c>
-      <c r="E35" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C36" t="s">
+      <c r="E52" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="D53" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C54" t="s">
         <v>0</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D54" t="s">
         <v>22</v>
       </c>
-      <c r="E36" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C37" t="s">
+      <c r="E54" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="D55" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C56" t="s">
         <v>0</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D56" t="s">
         <v>22</v>
       </c>
-      <c r="E37" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C38" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C39" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" t="s">
-        <v>22</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="E56" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="D57" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1849,7 +2180,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
         <v>51</v>
@@ -1860,55 +2191,55 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
         <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -1917,12 +2248,12 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
         <v>51</v>
@@ -1933,24 +2264,24 @@
         <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" s="5">
         <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D16">
         <v>57</v>
@@ -1958,13 +2289,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" s="5">
         <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17">
         <v>64</v>
@@ -1972,13 +2303,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18" s="6">
         <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18">
         <v>83</v>
@@ -1988,37 +2319,37 @@
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19">
         <v>129</v>
       </c>
       <c r="E19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D20">
         <v>131</v>
       </c>
       <c r="E20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21">
         <v>147</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
cdiscpilot01:visit_SCREENING1_P1 level complete. Create/QC the Child Triples
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="112">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -35,9 +35,6 @@
     <t>rdfs:label</t>
   </si>
   <si>
-    <t>Person,1^^xsd:string</t>
-  </si>
-  <si>
     <t>study:actualArm</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
   </si>
   <si>
     <t>study:deathFlag</t>
-  </si>
-  <si>
-    <t>Y^^xsd:string</t>
   </si>
   <si>
     <t>study:hasLifespan</t>
@@ -378,6 +372,15 @@
   </si>
   <si>
     <t>cdiscpilot01:sponsor_STUDYSPONSOR</t>
+  </si>
+  <si>
+    <t>SUPPDM/Hardcoded</t>
+  </si>
+  <si>
+    <t>"Person 1"</t>
+  </si>
+  <si>
+    <t>"Y"</t>
   </si>
 </sst>
 </file>
@@ -1334,8 +1337,8 @@
   <dimension ref="A1:K57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
+      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1345,7 +1348,7 @@
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.81640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.1796875" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="70" style="5" customWidth="1"/>
     <col min="8" max="8" width="67" style="6" customWidth="1"/>
     <col min="9" max="9" width="61.08984375" style="6" customWidth="1"/>
@@ -1355,48 +1358,48 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H1" s="15"/>
       <c r="I1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
         <v>44</v>
       </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -1410,7 +1413,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
@@ -1419,7 +1422,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -1427,10 +1430,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -1438,10 +1441,10 @@
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -1449,10 +1452,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -1463,10 +1466,10 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G8"/>
       <c r="H8" s="4"/>
@@ -1476,10 +1479,10 @@
     <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
       <c r="D9" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -1488,10 +1491,10 @@
     <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11"/>
       <c r="D10" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G10"/>
       <c r="I10" s="6"/>
@@ -1505,10 +1508,10 @@
         <v>0</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="8"/>
@@ -1517,10 +1520,10 @@
       <c r="A12" s="8"/>
       <c r="C12" s="9"/>
       <c r="D12" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="8"/>
@@ -1529,10 +1532,10 @@
       <c r="A13" s="8"/>
       <c r="C13" s="9"/>
       <c r="D13" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="8"/>
@@ -1545,10 +1548,10 @@
         <v>0</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="8"/>
@@ -1557,10 +1560,10 @@
       <c r="A15" s="8"/>
       <c r="C15" s="9"/>
       <c r="D15" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="8"/>
@@ -1573,10 +1576,10 @@
         <v>0</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G16"/>
       <c r="H16" s="4"/>
@@ -1587,10 +1590,10 @@
       <c r="A17" s="8"/>
       <c r="C17" s="9"/>
       <c r="D17" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="4"/>
@@ -1601,10 +1604,10 @@
       <c r="A18" s="8"/>
       <c r="C18" s="9"/>
       <c r="D18" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G18"/>
       <c r="H18" s="4"/>
@@ -1616,10 +1619,10 @@
         <v>0</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -1627,10 +1630,10 @@
         <v>0</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -1638,19 +1641,19 @@
         <v>0</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C22" s="9"/>
       <c r="D22" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G22" s="6"/>
     </row>
@@ -1659,10 +1662,10 @@
         <v>0</v>
       </c>
       <c r="D23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="6"/>
@@ -1670,10 +1673,10 @@
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
       <c r="D24" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="18"/>
@@ -1683,10 +1686,10 @@
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
       <c r="D25" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="19"/>
@@ -1701,10 +1704,10 @@
         <v>0</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -1713,10 +1716,10 @@
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="J27" s="11"/>
     </row>
@@ -1724,13 +1727,13 @@
       <c r="A28" s="8"/>
       <c r="C28" s="9"/>
       <c r="D28" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" t="s">
         <v>106</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H28" t="s">
-        <v>108</v>
       </c>
       <c r="J28" s="11"/>
     </row>
@@ -1738,10 +1741,10 @@
       <c r="A29" s="8"/>
       <c r="C29" s="9"/>
       <c r="D29" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J29" s="11"/>
     </row>
@@ -1753,10 +1756,10 @@
         <v>0</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G30"/>
       <c r="H30" s="4"/>
@@ -1766,68 +1769,68 @@
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E32" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.35">
       <c r="E33" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G33" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="34" spans="3:10" ht="29" x14ac:dyDescent="0.35">
       <c r="G34" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="3:10" ht="29" x14ac:dyDescent="0.35">
       <c r="G35" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.35">
       <c r="E36" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G36" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I36" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="H36" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="J36" s="11">
         <v>42870</v>
@@ -1859,30 +1862,30 @@
     </row>
     <row r="43" spans="3:10" x14ac:dyDescent="0.35">
       <c r="E43" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H43" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="I43" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="44" spans="3:10" x14ac:dyDescent="0.35">
       <c r="E44" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H44" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I44" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="45" spans="3:10" x14ac:dyDescent="0.35">
@@ -1893,25 +1896,25 @@
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G46" s="9"/>
     </row>
     <row r="47" spans="3:10" x14ac:dyDescent="0.35">
       <c r="D47" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="G47" s="9"/>
     </row>
@@ -1920,24 +1923,24 @@
         <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D49" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.35">
@@ -1945,24 +1948,24 @@
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D51" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.35">
@@ -1970,24 +1973,24 @@
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D53" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.35">
@@ -1995,24 +1998,24 @@
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D55" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.35">
@@ -2020,24 +2023,24 @@
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D57" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2066,55 +2069,55 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2140,106 +2143,106 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" t="s">
         <v>70</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
         <v>72</v>
-      </c>
-      <c r="C9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" t="s">
-        <v>75</v>
-      </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" t="s">
-        <v>76</v>
-      </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -2248,40 +2251,40 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B16" s="5">
         <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D16">
         <v>57</v>
@@ -2289,13 +2292,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B17" s="5">
         <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D17">
         <v>64</v>
@@ -2303,13 +2306,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B18" s="6">
         <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D18">
         <v>83</v>
@@ -2319,37 +2322,37 @@
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D19">
         <v>129</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D20">
         <v>131</v>
       </c>
       <c r="E20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D21">
         <v>147</v>
       </c>
       <c r="E21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
data imputation to match AO.  Moved most imputation from process scripts to build script.
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="106">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -266,63 +266,6 @@
     <t>bpoutcome_6</t>
   </si>
   <si>
-    <t>cdiscpilot01:visit_SCREENING1_P1  study:hasSubActivity  cdiscpilot01:vspos_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:visit_SCREENING1_P1  study:hasSubActivity  cdiscpilot01:vspos_2</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:visit_SCREENING1_P1  rdfs:label  SCREENING1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:visit_SCREENING1_P1  study:laterality  https://github.com/phuse-org/SDTMasRDF/blob/master/data/rdf/sdtm-terminology#C99073.C25228</t>
-  </si>
-  <si>
-    <t>NOT IN R?</t>
-  </si>
-  <si>
-    <t>SEE LATERALITY!</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:visit_SCREENING1_P1  study:laterality  https://github.com/phuse-org/SDTMasRDF/blob/master/data/rdf/sdtm-terminology#C99073.C25229</t>
-  </si>
-  <si>
-    <t>See VPOS</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">cdiscpilot01:visit_SCREENING1_P1  rdfs:label  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SCREENING1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">cdiscpilot01:visit_SCREENING1_P1  rdfs:label  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Person 1 Visit 1</t>
-    </r>
-  </si>
-  <si>
-    <t>Ont to match R. Is "Visit 1" proper, or show as Screening type of visit?</t>
-  </si>
-  <si>
     <t>DateLatestQC</t>
   </si>
   <si>
@@ -381,6 +324,21 @@
   </si>
   <si>
     <t>"Y"</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:AssumeBodyPositionStanding_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:AssumeBodyPositionSupine_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:DBP_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:DBP_3</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:DBP_2</t>
   </si>
 </sst>
 </file>
@@ -537,13 +495,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="7"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
@@ -556,6 +507,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="38">
@@ -938,7 +895,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -965,20 +922,24 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1336,9 +1297,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1358,12 +1319,12 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G1" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="15"/>
+      <c r="H1" s="19"/>
       <c r="I1" s="12" t="s">
         <v>57</v>
       </c>
@@ -1373,7 +1334,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
         <v>42</v>
@@ -1385,13 +1346,13 @@
         <v>44</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>99</v>
+        <v>82</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>46</v>
@@ -1422,7 +1383,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -1455,13 +1416,11 @@
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="8">
-        <v>42872</v>
-      </c>
+      <c r="A8" s="8"/>
       <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1478,11 +1437,11 @@
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
-      <c r="D9" s="17" t="s">
-        <v>103</v>
+      <c r="D9" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -1490,8 +1449,8 @@
     </row>
     <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11"/>
-      <c r="D10" s="17" t="s">
-        <v>103</v>
+      <c r="D10" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>39</v>
@@ -1501,9 +1460,7 @@
       <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="8">
-        <v>42873</v>
-      </c>
+      <c r="A11" s="8"/>
       <c r="C11" s="9" t="s">
         <v>0</v>
       </c>
@@ -1519,11 +1476,11 @@
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="17" t="s">
-        <v>103</v>
+      <c r="D12" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="8"/>
@@ -1531,19 +1488,17 @@
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="17" t="s">
-        <v>103</v>
+      <c r="D13" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="8">
-        <v>42872</v>
-      </c>
+      <c r="A14" s="8"/>
       <c r="C14" s="9" t="s">
         <v>0</v>
       </c>
@@ -1559,19 +1514,17 @@
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="8"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="17" t="s">
-        <v>103</v>
+      <c r="D15" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="8">
-        <v>42872</v>
-      </c>
+      <c r="A16" s="8"/>
       <c r="C16" s="9" t="s">
         <v>0</v>
       </c>
@@ -1589,8 +1542,8 @@
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="17" t="s">
-        <v>103</v>
+      <c r="D17" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>39</v>
@@ -1603,11 +1556,11 @@
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="17" t="s">
-        <v>103</v>
+      <c r="D18" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="G18"/>
       <c r="H18" s="4"/>
@@ -1649,8 +1602,8 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C22" s="9"/>
-      <c r="D22" s="17" t="s">
-        <v>103</v>
+      <c r="D22" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>39</v>
@@ -1672,34 +1625,32 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
-      <c r="D24" s="17" t="s">
-        <v>103</v>
+      <c r="D24" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="H24" s="5"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
       <c r="K24" s="6"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
-      <c r="D25" s="17" t="s">
-        <v>104</v>
+      <c r="D25" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H25" s="5"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="8">
-        <v>42873</v>
-      </c>
+      <c r="A26" s="8"/>
       <c r="C26" s="9" t="s">
         <v>0</v>
       </c>
@@ -1711,40 +1662,38 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="8">
-        <v>42873</v>
-      </c>
+      <c r="A27" s="8"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="17" t="s">
-        <v>103</v>
+      <c r="D27" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="J27" s="11"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="8"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="17" t="s">
-        <v>104</v>
+      <c r="D28" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="H28" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="8"/>
       <c r="C29" s="9"/>
-      <c r="D29" s="17" t="s">
-        <v>104</v>
+      <c r="D29" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="J29" s="11"/>
     </row>
@@ -1765,83 +1714,76 @@
       <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" s="20">
+        <v>42881</v>
+      </c>
       <c r="C31" t="s">
         <v>0</v>
       </c>
       <c r="D31" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G31" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>86</v>
-      </c>
+      <c r="G31" s="9"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E32" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>86</v>
+      <c r="D32" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="E33" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="3:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="G34" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="3:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="G35" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>87</v>
-      </c>
+      <c r="D33" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="D34" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="G34" s="9"/>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="D35" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="G35" s="9"/>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="E36" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="H36" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="J36" s="11">
-        <v>42870</v>
-      </c>
+      <c r="D36" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="G36" s="9"/>
+      <c r="H36" s="13"/>
+      <c r="J36" s="11"/>
     </row>
     <row r="37" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="E37" s="9"/>
+      <c r="D37" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>104</v>
+      </c>
       <c r="G37" s="9"/>
     </row>
     <row r="38" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="E38" s="9"/>
+      <c r="E38" s="22"/>
       <c r="G38" s="9"/>
     </row>
     <row r="39" spans="3:10" x14ac:dyDescent="0.35">
@@ -1902,19 +1844,19 @@
         <v>27</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="G46" s="9"/>
     </row>
     <row r="47" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="D47" s="17" t="s">
-        <v>103</v>
+      <c r="D47" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="G47" s="9"/>
     </row>
@@ -1929,18 +1871,18 @@
         <v>25</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="D49" s="17" t="s">
-        <v>103</v>
+      <c r="D49" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.35">
@@ -1954,18 +1896,18 @@
         <v>26</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="D51" s="17" t="s">
-        <v>103</v>
+      <c r="D51" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.35">
@@ -1979,18 +1921,18 @@
         <v>28</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="D53" s="17" t="s">
-        <v>103</v>
+      <c r="D53" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.35">
@@ -2004,18 +1946,18 @@
         <v>29</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="D55" s="17" t="s">
-        <v>103</v>
+      <c r="D55" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.35">
@@ -2029,18 +1971,18 @@
         <v>30</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="D57" s="17" t="s">
-        <v>103</v>
+      <c r="D57" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit prior to merge, prior to repo rename
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="140">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>study:hasSite</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:site_701</t>
   </si>
   <si>
     <t>study:hasStudyParticipationInterval</t>
@@ -363,12 +360,6 @@
     <t>change from</t>
   </si>
   <si>
-    <t>Interval_LS1</t>
-  </si>
-  <si>
-    <t>Interval_RI1</t>
-  </si>
-  <si>
     <t>cdiscpilot01:Site_1</t>
   </si>
   <si>
@@ -445,6 +436,12 @@
   </si>
   <si>
     <t>cdiscpilot01:BloodPressureOutcome_3</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>TO HERE. Questions about namespace and casing sent to AO</t>
   </si>
 </sst>
 </file>
@@ -1123,7 +1120,161 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="27">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1471,9 +1622,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1495,49 +1646,49 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J1" s="20"/>
       <c r="K1" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" t="s">
         <v>97</v>
       </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G2" t="s">
-        <v>98</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -1545,7 +1696,7 @@
         <v>42886</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>0</v>
@@ -1564,7 +1715,7 @@
         <v>42886</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>0</v>
@@ -1573,13 +1724,15 @@
         <v>3</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
+      <c r="A5" s="6">
+        <v>42886</v>
+      </c>
       <c r="C5" s="7" t="s">
         <v>0</v>
       </c>
@@ -1587,13 +1740,15 @@
         <v>4</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="6"/>
+      <c r="A6" s="6">
+        <v>42886</v>
+      </c>
       <c r="C6" s="7" t="s">
         <v>0</v>
       </c>
@@ -1601,13 +1756,15 @@
         <v>5</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="6"/>
+      <c r="A7" s="6">
+        <v>42886</v>
+      </c>
       <c r="C7" s="7" t="s">
         <v>0</v>
       </c>
@@ -1615,25 +1772,25 @@
         <v>6</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="6"/>
+      <c r="A8" s="6">
+        <v>42886</v>
+      </c>
       <c r="C8" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>113</v>
-      </c>
+      <c r="E8" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" s="22"/>
       <c r="G8" s="7"/>
       <c r="I8"/>
       <c r="J8" s="2"/>
@@ -1641,155 +1798,187 @@
       <c r="L8"/>
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
+      <c r="A9" s="6">
+        <v>42886</v>
+      </c>
       <c r="C9" s="7"/>
       <c r="D9" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6"/>
+      <c r="A10" s="6">
+        <v>42886</v>
+      </c>
       <c r="C10" s="7"/>
       <c r="D10" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I10"/>
       <c r="K10" s="4"/>
       <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="6"/>
+      <c r="A11" s="6">
+        <v>42886</v>
+      </c>
       <c r="C11" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>114</v>
-      </c>
+      <c r="E11" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11" s="22"/>
       <c r="G11" s="7"/>
       <c r="K11" s="2"/>
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="6"/>
+      <c r="A12" s="6">
+        <v>42886</v>
+      </c>
       <c r="C12" s="7"/>
       <c r="D12" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="6"/>
+      <c r="A13" s="6">
+        <v>42886</v>
+      </c>
       <c r="C13" s="7"/>
       <c r="D13" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="6"/>
+      <c r="A14" s="6">
+        <v>42886</v>
+      </c>
       <c r="C14" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="E14" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14" s="7"/>
       <c r="G14" s="7"/>
+      <c r="H14" s="7" t="s">
+        <v>138</v>
+      </c>
       <c r="K14" s="2"/>
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="6"/>
+      <c r="A15" s="6">
+        <v>42886</v>
+      </c>
       <c r="C15" s="7"/>
       <c r="D15" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>116</v>
+        <v>82</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G15" s="7"/>
+      <c r="H15" s="7" t="s">
+        <v>138</v>
+      </c>
       <c r="K15" s="2"/>
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="6"/>
+      <c r="A16" s="6">
+        <v>42886</v>
+      </c>
       <c r="C16" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="G16" s="7"/>
+      <c r="H16" s="7" t="s">
+        <v>138</v>
+      </c>
       <c r="I16"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="6"/>
+      <c r="A17" s="6">
+        <v>42886</v>
+      </c>
       <c r="C17" s="7"/>
       <c r="D17" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="2"/>
@@ -1797,17 +1986,22 @@
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="6"/>
+      <c r="A18" s="6">
+        <v>42886</v>
+      </c>
       <c r="C18" s="7"/>
       <c r="D18" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="I18"/>
       <c r="J18" s="2"/>
@@ -1815,123 +2009,163 @@
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="6"/>
+      <c r="A19" s="6">
+        <v>42886</v>
+      </c>
       <c r="C19" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
+      <c r="H19" s="7" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="6"/>
+      <c r="A20" s="6">
+        <v>42886</v>
+      </c>
       <c r="C20" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
+      <c r="H20" s="7" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="6"/>
+      <c r="A21" s="6">
+        <v>42886</v>
+      </c>
       <c r="C21" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
+      <c r="H21" s="7" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="6"/>
+      <c r="A22" s="6">
+        <v>42886</v>
+      </c>
       <c r="C22" s="7"/>
       <c r="D22" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="6"/>
+      <c r="A23" s="6">
+        <v>42886</v>
+      </c>
       <c r="C23" s="7"/>
       <c r="D23" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>119</v>
+        <v>82</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>116</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
+      <c r="H23" s="7" t="s">
+        <v>138</v>
+      </c>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="6"/>
+      <c r="A24" s="6">
+        <v>42886</v>
+      </c>
       <c r="C24" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>118</v>
+        <v>18</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G24" s="7"/>
+      <c r="H24" s="7" t="s">
+        <v>138</v>
+      </c>
       <c r="L24" s="6"/>
       <c r="M24" s="4"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
+      <c r="A25" s="6">
+        <v>42886</v>
+      </c>
       <c r="C25" s="7"/>
       <c r="D25" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>120</v>
+        <v>82</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G25" s="7"/>
+      <c r="H25" s="7" t="s">
+        <v>138</v>
+      </c>
       <c r="J25" s="3"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
       <c r="M25" s="4"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="6"/>
+      <c r="A26" s="6">
+        <v>42886</v>
+      </c>
       <c r="C26" s="7"/>
       <c r="D26" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="14"/>
@@ -1939,117 +2173,138 @@
       <c r="M26" s="4"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="6">
+        <v>42886</v>
+      </c>
       <c r="C27" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>121</v>
+        <v>18</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>118</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G27" s="7"/>
       <c r="H27" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" s="6">
+        <v>42886</v>
+      </c>
       <c r="C28" s="7"/>
       <c r="D28" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" s="6">
+        <v>42886</v>
+      </c>
       <c r="C29" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" s="6">
+        <v>42886</v>
+      </c>
       <c r="C30" s="7"/>
       <c r="D30" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31" s="6">
+        <v>42886</v>
+      </c>
       <c r="C31" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I31" s="7"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A32" s="6">
+        <v>42886</v>
+      </c>
       <c r="C32" s="7"/>
       <c r="D32" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G32" s="7"/>
       <c r="H32" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I32" s="7"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="6"/>
-      <c r="C33" s="7"/>
+      <c r="B33" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" s="12"/>
       <c r="D33" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G33" s="7"/>
       <c r="J33" s="3"/>
@@ -2058,16 +2313,18 @@
       <c r="M33" s="4"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="6"/>
+      <c r="A34" s="6">
+        <v>42886</v>
+      </c>
       <c r="C34" s="7"/>
       <c r="D34" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G34" s="7"/>
       <c r="J34" s="3"/>
@@ -2079,13 +2336,13 @@
       <c r="A35" s="6"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G35" s="7"/>
       <c r="J35" s="3"/>
@@ -2094,16 +2351,18 @@
       <c r="M35" s="4"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" s="6"/>
+      <c r="A36" s="6">
+        <v>42886</v>
+      </c>
       <c r="C36" s="7"/>
       <c r="D36" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G36" s="7"/>
       <c r="J36" s="3"/>
@@ -2115,13 +2374,13 @@
       <c r="A37" s="6"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G37" s="7"/>
       <c r="J37" s="3"/>
@@ -2130,16 +2389,18 @@
       <c r="M37" s="4"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="6"/>
+      <c r="A38" s="6">
+        <v>42886</v>
+      </c>
       <c r="C38" s="7"/>
       <c r="D38" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G38" s="7"/>
       <c r="J38" s="3"/>
@@ -2153,10 +2414,10 @@
         <v>0</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
@@ -2165,13 +2426,13 @@
       <c r="A40" s="6"/>
       <c r="C40" s="7"/>
       <c r="D40" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L40" s="9"/>
     </row>
@@ -2179,17 +2440,17 @@
       <c r="A41" s="6"/>
       <c r="C41" s="7"/>
       <c r="D41" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L41" s="9"/>
     </row>
@@ -2197,14 +2458,14 @@
       <c r="A42" s="6"/>
       <c r="C42" s="7"/>
       <c r="D42" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L42" s="9"/>
     </row>
@@ -2214,13 +2475,13 @@
         <v>0</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G43" s="7"/>
       <c r="I43"/>
@@ -2232,13 +2493,13 @@
         <v>0</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G44" s="7"/>
       <c r="I44" s="7"/>
@@ -2247,24 +2508,24 @@
       <c r="A45" s="18"/>
       <c r="C45" s="7"/>
       <c r="D45" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="12"/>
       <c r="C46" s="7"/>
       <c r="D46" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F46" s="17"/>
       <c r="G46" s="17"/>
@@ -2273,10 +2534,10 @@
       <c r="A47" s="12"/>
       <c r="C47" s="7"/>
       <c r="D47" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F47" s="17"/>
       <c r="G47" s="17"/>
@@ -2284,10 +2545,10 @@
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C48" s="7"/>
       <c r="D48" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F48" s="17"/>
       <c r="G48" s="17"/>
@@ -2296,10 +2557,10 @@
     <row r="49" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C49" s="7"/>
       <c r="D49" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E49" s="17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F49" s="17"/>
       <c r="G49" s="17"/>
@@ -2308,13 +2569,13 @@
     <row r="50" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C50" s="7"/>
       <c r="D50" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G50" s="17"/>
       <c r="I50" s="7"/>
@@ -2322,10 +2583,10 @@
     <row r="51" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C51" s="7"/>
       <c r="D51" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E51" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F51" s="17"/>
       <c r="G51" s="17"/>
@@ -2334,10 +2595,10 @@
     <row r="52" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C52" s="7"/>
       <c r="D52" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E52" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
@@ -2346,10 +2607,10 @@
     <row r="53" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C53" s="7"/>
       <c r="D53" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E53" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F53" s="17"/>
       <c r="G53" s="17"/>
@@ -2358,13 +2619,13 @@
     <row r="54" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C54" s="7"/>
       <c r="D54" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F54" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G54" s="17"/>
       <c r="I54" s="7"/>
@@ -2374,10 +2635,10 @@
     <row r="55" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C55" s="7"/>
       <c r="D55" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E55" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F55" s="17"/>
       <c r="G55" s="17"/>
@@ -2388,10 +2649,10 @@
     <row r="56" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C56" s="7"/>
       <c r="D56" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E56" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F56" s="17"/>
       <c r="G56" s="17"/>
@@ -2402,10 +2663,10 @@
     <row r="57" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C57" s="7"/>
       <c r="D57" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E57" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F57" s="17"/>
       <c r="G57" s="17"/>
@@ -2416,13 +2677,13 @@
     <row r="58" spans="3:13" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C58" s="24"/>
       <c r="D58" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F58" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G58" s="26"/>
       <c r="H58" s="27"/>
@@ -2435,10 +2696,10 @@
     <row r="59" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C59" s="7"/>
       <c r="D59" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E59" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F59" s="15"/>
       <c r="G59" s="15"/>
@@ -2447,10 +2708,10 @@
     <row r="60" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C60" s="7"/>
       <c r="D60" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E60" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
@@ -2459,10 +2720,10 @@
     <row r="61" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C61" s="7"/>
       <c r="D61" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E61" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
@@ -2577,29 +2838,139 @@
   <mergeCells count="1">
     <mergeCell ref="I1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3 A5:A26 A33:A39">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
+  <conditionalFormatting sqref="A3 A33 A35 A37 A39">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="28">
       <formula>LEN(TRIM(A3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:A42">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="26">
       <formula>LEN(TRIM(A40))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="25">
       <formula>LEN(TRIM(A43))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="24">
       <formula>LEN(TRIM(A44))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="23">
+      <formula>LEN(TRIM(A4))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:A10">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="22">
+      <formula>LEN(TRIM(A5))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11:A13">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="21">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="20">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="19">
+      <formula>LEN(TRIM(A15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="18">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="17">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="16">
+      <formula>LEN(TRIM(A18))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
+      <formula>LEN(TRIM(A19))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
+      <formula>LEN(TRIM(A21))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
+      <formula>LEN(TRIM(A22))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24:A26">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
+      <formula>LEN(TRIM(A24))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(A36))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(A38))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(A28))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(A27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(A29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A4))&gt;0</formula>
+      <formula>LEN(TRIM(A31))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2624,55 +2995,55 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
         <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
         <v>34</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
         <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2698,106 +3069,106 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -2806,40 +3177,40 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" s="3">
         <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16">
         <v>57</v>
@@ -2847,13 +3218,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="3">
         <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17">
         <v>64</v>
@@ -2861,13 +3232,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" s="4">
         <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D18">
         <v>83</v>
@@ -2877,37 +3248,37 @@
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19">
         <v>129</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20">
         <v>131</v>
       </c>
       <c r="E20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21">
         <v>147</v>
       </c>
       <c r="E21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
scripting work in progress
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_gitHub\SDTMasRDF\r\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_gitHub\CTDasRDF\r\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="122">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -38,9 +38,6 @@
     <t>study:actualArm</t>
   </si>
   <si>
-    <t>study:allocatedToArm</t>
-  </si>
-  <si>
     <t>study:deathFlag</t>
   </si>
   <si>
@@ -83,36 +80,9 @@
     <t>cdiscpilot01:DemographicDataCollection_1</t>
   </si>
   <si>
-    <t>cdiscpilot01:InformedConsent_1</t>
-  </si>
-  <si>
     <t>cdiscpilot01:ProductAdministration_1</t>
   </si>
   <si>
-    <t>cdiscpilot01:Randomization_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:popflag_C16WK_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:popflag_C24WK_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:popflag_C8WK_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:popflag_EFF_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:popflag_ITT_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:popflag_SAF_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:visit_SCREENING1_P1</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
@@ -266,27 +236,15 @@
     <t>cdiscpilot01:Date_30</t>
   </si>
   <si>
-    <t>cdiscpilot01:Interval_IC1</t>
-  </si>
-  <si>
     <t>CHILD</t>
   </si>
   <si>
     <t>CHILD-CHILD</t>
   </si>
   <si>
-    <t>cdiscpilot01:Interval_PA1</t>
-  </si>
-  <si>
     <t>cdiscpilot01:Date_20rdf:typestudy:StudyParticipationBegin</t>
   </si>
   <si>
-    <t>Checking does not extend past the cdiscpilot01 namespace. No checking of code:, custom:, study: etc.</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:sponsor_STUDYSPONSOR</t>
-  </si>
-  <si>
     <t>SUPPDM/Hardcoded</t>
   </si>
   <si>
@@ -300,15 +258,6 @@
   </si>
   <si>
     <t>cdiscpilot01:AssumeBodyPositionSupine_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:DBP_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:DBP_3</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:DBP_2</t>
   </si>
   <si>
     <t>Date
@@ -318,12 +267,6 @@
     <t>Additional Check(s)</t>
   </si>
   <si>
-    <t>Date Context (start interval): study:Birthdate</t>
-  </si>
-  <si>
-    <t>Date Context (end interval): study:Deathdate</t>
-  </si>
-  <si>
     <t>Date: study:ProductAdministationBegin</t>
   </si>
   <si>
@@ -336,21 +279,9 @@
     <t>Date: study:StudyParticipationEnd</t>
   </si>
   <si>
-    <t>Date: study:DemogDataCollectionDate</t>
-  </si>
-  <si>
-    <t>Date: study:InformedConsentBegin</t>
-  </si>
-  <si>
     <t>Date: study:ProductAdministrationBegin</t>
   </si>
   <si>
-    <t>AO Question 30MAy17: Does  Date_19 need Type ScreeningDate?</t>
-  </si>
-  <si>
-    <t>question out to AO</t>
-  </si>
-  <si>
     <t>cdiscpilot01:Lifespan_1</t>
   </si>
   <si>
@@ -441,7 +372,22 @@
     <t>DM</t>
   </si>
   <si>
-    <t>TO HERE. Questions about namespace and casing sent to AO</t>
+    <t>cd01p:ArmPlacebo</t>
+  </si>
+  <si>
+    <t>Date_19 is lacking a type:  study:VisitDate. Where is this created?</t>
+  </si>
+  <si>
+    <t>Checking does not extend past the cdiscpilot01 namespace. No checking of code:, cd01p, study, etc.</t>
+  </si>
+  <si>
+    <t>ERROR in ONT. Email to AO 2017-06-15</t>
+  </si>
+  <si>
+    <t>TO HERE</t>
+  </si>
+  <si>
+    <t>question to AO 2017-06-15: EFF/SAF/ITT to code: or cd01p: ??</t>
   </si>
 </sst>
 </file>
@@ -646,7 +592,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -847,6 +793,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1020,7 +984,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1056,13 +1020,6 @@
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1075,6 +1032,18 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1120,7 +1089,140 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="46">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1620,11 +1722,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M76"/>
+  <dimension ref="A1:M75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+      <pane ySplit="2" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1646,57 +1748,57 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="28"/>
+      <c r="K1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="10" t="s">
-        <v>55</v>
-      </c>
       <c r="L1" s="5" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="G2" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
-        <v>42886</v>
+        <v>42901</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>0</v>
@@ -1712,10 +1814,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
-        <v>42886</v>
+        <v>42901</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>0</v>
@@ -1724,14 +1826,14 @@
         <v>3</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
-        <v>42886</v>
+        <v>42901</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>0</v>
@@ -1739,15 +1841,15 @@
       <c r="D5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="F5" s="21"/>
+      <c r="E5" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
-        <v>42886</v>
+        <v>42901</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>0</v>
@@ -1755,15 +1857,15 @@
       <c r="D6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="F6" s="21"/>
+      <c r="E6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
-        <v>42886</v>
+        <v>42901</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>0</v>
@@ -1772,540 +1874,511 @@
         <v>6</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" s="7"/>
+        <v>86</v>
+      </c>
+      <c r="F7" s="19"/>
       <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I7"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7"/>
+    </row>
+    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>7</v>
+        <v>42901</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F8" s="22"/>
+        <v>64</v>
+      </c>
+      <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="I8"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
-        <v>42886</v>
-      </c>
+      <c r="A9" s="6"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>74</v>
+      <c r="D9" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="J9" s="4"/>
+        <v>117</v>
+      </c>
+      <c r="I9"/>
       <c r="K9" s="4"/>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="16" t="s">
-        <v>82</v>
+        <v>42901</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="I10"/>
-      <c r="K10" s="4"/>
-      <c r="M10" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="7"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>9</v>
+        <v>42901</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="7"/>
+        <v>65</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>115</v>
+      </c>
       <c r="K11" s="2"/>
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
-        <v>42886</v>
+        <v>42901</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="16" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="16" t="s">
-        <v>82</v>
+        <v>42901</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="F13" s="7"/>
-      <c r="G13" s="7" t="s">
-        <v>101</v>
-      </c>
+      <c r="G13" s="7"/>
       <c r="H13" s="7" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>11</v>
+        <v>42901</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F14" s="7"/>
+        <v>90</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="16" t="s">
-        <v>82</v>
+        <v>42901</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7" t="s">
-        <v>138</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="I15"/>
+      <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="7"/>
+      <c r="A16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>83</v>
+      </c>
       <c r="H16" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="I16"/>
+        <v>115</v>
+      </c>
+      <c r="I16" s="4"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
-        <v>42886</v>
+        <v>42901</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="16" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="I17" s="4"/>
+        <v>115</v>
+      </c>
+      <c r="I17"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="16" t="s">
-        <v>82</v>
+        <v>42901</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="F18" s="7"/>
-      <c r="G18" s="7" t="s">
-        <v>103</v>
-      </c>
+      <c r="G18" s="7"/>
       <c r="H18" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="I18"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="6"/>
+        <v>115</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
-        <v>42886</v>
+        <v>42901</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
-        <v>42886</v>
+        <v>42901</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>18</v>
+        <v>42901</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
-      <c r="H21" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="6">
-        <v>42886</v>
-      </c>
+      <c r="A22" s="30"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>37</v>
+      <c r="D22" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="F22" s="7"/>
-      <c r="G22" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="16" t="s">
-        <v>82</v>
+        <v>42901</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>115</v>
+      </c>
+      <c r="L23" s="6"/>
+      <c r="M23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>18</v>
+        <v>42901</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>20</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="L24" s="6"/>
+        <v>115</v>
+      </c>
+      <c r="J24" s="3"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
       <c r="M24" s="4"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="6">
-        <v>42886</v>
-      </c>
+      <c r="A25" s="6"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>81</v>
-      </c>
+      <c r="D25" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="7"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="J25" s="3"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
       <c r="M25" s="4"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="16" t="s">
-        <v>83</v>
+        <v>42901</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="F26" s="7"/>
-      <c r="G26" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="4"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>18</v>
+        <v>42901</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>23</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>87</v>
-      </c>
+        <v>42901</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="3" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>24</v>
-      </c>
+        <v>42901</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" s="22" t="s">
+      <c r="A30" s="31"/>
+      <c r="C30" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="F30" s="7" t="s">
-        <v>87</v>
-      </c>
       <c r="G30" s="7"/>
+      <c r="H30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I30" s="7"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>25</v>
-      </c>
+        <v>42901</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F31" s="7"/>
       <c r="G31" s="7"/>
       <c r="H31" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I31" s="7"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>87</v>
+      <c r="A32" s="32"/>
+      <c r="B32" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F32" s="34" t="s">
+        <v>121</v>
       </c>
       <c r="G32" s="7"/>
-      <c r="H32" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="I32" s="7"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="4"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A33" s="6"/>
-      <c r="B33" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="A33" s="6">
+        <v>42901</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="7"/>
       <c r="G33" s="7"/>
       <c r="J33" s="3"/>
       <c r="K33" s="14"/>
@@ -2313,19 +2386,15 @@
       <c r="M33" s="4"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="6">
-        <v>42886</v>
-      </c>
+      <c r="A34" s="6"/>
       <c r="C34" s="7"/>
-      <c r="D34" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>87</v>
-      </c>
+      <c r="D34" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34" s="7"/>
       <c r="G34" s="7"/>
       <c r="J34" s="3"/>
       <c r="K34" s="14"/>
@@ -2333,17 +2402,17 @@
       <c r="M34" s="4"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" s="6"/>
+      <c r="A35" s="6">
+        <v>42901</v>
+      </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="D35" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F35" s="7"/>
       <c r="G35" s="7"/>
       <c r="J35" s="3"/>
       <c r="K35" s="14"/>
@@ -2351,19 +2420,15 @@
       <c r="M35" s="4"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" s="6">
-        <v>42886</v>
-      </c>
+      <c r="A36" s="6"/>
       <c r="C36" s="7"/>
-      <c r="D36" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>87</v>
-      </c>
+      <c r="D36" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F36" s="7"/>
       <c r="G36" s="7"/>
       <c r="J36" s="3"/>
       <c r="K36" s="14"/>
@@ -2371,17 +2436,17 @@
       <c r="M36" s="4"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="6"/>
+      <c r="A37" s="6">
+        <v>42901</v>
+      </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>28</v>
-      </c>
+      <c r="D37" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F37" s="7"/>
       <c r="G37" s="7"/>
       <c r="J37" s="3"/>
       <c r="K37" s="14"/>
@@ -2389,50 +2454,46 @@
       <c r="M37" s="4"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="6">
-        <v>42886</v>
-      </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>87</v>
-      </c>
+      <c r="A38" s="6"/>
+      <c r="C38" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="7"/>
       <c r="G38" s="7"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="4"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="6"/>
-      <c r="C39" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>21</v>
+      <c r="C39" s="7"/>
+      <c r="D39" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>102</v>
       </c>
       <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
+      <c r="L39" s="9"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="6"/>
       <c r="C40" s="7"/>
       <c r="D40" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E40" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>84</v>
+        <v>72</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" t="s">
+        <v>85</v>
+      </c>
+      <c r="J40" t="s">
+        <v>73</v>
       </c>
       <c r="L40" s="9"/>
     </row>
@@ -2440,34 +2501,32 @@
       <c r="A41" s="6"/>
       <c r="C41" s="7"/>
       <c r="D41" s="16" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F41" s="7"/>
-      <c r="G41" t="s">
-        <v>106</v>
-      </c>
-      <c r="J41" t="s">
-        <v>85</v>
+      <c r="G41" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="L41" s="9"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="6"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>76</v>
+      <c r="C42" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>103</v>
       </c>
       <c r="F42" s="7"/>
-      <c r="G42" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="L42" s="9"/>
+      <c r="G42" s="7"/>
+      <c r="I42"/>
+      <c r="J42" s="2"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="6"/>
@@ -2475,80 +2534,70 @@
         <v>0</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E43" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>22</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="I43"/>
-      <c r="J43" s="2"/>
+      <c r="I43" s="7"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A44" s="6"/>
-      <c r="C44" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E44" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="A44" s="18"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F44" s="7"/>
       <c r="G44" s="7"/>
-      <c r="I44" s="7"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A45" s="18"/>
+      <c r="A45" s="12"/>
       <c r="C45" s="7"/>
       <c r="D45" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7" t="s">
-        <v>107</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="12"/>
       <c r="C46" s="7"/>
       <c r="D46" s="16" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="F46" s="17"/>
       <c r="G46" s="17"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A47" s="12"/>
       <c r="C47" s="7"/>
       <c r="D47" s="16" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
       <c r="F47" s="17"/>
       <c r="G47" s="17"/>
+      <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C48" s="7"/>
       <c r="D48" s="16" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="F48" s="17"/>
       <c r="G48" s="17"/>
@@ -2557,10 +2606,10 @@
     <row r="49" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C49" s="7"/>
       <c r="D49" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E49" s="17" t="s">
-        <v>128</v>
+        <v>71</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>106</v>
       </c>
       <c r="F49" s="17"/>
       <c r="G49" s="17"/>
@@ -2569,24 +2618,22 @@
     <row r="50" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C50" s="7"/>
       <c r="D50" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E50" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="F50" s="17" t="s">
-        <v>93</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="E50" t="s">
+        <v>109</v>
+      </c>
+      <c r="F50" s="17"/>
       <c r="G50" s="17"/>
       <c r="I50" s="7"/>
     </row>
     <row r="51" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C51" s="7"/>
       <c r="D51" s="16" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E51" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="F51" s="17"/>
       <c r="G51" s="17"/>
@@ -2595,10 +2642,10 @@
     <row r="52" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C52" s="7"/>
       <c r="D52" s="16" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E52" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
@@ -2607,26 +2654,26 @@
     <row r="53" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C53" s="7"/>
       <c r="D53" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E53" t="s">
-        <v>133</v>
+        <v>71</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>107</v>
       </c>
       <c r="F53" s="17"/>
       <c r="G53" s="17"/>
       <c r="I53" s="7"/>
+      <c r="J53" s="11"/>
+      <c r="L53" s="9"/>
     </row>
     <row r="54" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C54" s="7"/>
       <c r="D54" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E54" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="F54" s="17" t="s">
-        <v>95</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="E54" t="s">
+        <v>111</v>
+      </c>
+      <c r="F54" s="17"/>
       <c r="G54" s="17"/>
       <c r="I54" s="7"/>
       <c r="J54" s="11"/>
@@ -2635,10 +2682,10 @@
     <row r="55" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C55" s="7"/>
       <c r="D55" s="16" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E55" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="F55" s="17"/>
       <c r="G55" s="17"/>
@@ -2649,10 +2696,10 @@
     <row r="56" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C56" s="7"/>
       <c r="D56" s="16" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E56" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="F56" s="17"/>
       <c r="G56" s="17"/>
@@ -2660,58 +2707,54 @@
       <c r="J56" s="11"/>
       <c r="L56" s="9"/>
     </row>
-    <row r="57" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C57" s="7"/>
-      <c r="D57" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E57" t="s">
-        <v>135</v>
-      </c>
-      <c r="F57" s="17"/>
-      <c r="G57" s="17"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="11"/>
-      <c r="L57" s="9"/>
-    </row>
-    <row r="58" spans="3:13" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C58" s="24"/>
-      <c r="D58" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="E58" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="F58" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="G58" s="26"/>
-      <c r="H58" s="27"/>
-      <c r="I58" s="24"/>
-      <c r="J58" s="28"/>
-      <c r="K58" s="28"/>
-      <c r="L58" s="27"/>
-      <c r="M58" s="29"/>
+    <row r="57" spans="3:13" s="20" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C57" s="21"/>
+      <c r="D57" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="24"/>
+      <c r="I57" s="21"/>
+      <c r="J57" s="25"/>
+      <c r="K57" s="25"/>
+      <c r="L57" s="24"/>
+      <c r="M57" s="26"/>
+    </row>
+    <row r="58" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C58" s="7"/>
+      <c r="D58" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E58" t="s">
+        <v>114</v>
+      </c>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="I58" s="7"/>
     </row>
     <row r="59" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C59" s="7"/>
       <c r="D59" s="16" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E59" t="s">
-        <v>137</v>
-      </c>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15"/>
+        <v>105</v>
+      </c>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
       <c r="I59" s="7"/>
     </row>
     <row r="60" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C60" s="7"/>
       <c r="D60" s="16" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E60" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
@@ -2719,15 +2762,10 @@
     </row>
     <row r="61" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C61" s="7"/>
-      <c r="D61" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E61" t="s">
-        <v>136</v>
-      </c>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
-      <c r="I61" s="7"/>
     </row>
     <row r="62" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C62" s="7"/>
@@ -2827,65 +2865,103 @@
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C76" s="7"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="7"/>
-      <c r="F76" s="7"/>
-      <c r="G76" s="7"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="I1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3 A33 A35 A37 A39">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="28">
+  <conditionalFormatting sqref="A3 A32 A34 A36 A38 A9">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="56">
       <formula>LEN(TRIM(A3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A40:A42">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="26">
-      <formula>LEN(TRIM(A40))&gt;0</formula>
+  <conditionalFormatting sqref="A39:A41">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="54">
+      <formula>LEN(TRIM(A39))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="53">
+      <formula>LEN(TRIM(A42))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="25">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="52">
       <formula>LEN(TRIM(A43))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A44">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="24">
-      <formula>LEN(TRIM(A44))&gt;0</formula>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="45">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="41">
+      <formula>LEN(TRIM(A22))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="38">
+      <formula>LEN(TRIM(A25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="29">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="23">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="28">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A10">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="22">
+  <conditionalFormatting sqref="A5">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="27">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:A13">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="21">
+  <conditionalFormatting sqref="A6">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="26">
+      <formula>LEN(TRIM(A6))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="25">
+      <formula>LEN(TRIM(A7))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="24">
+      <formula>LEN(TRIM(A8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="23">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="22">
       <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="21">
+      <formula>LEN(TRIM(A12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="20">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="19">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="19">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="18">
       <formula>LEN(TRIM(A15))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="18">
-      <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
@@ -2903,74 +2979,64 @@
       <formula>LEN(TRIM(A19))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="11">
+      <formula>LEN(TRIM(A21))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
       <formula>LEN(TRIM(A20))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
-      <formula>LEN(TRIM(A21))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
-      <formula>LEN(TRIM(A22))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
       <formula>LEN(TRIM(A23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A24:A26">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
+  <conditionalFormatting sqref="A24">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
-      <formula>LEN(TRIM(A30))&gt;0</formula>
+  <conditionalFormatting sqref="A26">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(A26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
-      <formula>LEN(TRIM(A32))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
+  <conditionalFormatting sqref="A27">
     <cfRule type="notContainsBlanks" dxfId="6" priority="7">
-      <formula>LEN(TRIM(A34))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(A36))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
-      <formula>LEN(TRIM(A38))&gt;0</formula>
+      <formula>LEN(TRIM(A27))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
       <formula>LEN(TRIM(A28))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(A29))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(A31))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(A33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(A35))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A31))&gt;0</formula>
+      <formula>LEN(TRIM(A37))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2995,55 +3061,55 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3069,106 +3135,106 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -3177,40 +3243,40 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B16" s="3">
         <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D16">
         <v>57</v>
@@ -3218,13 +3284,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B17" s="3">
         <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D17">
         <v>64</v>
@@ -3232,13 +3298,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B18" s="4">
         <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D18">
         <v>83</v>
@@ -3248,37 +3314,37 @@
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D19">
         <v>129</v>
       </c>
       <c r="E19" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D20">
         <v>131</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D21">
         <v>147</v>
       </c>
       <c r="E21" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
DM, SUPPDM for Person_1 complete. Next: VS for Person_1
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="121">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Object</t>
   </si>
   <si>
-    <t>Person_1 Triples</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>ProposedFix</t>
   </si>
   <si>
-    <t>(and children)</t>
-  </si>
-  <si>
     <t>Reported</t>
   </si>
   <si>
@@ -243,9 +237,6 @@
   </si>
   <si>
     <t>cdiscpilot01:Date_20rdf:typestudy:StudyParticipationBegin</t>
-  </si>
-  <si>
-    <t>SUPPDM/Hardcoded</t>
   </si>
   <si>
     <t>"Person 1"</t>
@@ -309,27 +300,6 @@
     <t>cdiscpilot01:InformedConsentInterval_1</t>
   </si>
   <si>
-    <t xml:space="preserve">cdiscpilot01:PopulationFlagC16WK_1 </t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Sponsor_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:PopulationFlagC24WK_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:PopulationFlagC8WK_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:PopulationFlagEFF_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:PopulationFlagITT_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:PopulationFlagSAF_1</t>
-  </si>
-  <si>
     <t>cdiscpilot01:ProductAdministrationInterval_1</t>
   </si>
   <si>
@@ -384,17 +354,44 @@
     <t>ERROR in ONT. Email to AO 2017-06-15</t>
   </si>
   <si>
-    <t>TO HERE</t>
-  </si>
-  <si>
     <t>question to AO 2017-06-15: EFF/SAF/ITT to code: or cd01p: ??</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>no follow through to namespace</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:PopFlagCmpltr16Wk_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cdiscpilot01:PopFlagCmpltr24Wk_1 </t>
+  </si>
+  <si>
+    <t>cdiscpilot01:PopFlagCmpltr8Wk_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:PopFlagEff_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:PopFlagItt_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:PopFlagSaf_1</t>
+  </si>
+  <si>
+    <t>Src</t>
+  </si>
+  <si>
+    <t>ERROR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -591,8 +588,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="40">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -792,30 +795,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -939,6 +924,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -984,7 +984,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1017,13 +1017,10 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1032,18 +1029,26 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="15" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="15" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="15" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1089,14 +1094,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="46">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="45">
     <dxf>
       <fill>
         <patternFill>
@@ -1722,48 +1720,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M75"/>
+  <dimension ref="A1:N69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
+      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.81640625" customWidth="1"/>
-    <col min="7" max="7" width="40.36328125" customWidth="1"/>
-    <col min="8" max="8" width="18.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="70" style="3" customWidth="1"/>
-    <col min="10" max="10" width="67" style="4" customWidth="1"/>
-    <col min="11" max="11" width="61.08984375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="9.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="57.08984375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="49.81640625" customWidth="1"/>
+    <col min="8" max="8" width="40.36328125" customWidth="1"/>
+    <col min="9" max="9" width="18.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="70" style="3" customWidth="1"/>
+    <col min="11" max="11" width="67" style="4" customWidth="1"/>
+    <col min="12" max="12" width="61.08984375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="9.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="57.08984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="26"/>
+      <c r="L1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
@@ -1775,1268 +1776,1322 @@
         <v>32</v>
       </c>
       <c r="F2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="29"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="29"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B5" s="28"/>
+      <c r="C5" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="29"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="29"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="7"/>
+      <c r="J7"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7"/>
+    </row>
+    <row r="8" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="29"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="29"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J9"/>
+      <c r="L9" s="4"/>
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="29"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="7"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B11" s="28"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="29"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="29"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="29"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" s="29"/>
+      <c r="G14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B15" s="28"/>
+      <c r="C15" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F15" s="29"/>
+      <c r="G15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="J15"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="6"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="29"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="12" t="s">
+      <c r="I16" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B17" s="28"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
-        <v>42901</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="F17" s="29"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="J17"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="6"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B18" s="28"/>
+      <c r="C18" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
-        <v>42901</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="D18" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="29"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="D19" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="29"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="7"/>
-      <c r="I7"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7"/>
-    </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="M8" s="4"/>
-    </row>
-    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="I9"/>
-      <c r="K9" s="4"/>
-      <c r="M9" s="4"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="7"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="6"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="6"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="6"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="6"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="7" t="s">
+      <c r="D20" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="29"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="27">
+        <v>42915</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="6"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I15"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="6"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="6"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I17"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="6"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="7"/>
+      <c r="F21" s="29"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="30"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="12" t="s">
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="32">
+        <v>42915</v>
+      </c>
+      <c r="B22" s="28"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="7"/>
+      <c r="F22" s="29"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C23" s="7" t="s">
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="32">
+        <v>42915</v>
+      </c>
+      <c r="B23" s="28"/>
+      <c r="C23" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="29"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="M23" s="6"/>
+      <c r="N23" s="4"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" s="32">
+        <v>42915</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="29"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="K24" s="3"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="4"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" s="32">
+        <v>42916</v>
+      </c>
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="29"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="K25" s="3"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="4"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" s="32">
+        <v>42916</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="29"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" s="32">
+        <v>42916</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="29"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" s="32">
+        <v>42916</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" s="34"/>
+      <c r="G28" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="I28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29" s="32">
+        <v>42916</v>
+      </c>
+      <c r="B29" s="29"/>
+      <c r="C29" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="F29" s="34"/>
+      <c r="G29" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="H29" s="7"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="4"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" s="32">
+        <v>42916</v>
+      </c>
+      <c r="B30" s="28"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="F30" s="34"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="4"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31" s="32">
+        <v>42916</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="F31" s="34"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="4"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" s="32">
+        <v>42916</v>
+      </c>
+      <c r="B32" s="28"/>
+      <c r="C32" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="29"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A33" s="32">
+        <v>42916</v>
+      </c>
+      <c r="B33" s="28"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="L23" s="6"/>
-      <c r="M23" s="4"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="16" t="s">
+      <c r="F33" s="34"/>
+      <c r="G33" s="7"/>
+      <c r="M33" s="9"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A34" s="32">
+        <v>42916</v>
+      </c>
+      <c r="B34" s="28"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" s="29"/>
+      <c r="G34" s="7"/>
+      <c r="H34" t="s">
+        <v>82</v>
+      </c>
+      <c r="K34" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="M34" s="9"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35" s="32">
+        <v>42916</v>
+      </c>
+      <c r="B35" s="28"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" s="29"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="M35" s="9"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36" s="32">
+        <v>42916</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36" s="34"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="J36"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37" s="27"/>
+      <c r="B37" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="4"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="12" t="s">
+      <c r="F37" s="34"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="J37" s="7"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A38" s="27"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="J25" s="3"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="4"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="7" t="s">
+      <c r="F38" s="29"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A39" s="29"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="F39" s="36"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A40" s="29"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E40" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" s="7" t="s">
+      <c r="F40" s="36"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A41" s="29"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="F41" s="36"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="J41" s="7"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A42" s="28"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E42" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="F42" s="36"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="J42" s="7"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A43" s="28"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E43" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="7" t="s">
+      <c r="F43" s="34"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="J43" s="7"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A44" s="28"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="F44" s="28"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="J44" s="7"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A45" s="28"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E45" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="F45" s="28"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="J45" s="7"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A46" s="28"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F46" s="28"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="J46" s="7"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A47" s="28"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E47" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="31"/>
-      <c r="C30" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="19" t="s">
+      <c r="F47" s="34"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="11"/>
+      <c r="M47" s="9"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A48" s="28"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E48" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="F48" s="28"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="11"/>
+      <c r="M48" s="9"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A49" s="28"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="F49" s="28"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="11"/>
+      <c r="M49" s="9"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A50" s="28"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E50" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="F50" s="28"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="11"/>
+      <c r="M50" s="9"/>
+    </row>
+    <row r="51" spans="1:14" s="18" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="37"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="E51" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="F30" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="G30" s="7"/>
-      <c r="H30" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I30" s="7"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I31" s="7"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32" s="32"/>
-      <c r="B32" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F32" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="G32" s="7"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="4"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A33" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="4"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="6"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="4"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="4"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" s="6"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="4"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="6">
-        <v>42901</v>
-      </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="4"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="6"/>
-      <c r="C38" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="6"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="F39" s="7"/>
-      <c r="L39" s="9"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A40" s="6"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F40" s="7"/>
-      <c r="G40" t="s">
-        <v>85</v>
-      </c>
-      <c r="J40" t="s">
-        <v>73</v>
-      </c>
-      <c r="L40" s="9"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A41" s="6"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="L41" s="9"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42" s="6"/>
-      <c r="C42" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E42" s="19" t="s">
+      <c r="F51" s="34"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="22"/>
+      <c r="L51" s="22"/>
+      <c r="M51" s="21"/>
+      <c r="N51" s="23"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A52" s="28"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E52" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="F52" s="28"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="J52" s="7"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A53" s="28"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E53" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="F53" s="28"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="J53" s="7"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A54" s="28"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E54" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="I42"/>
-      <c r="J42" s="2"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A43" s="6"/>
-      <c r="C43" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E43" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="I43" s="7"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A44" s="18"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A45" s="12"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A46" s="12"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E46" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C47" s="7"/>
-      <c r="D47" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E47" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="I47" s="7"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C48" s="7"/>
-      <c r="D48" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E48" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="I48" s="7"/>
-    </row>
-    <row r="49" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C49" s="7"/>
-      <c r="D49" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E49" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
-      <c r="I49" s="7"/>
-    </row>
-    <row r="50" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C50" s="7"/>
-      <c r="D50" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E50" t="s">
-        <v>109</v>
-      </c>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
-      <c r="I50" s="7"/>
-    </row>
-    <row r="51" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C51" s="7"/>
-      <c r="D51" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E51" t="s">
-        <v>105</v>
-      </c>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
-      <c r="I51" s="7"/>
-    </row>
-    <row r="52" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C52" s="7"/>
-      <c r="D52" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E52" t="s">
-        <v>110</v>
-      </c>
-      <c r="F52" s="17"/>
-      <c r="G52" s="17"/>
-      <c r="I52" s="7"/>
-    </row>
-    <row r="53" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C53" s="7"/>
-      <c r="D53" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E53" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="F53" s="17"/>
-      <c r="G53" s="17"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="11"/>
-      <c r="L53" s="9"/>
-    </row>
-    <row r="54" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C54" s="7"/>
-      <c r="D54" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E54" t="s">
-        <v>111</v>
-      </c>
-      <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="11"/>
-      <c r="L54" s="9"/>
-    </row>
-    <row r="55" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="F54" s="28"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="J54" s="7"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C55" s="7"/>
-      <c r="D55" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E55" t="s">
-        <v>105</v>
-      </c>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-      <c r="I55" s="7"/>
-      <c r="J55" s="11"/>
-      <c r="L55" s="9"/>
-    </row>
-    <row r="56" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C56" s="7"/>
-      <c r="D56" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E56" t="s">
-        <v>112</v>
-      </c>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="11"/>
-      <c r="L56" s="9"/>
-    </row>
-    <row r="57" spans="3:13" s="20" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C57" s="21"/>
-      <c r="D57" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="E57" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="F57" s="23"/>
-      <c r="G57" s="23"/>
-      <c r="H57" s="24"/>
-      <c r="I57" s="21"/>
-      <c r="J57" s="25"/>
-      <c r="K57" s="25"/>
-      <c r="L57" s="24"/>
-      <c r="M57" s="26"/>
-    </row>
-    <row r="58" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C58" s="7"/>
-      <c r="D58" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E58" t="s">
-        <v>114</v>
-      </c>
-      <c r="F58" s="15"/>
-      <c r="G58" s="15"/>
-      <c r="I58" s="7"/>
-    </row>
-    <row r="59" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C59" s="7"/>
-      <c r="D59" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E59" t="s">
-        <v>105</v>
-      </c>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
-      <c r="I59" s="7"/>
-    </row>
-    <row r="60" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="H59" s="7"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C60" s="7"/>
-      <c r="D60" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E60" t="s">
-        <v>113</v>
-      </c>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
-      <c r="I60" s="7"/>
-    </row>
-    <row r="61" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="H60" s="7"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
-    </row>
-    <row r="62" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
-    </row>
-    <row r="63" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
-    </row>
-    <row r="64" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="H63" s="7"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
-    </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="H64" s="7"/>
+    </row>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
-    </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="H65" s="7"/>
+    </row>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
-    </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="H66" s="7"/>
+    </row>
+    <row r="67" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
-    </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="H67" s="7"/>
+    </row>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
-    </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="H68" s="7"/>
+    </row>
+    <row r="69" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
-    </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C70" s="7"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
-      <c r="G70" s="7"/>
-    </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C71" s="7"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="7"/>
-      <c r="G71" s="7"/>
-    </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C72" s="7"/>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="7"/>
-      <c r="G72" s="7"/>
-    </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C73" s="7"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
-      <c r="F73" s="7"/>
-      <c r="G73" s="7"/>
-    </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="7"/>
-      <c r="F74" s="7"/>
-      <c r="G74" s="7"/>
-    </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="7"/>
-      <c r="G75" s="7"/>
+      <c r="H69" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3 A32 A34 A36 A38 A9">
-    <cfRule type="notContainsBlanks" dxfId="45" priority="56">
+  <conditionalFormatting sqref="A37">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="82">
+      <formula>LEN(TRIM(A37))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="71">
+      <formula>LEN(TRIM(A22))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="55">
+      <formula>LEN(TRIM(A7))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:A6">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="30">
       <formula>LEN(TRIM(A3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39:A41">
-    <cfRule type="notContainsBlanks" dxfId="44" priority="54">
-      <formula>LEN(TRIM(A39))&gt;0</formula>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="29">
+      <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A42">
-    <cfRule type="notContainsBlanks" dxfId="43" priority="53">
-      <formula>LEN(TRIM(A42))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A43">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="52">
-      <formula>LEN(TRIM(A43))&gt;0</formula>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="28">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="45">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="27">
       <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="41">
-      <formula>LEN(TRIM(A22))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="38">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="26">
       <formula>LEN(TRIM(A25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="29">
-      <formula>LEN(TRIM(A30))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="28">
-      <formula>LEN(TRIM(A4))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="27">
-      <formula>LEN(TRIM(A5))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A6">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="26">
-      <formula>LEN(TRIM(A6))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
+  <conditionalFormatting sqref="A10">
     <cfRule type="notContainsBlanks" dxfId="24" priority="25">
-      <formula>LEN(TRIM(A7))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="24">
-      <formula>LEN(TRIM(A8))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="23">
       <formula>LEN(TRIM(A10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="22">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="24">
       <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="23">
       <formula>LEN(TRIM(A12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="22">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="21">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="19">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="20">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="19">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="17">
-      <formula>LEN(TRIM(A17))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A18">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="18">
       <formula>LEN(TRIM(A18))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="17">
       <formula>LEN(TRIM(A19))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A20">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="16">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="11">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
       <formula>LEN(TRIM(A21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
-      <formula>LEN(TRIM(A20))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
       <formula>LEN(TRIM(A23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
       <formula>LEN(TRIM(A26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
       <formula>LEN(TRIM(A27))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
       <formula>LEN(TRIM(A28))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
       <formula>LEN(TRIM(A29))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
       <formula>LEN(TRIM(A31))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A33">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(A33))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(A35))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
+  <conditionalFormatting sqref="A38">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(A38))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A37))&gt;0</formula>
+      <formula>LEN(TRIM(A36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3135,50 +3190,50 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -3186,55 +3241,55 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
         <v>49</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
         <v>51</v>
-      </c>
-      <c r="C9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
         <v>52</v>
       </c>
-      <c r="C10" t="s">
-        <v>54</v>
-      </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
         <v>53</v>
       </c>
-      <c r="C11" t="s">
-        <v>55</v>
-      </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -3243,15 +3298,15 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -3259,24 +3314,24 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B16" s="3">
         <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D16">
         <v>57</v>
@@ -3284,13 +3339,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" s="3">
         <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D17">
         <v>64</v>
@@ -3298,13 +3353,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B18" s="4">
         <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D18">
         <v>83</v>
@@ -3314,37 +3369,37 @@
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D19">
         <v>129</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D20">
         <v>131</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D21">
         <v>147</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
starting work on VS_frag.R and VS_process.R
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="120">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -382,9 +382,6 @@
   </si>
   <si>
     <t>Src</t>
-  </si>
-  <si>
-    <t>ERROR</t>
   </si>
 </sst>
 </file>
@@ -984,7 +981,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1049,6 +1046,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1723,8 +1721,8 @@
   <dimension ref="A1:N69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
+      <pane ySplit="2" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2523,9 +2521,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="27"/>
-      <c r="B37" s="28" t="s">
-        <v>120</v>
-      </c>
+      <c r="B37" s="40"/>
       <c r="C37" s="29" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Proofing subtriples at cdiscpilot01:VisitScreening1_1. Code runs. Questions out to AO re. vsseq matching with source data.
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="126">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -312,15 +312,6 @@
     <t xml:space="preserve">cdiscpilot01:Date_19 </t>
   </si>
   <si>
-    <t>#C67153.C25299_1</t>
-  </si>
-  <si>
-    <t>#C67153.C25299_2</t>
-  </si>
-  <si>
-    <t>#C67153.C25299_3</t>
-  </si>
-  <si>
     <t>cdiscpilot01:BloodPressureOutcome_1</t>
   </si>
   <si>
@@ -382,6 +373,33 @@
   </si>
   <si>
     <t>Src</t>
+  </si>
+  <si>
+    <t>VS</t>
+  </si>
+  <si>
+    <t>C67153.C25298_1</t>
+  </si>
+  <si>
+    <t>Not yet in file from AO: 2017-07-07</t>
+  </si>
+  <si>
+    <t>See greyed out section, below.</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:C67153.C25299_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:C67153.C25298_3</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:C67153.C25298_2</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:C67153.C25299_2</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:C67153.C25299_3</t>
   </si>
 </sst>
 </file>
@@ -592,7 +610,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -796,6 +814,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -981,7 +1005,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1027,18 +1051,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1046,7 +1062,24 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1092,21 +1125,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="45">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="43">
     <dxf>
       <fill>
         <patternFill>
@@ -1718,11 +1737,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N69"/>
+  <dimension ref="A1:N80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1744,12 +1763,12 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
-        <v>108</v>
-      </c>
-      <c r="J1" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="26"/>
+      <c r="K1" s="37"/>
       <c r="L1" s="10" t="s">
         <v>44</v>
       </c>
@@ -1762,7 +1781,7 @@
         <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
@@ -1774,7 +1793,7 @@
         <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G2" t="s">
         <v>85</v>
@@ -1796,94 +1815,104 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29" t="s">
+      <c r="A3" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="29"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="29" t="s">
+      <c r="A4" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="29"/>
+      <c r="F4" s="27"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="29" t="s">
+      <c r="A5" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>112</v>
+      <c r="E5" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>109</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="29" t="s">
+      <c r="A6" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="29"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="29" t="s">
+      <c r="A7" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="29"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="17"/>
       <c r="H7" s="7"/>
       <c r="J7"/>
@@ -1892,18 +1921,20 @@
       <c r="M7"/>
     </row>
     <row r="8" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="31" t="s">
+      <c r="A8" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="27"/>
+      <c r="D8" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="29"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="K8" s="4"/>
@@ -1911,159 +1942,173 @@
       <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="31" t="s">
+      <c r="A9" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="29"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J9"/>
       <c r="L9" s="4"/>
       <c r="N9" s="4"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="29" t="s">
+      <c r="A10" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="F10" s="29"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="17"/>
       <c r="H10" s="7"/>
       <c r="L10" s="2"/>
       <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="31" t="s">
+      <c r="A11" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="29"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7" t="s">
         <v>78</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="31" t="s">
+      <c r="A12" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="29"/>
+      <c r="F12" s="27"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7" t="s">
         <v>79</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="29" t="s">
+      <c r="A13" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="29"/>
+      <c r="F13" s="27"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="31" t="s">
+      <c r="A14" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="F14" s="29"/>
+      <c r="F14" s="27"/>
       <c r="G14" s="7" t="s">
         <v>67</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29" t="s">
+      <c r="A15" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="29"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="J15"/>
       <c r="K15" s="2"/>
@@ -2071,24 +2116,26 @@
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="31" t="s">
+      <c r="A16" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="29"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7" t="s">
         <v>80</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="2"/>
@@ -2096,24 +2143,26 @@
       <c r="M16" s="6"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="31" t="s">
+      <c r="A17" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="29"/>
+      <c r="F17" s="27"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7" t="s">
         <v>81</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="J17"/>
       <c r="K17" s="2"/>
@@ -2121,142 +2170,156 @@
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="29" t="s">
+      <c r="A18" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="29"/>
+      <c r="F18" s="27"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29" t="s">
+      <c r="A19" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="29" t="s">
+      <c r="E19" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="29"/>
+      <c r="F19" s="27"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="29" t="s">
+      <c r="A20" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="29" t="s">
+      <c r="E20" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="29"/>
+      <c r="F20" s="27"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="27">
-        <v>42915</v>
-      </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="31" t="s">
+      <c r="A21" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="29"/>
+      <c r="F21" s="27"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="32">
-        <v>42915</v>
-      </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="31" t="s">
+      <c r="A22" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" s="27"/>
+      <c r="D22" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="29" t="s">
+      <c r="E22" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="29"/>
+      <c r="F22" s="27"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
     </row>
     <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="32">
-        <v>42915</v>
-      </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29" t="s">
+      <c r="A23" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="29" t="s">
+      <c r="E23" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="F23" s="29"/>
+      <c r="F23" s="27"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="M23" s="6"/>
       <c r="N23" s="4"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="32">
-        <v>42915</v>
-      </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="31" t="s">
+      <c r="A24" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="27"/>
+      <c r="D24" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="29" t="s">
+      <c r="E24" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="F24" s="29"/>
+      <c r="F24" s="27"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="13"/>
@@ -2264,22 +2327,24 @@
       <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" s="32">
-        <v>42916</v>
-      </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="31" t="s">
+      <c r="A25" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="27"/>
+      <c r="D25" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="29" t="s">
+      <c r="E25" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="29"/>
+      <c r="F25" s="27"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="14"/>
@@ -2287,22 +2352,22 @@
       <c r="N25" s="4"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" s="32">
-        <v>42916</v>
-      </c>
-      <c r="B26" s="29" t="s">
+      <c r="A26" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B26" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="D26" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="F26" s="29"/>
+      <c r="E26" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="F26" s="27"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="3" t="s">
@@ -2310,22 +2375,22 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A27" s="32">
-        <v>42916</v>
-      </c>
-      <c r="B27" s="29" t="s">
+      <c r="A27" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B27" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D27" s="29" t="s">
+      <c r="D27" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="F27" s="29"/>
+      <c r="E27" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27" s="27"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="3" t="s">
@@ -2333,24 +2398,24 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" s="32">
-        <v>42916</v>
-      </c>
-      <c r="B28" s="29" t="s">
+      <c r="A28" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B28" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E28" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="F28" s="34"/>
+      <c r="E28" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="F28" s="30"/>
       <c r="G28" s="24" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="3" t="s">
@@ -2359,22 +2424,22 @@
       <c r="J28" s="7"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A29" s="32">
-        <v>42916</v>
-      </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="35" t="s">
+      <c r="A29" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="F29" s="34"/>
+      <c r="E29" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="F29" s="30"/>
       <c r="G29" s="24" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H29" s="7"/>
       <c r="K29" s="3"/>
@@ -2383,18 +2448,18 @@
       <c r="N29" s="4"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A30" s="32">
-        <v>42916</v>
-      </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29" t="s">
+      <c r="A30" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B30" s="26"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="F30" s="34"/>
+      <c r="E30" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="F30" s="30"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="K30" s="3"/>
@@ -2403,18 +2468,18 @@
       <c r="N30" s="4"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A31" s="32">
-        <v>42916</v>
-      </c>
-      <c r="B31" s="28"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29" t="s">
+      <c r="A31" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B31" s="26"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="F31" s="34"/>
+      <c r="E31" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="30"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="K31" s="3"/>
@@ -2423,52 +2488,52 @@
       <c r="N31" s="4"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A32" s="32">
-        <v>42916</v>
-      </c>
-      <c r="B32" s="28"/>
-      <c r="C32" s="29" t="s">
+      <c r="A32" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B32" s="26"/>
+      <c r="C32" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E32" s="29" t="s">
+      <c r="E32" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F32" s="29"/>
+      <c r="F32" s="27"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A33" s="32">
-        <v>42916</v>
-      </c>
-      <c r="B33" s="28"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="31" t="s">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A33" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B33" s="26"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="29" t="s">
+      <c r="E33" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="30"/>
       <c r="G33" s="7"/>
       <c r="M33" s="9"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="32">
-        <v>42916</v>
-      </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="31" t="s">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A34" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B34" s="26"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E34" s="29" t="s">
+      <c r="E34" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="F34" s="29"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="7"/>
       <c r="H34" t="s">
         <v>82</v>
@@ -2478,418 +2543,535 @@
       </c>
       <c r="M34" s="9"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" s="32">
-        <v>42916</v>
-      </c>
-      <c r="B35" s="28"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="31" t="s">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A35" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B35" s="26"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E35" s="29" t="s">
+      <c r="E35" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="F35" s="29"/>
+      <c r="F35" s="27"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7" t="s">
         <v>79</v>
       </c>
       <c r="M35" s="9"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" s="32">
-        <v>42916</v>
-      </c>
-      <c r="B36" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="C36" s="29" t="s">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A36" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E36" s="34" t="s">
+      <c r="E36" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="F36" s="34"/>
+      <c r="F36" s="30"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="J36"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="27"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="29" t="s">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A37" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D37" s="29" t="s">
+      <c r="D37" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E37" s="34" t="s">
+      <c r="E37" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="F37" s="34"/>
+      <c r="F37" s="43" t="s">
+        <v>120</v>
+      </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="J37" s="7"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="27"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="31" t="s">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A38" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B38" s="26"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="29" t="s">
+      <c r="E38" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="F38" s="29"/>
+      <c r="F38" s="27"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="29"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="31" t="s">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A39" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B39" s="26"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E39" s="36" t="s">
+      <c r="E39" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="F39" s="36"/>
+      <c r="F39" s="32"/>
       <c r="G39" s="16"/>
       <c r="H39" s="16"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A40" s="29"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="31" t="s">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A40" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B40" s="26"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E40" s="36" t="s">
+      <c r="E40" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="F40" s="36"/>
+      <c r="F40" s="32"/>
       <c r="G40" s="16"/>
       <c r="H40" s="16"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A41" s="29"/>
-      <c r="B41" s="28"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="31" t="s">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A41" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B41" s="26"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E41" s="36" t="s">
+      <c r="E41" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F41" s="36"/>
+      <c r="F41" s="32"/>
       <c r="G41" s="16"/>
       <c r="H41" s="16"/>
       <c r="J41" s="7"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42" s="28"/>
-      <c r="B42" s="28"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="31" t="s">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A42" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B42" s="26"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E42" s="36" t="s">
+      <c r="E42" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="F42" s="36"/>
+      <c r="F42" s="32"/>
       <c r="G42" s="16"/>
       <c r="H42" s="16"/>
       <c r="J42" s="7"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A43" s="28"/>
-      <c r="B43" s="28"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="31" t="s">
+    <row r="43" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="39"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="F43" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="K43" s="46"/>
+      <c r="L43" s="46"/>
+      <c r="N43" s="46"/>
+    </row>
+    <row r="44" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="39"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="F44" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="G44" s="44"/>
+      <c r="H44" s="44"/>
+      <c r="K44" s="46"/>
+      <c r="L44" s="46"/>
+      <c r="N44" s="46"/>
+    </row>
+    <row r="45" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="39"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="41"/>
+      <c r="E45" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="G45" s="44"/>
+      <c r="H45" s="44"/>
+      <c r="K45" s="46"/>
+      <c r="L45" s="46"/>
+      <c r="N45" s="46"/>
+    </row>
+    <row r="46" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="39"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="41"/>
+      <c r="E46" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="F46" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="G46" s="44"/>
+      <c r="H46" s="44"/>
+      <c r="K46" s="46"/>
+      <c r="L46" s="46"/>
+      <c r="N46" s="46"/>
+    </row>
+    <row r="47" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="39"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="F47" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="G47" s="44"/>
+      <c r="H47" s="44"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="46"/>
+      <c r="N47" s="46"/>
+    </row>
+    <row r="48" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="39"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="F48" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="G48" s="44"/>
+      <c r="H48" s="44"/>
+      <c r="K48" s="46"/>
+      <c r="L48" s="46"/>
+      <c r="N48" s="46"/>
+    </row>
+    <row r="49" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="39"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="F49" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="G49" s="44"/>
+      <c r="H49" s="44"/>
+      <c r="K49" s="46"/>
+      <c r="L49" s="46"/>
+      <c r="N49" s="46"/>
+    </row>
+    <row r="50" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="39"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="F50" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="G50" s="44"/>
+      <c r="H50" s="44"/>
+      <c r="K50" s="46"/>
+      <c r="L50" s="46"/>
+      <c r="N50" s="46"/>
+    </row>
+    <row r="51" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="39"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="41"/>
+      <c r="E51" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="F51" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="G51" s="44"/>
+      <c r="H51" s="44"/>
+      <c r="K51" s="46"/>
+      <c r="L51" s="46"/>
+      <c r="N51" s="46"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A52" s="26"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E43" s="34" t="s">
+      <c r="E52" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="F52" s="30"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="J52" s="7"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A53" s="26"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E53" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F53" s="30"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="J53" s="7"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A54" s="26"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E54" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="F54" s="30"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+      <c r="J54" s="7"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A55" s="26"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E55" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="F43" s="34"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-      <c r="J43" s="7"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A44" s="28"/>
-      <c r="B44" s="28"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="31" t="s">
+      <c r="F55" s="26"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="J55" s="7"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A56" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B56" s="26"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E44" s="28" t="s">
+      <c r="E56" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F56" s="26"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="J56" s="7"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A57" s="26"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E57" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="F57" s="26"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="16"/>
+      <c r="J57" s="7"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A58" s="26"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E58" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="F58" s="30"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="11"/>
+      <c r="M58" s="9"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A59" s="26"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E59" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="F59" s="26"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="11"/>
+      <c r="M59" s="9"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A60" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B60" s="26"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E60" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="F60" s="26"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="16"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="11"/>
+      <c r="M60" s="9"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A61" s="26"/>
+      <c r="B61" s="26"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E61" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="F44" s="28"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
-      <c r="J44" s="7"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A45" s="28"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="31" t="s">
+      <c r="F61" s="26"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="16"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="11"/>
+      <c r="M61" s="9"/>
+    </row>
+    <row r="62" spans="1:14" s="18" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="33"/>
+      <c r="B62" s="33"/>
+      <c r="C62" s="34"/>
+      <c r="D62" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="E62" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="F62" s="30"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="21"/>
+      <c r="J62" s="19"/>
+      <c r="K62" s="22"/>
+      <c r="L62" s="22"/>
+      <c r="M62" s="21"/>
+      <c r="N62" s="23"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A63" s="26"/>
+      <c r="B63" s="26"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E45" s="28" t="s">
+      <c r="E63" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="F63" s="26"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="J63" s="7"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A64" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B64" s="26"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E64" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="F45" s="28"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-      <c r="J45" s="7"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A46" s="28"/>
-      <c r="B46" s="28"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="E46" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="F46" s="28"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
-      <c r="J46" s="7"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A47" s="28"/>
-      <c r="B47" s="28"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="E47" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="F47" s="34"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="11"/>
-      <c r="M47" s="9"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A48" s="28"/>
-      <c r="B48" s="28"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="E48" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="F48" s="28"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="11"/>
-      <c r="M48" s="9"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A49" s="28"/>
-      <c r="B49" s="28"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="E49" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="F49" s="28"/>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="11"/>
-      <c r="M49" s="9"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A50" s="28"/>
-      <c r="B50" s="28"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="E50" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="F50" s="28"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="16"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="11"/>
-      <c r="M50" s="9"/>
-    </row>
-    <row r="51" spans="1:14" s="18" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="37"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="E51" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="F51" s="34"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="21"/>
-      <c r="J51" s="19"/>
-      <c r="K51" s="22"/>
-      <c r="L51" s="22"/>
-      <c r="M51" s="21"/>
-      <c r="N51" s="23"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A52" s="28"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="E52" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="F52" s="28"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="J52" s="7"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A53" s="28"/>
-      <c r="B53" s="28"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="E53" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="F53" s="28"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-      <c r="J53" s="7"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A54" s="28"/>
-      <c r="B54" s="28"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="E54" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="F54" s="28"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
-      <c r="J54" s="7"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="7"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C59" s="7"/>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
-      <c r="F59" s="7"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
-      <c r="G61" s="7"/>
-      <c r="H61" s="7"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="7"/>
-      <c r="F64" s="7"/>
+      <c r="F64" s="26"/>
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
-    </row>
-    <row r="65" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C65" s="7"/>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7"/>
-      <c r="F65" s="7"/>
+      <c r="J64" s="7"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A65" s="26"/>
+      <c r="B65" s="26"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E65" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="F65" s="26"/>
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
-    </row>
-    <row r="66" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="J65" s="7"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
@@ -2897,7 +3079,7 @@
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
     </row>
-    <row r="67" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
@@ -2905,7 +3087,7 @@
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
     </row>
-    <row r="68" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
@@ -2913,7 +3095,7 @@
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
     </row>
-    <row r="69" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
       <c r="E69" s="7"/>
@@ -2921,173 +3103,296 @@
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
     </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
+      <c r="H73" s="7"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="7"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="J1:K1"/>
   </mergeCells>
+  <conditionalFormatting sqref="A42:A51">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="87">
+      <formula>LEN(TRIM(A42))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:A6">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="72">
+      <formula>LEN(TRIM(A3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="37">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="38">
+      <formula>LEN(TRIM(A8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="16">
+      <formula>LEN(TRIM(A21))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="15">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="14">
+      <formula>LEN(TRIM(A24))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="13">
+      <formula>LEN(TRIM(A26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="12">
+      <formula>LEN(TRIM(A27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="11">
+      <formula>LEN(TRIM(A28))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="10">
+      <formula>LEN(TRIM(A29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="9">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="8">
+      <formula>LEN(TRIM(A31))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="5">
+      <formula>LEN(TRIM(A36))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="36">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="39">
+      <formula>LEN(TRIM(A7))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="35">
+      <formula>LEN(TRIM(A22))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="34">
+      <formula>LEN(TRIM(A25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="33">
+      <formula>LEN(TRIM(A40))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="31">
+      <formula>LEN(TRIM(A56))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="30">
+      <formula>LEN(TRIM(A60))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="29">
+      <formula>LEN(TRIM(A64))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="28">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="27">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="26">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="25">
+      <formula>LEN(TRIM(A35))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="24">
+      <formula>LEN(TRIM(A12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="23">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="22">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="21">
+      <formula>LEN(TRIM(A15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="20">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="19">
+      <formula>LEN(TRIM(A18))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="18">
+      <formula>LEN(TRIM(A19))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="17">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="7">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
+      <formula>LEN(TRIM(A33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="82">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(A37))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="71">
-      <formula>LEN(TRIM(A22))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="55">
-      <formula>LEN(TRIM(A7))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A6">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="30">
-      <formula>LEN(TRIM(A3))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="29">
-      <formula>LEN(TRIM(A8))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="28">
-      <formula>LEN(TRIM(A9))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="27">
-      <formula>LEN(TRIM(A16))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="26">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="25">
-      <formula>LEN(TRIM(A10))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="24">
-      <formula>LEN(TRIM(A11))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="23">
-      <formula>LEN(TRIM(A12))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="22">
-      <formula>LEN(TRIM(A17))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="21">
-      <formula>LEN(TRIM(A13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="20">
-      <formula>LEN(TRIM(A14))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="19">
-      <formula>LEN(TRIM(A15))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="18">
-      <formula>LEN(TRIM(A18))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="17">
-      <formula>LEN(TRIM(A19))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="16">
-      <formula>LEN(TRIM(A20))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
-      <formula>LEN(TRIM(A21))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
-      <formula>LEN(TRIM(A23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
-      <formula>LEN(TRIM(A24))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
-      <formula>LEN(TRIM(A26))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
-      <formula>LEN(TRIM(A28))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
-      <formula>LEN(TRIM(A29))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
-      <formula>LEN(TRIM(A30))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
-      <formula>LEN(TRIM(A31))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(A32))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(A34))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35">
+  <conditionalFormatting sqref="A38">
     <cfRule type="notContainsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(A35))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
+      <formula>LEN(TRIM(A38))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(A38))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
+      <formula>LEN(TRIM(A39))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A36))&gt;0</formula>
+      <formula>LEN(TRIM(A41))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added outcome result triples. Sorting on result differs from AO. Next steps. Move hard coding from the XX_process.R scripts to XX_impute and XX_Frag scripts
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="person_1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="125">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -318,18 +318,12 @@
     <t>cdiscpilot01:StartRuleLying5_1</t>
   </si>
   <si>
-    <t>cdiscpilot01:BloodPressureOutcome_2</t>
-  </si>
-  <si>
     <t>cdiscpilot01:StartRuleStanding1_1</t>
   </si>
   <si>
     <t>cdiscpilot01:StartRuleStanding3_1</t>
   </si>
   <si>
-    <t>cdiscpilot01:BloodPressureOutcome_3</t>
-  </si>
-  <si>
     <t>DM</t>
   </si>
   <si>
@@ -400,6 +394,9 @@
   </si>
   <si>
     <t>cdiscpilot01:C67153.C25299_3</t>
+  </si>
+  <si>
+    <t>TO HERE 201707-07</t>
   </si>
 </sst>
 </file>
@@ -610,7 +607,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -811,6 +808,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1005,7 +1008,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1069,17 +1072,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="38" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1740,8 +1745,8 @@
   <dimension ref="A1:N80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1763,7 +1768,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J1" s="36" t="s">
         <v>34</v>
@@ -1781,7 +1786,7 @@
         <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
@@ -1793,7 +1798,7 @@
         <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G2" t="s">
         <v>85</v>
@@ -1819,7 +1824,7 @@
         <v>42923</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C3" s="27" t="s">
         <v>0</v>
@@ -1839,7 +1844,7 @@
         <v>42923</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C4" s="27" t="s">
         <v>0</v>
@@ -1859,7 +1864,7 @@
         <v>42923</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C5" s="27" t="s">
         <v>0</v>
@@ -1868,10 +1873,10 @@
         <v>4</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -1881,7 +1886,7 @@
         <v>42923</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C6" s="27" t="s">
         <v>0</v>
@@ -1901,7 +1906,7 @@
         <v>42923</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C7" s="27" t="s">
         <v>0</v>
@@ -1925,7 +1930,7 @@
         <v>42923</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="28" t="s">
@@ -1946,7 +1951,7 @@
         <v>42923</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C9" s="27"/>
       <c r="D9" s="28" t="s">
@@ -1958,7 +1963,7 @@
       <c r="F9" s="27"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J9"/>
       <c r="L9" s="4"/>
@@ -1969,7 +1974,7 @@
         <v>42923</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>0</v>
@@ -1991,7 +1996,7 @@
         <v>42923</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C11" s="27"/>
       <c r="D11" s="28" t="s">
@@ -2006,7 +2011,7 @@
         <v>78</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="6"/>
@@ -2016,7 +2021,7 @@
         <v>42923</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="28" t="s">
@@ -2031,7 +2036,7 @@
         <v>79</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="6"/>
@@ -2041,7 +2046,7 @@
         <v>42923</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>0</v>
@@ -2056,7 +2061,7 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="6"/>
@@ -2066,7 +2071,7 @@
         <v>42923</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="28" t="s">
@@ -2081,7 +2086,7 @@
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="6"/>
@@ -2091,7 +2096,7 @@
         <v>42923</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C15" s="27" t="s">
         <v>0</v>
@@ -2108,7 +2113,7 @@
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J15"/>
       <c r="K15" s="2"/>
@@ -2120,7 +2125,7 @@
         <v>42923</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="28" t="s">
@@ -2135,7 +2140,7 @@
         <v>80</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="2"/>
@@ -2147,7 +2152,7 @@
         <v>42923</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="28" t="s">
@@ -2162,7 +2167,7 @@
         <v>81</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J17"/>
       <c r="K17" s="2"/>
@@ -2174,7 +2179,7 @@
         <v>42923</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>0</v>
@@ -2189,7 +2194,7 @@
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
@@ -2197,7 +2202,7 @@
         <v>42923</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C19" s="27" t="s">
         <v>0</v>
@@ -2212,7 +2217,7 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
@@ -2220,7 +2225,7 @@
         <v>42923</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C20" s="27" t="s">
         <v>0</v>
@@ -2235,7 +2240,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
@@ -2243,7 +2248,7 @@
         <v>42923</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="28" t="s">
@@ -2262,7 +2267,7 @@
         <v>42923</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C22" s="27"/>
       <c r="D22" s="28" t="s">
@@ -2281,7 +2286,7 @@
         <v>42923</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C23" s="27" t="s">
         <v>0</v>
@@ -2296,7 +2301,7 @@
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="M23" s="6"/>
       <c r="N23" s="4"/>
@@ -2306,7 +2311,7 @@
         <v>42923</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="28" t="s">
@@ -2319,7 +2324,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="13"/>
@@ -2331,7 +2336,7 @@
         <v>42923</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C25" s="27"/>
       <c r="D25" s="28" t="s">
@@ -2344,7 +2349,7 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="14"/>
@@ -2365,7 +2370,7 @@
         <v>17</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F26" s="27"/>
       <c r="G26" s="7"/>
@@ -2388,7 +2393,7 @@
         <v>17</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F27" s="27"/>
       <c r="G27" s="7"/>
@@ -2411,11 +2416,11 @@
         <v>17</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F28" s="30"/>
       <c r="G28" s="24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="3" t="s">
@@ -2435,11 +2440,11 @@
         <v>17</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F29" s="30"/>
       <c r="G29" s="24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H29" s="7"/>
       <c r="K29" s="3"/>
@@ -2457,7 +2462,7 @@
         <v>17</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F30" s="30"/>
       <c r="G30" s="7"/>
@@ -2477,7 +2482,7 @@
         <v>17</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F31" s="30"/>
       <c r="G31" s="7"/>
@@ -2567,7 +2572,7 @@
         <v>42923</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>0</v>
@@ -2589,7 +2594,7 @@
         <v>42923</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C37" s="27" t="s">
         <v>0</v>
@@ -2600,8 +2605,8 @@
       <c r="E37" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="F37" s="43" t="s">
-        <v>120</v>
+      <c r="F37" s="44" t="s">
+        <v>118</v>
       </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
@@ -2689,168 +2694,170 @@
       <c r="H42" s="16"/>
       <c r="J42" s="7"/>
     </row>
-    <row r="43" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="39"/>
-      <c r="B43" s="40"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="F43" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="K43" s="46"/>
-      <c r="L43" s="46"/>
-      <c r="N43" s="46"/>
-    </row>
-    <row r="44" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="39"/>
-      <c r="B44" s="40"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="40" t="s">
+    <row r="43" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="40"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="F43" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="K43" s="47"/>
+      <c r="L43" s="47"/>
+      <c r="N43" s="47"/>
+    </row>
+    <row r="44" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="40"/>
+      <c r="B44" s="41"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="F44" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="K44" s="46"/>
-      <c r="L44" s="46"/>
-      <c r="N44" s="46"/>
-    </row>
-    <row r="45" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="39"/>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="41"/>
-      <c r="E45" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="F45" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="K45" s="46"/>
-      <c r="L45" s="46"/>
-      <c r="N45" s="46"/>
-    </row>
-    <row r="46" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="39"/>
-      <c r="B46" s="40"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="41"/>
-      <c r="E46" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="F46" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="G46" s="44"/>
-      <c r="H46" s="44"/>
-      <c r="K46" s="46"/>
-      <c r="L46" s="46"/>
-      <c r="N46" s="46"/>
-    </row>
-    <row r="47" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="39"/>
-      <c r="B47" s="40"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="41"/>
-      <c r="E47" s="40" t="s">
+      <c r="F44" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
+      <c r="K44" s="47"/>
+      <c r="L44" s="47"/>
+      <c r="N44" s="47"/>
+    </row>
+    <row r="45" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="40"/>
+      <c r="B45" s="41"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="F45" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="K45" s="47"/>
+      <c r="L45" s="47"/>
+      <c r="N45" s="47"/>
+    </row>
+    <row r="46" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="40"/>
+      <c r="B46" s="41"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="F46" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="G46" s="45"/>
+      <c r="H46" s="45"/>
+      <c r="K46" s="47"/>
+      <c r="L46" s="47"/>
+      <c r="N46" s="47"/>
+    </row>
+    <row r="47" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="40"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="42"/>
+      <c r="E47" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="F47" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="G47" s="44"/>
-      <c r="H47" s="44"/>
-      <c r="K47" s="46"/>
-      <c r="L47" s="46"/>
-      <c r="N47" s="46"/>
-    </row>
-    <row r="48" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="39"/>
-      <c r="B48" s="40"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="41"/>
-      <c r="E48" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="F48" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="G48" s="44"/>
-      <c r="H48" s="44"/>
-      <c r="K48" s="46"/>
-      <c r="L48" s="46"/>
-      <c r="N48" s="46"/>
-    </row>
-    <row r="49" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="39"/>
-      <c r="B49" s="40"/>
-      <c r="C49" s="40"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="42" t="s">
-        <v>122</v>
-      </c>
-      <c r="F49" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="G49" s="44"/>
-      <c r="H49" s="44"/>
-      <c r="K49" s="46"/>
-      <c r="L49" s="46"/>
-      <c r="N49" s="46"/>
-    </row>
-    <row r="50" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="39"/>
-      <c r="B50" s="40"/>
-      <c r="C50" s="40"/>
-      <c r="D50" s="41"/>
-      <c r="E50" s="40" t="s">
+      <c r="F47" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="G47" s="45"/>
+      <c r="H47" s="45"/>
+      <c r="K47" s="47"/>
+      <c r="L47" s="47"/>
+      <c r="N47" s="47"/>
+    </row>
+    <row r="48" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="40"/>
+      <c r="B48" s="41"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="F48" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="G48" s="45"/>
+      <c r="H48" s="45"/>
+      <c r="K48" s="47"/>
+      <c r="L48" s="47"/>
+      <c r="N48" s="47"/>
+    </row>
+    <row r="49" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="40"/>
+      <c r="B49" s="41"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="F49" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="G49" s="45"/>
+      <c r="H49" s="45"/>
+      <c r="K49" s="47"/>
+      <c r="L49" s="47"/>
+      <c r="N49" s="47"/>
+    </row>
+    <row r="50" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="40"/>
+      <c r="B50" s="41"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="42"/>
+      <c r="E50" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="F50" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="G50" s="44"/>
-      <c r="H50" s="44"/>
-      <c r="K50" s="46"/>
-      <c r="L50" s="46"/>
-      <c r="N50" s="46"/>
-    </row>
-    <row r="51" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="39"/>
-      <c r="B51" s="40"/>
-      <c r="C51" s="40"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="F51" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="G51" s="44"/>
-      <c r="H51" s="44"/>
-      <c r="K51" s="46"/>
-      <c r="L51" s="46"/>
-      <c r="N51" s="46"/>
+      <c r="F50" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
+      <c r="K50" s="47"/>
+      <c r="L50" s="47"/>
+      <c r="N50" s="47"/>
+    </row>
+    <row r="51" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="40"/>
+      <c r="B51" s="41"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="42"/>
+      <c r="E51" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="F51" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="G51" s="45"/>
+      <c r="H51" s="45"/>
+      <c r="K51" s="47"/>
+      <c r="L51" s="47"/>
+      <c r="N51" s="47"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" s="26"/>
       <c r="B52" s="26"/>
-      <c r="C52" s="27"/>
+      <c r="C52" s="49" t="s">
+        <v>124</v>
+      </c>
       <c r="D52" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E52" s="47" t="s">
-        <v>121</v>
+      <c r="E52" s="48" t="s">
+        <v>119</v>
       </c>
       <c r="F52" s="30"/>
       <c r="G52" s="16"/>
@@ -2894,7 +2901,7 @@
       <c r="D55" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E55" s="27" t="s">
+      <c r="E55" s="39" t="s">
         <v>96</v>
       </c>
       <c r="F55" s="26"/>
@@ -2942,7 +2949,7 @@
         <v>69</v>
       </c>
       <c r="E58" s="38" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F58" s="30"/>
       <c r="G58" s="16"/>
@@ -2958,8 +2965,8 @@
       <c r="D59" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E59" s="26" t="s">
-        <v>98</v>
+      <c r="E59" s="39" t="s">
+        <v>96</v>
       </c>
       <c r="F59" s="26"/>
       <c r="G59" s="16"/>
@@ -2995,7 +3002,7 @@
         <v>70</v>
       </c>
       <c r="E61" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F61" s="26"/>
       <c r="G61" s="16"/>
@@ -3012,7 +3019,7 @@
         <v>69</v>
       </c>
       <c r="E62" s="38" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F62" s="30"/>
       <c r="G62" s="20"/>
@@ -3031,8 +3038,8 @@
       <c r="D63" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E63" s="26" t="s">
-        <v>101</v>
+      <c r="E63" s="39" t="s">
+        <v>96</v>
       </c>
       <c r="F63" s="26"/>
       <c r="G63" s="15"/>
@@ -3064,7 +3071,7 @@
         <v>70</v>
       </c>
       <c r="E65" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F65" s="26"/>
       <c r="G65" s="7"/>

</xml_diff>

<commit_message>
next: rework of vstestCat/outcome
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="person_1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="139">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -372,9 +372,6 @@
     <t>VS</t>
   </si>
   <si>
-    <t>C67153.C25298_1</t>
-  </si>
-  <si>
     <t>Not yet in file from AO: 2017-07-07</t>
   </si>
   <si>
@@ -396,7 +393,52 @@
     <t>cdiscpilot01:C67153.C25299_3</t>
   </si>
   <si>
-    <t>TO HERE 201707-07</t>
+    <t>Ties into the OWL. Part of original triples</t>
+  </si>
+  <si>
+    <t>Checking occurs with owl:imports REMOVED.</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:C67153.C25206_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:C67153.C25208_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:C67153.C25347_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:C67153.C49676_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:C67153.C49676_2</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:C67153.C49676_3</t>
+  </si>
+  <si>
+    <t>AO needs to change formatting of label to match R</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:StartRuleNone_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:TemperatureOutcome_1</t>
+  </si>
+  <si>
+    <t>study:hasSubActivity</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:C67153.C25298_1</t>
+  </si>
+  <si>
+    <t>Label issue email to AO TBD sent</t>
+  </si>
+  <si>
+    <t>Change label. Screening1 (ont) to Screening 1 ®</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:WeightMassOutcome_1</t>
   </si>
 </sst>
 </file>
@@ -607,7 +649,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -823,6 +865,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -1008,7 +1056,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1063,7 +1111,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1084,7 +1131,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="39" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1130,7 +1185,70 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="52">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1742,18 +1860,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N80"/>
+  <dimension ref="A1:N94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" customWidth="1"/>
     <col min="4" max="4" width="30.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="49.81640625" customWidth="1"/>
@@ -1770,10 +1888,10 @@
       <c r="C1" t="s">
         <v>103</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="37"/>
+      <c r="K1" s="49"/>
       <c r="L1" s="10" t="s">
         <v>44</v>
       </c>
@@ -1781,67 +1899,56 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J2" s="35"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="36"/>
+    </row>
+    <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>114</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>31</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>32</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>106</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" t="s">
         <v>85</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H3" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J3" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="25">
-        <v>42923</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>100</v>
@@ -1850,18 +1957,20 @@
         <v>0</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="27"/>
+        <v>2</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>123</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>100</v>
@@ -1870,20 +1979,18 @@
         <v>0</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>107</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F5" s="27"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B6" s="26" t="s">
         <v>100</v>
@@ -1892,18 +1999,20 @@
         <v>0</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="27"/>
+        <v>101</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>107</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B7" s="26" t="s">
         <v>100</v>
@@ -1912,43 +2021,42 @@
         <v>0</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F7" s="27"/>
-      <c r="G7" s="17"/>
+      <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="J7"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7"/>
-    </row>
-    <row r="8" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B8" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28" t="s">
-        <v>69</v>
+      <c r="C8" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>6</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F8" s="27"/>
-      <c r="G8" s="7"/>
+      <c r="G8" s="17"/>
       <c r="H8" s="7"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="N8" s="4"/>
+      <c r="J8"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8"/>
     </row>
     <row r="9" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B9" s="26" t="s">
         <v>100</v>
@@ -1958,67 +2066,63 @@
         <v>69</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="J9"/>
+      <c r="H9" s="7"/>
+      <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="N9" s="4"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>8</v>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28" t="s">
+        <v>69</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="F10" s="27"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="7"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="J10"/>
+      <c r="L10" s="4"/>
+      <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B11" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="28" t="s">
-        <v>69</v>
+      <c r="C11" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>8</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="F11" s="27"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>100</v>
-      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="7"/>
       <c r="L11" s="2"/>
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>100</v>
@@ -2028,12 +2132,12 @@
         <v>69</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F12" s="27"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>100</v>
@@ -2043,23 +2147,23 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B13" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>10</v>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28" t="s">
+        <v>69</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="F13" s="27"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="I13" s="7" t="s">
         <v>100</v>
       </c>
@@ -2068,22 +2172,22 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B14" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="28" t="s">
-        <v>69</v>
+      <c r="C14" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>10</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F14" s="27"/>
-      <c r="G14" s="7" t="s">
-        <v>67</v>
-      </c>
+      <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7" t="s">
         <v>100</v>
@@ -2093,63 +2197,61 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B15" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>11</v>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28" t="s">
+        <v>69</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F15" s="27"/>
       <c r="G15" s="7" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="J15"/>
-      <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B16" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="28" t="s">
-        <v>69</v>
+      <c r="C16" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>11</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="F16" s="27"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7" t="s">
-        <v>80</v>
-      </c>
+      <c r="G16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="7"/>
       <c r="I16" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="J16" s="4"/>
+      <c r="J16"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="6"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B17" s="26" t="s">
         <v>100</v>
@@ -2159,47 +2261,51 @@
         <v>69</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="F17" s="27"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="J17"/>
+      <c r="J17" s="4"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>13</v>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28" t="s">
+        <v>69</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="F18" s="27"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="H18" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="I18" s="7" t="s">
         <v>100</v>
       </c>
+      <c r="J18"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="6"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B19" s="26" t="s">
         <v>100</v>
@@ -2208,10 +2314,10 @@
         <v>0</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F19" s="27"/>
       <c r="G19" s="7"/>
@@ -2222,7 +2328,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>100</v>
@@ -2231,10 +2337,10 @@
         <v>0</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F20" s="27"/>
       <c r="G20" s="7"/>
@@ -2245,26 +2351,27 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="28" t="s">
-        <v>69</v>
+      <c r="C21" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>17</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
       <c r="F21" s="27"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B22" s="26" t="s">
         <v>100</v>
@@ -2274,51 +2381,45 @@
         <v>69</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="F22" s="27"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B23" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>17</v>
+      <c r="C23" s="27"/>
+      <c r="D23" s="28" t="s">
+        <v>69</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="F23" s="27"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
-      <c r="I23" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="M23" s="6"/>
-      <c r="N23" s="4"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="28" t="s">
-        <v>69</v>
+      <c r="C24" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>17</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F24" s="27"/>
       <c r="G24" s="7"/>
@@ -2326,24 +2427,22 @@
       <c r="I24" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="K24" s="3"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
+      <c r="M24" s="6"/>
       <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B25" s="26" t="s">
         <v>100</v>
       </c>
       <c r="C25" s="27"/>
       <c r="D25" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="F25" s="27"/>
       <c r="G25" s="7"/>
@@ -2352,36 +2451,38 @@
         <v>100</v>
       </c>
       <c r="K25" s="3"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
       <c r="N25" s="4"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="25">
-        <v>42923</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>17</v>
+        <v>42942</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="27"/>
+      <c r="D26" s="28" t="s">
+        <v>70</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="F26" s="27"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
-      <c r="I26" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="I26" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="K26" s="3"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="4"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B27" s="27" t="s">
         <v>61</v>
@@ -2393,7 +2494,7 @@
         <v>17</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F27" s="27"/>
       <c r="G27" s="7"/>
@@ -2404,7 +2505,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B28" s="27" t="s">
         <v>61</v>
@@ -2415,57 +2516,60 @@
       <c r="D28" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E28" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="F28" s="30"/>
-      <c r="G28" s="24" t="s">
-        <v>104</v>
-      </c>
+      <c r="E28" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="F28" s="27"/>
+      <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="J28" s="7"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="25">
-        <v>42923</v>
-      </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="31" t="s">
+        <v>42942</v>
+      </c>
+      <c r="B29" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="27" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="27" t="s">
         <v>17</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F29" s="30"/>
       <c r="G29" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H29" s="7"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="4"/>
+      <c r="I29" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J29" s="7"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="25">
-        <v>42923</v>
-      </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="27"/>
+        <v>42942</v>
+      </c>
+      <c r="B30" s="27"/>
+      <c r="C30" s="31" t="s">
+        <v>0</v>
+      </c>
       <c r="D30" s="27" t="s">
         <v>17</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F30" s="30"/>
-      <c r="G30" s="7"/>
+      <c r="G30" s="24" t="s">
+        <v>105</v>
+      </c>
       <c r="H30" s="7"/>
       <c r="K30" s="3"/>
       <c r="L30" s="14"/>
@@ -2474,7 +2578,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B31" s="26"/>
       <c r="C31" s="27"/>
@@ -2482,7 +2586,7 @@
         <v>17</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F31" s="30"/>
       <c r="G31" s="7"/>
@@ -2494,63 +2598,61 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B32" s="26"/>
-      <c r="C32" s="27" t="s">
-        <v>0</v>
-      </c>
+      <c r="C32" s="27"/>
       <c r="D32" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E32" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="27"/>
+      <c r="E32" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="F32" s="30"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K32" s="3"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="4"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B33" s="26"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="28" t="s">
-        <v>69</v>
+      <c r="C33" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>17</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="F33" s="30"/>
+        <v>19</v>
+      </c>
+      <c r="F33" s="27"/>
       <c r="G33" s="7"/>
-      <c r="M33" s="9"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B34" s="26"/>
       <c r="C34" s="27"/>
       <c r="D34" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="F34" s="27"/>
+        <v>92</v>
+      </c>
+      <c r="F34" s="30"/>
       <c r="G34" s="7"/>
-      <c r="H34" t="s">
-        <v>82</v>
-      </c>
-      <c r="K34" t="s">
-        <v>71</v>
-      </c>
       <c r="M34" s="9"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B35" s="26"/>
       <c r="C35" s="27"/>
@@ -2558,43 +2660,43 @@
         <v>70</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F35" s="27"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="7" t="s">
+      <c r="H35" t="s">
+        <v>82</v>
+      </c>
+      <c r="K35" t="s">
+        <v>71</v>
+      </c>
+      <c r="M35" s="9"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36" s="25">
+        <v>42942</v>
+      </c>
+      <c r="B36" s="26"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" s="27"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="M35" s="9"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A36" s="25">
-        <v>42923</v>
-      </c>
-      <c r="B36" s="26" t="s">
+      <c r="M36" s="9"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37" s="25">
+        <v>42942</v>
+      </c>
+      <c r="B37" s="26" t="s">
         <v>100</v>
-      </c>
-      <c r="C36" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D36" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="F36" s="30"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="J36"/>
-      <c r="K36" s="2"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A37" s="25">
-        <v>42923</v>
-      </c>
-      <c r="B37" s="27" t="s">
-        <v>115</v>
       </c>
       <c r="C37" s="27" t="s">
         <v>0</v>
@@ -2603,433 +2705,455 @@
         <v>17</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="F37" s="44" t="s">
-        <v>118</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="F37" s="30"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
-      <c r="J37" s="7"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J37"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="25">
-        <v>42923</v>
-      </c>
-      <c r="B38" s="26"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E38" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="F38" s="27"/>
+        <v>42942</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="F38" s="43" t="s">
+        <v>117</v>
+      </c>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J38" s="7"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B39" s="26"/>
       <c r="C39" s="27"/>
       <c r="D39" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E39" s="38" t="s">
+      <c r="E39" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" s="27"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A40" s="25">
+        <v>42942</v>
+      </c>
+      <c r="B40" s="26"/>
+      <c r="C40" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" s="37" t="s">
         <v>74</v>
-      </c>
-      <c r="F39" s="32"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A40" s="25">
-        <v>42923</v>
-      </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E40" s="27" t="s">
-        <v>95</v>
       </c>
       <c r="F40" s="32"/>
       <c r="G40" s="16"/>
       <c r="H40" s="16"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B41" s="26"/>
       <c r="C41" s="27"/>
       <c r="D41" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E41" s="38" t="s">
-        <v>75</v>
+        <v>70</v>
+      </c>
+      <c r="E41" s="27" t="s">
+        <v>95</v>
       </c>
       <c r="F41" s="32"/>
       <c r="G41" s="16"/>
       <c r="H41" s="16"/>
-      <c r="J41" s="7"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="25">
-        <v>42923</v>
+        <v>42942</v>
       </c>
       <c r="B42" s="26"/>
-      <c r="C42" s="27"/>
+      <c r="C42" s="30" t="s">
+        <v>94</v>
+      </c>
       <c r="D42" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E42" s="27" t="s">
-        <v>95</v>
+        <v>69</v>
+      </c>
+      <c r="E42" s="37" t="s">
+        <v>75</v>
       </c>
       <c r="F42" s="32"/>
       <c r="G42" s="16"/>
       <c r="H42" s="16"/>
       <c r="J42" s="7"/>
     </row>
-    <row r="43" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="40"/>
-      <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="43" t="s">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A43" s="25">
+        <v>42942</v>
+      </c>
+      <c r="B43" s="26"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E43" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F43" s="32"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="J43" s="7"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A44" s="51">
+        <v>42944</v>
+      </c>
+      <c r="B44" s="26"/>
+      <c r="C44" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="E44" s="50" t="s">
+        <v>125</v>
+      </c>
+      <c r="F44" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="J44" s="7"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A45" s="25">
+        <v>42944</v>
+      </c>
+      <c r="B45" s="26"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E45" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" s="32"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="J45" s="7"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A46" s="25">
+        <v>42944</v>
+      </c>
+      <c r="B46" s="26"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" s="52" t="s">
+        <v>132</v>
+      </c>
+      <c r="F46" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="J46" s="7"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A47" s="25">
+        <v>42944</v>
+      </c>
+      <c r="B47" s="26"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E47" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="F47" s="32"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="J47" s="7"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A48" s="25">
+        <v>42944</v>
+      </c>
+      <c r="B48" s="26"/>
+      <c r="C48" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D48" s="28"/>
+      <c r="E48" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="F48" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="J48" s="7"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A49" s="25">
+        <v>42944</v>
+      </c>
+      <c r="B49" s="26"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F49" s="32"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+      <c r="J49" s="7"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A50" s="25"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="F50" s="32"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+      <c r="J50" s="7"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A51" s="25"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="F51" s="32"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
+      <c r="J51" s="7"/>
+    </row>
+    <row r="52" spans="1:14" s="45" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="25">
+        <v>42944</v>
+      </c>
+      <c r="B52" s="40"/>
+      <c r="C52" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D52" s="41"/>
+      <c r="E52" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="F52" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="F43" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-      <c r="K43" s="47"/>
-      <c r="L43" s="47"/>
-      <c r="N43" s="47"/>
-    </row>
-    <row r="44" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="40"/>
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="41" t="s">
+      <c r="G52" s="44"/>
+      <c r="H52" s="44"/>
+      <c r="K52" s="46"/>
+      <c r="L52" s="46"/>
+      <c r="N52" s="46"/>
+    </row>
+    <row r="53" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="39"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="40"/>
+      <c r="D53" s="41"/>
+      <c r="E53" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="F44" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
-      <c r="K44" s="47"/>
-      <c r="L44" s="47"/>
-      <c r="N44" s="47"/>
-    </row>
-    <row r="45" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="40"/>
-      <c r="B45" s="41"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="41" t="s">
+      <c r="F53" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="G53" s="44"/>
+      <c r="H53" s="44"/>
+      <c r="K53" s="46"/>
+      <c r="L53" s="46"/>
+      <c r="N53" s="46"/>
+    </row>
+    <row r="54" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="39"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="41"/>
+      <c r="E54" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="F45" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="K45" s="47"/>
-      <c r="L45" s="47"/>
-      <c r="N45" s="47"/>
-    </row>
-    <row r="46" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="40"/>
-      <c r="B46" s="41"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="F46" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="G46" s="45"/>
-      <c r="H46" s="45"/>
-      <c r="K46" s="47"/>
-      <c r="L46" s="47"/>
-      <c r="N46" s="47"/>
-    </row>
-    <row r="47" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="40"/>
-      <c r="B47" s="41"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="41" t="s">
+      <c r="F54" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="G54" s="44"/>
+      <c r="H54" s="44"/>
+      <c r="K54" s="46"/>
+      <c r="L54" s="46"/>
+      <c r="N54" s="46"/>
+    </row>
+    <row r="55" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="25">
+        <v>42944</v>
+      </c>
+      <c r="B55" s="40"/>
+      <c r="C55" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D55" s="41"/>
+      <c r="E55" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="F55" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="G55" s="44"/>
+      <c r="H55" s="44"/>
+      <c r="K55" s="46"/>
+      <c r="L55" s="46"/>
+      <c r="N55" s="46"/>
+    </row>
+    <row r="56" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="39"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="F47" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
-      <c r="K47" s="47"/>
-      <c r="L47" s="47"/>
-      <c r="N47" s="47"/>
-    </row>
-    <row r="48" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="40"/>
-      <c r="B48" s="41"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="42"/>
-      <c r="E48" s="41" t="s">
+      <c r="F56" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="G56" s="44"/>
+      <c r="H56" s="44"/>
+      <c r="K56" s="46"/>
+      <c r="L56" s="46"/>
+      <c r="N56" s="46"/>
+    </row>
+    <row r="57" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="39"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="41"/>
+      <c r="E57" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="F48" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="G48" s="45"/>
-      <c r="H48" s="45"/>
-      <c r="K48" s="47"/>
-      <c r="L48" s="47"/>
-      <c r="N48" s="47"/>
-    </row>
-    <row r="49" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="40"/>
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="43" t="s">
-        <v>120</v>
-      </c>
-      <c r="F49" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="G49" s="45"/>
-      <c r="H49" s="45"/>
-      <c r="K49" s="47"/>
-      <c r="L49" s="47"/>
-      <c r="N49" s="47"/>
-    </row>
-    <row r="50" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="40"/>
-      <c r="B50" s="41"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="42"/>
-      <c r="E50" s="41" t="s">
+      <c r="F57" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="G57" s="44"/>
+      <c r="H57" s="44"/>
+      <c r="K57" s="46"/>
+      <c r="L57" s="46"/>
+      <c r="N57" s="46"/>
+    </row>
+    <row r="58" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="25">
+        <v>42944</v>
+      </c>
+      <c r="B58" s="40"/>
+      <c r="C58" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D58" s="41"/>
+      <c r="E58" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="F58" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="G58" s="44"/>
+      <c r="H58" s="44"/>
+      <c r="K58" s="46"/>
+      <c r="L58" s="46"/>
+      <c r="N58" s="46"/>
+    </row>
+    <row r="59" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="39"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="41"/>
+      <c r="E59" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="F50" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="G50" s="45"/>
-      <c r="H50" s="45"/>
-      <c r="K50" s="47"/>
-      <c r="L50" s="47"/>
-      <c r="N50" s="47"/>
-    </row>
-    <row r="51" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="40"/>
-      <c r="B51" s="41"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="41" t="s">
+      <c r="F59" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="G59" s="44"/>
+      <c r="H59" s="44"/>
+      <c r="K59" s="46"/>
+      <c r="L59" s="46"/>
+      <c r="N59" s="46"/>
+    </row>
+    <row r="60" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="39"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="41"/>
+      <c r="E60" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="F51" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="G51" s="45"/>
-      <c r="H51" s="45"/>
-      <c r="K51" s="47"/>
-      <c r="L51" s="47"/>
-      <c r="N51" s="47"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A52" s="26"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="49" t="s">
-        <v>124</v>
-      </c>
-      <c r="D52" s="28" t="s">
+      <c r="F60" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="G60" s="44"/>
+      <c r="H60" s="44"/>
+      <c r="K60" s="46"/>
+      <c r="L60" s="46"/>
+      <c r="N60" s="46"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A61" s="25">
+        <v>42944</v>
+      </c>
+      <c r="B61" s="26"/>
+      <c r="C61" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D61" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E52" s="48" t="s">
-        <v>119</v>
-      </c>
-      <c r="F52" s="30"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="16"/>
-      <c r="J52" s="7"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A53" s="26"/>
-      <c r="B53" s="26"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E53" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="F53" s="30"/>
-      <c r="G53" s="16"/>
-      <c r="H53" s="16"/>
-      <c r="J53" s="7"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A54" s="26"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E54" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="F54" s="30"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="16"/>
-      <c r="J54" s="7"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A55" s="26"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E55" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="F55" s="26"/>
-      <c r="G55" s="16"/>
-      <c r="H55" s="16"/>
-      <c r="J55" s="7"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A56" s="25">
-        <v>42923</v>
-      </c>
-      <c r="B56" s="26"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E56" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="F56" s="26"/>
-      <c r="G56" s="16"/>
-      <c r="H56" s="16"/>
-      <c r="J56" s="7"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A57" s="26"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="27"/>
-      <c r="D57" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E57" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="F57" s="26"/>
-      <c r="G57" s="16"/>
-      <c r="H57" s="16"/>
-      <c r="J57" s="7"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A58" s="26"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="27"/>
-      <c r="D58" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E58" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="F58" s="30"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="J58" s="7"/>
-      <c r="K58" s="11"/>
-      <c r="M58" s="9"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A59" s="26"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E59" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="F59" s="26"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="16"/>
-      <c r="J59" s="7"/>
-      <c r="K59" s="11"/>
-      <c r="M59" s="9"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A60" s="25">
-        <v>42923</v>
-      </c>
-      <c r="B60" s="26"/>
-      <c r="C60" s="27"/>
-      <c r="D60" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E60" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="F60" s="26"/>
-      <c r="G60" s="16"/>
-      <c r="H60" s="16"/>
-      <c r="J60" s="7"/>
-      <c r="K60" s="11"/>
-      <c r="M60" s="9"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A61" s="26"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="27"/>
-      <c r="D61" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E61" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="F61" s="26"/>
+      <c r="E61" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="F61" s="30"/>
       <c r="G61" s="16"/>
       <c r="H61" s="16"/>
       <c r="J61" s="7"/>
-      <c r="K61" s="11"/>
-      <c r="M61" s="9"/>
-    </row>
-    <row r="62" spans="1:14" s="18" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="33"/>
-      <c r="B62" s="33"/>
-      <c r="C62" s="34"/>
-      <c r="D62" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="E62" s="38" t="s">
-        <v>123</v>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A62" s="26"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E62" s="27" t="s">
+        <v>95</v>
       </c>
       <c r="F62" s="30"/>
-      <c r="G62" s="20"/>
-      <c r="H62" s="20"/>
-      <c r="I62" s="21"/>
-      <c r="J62" s="19"/>
-      <c r="K62" s="22"/>
-      <c r="L62" s="22"/>
-      <c r="M62" s="21"/>
-      <c r="N62" s="23"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
+      <c r="J62" s="7"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A63" s="26"/>
@@ -3038,368 +3162,662 @@
       <c r="D63" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E63" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="F63" s="26"/>
-      <c r="G63" s="15"/>
-      <c r="H63" s="15"/>
+      <c r="E63" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="F63" s="30"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="16"/>
       <c r="J63" s="7"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A64" s="25">
-        <v>42923</v>
-      </c>
+      <c r="A64" s="26"/>
       <c r="B64" s="26"/>
       <c r="C64" s="27"/>
       <c r="D64" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E64" s="26" t="s">
-        <v>95</v>
+      <c r="E64" s="38" t="s">
+        <v>96</v>
       </c>
       <c r="F64" s="26"/>
-      <c r="G64" s="7"/>
-      <c r="H64" s="7"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16"/>
       <c r="J64" s="7"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A65" s="26"/>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A65" s="25">
+        <v>42923</v>
+      </c>
       <c r="B65" s="26"/>
       <c r="C65" s="27"/>
       <c r="D65" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E65" s="26" t="s">
-        <v>99</v>
+      <c r="E65" s="27" t="s">
+        <v>95</v>
       </c>
       <c r="F65" s="26"/>
-      <c r="G65" s="7"/>
-      <c r="H65" s="7"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="16"/>
       <c r="J65" s="7"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="7"/>
-      <c r="G67" s="7"/>
-      <c r="H67" s="7"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
-      <c r="E68" s="7"/>
-      <c r="F68" s="7"/>
-      <c r="G68" s="7"/>
-      <c r="H68" s="7"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C69" s="7"/>
-      <c r="D69" s="7"/>
-      <c r="E69" s="7"/>
-      <c r="F69" s="7"/>
-      <c r="G69" s="7"/>
-      <c r="H69" s="7"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C70" s="7"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
-      <c r="G70" s="7"/>
-      <c r="H70" s="7"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C71" s="7"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="7"/>
-      <c r="G71" s="7"/>
-      <c r="H71" s="7"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C72" s="7"/>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="7"/>
-      <c r="G72" s="7"/>
-      <c r="H72" s="7"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C73" s="7"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
-      <c r="F73" s="7"/>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A66" s="26"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E66" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="F66" s="26"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="16"/>
+      <c r="J66" s="7"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A67" s="25">
+        <v>42944</v>
+      </c>
+      <c r="B67" s="26"/>
+      <c r="C67" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D67" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E67" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="F67" s="30"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
+      <c r="J67" s="7"/>
+      <c r="K67" s="11"/>
+      <c r="M67" s="9"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A68" s="26"/>
+      <c r="B68" s="26"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E68" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="F68" s="26"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="16"/>
+      <c r="J68" s="7"/>
+      <c r="K68" s="11"/>
+      <c r="M68" s="9"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A69" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B69" s="26"/>
+      <c r="C69" s="27"/>
+      <c r="D69" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E69" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="F69" s="26"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="16"/>
+      <c r="J69" s="7"/>
+      <c r="K69" s="11"/>
+      <c r="M69" s="9"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A70" s="26"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="27"/>
+      <c r="D70" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E70" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="F70" s="26"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
+      <c r="J70" s="7"/>
+      <c r="K70" s="11"/>
+      <c r="M70" s="9"/>
+    </row>
+    <row r="71" spans="1:14" s="18" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A71" s="25">
+        <v>42944</v>
+      </c>
+      <c r="B71" s="33"/>
+      <c r="C71" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D71" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E71" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="F71" s="30"/>
+      <c r="G71" s="20"/>
+      <c r="H71" s="20"/>
+      <c r="I71" s="21"/>
+      <c r="J71" s="19"/>
+      <c r="K71" s="22"/>
+      <c r="L71" s="22"/>
+      <c r="M71" s="21"/>
+      <c r="N71" s="23"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A72" s="26"/>
+      <c r="B72" s="26"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E72" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="F72" s="26"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
+      <c r="J72" s="7"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A73" s="25">
+        <v>42923</v>
+      </c>
+      <c r="B73" s="26"/>
+      <c r="C73" s="27"/>
+      <c r="D73" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E73" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="F73" s="26"/>
       <c r="G73" s="7"/>
       <c r="H73" s="7"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="7"/>
-      <c r="F74" s="7"/>
+      <c r="J73" s="7"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A74" s="26"/>
+      <c r="B74" s="26"/>
+      <c r="C74" s="27"/>
+      <c r="D74" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E74" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="F74" s="26"/>
       <c r="G74" s="7"/>
       <c r="H74" s="7"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="7"/>
-      <c r="G75" s="7"/>
-      <c r="H75" s="7"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C76" s="7"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="7"/>
-      <c r="F76" s="7"/>
-      <c r="G76" s="7"/>
-      <c r="H76" s="7"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C77" s="7"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="7"/>
-      <c r="F77" s="7"/>
-      <c r="G77" s="7"/>
-      <c r="H77" s="7"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C78" s="7"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
-      <c r="F78" s="7"/>
-      <c r="G78" s="7"/>
-      <c r="H78" s="7"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C79" s="7"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7"/>
-      <c r="F79" s="7"/>
-      <c r="G79" s="7"/>
-      <c r="H79" s="7"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C80" s="7"/>
-      <c r="D80" s="7"/>
-      <c r="E80" s="7"/>
-      <c r="F80" s="7"/>
+      <c r="J74" s="7"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A75" s="25">
+        <v>42944</v>
+      </c>
+      <c r="B75" s="26"/>
+      <c r="C75" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D75" s="26"/>
+      <c r="E75" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="F75" s="26"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A76" s="26"/>
+      <c r="B76" s="26"/>
+      <c r="C76" s="26"/>
+      <c r="D76" s="26"/>
+      <c r="E76" s="26"/>
+      <c r="F76" s="26"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A77" s="25">
+        <v>42944</v>
+      </c>
+      <c r="B77" s="26"/>
+      <c r="C77" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D77" s="26"/>
+      <c r="E77" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F77" s="26"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A78" s="26"/>
+      <c r="B78" s="26"/>
+      <c r="C78" s="26"/>
+      <c r="D78" s="26"/>
+      <c r="E78" s="26"/>
+      <c r="F78" s="26"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A79" s="26"/>
+      <c r="B79" s="26"/>
+      <c r="C79" s="26"/>
+      <c r="D79" s="26"/>
+      <c r="E79" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="F79" s="26"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A80" s="25">
+        <v>42944</v>
+      </c>
+      <c r="B80" s="26"/>
+      <c r="C80" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D80" s="27"/>
+      <c r="E80" s="27"/>
+      <c r="F80" s="27"/>
       <c r="G80" s="7"/>
       <c r="H80" s="7"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A81" s="26"/>
+      <c r="B81" s="26"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
+      <c r="E81" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="F81" s="27"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A82" s="25">
+        <v>42944</v>
+      </c>
+      <c r="B82" s="26"/>
+      <c r="C82" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D82" s="27"/>
+      <c r="E82" s="26"/>
+      <c r="F82" s="27"/>
+      <c r="G82" s="7"/>
+      <c r="H82" s="7"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A83" s="26"/>
+      <c r="B83" s="26"/>
+      <c r="C83" s="27"/>
+      <c r="D83" s="27"/>
+      <c r="E83" s="27"/>
+      <c r="F83" s="27"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="7"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A84" s="26"/>
+      <c r="B84" s="26"/>
+      <c r="C84" s="27"/>
+      <c r="D84" s="27"/>
+      <c r="E84" s="27"/>
+      <c r="F84" s="27"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="7"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7"/>
+      <c r="H86" s="7"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7"/>
+      <c r="G87" s="7"/>
+      <c r="H87" s="7"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C88" s="7"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="7"/>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7"/>
+      <c r="H88" s="7"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C89" s="7"/>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7"/>
+      <c r="H89" s="7"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C90" s="7"/>
+      <c r="D90" s="7"/>
+      <c r="E90" s="7"/>
+      <c r="F90" s="7"/>
+      <c r="G90" s="7"/>
+      <c r="H90" s="7"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C91" s="7"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="7"/>
+      <c r="F91" s="7"/>
+      <c r="G91" s="7"/>
+      <c r="H91" s="7"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C92" s="7"/>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7"/>
+      <c r="F92" s="7"/>
+      <c r="G92" s="7"/>
+      <c r="H92" s="7"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C93" s="7"/>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
+      <c r="F93" s="7"/>
+      <c r="G93" s="7"/>
+      <c r="H93" s="7"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="J1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A42:A51">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="87">
+  <conditionalFormatting sqref="A4:A7 A51 A53:A54 A56:A57 A59:A60">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="136">
+      <formula>LEN(TRIM(A4))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="80">
+      <formula>LEN(TRIM(A65))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="notContainsBlanks" dxfId="49" priority="79">
+      <formula>LEN(TRIM(A69))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A73">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="78">
+      <formula>LEN(TRIM(A73))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="48">
+      <formula>LEN(TRIM(A8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="47">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="46">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11:A13">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="45">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="44">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="43">
+      <formula>LEN(TRIM(A26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="42">
+      <formula>LEN(TRIM(A35))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="41">
+      <formula>LEN(TRIM(A36))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="40">
+      <formula>LEN(TRIM(A39))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:A15">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="39">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="38">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="37">
+      <formula>LEN(TRIM(A18))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="36">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="35">
+      <formula>LEN(TRIM(A19))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="34">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="33">
+      <formula>LEN(TRIM(A21))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="32">
+      <formula>LEN(TRIM(A22))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="31">
+      <formula>LEN(TRIM(A24))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="30">
+      <formula>LEN(TRIM(A25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="29">
+      <formula>LEN(TRIM(A27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="28">
+      <formula>LEN(TRIM(A28))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="27">
+      <formula>LEN(TRIM(A29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="26">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="25">
+      <formula>LEN(TRIM(A31))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="24">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="23">
+      <formula>LEN(TRIM(A33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="22">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="21">
+      <formula>LEN(TRIM(A37))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="20">
+      <formula>LEN(TRIM(A38))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="19">
+      <formula>LEN(TRIM(A40))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="18">
+      <formula>LEN(TRIM(A41))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="17">
       <formula>LEN(TRIM(A42))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A6">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="72">
-      <formula>LEN(TRIM(A3))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="37">
-      <formula>LEN(TRIM(A9))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="38">
-      <formula>LEN(TRIM(A8))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="16">
-      <formula>LEN(TRIM(A21))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="15">
-      <formula>LEN(TRIM(A23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24">
-    <cfRule type="notContainsBlanks" dxfId="35" priority="14">
-      <formula>LEN(TRIM(A24))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="13">
-      <formula>LEN(TRIM(A26))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="12">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="11">
-      <formula>LEN(TRIM(A28))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="10">
-      <formula>LEN(TRIM(A29))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
-    <cfRule type="notContainsBlanks" dxfId="30" priority="9">
-      <formula>LEN(TRIM(A30))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="8">
-      <formula>LEN(TRIM(A31))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="5">
-      <formula>LEN(TRIM(A36))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="36">
-      <formula>LEN(TRIM(A16))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="39">
-      <formula>LEN(TRIM(A7))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="35">
-      <formula>LEN(TRIM(A22))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="34">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="33">
-      <formula>LEN(TRIM(A40))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="31">
-      <formula>LEN(TRIM(A56))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="30">
-      <formula>LEN(TRIM(A60))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A64">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="29">
-      <formula>LEN(TRIM(A64))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="28">
-      <formula>LEN(TRIM(A10))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="27">
-      <formula>LEN(TRIM(A11))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="26">
-      <formula>LEN(TRIM(A34))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="25">
-      <formula>LEN(TRIM(A35))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="24">
-      <formula>LEN(TRIM(A12))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="23">
-      <formula>LEN(TRIM(A13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="22">
-      <formula>LEN(TRIM(A14))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="21">
-      <formula>LEN(TRIM(A15))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="20">
-      <formula>LEN(TRIM(A17))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="19">
-      <formula>LEN(TRIM(A18))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="18">
-      <formula>LEN(TRIM(A19))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="17">
-      <formula>LEN(TRIM(A20))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="7">
-      <formula>LEN(TRIM(A32))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
+  <conditionalFormatting sqref="A43">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="16">
+      <formula>LEN(TRIM(A43))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
+      <formula>LEN(TRIM(A44))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48:A50">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
+      <formula>LEN(TRIM(A48))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
+      <formula>LEN(TRIM(A52))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
+      <formula>LEN(TRIM(A55))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
+      <formula>LEN(TRIM(A58))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
+      <formula>LEN(TRIM(A61))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
+      <formula>LEN(TRIM(A67))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(A71))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A75">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(A75))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A77">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(A77))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A80">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(A80))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82">
     <cfRule type="notContainsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(A37))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
+      <formula>LEN(TRIM(A82))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45">
     <cfRule type="notContainsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(A38))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A39">
+      <formula>LEN(TRIM(A45))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(A39))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41">
+      <formula>LEN(TRIM(A46))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A41))&gt;0</formula>
+      <formula>LEN(TRIM(A47))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working on VS result triples.
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="139">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -372,9 +372,6 @@
     <t>VS</t>
   </si>
   <si>
-    <t>Not yet in file from AO: 2017-07-07</t>
-  </si>
-  <si>
     <t>See greyed out section, below.</t>
   </si>
   <si>
@@ -439,6 +436,9 @@
   </si>
   <si>
     <t>cdiscpilot01:WeightMassOutcome_1</t>
+  </si>
+  <si>
+    <t>decimal point issue in hasValue. Email to AO.</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1056,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1120,17 +1120,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="38" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1185,7 +1175,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="53">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1863,8 +1860,8 @@
   <dimension ref="A1:N94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
+      <pane ySplit="3" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1888,10 +1885,10 @@
       <c r="C1" t="s">
         <v>103</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="49"/>
+      <c r="K1" s="41"/>
       <c r="L1" s="10" t="s">
         <v>44</v>
       </c>
@@ -1901,7 +1898,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J2" s="35"/>
       <c r="K2" s="36"/>
@@ -1963,7 +1960,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -2729,8 +2726,8 @@
       <c r="E38" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="F38" s="43" t="s">
-        <v>117</v>
+      <c r="F38" s="39" t="s">
+        <v>116</v>
       </c>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
@@ -2823,21 +2820,19 @@
       <c r="J43" s="7"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A44" s="51">
-        <v>42944</v>
-      </c>
+      <c r="A44" s="43"/>
       <c r="B44" s="26"/>
       <c r="C44" s="30" t="s">
         <v>94</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="E44" s="50" t="s">
-        <v>125</v>
+        <v>133</v>
+      </c>
+      <c r="E44" s="42" t="s">
+        <v>124</v>
       </c>
       <c r="F44" s="32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G44" s="16"/>
       <c r="H44" s="16"/>
@@ -2869,11 +2864,11 @@
       <c r="D46" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E46" s="52" t="s">
-        <v>132</v>
+      <c r="E46" s="44" t="s">
+        <v>131</v>
       </c>
       <c r="F46" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G46" s="16"/>
       <c r="H46" s="16"/>
@@ -2889,7 +2884,7 @@
         <v>69</v>
       </c>
       <c r="E47" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F47" s="32"/>
       <c r="G47" s="16"/>
@@ -2897,19 +2892,17 @@
       <c r="J47" s="7"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A48" s="25">
-        <v>42944</v>
-      </c>
+      <c r="A48" s="25"/>
       <c r="B48" s="26"/>
       <c r="C48" s="30" t="s">
         <v>94</v>
       </c>
       <c r="D48" s="28"/>
-      <c r="E48" s="50" t="s">
-        <v>126</v>
+      <c r="E48" s="42" t="s">
+        <v>125</v>
       </c>
       <c r="F48" s="32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G48" s="16"/>
       <c r="H48" s="16"/>
@@ -2931,195 +2924,185 @@
       <c r="J49" s="7"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A50" s="25"/>
+      <c r="A50" s="25">
+        <v>42944</v>
+      </c>
       <c r="B50" s="26"/>
       <c r="C50" s="30"/>
       <c r="D50" s="28"/>
-      <c r="E50" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="F50" s="32"/>
+      <c r="E50" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="F50" s="32" t="s">
+        <v>135</v>
+      </c>
       <c r="G50" s="16"/>
       <c r="H50" s="16"/>
       <c r="J50" s="7"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A51" s="25"/>
+      <c r="A51" s="25">
+        <v>42944</v>
+      </c>
       <c r="B51" s="26"/>
       <c r="C51" s="27"/>
       <c r="D51" s="28"/>
-      <c r="E51" s="27" t="s">
+      <c r="E51" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="F51" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="F51" s="32"/>
       <c r="G51" s="16"/>
       <c r="H51" s="16"/>
       <c r="J51" s="7"/>
     </row>
-    <row r="52" spans="1:14" s="45" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" s="7" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="25">
         <v>42944</v>
       </c>
-      <c r="B52" s="40"/>
+      <c r="B52" s="28"/>
       <c r="C52" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="D52" s="41"/>
-      <c r="E52" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="F52" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="G52" s="44"/>
-      <c r="H52" s="44"/>
-      <c r="K52" s="46"/>
-      <c r="L52" s="46"/>
-      <c r="N52" s="46"/>
-    </row>
-    <row r="53" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="39"/>
-      <c r="B53" s="40"/>
-      <c r="C53" s="40"/>
-      <c r="D53" s="41"/>
-      <c r="E53" s="40" t="s">
+      <c r="D52" s="28"/>
+      <c r="E52" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="F52" s="32"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="11"/>
+      <c r="N52" s="11"/>
+    </row>
+    <row r="53" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="28"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="F53" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="G53" s="44"/>
-      <c r="H53" s="44"/>
-      <c r="K53" s="46"/>
-      <c r="L53" s="46"/>
-      <c r="N53" s="46"/>
-    </row>
-    <row r="54" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="39"/>
-      <c r="B54" s="40"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="41"/>
-      <c r="E54" s="40" t="s">
+      <c r="F53" s="32"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="K53" s="11"/>
+      <c r="L53" s="11"/>
+      <c r="N53" s="11"/>
+    </row>
+    <row r="54" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="28"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="F54" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="G54" s="44"/>
-      <c r="H54" s="44"/>
-      <c r="K54" s="46"/>
-      <c r="L54" s="46"/>
-      <c r="N54" s="46"/>
-    </row>
-    <row r="55" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F54" s="32"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+      <c r="K54" s="11"/>
+      <c r="L54" s="11"/>
+      <c r="N54" s="11"/>
+    </row>
+    <row r="55" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="25">
         <v>42944</v>
       </c>
-      <c r="B55" s="40"/>
+      <c r="B55" s="28"/>
       <c r="C55" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="41"/>
-      <c r="E55" s="42" t="s">
-        <v>120</v>
-      </c>
-      <c r="F55" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="G55" s="44"/>
-      <c r="H55" s="44"/>
-      <c r="K55" s="46"/>
-      <c r="L55" s="46"/>
-      <c r="N55" s="46"/>
-    </row>
-    <row r="56" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="39"/>
-      <c r="B56" s="40"/>
-      <c r="C56" s="40"/>
-      <c r="D56" s="41"/>
-      <c r="E56" s="40" t="s">
+      <c r="D55" s="28"/>
+      <c r="E55" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="F55" s="32"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="11"/>
+      <c r="N55" s="11"/>
+    </row>
+    <row r="56" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="28"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="F56" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="G56" s="44"/>
-      <c r="H56" s="44"/>
-      <c r="K56" s="46"/>
-      <c r="L56" s="46"/>
-      <c r="N56" s="46"/>
-    </row>
-    <row r="57" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="39"/>
-      <c r="B57" s="40"/>
-      <c r="C57" s="40"/>
-      <c r="D57" s="41"/>
-      <c r="E57" s="40" t="s">
+      <c r="F56" s="32"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="N56" s="11"/>
+    </row>
+    <row r="57" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="28"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="F57" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="G57" s="44"/>
-      <c r="H57" s="44"/>
-      <c r="K57" s="46"/>
-      <c r="L57" s="46"/>
-      <c r="N57" s="46"/>
-    </row>
-    <row r="58" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F57" s="32"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="16"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="11"/>
+      <c r="N57" s="11"/>
+    </row>
+    <row r="58" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="25">
         <v>42944</v>
       </c>
-      <c r="B58" s="40"/>
+      <c r="B58" s="28"/>
       <c r="C58" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="D58" s="41"/>
-      <c r="E58" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="F58" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="G58" s="44"/>
-      <c r="H58" s="44"/>
-      <c r="K58" s="46"/>
-      <c r="L58" s="46"/>
-      <c r="N58" s="46"/>
-    </row>
-    <row r="59" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="39"/>
-      <c r="B59" s="40"/>
-      <c r="C59" s="40"/>
-      <c r="D59" s="41"/>
-      <c r="E59" s="40" t="s">
+      <c r="D58" s="28"/>
+      <c r="E58" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="F58" s="32"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="11"/>
+      <c r="N58" s="11"/>
+    </row>
+    <row r="59" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="28"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="F59" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="G59" s="44"/>
-      <c r="H59" s="44"/>
-      <c r="K59" s="46"/>
-      <c r="L59" s="46"/>
-      <c r="N59" s="46"/>
-    </row>
-    <row r="60" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="39"/>
-      <c r="B60" s="40"/>
-      <c r="C60" s="40"/>
-      <c r="D60" s="41"/>
-      <c r="E60" s="40" t="s">
+      <c r="F59" s="32"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="K59" s="11"/>
+      <c r="L59" s="11"/>
+      <c r="N59" s="11"/>
+    </row>
+    <row r="60" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="28"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="F60" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="G60" s="44"/>
-      <c r="H60" s="44"/>
-      <c r="K60" s="46"/>
-      <c r="L60" s="46"/>
-      <c r="N60" s="46"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="16"/>
+      <c r="K60" s="11"/>
+      <c r="L60" s="11"/>
+      <c r="N60" s="11"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A61" s="25">
@@ -3132,8 +3115,8 @@
       <c r="D61" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E61" s="47" t="s">
-        <v>118</v>
+      <c r="E61" s="37" t="s">
+        <v>117</v>
       </c>
       <c r="F61" s="30"/>
       <c r="G61" s="16"/>
@@ -3229,7 +3212,7 @@
         <v>69</v>
       </c>
       <c r="E67" s="37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F67" s="30"/>
       <c r="G67" s="16"/>
@@ -3303,7 +3286,7 @@
         <v>69</v>
       </c>
       <c r="E71" s="37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F71" s="30"/>
       <c r="G71" s="20"/>
@@ -3372,7 +3355,7 @@
       </c>
       <c r="D75" s="26"/>
       <c r="E75" s="37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F75" s="26"/>
     </row>
@@ -3394,7 +3377,7 @@
       </c>
       <c r="D77" s="26"/>
       <c r="E77" s="37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F77" s="26"/>
     </row>
@@ -3412,7 +3395,7 @@
       <c r="C79" s="26"/>
       <c r="D79" s="26"/>
       <c r="E79" s="37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F79" s="26"/>
     </row>
@@ -3436,7 +3419,7 @@
       <c r="C81" s="27"/>
       <c r="D81" s="27"/>
       <c r="E81" s="37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F81" s="27"/>
       <c r="G81" s="7"/>
@@ -3560,264 +3543,269 @@
   <mergeCells count="1">
     <mergeCell ref="J1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A4:A7 A51 A53:A54 A56:A57 A59:A60">
-    <cfRule type="notContainsBlanks" dxfId="51" priority="136">
+  <conditionalFormatting sqref="A4:A7">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="137">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="81">
+      <formula>LEN(TRIM(A65))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
     <cfRule type="notContainsBlanks" dxfId="50" priority="80">
-      <formula>LEN(TRIM(A65))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
+      <formula>LEN(TRIM(A69))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A73">
     <cfRule type="notContainsBlanks" dxfId="49" priority="79">
-      <formula>LEN(TRIM(A69))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A73">
-    <cfRule type="notContainsBlanks" dxfId="48" priority="78">
       <formula>LEN(TRIM(A73))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="49">
+      <formula>LEN(TRIM(A8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
     <cfRule type="notContainsBlanks" dxfId="47" priority="48">
-      <formula>LEN(TRIM(A8))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
     <cfRule type="notContainsBlanks" dxfId="46" priority="47">
-      <formula>LEN(TRIM(A9))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11:A13">
     <cfRule type="notContainsBlanks" dxfId="45" priority="46">
-      <formula>LEN(TRIM(A10))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11:A13">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
     <cfRule type="notContainsBlanks" dxfId="44" priority="45">
-      <formula>LEN(TRIM(A11))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26">
     <cfRule type="notContainsBlanks" dxfId="43" priority="44">
-      <formula>LEN(TRIM(A23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
+      <formula>LEN(TRIM(A26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
     <cfRule type="notContainsBlanks" dxfId="42" priority="43">
-      <formula>LEN(TRIM(A26))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35">
+      <formula>LEN(TRIM(A35))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
     <cfRule type="notContainsBlanks" dxfId="41" priority="42">
-      <formula>LEN(TRIM(A35))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
+      <formula>LEN(TRIM(A36))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39">
     <cfRule type="notContainsBlanks" dxfId="40" priority="41">
-      <formula>LEN(TRIM(A36))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A39">
+      <formula>LEN(TRIM(A39))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:A15">
     <cfRule type="notContainsBlanks" dxfId="39" priority="40">
-      <formula>LEN(TRIM(A39))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:A15">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
     <cfRule type="notContainsBlanks" dxfId="38" priority="39">
-      <formula>LEN(TRIM(A14))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
     <cfRule type="notContainsBlanks" dxfId="37" priority="38">
-      <formula>LEN(TRIM(A17))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
+      <formula>LEN(TRIM(A18))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
     <cfRule type="notContainsBlanks" dxfId="36" priority="37">
-      <formula>LEN(TRIM(A18))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19">
     <cfRule type="notContainsBlanks" dxfId="35" priority="36">
-      <formula>LEN(TRIM(A16))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
+      <formula>LEN(TRIM(A19))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20">
     <cfRule type="notContainsBlanks" dxfId="34" priority="35">
-      <formula>LEN(TRIM(A19))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
     <cfRule type="notContainsBlanks" dxfId="33" priority="34">
-      <formula>LEN(TRIM(A20))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
+      <formula>LEN(TRIM(A21))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
     <cfRule type="notContainsBlanks" dxfId="32" priority="33">
-      <formula>LEN(TRIM(A21))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
+      <formula>LEN(TRIM(A22))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
     <cfRule type="notContainsBlanks" dxfId="31" priority="32">
-      <formula>LEN(TRIM(A22))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24">
+      <formula>LEN(TRIM(A24))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
     <cfRule type="notContainsBlanks" dxfId="30" priority="31">
-      <formula>LEN(TRIM(A24))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
+      <formula>LEN(TRIM(A25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27">
     <cfRule type="notContainsBlanks" dxfId="29" priority="30">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
+      <formula>LEN(TRIM(A27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28">
     <cfRule type="notContainsBlanks" dxfId="28" priority="29">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
+      <formula>LEN(TRIM(A28))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29">
     <cfRule type="notContainsBlanks" dxfId="27" priority="28">
-      <formula>LEN(TRIM(A28))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29">
+      <formula>LEN(TRIM(A29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
     <cfRule type="notContainsBlanks" dxfId="26" priority="27">
-      <formula>LEN(TRIM(A29))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31">
     <cfRule type="notContainsBlanks" dxfId="25" priority="26">
-      <formula>LEN(TRIM(A30))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
+      <formula>LEN(TRIM(A31))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
     <cfRule type="notContainsBlanks" dxfId="24" priority="25">
-      <formula>LEN(TRIM(A31))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
     <cfRule type="notContainsBlanks" dxfId="23" priority="24">
-      <formula>LEN(TRIM(A32))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
+      <formula>LEN(TRIM(A33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
     <cfRule type="notContainsBlanks" dxfId="22" priority="23">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
     <cfRule type="notContainsBlanks" dxfId="21" priority="22">
-      <formula>LEN(TRIM(A34))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
+      <formula>LEN(TRIM(A37))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38">
     <cfRule type="notContainsBlanks" dxfId="20" priority="21">
-      <formula>LEN(TRIM(A37))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
+      <formula>LEN(TRIM(A38))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
     <cfRule type="notContainsBlanks" dxfId="19" priority="20">
-      <formula>LEN(TRIM(A38))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
+      <formula>LEN(TRIM(A40))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41">
     <cfRule type="notContainsBlanks" dxfId="18" priority="19">
-      <formula>LEN(TRIM(A40))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41">
+      <formula>LEN(TRIM(A41))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42">
     <cfRule type="notContainsBlanks" dxfId="17" priority="18">
-      <formula>LEN(TRIM(A41))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A42">
+      <formula>LEN(TRIM(A42))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43">
     <cfRule type="notContainsBlanks" dxfId="16" priority="17">
-      <formula>LEN(TRIM(A42))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A43">
+      <formula>LEN(TRIM(A43))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44">
     <cfRule type="notContainsBlanks" dxfId="15" priority="16">
-      <formula>LEN(TRIM(A43))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A44">
+      <formula>LEN(TRIM(A44))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48:A50">
     <cfRule type="notContainsBlanks" dxfId="14" priority="15">
-      <formula>LEN(TRIM(A44))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48:A50">
+      <formula>LEN(TRIM(A48))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52">
     <cfRule type="notContainsBlanks" dxfId="13" priority="14">
-      <formula>LEN(TRIM(A48))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A52">
+      <formula>LEN(TRIM(A52))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55">
     <cfRule type="notContainsBlanks" dxfId="12" priority="13">
-      <formula>LEN(TRIM(A52))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55">
+      <formula>LEN(TRIM(A55))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58">
     <cfRule type="notContainsBlanks" dxfId="11" priority="12">
-      <formula>LEN(TRIM(A55))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A58">
+      <formula>LEN(TRIM(A58))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61">
     <cfRule type="notContainsBlanks" dxfId="10" priority="11">
-      <formula>LEN(TRIM(A58))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61">
+      <formula>LEN(TRIM(A61))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67">
     <cfRule type="notContainsBlanks" dxfId="9" priority="10">
-      <formula>LEN(TRIM(A61))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67">
+      <formula>LEN(TRIM(A67))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71">
     <cfRule type="notContainsBlanks" dxfId="8" priority="9">
-      <formula>LEN(TRIM(A67))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71">
+      <formula>LEN(TRIM(A71))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A75">
     <cfRule type="notContainsBlanks" dxfId="7" priority="8">
-      <formula>LEN(TRIM(A71))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A75">
+      <formula>LEN(TRIM(A75))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A77">
     <cfRule type="notContainsBlanks" dxfId="6" priority="7">
-      <formula>LEN(TRIM(A75))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A77">
+      <formula>LEN(TRIM(A77))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A80">
     <cfRule type="notContainsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(A77))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A80">
+      <formula>LEN(TRIM(A80))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82">
     <cfRule type="notContainsBlanks" dxfId="4" priority="5">
-      <formula>LEN(TRIM(A80))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A82">
+      <formula>LEN(TRIM(A82))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45">
     <cfRule type="notContainsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(A82))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45">
+      <formula>LEN(TRIM(A45))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46">
     <cfRule type="notContainsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(A45))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46">
+      <formula>LEN(TRIM(A46))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(A46))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
+      <formula>LEN(TRIM(A47))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A47))&gt;0</formula>
+      <formula>LEN(TRIM(A51))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
WIP for VS. Next: StartRule Creation and Resolution.
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -438,7 +438,7 @@
     <t>cdiscpilot01:WeightMassOutcome_1</t>
   </si>
   <si>
-    <t>decimal point issue in hasValue. Email to AO.</t>
+    <t>decimal point issue in hasValue. Label should be value + unit (119.0 LB) Email to AO.</t>
   </si>
 </sst>
 </file>
@@ -1121,15 +1121,15 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="39" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="39" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1859,9 +1859,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1885,10 +1885,10 @@
       <c r="C1" t="s">
         <v>103</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="41"/>
+      <c r="K1" s="44"/>
       <c r="L1" s="10" t="s">
         <v>44</v>
       </c>
@@ -2820,7 +2820,7 @@
       <c r="J43" s="7"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A44" s="43"/>
+      <c r="A44" s="41"/>
       <c r="B44" s="26"/>
       <c r="C44" s="30" t="s">
         <v>94</v>
@@ -2828,7 +2828,7 @@
       <c r="D44" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="E44" s="42" t="s">
+      <c r="E44" s="40" t="s">
         <v>124</v>
       </c>
       <c r="F44" s="32" t="s">
@@ -2864,7 +2864,7 @@
       <c r="D46" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E46" s="44" t="s">
+      <c r="E46" s="42" t="s">
         <v>131</v>
       </c>
       <c r="F46" s="32" t="s">
@@ -2898,7 +2898,7 @@
         <v>94</v>
       </c>
       <c r="D48" s="28"/>
-      <c r="E48" s="42" t="s">
+      <c r="E48" s="40" t="s">
         <v>125</v>
       </c>
       <c r="F48" s="32" t="s">
@@ -2930,7 +2930,7 @@
       <c r="B50" s="26"/>
       <c r="C50" s="30"/>
       <c r="D50" s="28"/>
-      <c r="E50" s="44" t="s">
+      <c r="E50" s="42" t="s">
         <v>131</v>
       </c>
       <c r="F50" s="32" t="s">
@@ -2947,7 +2947,7 @@
       <c r="B51" s="26"/>
       <c r="C51" s="27"/>
       <c r="D51" s="28"/>
-      <c r="E51" s="44" t="s">
+      <c r="E51" s="42" t="s">
         <v>137</v>
       </c>
       <c r="F51" s="32" t="s">

</xml_diff>

<commit_message>
ready to fix issue in createFrag_F.R
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -1175,7 +1175,231 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="85">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1859,9 +2083,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1945,7 +2169,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>100</v>
@@ -1967,7 +2191,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>100</v>
@@ -1987,7 +2211,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B6" s="26" t="s">
         <v>100</v>
@@ -2009,7 +2233,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B7" s="26" t="s">
         <v>100</v>
@@ -2029,7 +2253,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B8" s="26" t="s">
         <v>100</v>
@@ -2053,7 +2277,7 @@
     </row>
     <row r="9" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B9" s="26" t="s">
         <v>100</v>
@@ -2074,7 +2298,7 @@
     </row>
     <row r="10" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>100</v>
@@ -2097,7 +2321,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B11" s="26" t="s">
         <v>100</v>
@@ -2119,7 +2343,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>100</v>
@@ -2144,7 +2368,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B13" s="26" t="s">
         <v>100</v>
@@ -2169,7 +2393,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B14" s="26" t="s">
         <v>100</v>
@@ -2194,7 +2418,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B15" s="26" t="s">
         <v>100</v>
@@ -2219,7 +2443,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B16" s="26" t="s">
         <v>100</v>
@@ -2248,7 +2472,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B17" s="26" t="s">
         <v>100</v>
@@ -2275,7 +2499,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>100</v>
@@ -2302,7 +2526,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B19" s="26" t="s">
         <v>100</v>
@@ -2325,7 +2549,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>100</v>
@@ -2348,7 +2572,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>100</v>
@@ -2368,7 +2592,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B22" s="26" t="s">
         <v>100</v>
@@ -2386,7 +2610,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B23" s="26" t="s">
         <v>100</v>
@@ -2404,7 +2628,7 @@
     </row>
     <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>100</v>
@@ -2429,7 +2653,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B25" s="26" t="s">
         <v>100</v>
@@ -2454,7 +2678,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B26" s="26" t="s">
         <v>100</v>
@@ -2479,7 +2703,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B27" s="27" t="s">
         <v>61</v>
@@ -2502,7 +2726,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B28" s="27" t="s">
         <v>61</v>
@@ -2525,7 +2749,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B29" s="27" t="s">
         <v>61</v>
@@ -2550,9 +2774,7 @@
       <c r="J29" s="7"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A30" s="25">
-        <v>42942</v>
-      </c>
+      <c r="A30" s="25"/>
       <c r="B30" s="27"/>
       <c r="C30" s="31" t="s">
         <v>0</v>
@@ -2574,9 +2796,7 @@
       <c r="N30" s="4"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A31" s="25">
-        <v>42942</v>
-      </c>
+      <c r="A31" s="25"/>
       <c r="B31" s="26"/>
       <c r="C31" s="27"/>
       <c r="D31" s="27" t="s">
@@ -2594,9 +2814,7 @@
       <c r="N31" s="4"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A32" s="25">
-        <v>42942</v>
-      </c>
+      <c r="A32" s="25"/>
       <c r="B32" s="26"/>
       <c r="C32" s="27"/>
       <c r="D32" s="27" t="s">
@@ -2614,9 +2832,7 @@
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A33" s="25">
-        <v>42942</v>
-      </c>
+      <c r="A33" s="25"/>
       <c r="B33" s="26"/>
       <c r="C33" s="27" t="s">
         <v>0</v>
@@ -2632,9 +2848,7 @@
       <c r="H33" s="7"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="25">
-        <v>42942</v>
-      </c>
+      <c r="A34" s="25"/>
       <c r="B34" s="26"/>
       <c r="C34" s="27"/>
       <c r="D34" s="28" t="s">
@@ -2649,7 +2863,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B35" s="26"/>
       <c r="C35" s="27"/>
@@ -2671,7 +2885,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B36" s="26"/>
       <c r="C36" s="27"/>
@@ -2689,9 +2903,7 @@
       <c r="M36" s="9"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="25">
-        <v>42942</v>
-      </c>
+      <c r="A37" s="25"/>
       <c r="B37" s="26" t="s">
         <v>100</v>
       </c>
@@ -2711,9 +2923,7 @@
       <c r="K37" s="2"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="25">
-        <v>42942</v>
-      </c>
+      <c r="A38" s="25"/>
       <c r="B38" s="27" t="s">
         <v>115</v>
       </c>
@@ -2734,9 +2944,7 @@
       <c r="J38" s="7"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="25">
-        <v>42942</v>
-      </c>
+      <c r="A39" s="25"/>
       <c r="B39" s="26"/>
       <c r="C39" s="27"/>
       <c r="D39" s="28" t="s">
@@ -2750,9 +2958,7 @@
       <c r="H39" s="7"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A40" s="25">
-        <v>42942</v>
-      </c>
+      <c r="A40" s="25"/>
       <c r="B40" s="26"/>
       <c r="C40" s="30" t="s">
         <v>94</v>
@@ -2769,7 +2975,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B41" s="26"/>
       <c r="C41" s="27"/>
@@ -2784,9 +2990,7 @@
       <c r="H41" s="16"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42" s="25">
-        <v>42942</v>
-      </c>
+      <c r="A42" s="25"/>
       <c r="B42" s="26"/>
       <c r="C42" s="30" t="s">
         <v>94</v>
@@ -2804,7 +3008,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="25">
-        <v>42942</v>
+        <v>42956</v>
       </c>
       <c r="B43" s="26"/>
       <c r="C43" s="27"/>
@@ -2840,7 +3044,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="25">
-        <v>42944</v>
+        <v>42956</v>
       </c>
       <c r="B45" s="26"/>
       <c r="C45" s="27"/>
@@ -2856,9 +3060,7 @@
       <c r="J45" s="7"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A46" s="25">
-        <v>42944</v>
-      </c>
+      <c r="A46" s="25"/>
       <c r="B46" s="26"/>
       <c r="C46" s="27"/>
       <c r="D46" s="28" t="s">
@@ -2875,9 +3077,7 @@
       <c r="J46" s="7"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A47" s="25">
-        <v>42944</v>
-      </c>
+      <c r="A47" s="25"/>
       <c r="B47" s="26"/>
       <c r="C47" s="27"/>
       <c r="D47" s="28" t="s">
@@ -2910,7 +3110,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" s="25">
-        <v>42944</v>
+        <v>42956</v>
       </c>
       <c r="B49" s="26"/>
       <c r="C49" s="30"/>
@@ -2924,9 +3124,7 @@
       <c r="J49" s="7"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A50" s="25">
-        <v>42944</v>
-      </c>
+      <c r="A50" s="25"/>
       <c r="B50" s="26"/>
       <c r="C50" s="30"/>
       <c r="D50" s="28"/>
@@ -2941,9 +3139,7 @@
       <c r="J50" s="7"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A51" s="25">
-        <v>42944</v>
-      </c>
+      <c r="A51" s="25"/>
       <c r="B51" s="26"/>
       <c r="C51" s="27"/>
       <c r="D51" s="28"/>
@@ -2958,9 +3154,7 @@
       <c r="J51" s="7"/>
     </row>
     <row r="52" spans="1:14" s="7" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="25">
-        <v>42944</v>
-      </c>
+      <c r="A52" s="25"/>
       <c r="B52" s="28"/>
       <c r="C52" s="30" t="s">
         <v>94</v>
@@ -3007,9 +3201,7 @@
       <c r="N54" s="11"/>
     </row>
     <row r="55" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="25">
-        <v>42944</v>
-      </c>
+      <c r="A55" s="25"/>
       <c r="B55" s="28"/>
       <c r="C55" s="30" t="s">
         <v>94</v>
@@ -3026,7 +3218,9 @@
       <c r="N55" s="11"/>
     </row>
     <row r="56" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="28"/>
+      <c r="A56" s="25">
+        <v>42956</v>
+      </c>
       <c r="B56" s="28"/>
       <c r="C56" s="28"/>
       <c r="D56" s="28"/>
@@ -3056,9 +3250,7 @@
       <c r="N57" s="11"/>
     </row>
     <row r="58" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="25">
-        <v>42944</v>
-      </c>
+      <c r="A58" s="25"/>
       <c r="B58" s="28"/>
       <c r="C58" s="30" t="s">
         <v>94</v>
@@ -3075,7 +3267,9 @@
       <c r="N58" s="11"/>
     </row>
     <row r="59" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="28"/>
+      <c r="A59" s="25">
+        <v>42956</v>
+      </c>
       <c r="B59" s="28"/>
       <c r="C59" s="28"/>
       <c r="D59" s="28"/>
@@ -3105,9 +3299,7 @@
       <c r="N60" s="11"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A61" s="25">
-        <v>42944</v>
-      </c>
+      <c r="A61" s="25"/>
       <c r="B61" s="26"/>
       <c r="C61" s="30" t="s">
         <v>94</v>
@@ -3124,7 +3316,9 @@
       <c r="J61" s="7"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A62" s="26"/>
+      <c r="A62" s="25">
+        <v>42956</v>
+      </c>
       <c r="B62" s="26"/>
       <c r="C62" s="27"/>
       <c r="D62" s="28" t="s">
@@ -3170,7 +3364,7 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A65" s="25">
-        <v>42923</v>
+        <v>42956</v>
       </c>
       <c r="B65" s="26"/>
       <c r="C65" s="27"/>
@@ -3201,9 +3395,7 @@
       <c r="J66" s="7"/>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A67" s="25">
-        <v>42944</v>
-      </c>
+      <c r="A67" s="25"/>
       <c r="B67" s="26"/>
       <c r="C67" s="30" t="s">
         <v>94</v>
@@ -3240,7 +3432,7 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A69" s="25">
-        <v>42923</v>
+        <v>42956</v>
       </c>
       <c r="B69" s="26"/>
       <c r="C69" s="27"/>
@@ -3275,9 +3467,7 @@
       <c r="M70" s="9"/>
     </row>
     <row r="71" spans="1:14" s="18" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="25">
-        <v>42944</v>
-      </c>
+      <c r="A71" s="25"/>
       <c r="B71" s="33"/>
       <c r="C71" s="30" t="s">
         <v>94</v>
@@ -3315,7 +3505,7 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A73" s="25">
-        <v>42923</v>
+        <v>42956</v>
       </c>
       <c r="B73" s="26"/>
       <c r="C73" s="27"/>
@@ -3346,9 +3536,7 @@
       <c r="J74" s="7"/>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A75" s="25">
-        <v>42944</v>
-      </c>
+      <c r="A75" s="25"/>
       <c r="B75" s="26"/>
       <c r="C75" s="30" t="s">
         <v>94</v>
@@ -3368,9 +3556,7 @@
       <c r="F76" s="26"/>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A77" s="25">
-        <v>42944</v>
-      </c>
+      <c r="A77" s="25"/>
       <c r="B77" s="26"/>
       <c r="C77" s="30" t="s">
         <v>94</v>
@@ -3400,9 +3586,7 @@
       <c r="F79" s="26"/>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A80" s="25">
-        <v>42944</v>
-      </c>
+      <c r="A80" s="25"/>
       <c r="B80" s="26"/>
       <c r="C80" s="30" t="s">
         <v>94</v>
@@ -3426,9 +3610,7 @@
       <c r="H81" s="7"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A82" s="25">
-        <v>42944</v>
-      </c>
+      <c r="A82" s="25"/>
       <c r="B82" s="26"/>
       <c r="C82" s="30" t="s">
         <v>94</v>
@@ -3544,268 +3726,288 @@
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:A7">
-    <cfRule type="notContainsBlanks" dxfId="52" priority="137">
+    <cfRule type="notContainsBlanks" dxfId="84" priority="168">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A39">
+    <cfRule type="notContainsBlanks" dxfId="72" priority="72">
+      <formula>LEN(TRIM(A39))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="58">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="57">
+      <formula>LEN(TRIM(A31))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="56">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="55">
+      <formula>LEN(TRIM(A33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="54">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="53">
+      <formula>LEN(TRIM(A37))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="52">
+      <formula>LEN(TRIM(A38))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="51">
+      <formula>LEN(TRIM(A40))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42">
+    <cfRule type="notContainsBlanks" dxfId="49" priority="49">
+      <formula>LEN(TRIM(A42))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="47">
+      <formula>LEN(TRIM(A44))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48 A50">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="46">
+      <formula>LEN(TRIM(A48))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="45">
+      <formula>LEN(TRIM(A52))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="44">
+      <formula>LEN(TRIM(A55))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="43">
+      <formula>LEN(TRIM(A58))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="42">
+      <formula>LEN(TRIM(A61))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="41">
+      <formula>LEN(TRIM(A67))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="40">
+      <formula>LEN(TRIM(A71))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A75">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="39">
+      <formula>LEN(TRIM(A75))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A77">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="38">
+      <formula>LEN(TRIM(A77))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A80">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="37">
+      <formula>LEN(TRIM(A80))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="36">
+      <formula>LEN(TRIM(A82))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="34">
+      <formula>LEN(TRIM(A46))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="33">
+      <formula>LEN(TRIM(A47))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="32">
+      <formula>LEN(TRIM(A51))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="31">
+      <formula>LEN(TRIM(A8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="30">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="29">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="28">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="27">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="26">
+      <formula>LEN(TRIM(A26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="25">
+      <formula>LEN(TRIM(A41))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="24">
+      <formula>LEN(TRIM(A43))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="23">
+      <formula>LEN(TRIM(A45))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="22">
+      <formula>LEN(TRIM(A49))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="21">
+      <formula>LEN(TRIM(A56))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="20">
+      <formula>LEN(TRIM(A59))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="19">
+      <formula>LEN(TRIM(A62))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="notContainsBlanks" dxfId="51" priority="81">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="18">
       <formula>LEN(TRIM(A65))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="notContainsBlanks" dxfId="50" priority="80">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="17">
       <formula>LEN(TRIM(A69))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A73">
-    <cfRule type="notContainsBlanks" dxfId="49" priority="79">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="16">
       <formula>LEN(TRIM(A73))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="notContainsBlanks" dxfId="48" priority="49">
-      <formula>LEN(TRIM(A8))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="notContainsBlanks" dxfId="47" priority="48">
-      <formula>LEN(TRIM(A9))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="notContainsBlanks" dxfId="46" priority="47">
-      <formula>LEN(TRIM(A10))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11:A13">
-    <cfRule type="notContainsBlanks" dxfId="45" priority="46">
+  <conditionalFormatting sqref="A11">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
       <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="notContainsBlanks" dxfId="44" priority="45">
-      <formula>LEN(TRIM(A23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="notContainsBlanks" dxfId="43" priority="44">
-      <formula>LEN(TRIM(A26))&gt;0</formula>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
+      <formula>LEN(TRIM(A12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="43">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
       <formula>LEN(TRIM(A35))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="42">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
       <formula>LEN(TRIM(A36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="41">
-      <formula>LEN(TRIM(A39))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:A15">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="40">
+  <conditionalFormatting sqref="A13">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="39">
-      <formula>LEN(TRIM(A17))&gt;0</formula>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
+      <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="38">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
       <formula>LEN(TRIM(A18))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="37">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
       <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19">
-    <cfRule type="notContainsBlanks" dxfId="35" priority="36">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
       <formula>LEN(TRIM(A19))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="35">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(A20))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="34">
+  <conditionalFormatting sqref="A21:A22">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(A21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="33">
-      <formula>LEN(TRIM(A22))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="32">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="30" priority="31">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="30">
+  <conditionalFormatting sqref="A27:A29">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="29">
-      <formula>LEN(TRIM(A28))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="28">
-      <formula>LEN(TRIM(A29))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="27">
-      <formula>LEN(TRIM(A30))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="26">
-      <formula>LEN(TRIM(A31))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="25">
-      <formula>LEN(TRIM(A32))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="24">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="23">
-      <formula>LEN(TRIM(A34))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="22">
-      <formula>LEN(TRIM(A37))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="21">
-      <formula>LEN(TRIM(A38))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="20">
-      <formula>LEN(TRIM(A40))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="19">
-      <formula>LEN(TRIM(A41))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A42">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="18">
-      <formula>LEN(TRIM(A42))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A43">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="17">
-      <formula>LEN(TRIM(A43))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A44">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="16">
-      <formula>LEN(TRIM(A44))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48:A50">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
-      <formula>LEN(TRIM(A48))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A52">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
-      <formula>LEN(TRIM(A52))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
-      <formula>LEN(TRIM(A55))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A58">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
-      <formula>LEN(TRIM(A58))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
-      <formula>LEN(TRIM(A61))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
-      <formula>LEN(TRIM(A67))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
-      <formula>LEN(TRIM(A71))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A75">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
-      <formula>LEN(TRIM(A75))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A77">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
-      <formula>LEN(TRIM(A77))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A80">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(A80))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A82">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
-      <formula>LEN(TRIM(A82))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(A45))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(A46))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(A47))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A51))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New files in prep for pull to PhUSE server
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="140">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -336,12 +336,6 @@
     <t>Checking does not extend past the cdiscpilot01 namespace. No checking of code:, cd01p, study, etc.</t>
   </si>
   <si>
-    <t>ERROR in ONT. Email to AO 2017-06-15</t>
-  </si>
-  <si>
-    <t>question to AO 2017-06-15: EFF/SAF/ITT to code: or cd01p: ??</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
@@ -372,9 +366,6 @@
     <t>VS</t>
   </si>
   <si>
-    <t>See greyed out section, below.</t>
-  </si>
-  <si>
     <t>cdiscpilot01:C67153.C25299_1</t>
   </si>
   <si>
@@ -414,9 +405,6 @@
     <t>cdiscpilot01:C67153.C49676_3</t>
   </si>
   <si>
-    <t>AO needs to change formatting of label to match R</t>
-  </si>
-  <si>
     <t>cdiscpilot01:StartRuleNone_1</t>
   </si>
   <si>
@@ -429,23 +417,38 @@
     <t>cdiscpilot01:C67153.C25298_1</t>
   </si>
   <si>
-    <t>Label issue email to AO TBD sent</t>
-  </si>
-  <si>
-    <t>Change label. Screening1 (ont) to Screening 1 ®</t>
-  </si>
-  <si>
     <t>cdiscpilot01:WeightMassOutcome_1</t>
   </si>
   <si>
-    <t>decimal point issue in hasValue. Label should be value + unit (119.0 LB) Email to AO.</t>
+    <t>Child of prev</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:HeightLengthOutcome_1</t>
+  </si>
+  <si>
+    <t>missing decimal. Email to AO 9 Aug17</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:PulseHROutcome_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:PulseHROutcome_2</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:PulseHROutcome_3</t>
+  </si>
+  <si>
+    <t>BLOOD PRESSURE</t>
+  </si>
+  <si>
+    <t>PULSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -648,8 +651,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="40">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -849,12 +860,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -862,12 +867,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1056,7 +1055,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1088,12 +1087,8 @@
     <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1101,7 +1096,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1119,11 +1113,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="39" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1175,91 +1171,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="85">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="73">
     <dxf>
       <fill>
         <patternFill>
@@ -2081,19 +1993,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N94"/>
+  <dimension ref="A1:N103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <pane ySplit="3" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.453125" customWidth="1"/>
-    <col min="4" max="4" width="30.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" customWidth="1"/>
     <col min="5" max="5" width="49.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="49.81640625" customWidth="1"/>
     <col min="8" max="8" width="40.36328125" customWidth="1"/>
@@ -2109,10 +2021,10 @@
       <c r="C1" t="s">
         <v>103</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="44"/>
+      <c r="K1" s="41"/>
       <c r="L1" s="10" t="s">
         <v>44</v>
       </c>
@@ -2122,19 +2034,19 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
-        <v>123</v>
-      </c>
-      <c r="J2" s="35"/>
-      <c r="K2" s="36"/>
+        <v>120</v>
+      </c>
+      <c r="J2" s="30"/>
+      <c r="K2" s="31"/>
       <c r="L2" s="10"/>
-      <c r="M2" s="36"/>
+      <c r="M2" s="31"/>
     </row>
     <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
@@ -2146,7 +2058,7 @@
         <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G3" t="s">
         <v>85</v>
@@ -2168,301 +2080,309 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B4" s="26" t="s">
+      <c r="A4" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="F4" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="35"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B5" s="26" t="s">
+      <c r="A5" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="35"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B6" s="26" t="s">
+      <c r="A6" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="F6" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="35"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B7" s="26" t="s">
+      <c r="A7" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="35"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B8" s="26" t="s">
+      <c r="A8" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B8" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="7"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="35"/>
       <c r="J8"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8"/>
     </row>
     <row r="9" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B9" s="26" t="s">
+      <c r="A9" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B9" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28" t="s">
+      <c r="C9" s="22"/>
+      <c r="D9" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="35"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="N9" s="4"/>
     </row>
     <row r="10" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B10" s="26" t="s">
+      <c r="A10" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28" t="s">
+      <c r="C10" s="22"/>
+      <c r="D10" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="27"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7" t="s">
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22" t="s">
         <v>102</v>
       </c>
+      <c r="I10" s="35"/>
       <c r="J10"/>
       <c r="L10" s="4"/>
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B11" s="26" t="s">
+      <c r="A11" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="7"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="35"/>
       <c r="L11" s="2"/>
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B12" s="26" t="s">
+      <c r="A12" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28" t="s">
+      <c r="C12" s="22"/>
+      <c r="D12" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7" t="s">
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="22" t="s">
         <v>100</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B13" s="26" t="s">
+      <c r="A13" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B13" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="28" t="s">
+      <c r="C13" s="22"/>
+      <c r="D13" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7" t="s">
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="I13" s="22" t="s">
         <v>100</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B14" s="26" t="s">
+      <c r="A14" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B14" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7" t="s">
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22" t="s">
         <v>100</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B15" s="26" t="s">
+      <c r="A15" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="28" t="s">
+      <c r="C15" s="22"/>
+      <c r="D15" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="7" t="s">
+      <c r="F15" s="22"/>
+      <c r="G15" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7" t="s">
+      <c r="H15" s="22"/>
+      <c r="I15" s="22" t="s">
         <v>100</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B16" s="26" t="s">
+      <c r="A16" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="F16" s="27"/>
-      <c r="G16" s="7" t="s">
+      <c r="F16" s="22"/>
+      <c r="G16" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7" t="s">
+      <c r="H16" s="22"/>
+      <c r="I16" s="22" t="s">
         <v>100</v>
       </c>
       <c r="J16"/>
@@ -2471,25 +2391,25 @@
       <c r="M16" s="6"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B17" s="26" t="s">
+      <c r="A17" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28" t="s">
+      <c r="C17" s="22"/>
+      <c r="D17" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="27"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7" t="s">
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="I17" s="22" t="s">
         <v>100</v>
       </c>
       <c r="J17" s="4"/>
@@ -2498,25 +2418,25 @@
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B18" s="26" t="s">
+      <c r="A18" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B18" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="28" t="s">
+      <c r="C18" s="22"/>
+      <c r="D18" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="27"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7" t="s">
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="22" t="s">
         <v>100</v>
       </c>
       <c r="J18"/>
@@ -2525,150 +2445,153 @@
       <c r="M18" s="6"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B19" s="26" t="s">
+      <c r="A19" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B19" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7" t="s">
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B20" s="26" t="s">
+      <c r="A20" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B20" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7" t="s">
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B21" s="26" t="s">
+      <c r="A21" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B21" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="27"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="35"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B22" s="26" t="s">
+      <c r="A22" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B22" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="28" t="s">
+      <c r="C22" s="22"/>
+      <c r="D22" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="27"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="35"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B23" s="26" t="s">
+      <c r="A23" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B23" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="28" t="s">
+      <c r="C23" s="22"/>
+      <c r="D23" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="27"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="35"/>
     </row>
     <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B24" s="26" t="s">
+      <c r="A24" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B24" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="F24" s="27"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7" t="s">
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22" t="s">
         <v>100</v>
       </c>
       <c r="M24" s="6"/>
       <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B25" s="26" t="s">
+      <c r="A25" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B25" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="28" t="s">
+      <c r="C25" s="22"/>
+      <c r="D25" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E25" s="27" t="s">
+      <c r="E25" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="F25" s="27"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7" t="s">
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22" t="s">
         <v>100</v>
       </c>
       <c r="K25" s="3"/>
@@ -2677,23 +2600,23 @@
       <c r="N25" s="4"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B26" s="26" t="s">
+      <c r="A26" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B26" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="28" t="s">
+      <c r="C26" s="22"/>
+      <c r="D26" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F26" s="27"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7" t="s">
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22" t="s">
         <v>100</v>
       </c>
       <c r="K26" s="3"/>
@@ -2702,1018 +2625,1254 @@
       <c r="N26" s="4"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A27" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B27" s="27" t="s">
+      <c r="A27" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B27" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="F27" s="27"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="3" t="s">
+      <c r="F29" s="25"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="35" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="27" t="s">
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D30" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E30" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="F28" s="27"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A29" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B29" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="F29" s="30"/>
-      <c r="G29" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="H29" s="7"/>
-      <c r="I29" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J29" s="7"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A30" s="25"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="F30" s="30"/>
-      <c r="G30" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="H30" s="7"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="35"/>
       <c r="K30" s="3"/>
       <c r="L30" s="14"/>
       <c r="M30" s="14"/>
       <c r="N30" s="4"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A31" s="25"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27" t="s">
+      <c r="A31" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="F31" s="30"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
+      <c r="E31" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="F31" s="25"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="35"/>
       <c r="K31" s="3"/>
       <c r="L31" s="14"/>
       <c r="M31" s="14"/>
       <c r="N31" s="4"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A32" s="25"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27" t="s">
+      <c r="A32" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E32" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="F32" s="30"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
+      <c r="E32" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="F32" s="25"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="35"/>
       <c r="K32" s="3"/>
       <c r="L32" s="14"/>
       <c r="M32" s="14"/>
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A33" s="25"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="27" t="s">
+      <c r="A33" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D33" s="27" t="s">
+      <c r="D33" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="27" t="s">
+      <c r="E33" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="27"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="35"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="25"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="28" t="s">
+      <c r="A34" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E34" s="27" t="s">
+      <c r="E34" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="F34" s="30"/>
-      <c r="G34" s="7"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="35"/>
       <c r="M34" s="9"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B35" s="26"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="28" t="s">
+      <c r="A35" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="22"/>
+      <c r="D35" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E35" s="27" t="s">
+      <c r="E35" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="F35" s="27"/>
-      <c r="G35" s="7"/>
-      <c r="H35" t="s">
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="21" t="s">
         <v>82</v>
       </c>
+      <c r="I35" s="35"/>
       <c r="K35" t="s">
         <v>71</v>
       </c>
       <c r="M35" s="9"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B36" s="26"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="28" t="s">
+      <c r="A36" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="22"/>
+      <c r="D36" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E36" s="27" t="s">
+      <c r="E36" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F36" s="27"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7" t="s">
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22" t="s">
         <v>79</v>
       </c>
+      <c r="I36" s="35"/>
       <c r="M36" s="9"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="25"/>
-      <c r="B37" s="26" t="s">
+      <c r="A37" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B37" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C37" s="27" t="s">
+      <c r="C37" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D37" s="27" t="s">
+      <c r="D37" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E37" s="27" t="s">
+      <c r="E37" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="F37" s="30"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="35"/>
       <c r="J37"/>
       <c r="K37" s="2"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="25"/>
-      <c r="B38" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="C38" s="27" t="s">
+      <c r="A38" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="27" t="s">
+      <c r="D38" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E38" s="30" t="s">
+      <c r="E38" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F38" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="35"/>
       <c r="J38" s="7"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="25"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="28" t="s">
+      <c r="A39" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="22"/>
+      <c r="D39" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E39" s="27" t="s">
+      <c r="E39" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F39" s="27"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="35"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A40" s="25"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="30" t="s">
+      <c r="A40" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D40" s="28" t="s">
+      <c r="D40" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E40" s="37" t="s">
+      <c r="E40" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="F40" s="32"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="35"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A41" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B41" s="26"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="28" t="s">
+      <c r="A41" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41" s="22"/>
+      <c r="D41" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E41" s="27" t="s">
+      <c r="E41" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="F41" s="32"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="35"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42" s="25"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="30" t="s">
+      <c r="A42" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D42" s="28" t="s">
+      <c r="D42" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E42" s="37" t="s">
+      <c r="E42" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="F42" s="32"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="35"/>
       <c r="J42" s="7"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A43" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B43" s="26"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="28" t="s">
+      <c r="A43" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" s="22"/>
+      <c r="D43" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E43" s="27" t="s">
+      <c r="E43" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="F43" s="32"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="35"/>
       <c r="J43" s="7"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A44" s="41"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="30" t="s">
+      <c r="A44" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="E44" s="40" t="s">
-        <v>124</v>
-      </c>
-      <c r="F44" s="32" t="s">
+      <c r="D44" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E44" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="7"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A45" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C45" s="22"/>
+      <c r="D45" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="7"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A46" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46" s="22"/>
+      <c r="D46" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F46" s="27"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="7"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A47" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" s="22"/>
+      <c r="D47" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="35"/>
+      <c r="J47" s="7"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A48" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D48" s="23"/>
+      <c r="E48" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="35"/>
+      <c r="J48" s="7"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A49" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C49" s="25"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F49" s="27"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="7"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A50" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C50" s="25"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="35"/>
+      <c r="J50" s="7"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A51" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B51" s="21"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="F51" s="27"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="7"/>
+    </row>
+    <row r="52" spans="1:14" s="7" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="20"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D52" s="23"/>
+      <c r="E52" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
-      <c r="J44" s="7"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A45" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B45" s="26"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E45" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="F45" s="32"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-      <c r="J45" s="7"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A46" s="25"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E46" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="F46" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
-      <c r="J46" s="7"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A47" s="25"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E47" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="F47" s="32"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
-      <c r="J47" s="7"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A48" s="25"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="D48" s="28"/>
-      <c r="E48" s="40" t="s">
-        <v>125</v>
-      </c>
-      <c r="F48" s="32" t="s">
-        <v>136</v>
-      </c>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
-      <c r="J48" s="7"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A49" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B49" s="26"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="F49" s="32"/>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16"/>
-      <c r="J49" s="7"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A50" s="25"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="F50" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="G50" s="16"/>
-      <c r="H50" s="16"/>
-      <c r="J50" s="7"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A51" s="25"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="F51" s="32" t="s">
+      <c r="F52" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="G51" s="16"/>
-      <c r="H51" s="16"/>
-      <c r="J51" s="7"/>
-    </row>
-    <row r="52" spans="1:14" s="7" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="25"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="D52" s="28"/>
-      <c r="E52" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="F52" s="32"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="16"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="27"/>
+      <c r="I52" s="22"/>
       <c r="K52" s="11"/>
       <c r="L52" s="11"/>
       <c r="N52" s="11"/>
     </row>
     <row r="53" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="28"/>
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="27" t="s">
+      <c r="A53" s="23"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="F53" s="32"/>
-      <c r="G53" s="16"/>
-      <c r="H53" s="16"/>
+      <c r="F53" s="27"/>
+      <c r="G53" s="27"/>
+      <c r="H53" s="27"/>
+      <c r="I53" s="22"/>
       <c r="K53" s="11"/>
       <c r="L53" s="11"/>
       <c r="N53" s="11"/>
     </row>
     <row r="54" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="28"/>
-      <c r="B54" s="28"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="27" t="s">
+      <c r="A54" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B54" s="23"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="F54" s="32"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="16"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="22"/>
       <c r="K54" s="11"/>
       <c r="L54" s="11"/>
       <c r="N54" s="11"/>
     </row>
     <row r="55" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="25"/>
-      <c r="B55" s="28"/>
-      <c r="C55" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="D55" s="28"/>
-      <c r="E55" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="F55" s="32"/>
-      <c r="G55" s="16"/>
-      <c r="H55" s="16"/>
+      <c r="A55" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B55" s="23"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="27"/>
+      <c r="I55" s="22"/>
       <c r="K55" s="11"/>
       <c r="L55" s="11"/>
       <c r="N55" s="11"/>
     </row>
     <row r="56" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B56" s="28"/>
-      <c r="C56" s="28"/>
-      <c r="D56" s="28"/>
-      <c r="E56" s="27" t="s">
+      <c r="A56" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="E56" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="F56" s="32"/>
-      <c r="G56" s="16"/>
-      <c r="H56" s="16"/>
+      <c r="F56" s="27"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="27"/>
+      <c r="I56" s="22"/>
       <c r="K56" s="11"/>
       <c r="L56" s="11"/>
       <c r="N56" s="11"/>
     </row>
     <row r="57" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="28"/>
-      <c r="B57" s="28"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="F57" s="32"/>
-      <c r="G57" s="16"/>
-      <c r="H57" s="16"/>
+      <c r="A57" s="20"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D57" s="23"/>
+      <c r="E57" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="F57" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="G57" s="27"/>
+      <c r="H57" s="27"/>
+      <c r="I57" s="22"/>
       <c r="K57" s="11"/>
       <c r="L57" s="11"/>
       <c r="N57" s="11"/>
     </row>
     <row r="58" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="25"/>
-      <c r="B58" s="28"/>
-      <c r="C58" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="D58" s="28"/>
-      <c r="E58" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="F58" s="32"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
+      <c r="A58" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B58" s="23"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F58" s="27"/>
+      <c r="G58" s="27"/>
+      <c r="H58" s="27"/>
+      <c r="I58" s="22"/>
       <c r="K58" s="11"/>
       <c r="L58" s="11"/>
       <c r="N58" s="11"/>
     </row>
     <row r="59" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B59" s="28"/>
-      <c r="C59" s="28"/>
-      <c r="D59" s="28"/>
-      <c r="E59" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="F59" s="32"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="16"/>
+      <c r="A59" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B59" s="23"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="F59" s="27"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="27"/>
+      <c r="I59" s="22"/>
       <c r="K59" s="11"/>
       <c r="L59" s="11"/>
       <c r="N59" s="11"/>
     </row>
     <row r="60" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="28"/>
-      <c r="B60" s="28"/>
-      <c r="C60" s="28"/>
-      <c r="D60" s="28"/>
-      <c r="E60" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="F60" s="32"/>
-      <c r="G60" s="16"/>
-      <c r="H60" s="16"/>
+      <c r="A60" s="20"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D60" s="23"/>
+      <c r="E60" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="F60" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="G60" s="27"/>
+      <c r="H60" s="27"/>
+      <c r="I60" s="22"/>
       <c r="K60" s="11"/>
       <c r="L60" s="11"/>
       <c r="N60" s="11"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A61" s="25"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="30" t="s">
+    <row r="61" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B61" s="23"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F61" s="27"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="27"/>
+      <c r="I61" s="22"/>
+      <c r="K61" s="11"/>
+      <c r="L61" s="11"/>
+      <c r="N61" s="11"/>
+    </row>
+    <row r="62" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="F62" s="27"/>
+      <c r="G62" s="27"/>
+      <c r="H62" s="27"/>
+      <c r="I62" s="22"/>
+      <c r="K62" s="11"/>
+      <c r="L62" s="11"/>
+      <c r="N62" s="11"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A63" s="20"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D61" s="28" t="s">
+      <c r="D63" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E61" s="37" t="s">
+      <c r="E63" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="F63" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="G63" s="27"/>
+      <c r="H63" s="27"/>
+      <c r="I63" s="35"/>
+      <c r="J63" s="7"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A64" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B64" s="21"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E64" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F64" s="25"/>
+      <c r="G64" s="27"/>
+      <c r="H64" s="27"/>
+      <c r="I64" s="35"/>
+      <c r="J64" s="7"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A65" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B65" s="21"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E65" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="F65" s="25"/>
+      <c r="G65" s="27"/>
+      <c r="H65" s="27"/>
+      <c r="I65" s="35"/>
+      <c r="J65" s="7"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A66" s="21"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="22"/>
+      <c r="D66" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E66" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="F66" s="21"/>
+      <c r="G66" s="27"/>
+      <c r="H66" s="27"/>
+      <c r="I66" s="35"/>
+      <c r="J66" s="7"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A67" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B67" s="21"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E67" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F67" s="21"/>
+      <c r="G67" s="27"/>
+      <c r="H67" s="27"/>
+      <c r="I67" s="35"/>
+      <c r="J67" s="7"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A68" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B68" s="21"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E68" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="F68" s="21"/>
+      <c r="G68" s="27"/>
+      <c r="H68" s="27"/>
+      <c r="I68" s="35"/>
+      <c r="J68" s="7"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A69" s="20"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D69" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E69" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="F61" s="30"/>
-      <c r="G61" s="16"/>
-      <c r="H61" s="16"/>
-      <c r="J61" s="7"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A62" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B62" s="26"/>
-      <c r="C62" s="27"/>
-      <c r="D62" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E62" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="F62" s="30"/>
-      <c r="G62" s="16"/>
-      <c r="H62" s="16"/>
-      <c r="J62" s="7"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A63" s="26"/>
-      <c r="B63" s="26"/>
-      <c r="C63" s="27"/>
-      <c r="D63" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E63" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="F63" s="30"/>
-      <c r="G63" s="16"/>
-      <c r="H63" s="16"/>
-      <c r="J63" s="7"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A64" s="26"/>
-      <c r="B64" s="26"/>
-      <c r="C64" s="27"/>
-      <c r="D64" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E64" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="F64" s="26"/>
-      <c r="G64" s="16"/>
-      <c r="H64" s="16"/>
-      <c r="J64" s="7"/>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A65" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B65" s="26"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E65" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="F65" s="26"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
-      <c r="J65" s="7"/>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A66" s="26"/>
-      <c r="B66" s="26"/>
-      <c r="C66" s="27"/>
-      <c r="D66" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E66" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="F66" s="26"/>
-      <c r="G66" s="16"/>
-      <c r="H66" s="16"/>
-      <c r="J66" s="7"/>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A67" s="25"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="D67" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E67" s="37" t="s">
-        <v>120</v>
-      </c>
-      <c r="F67" s="30"/>
-      <c r="G67" s="16"/>
-      <c r="H67" s="16"/>
-      <c r="J67" s="7"/>
-      <c r="K67" s="11"/>
-      <c r="M67" s="9"/>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A68" s="26"/>
-      <c r="B68" s="26"/>
-      <c r="C68" s="27"/>
-      <c r="D68" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E68" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="F68" s="26"/>
-      <c r="G68" s="16"/>
-      <c r="H68" s="16"/>
-      <c r="J68" s="7"/>
-      <c r="K68" s="11"/>
-      <c r="M68" s="9"/>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A69" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B69" s="26"/>
-      <c r="C69" s="27"/>
-      <c r="D69" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E69" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="F69" s="26"/>
-      <c r="G69" s="16"/>
-      <c r="H69" s="16"/>
+      <c r="F69" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="G69" s="27"/>
+      <c r="H69" s="27"/>
+      <c r="I69" s="35"/>
       <c r="J69" s="7"/>
       <c r="K69" s="11"/>
       <c r="M69" s="9"/>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A70" s="26"/>
-      <c r="B70" s="26"/>
-      <c r="C70" s="27"/>
-      <c r="D70" s="28" t="s">
+      <c r="A70" s="21"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E70" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="F70" s="26"/>
-      <c r="G70" s="16"/>
-      <c r="H70" s="16"/>
+      <c r="E70" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="F70" s="21"/>
+      <c r="G70" s="27"/>
+      <c r="H70" s="27"/>
+      <c r="I70" s="35"/>
       <c r="J70" s="7"/>
       <c r="K70" s="11"/>
       <c r="M70" s="9"/>
     </row>
-    <row r="71" spans="1:14" s="18" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="25"/>
-      <c r="B71" s="33"/>
-      <c r="C71" s="30" t="s">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A71" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B71" s="21"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E71" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="F71" s="21"/>
+      <c r="G71" s="27"/>
+      <c r="H71" s="27"/>
+      <c r="I71" s="35"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="11"/>
+      <c r="M71" s="9"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A72" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B72" s="21"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E72" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F72" s="21"/>
+      <c r="G72" s="27"/>
+      <c r="H72" s="27"/>
+      <c r="I72" s="35"/>
+      <c r="J72" s="7"/>
+      <c r="K72" s="11"/>
+      <c r="M72" s="9"/>
+    </row>
+    <row r="73" spans="1:14" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="20"/>
+      <c r="B73" s="28"/>
+      <c r="C73" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D71" s="34" t="s">
+      <c r="D73" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="E71" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="F71" s="30"/>
-      <c r="G71" s="20"/>
-      <c r="H71" s="20"/>
-      <c r="I71" s="21"/>
-      <c r="J71" s="19"/>
-      <c r="K71" s="22"/>
-      <c r="L71" s="22"/>
-      <c r="M71" s="21"/>
-      <c r="N71" s="23"/>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A72" s="26"/>
-      <c r="B72" s="26"/>
-      <c r="C72" s="27"/>
-      <c r="D72" s="28" t="s">
+      <c r="E73" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="F73" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="G73" s="36"/>
+      <c r="H73" s="36"/>
+      <c r="I73" s="37"/>
+      <c r="J73" s="16"/>
+      <c r="K73" s="18"/>
+      <c r="L73" s="18"/>
+      <c r="M73" s="17"/>
+      <c r="N73" s="19"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A74" s="21"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="22"/>
+      <c r="D74" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E72" s="38" t="s">
+      <c r="E74" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="F72" s="26"/>
-      <c r="G72" s="15"/>
-      <c r="H72" s="15"/>
-      <c r="J72" s="7"/>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A73" s="25">
-        <v>42956</v>
-      </c>
-      <c r="B73" s="26"/>
-      <c r="C73" s="27"/>
-      <c r="D73" s="28" t="s">
+      <c r="F74" s="21"/>
+      <c r="G74" s="26"/>
+      <c r="H74" s="26"/>
+      <c r="I74" s="35"/>
+      <c r="J74" s="7"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A75" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B75" s="21"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E73" s="26" t="s">
+      <c r="E75" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="F73" s="26"/>
-      <c r="G73" s="7"/>
-      <c r="H73" s="7"/>
-      <c r="J73" s="7"/>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A74" s="26"/>
-      <c r="B74" s="26"/>
-      <c r="C74" s="27"/>
-      <c r="D74" s="28" t="s">
+      <c r="F75" s="21"/>
+      <c r="G75" s="22"/>
+      <c r="H75" s="22"/>
+      <c r="I75" s="35"/>
+      <c r="J75" s="7"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A76" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B76" s="21"/>
+      <c r="C76" s="22"/>
+      <c r="D76" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E74" s="26" t="s">
+      <c r="E76" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="F74" s="26"/>
-      <c r="G74" s="7"/>
-      <c r="H74" s="7"/>
-      <c r="J74" s="7"/>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A75" s="25"/>
-      <c r="B75" s="26"/>
-      <c r="C75" s="30" t="s">
+      <c r="F76" s="21"/>
+      <c r="G76" s="22"/>
+      <c r="H76" s="22"/>
+      <c r="I76" s="35"/>
+      <c r="J76" s="7"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A77" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B77" s="21"/>
+      <c r="C77" s="22"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F77" s="21"/>
+      <c r="G77" s="22"/>
+      <c r="H77" s="22"/>
+      <c r="I77" s="35"/>
+      <c r="J77" s="7"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A78" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B78" s="21"/>
+      <c r="C78" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D75" s="26"/>
-      <c r="E75" s="37" t="s">
+      <c r="D78" s="21"/>
+      <c r="E78" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="F78" s="21"/>
+      <c r="G78" s="21"/>
+      <c r="H78" s="21"/>
+      <c r="I78" s="35"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A79" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B79" s="21"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F79" s="21"/>
+      <c r="G79" s="21"/>
+      <c r="H79" s="21"/>
+      <c r="I79" s="35"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A80" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B80" s="21"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="21"/>
+      <c r="E80" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F80" s="21"/>
+      <c r="G80" s="21"/>
+      <c r="H80" s="21"/>
+      <c r="I80" s="35"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A81" s="21"/>
+      <c r="B81" s="21"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="21"/>
+      <c r="E81" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="F81" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="G81" s="21"/>
+      <c r="H81" s="21"/>
+      <c r="I81" s="35"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A82" s="20"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D82" s="21"/>
+      <c r="E82" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="F82" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="G82" s="21"/>
+      <c r="H82" s="21"/>
+      <c r="I82" s="35"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A83" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B83" s="21"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="21"/>
+      <c r="E83" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F83" s="21"/>
+      <c r="G83" s="21"/>
+      <c r="H83" s="21"/>
+      <c r="I83" s="35"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A84" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B84" s="21"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F84" s="21"/>
+      <c r="G84" s="21"/>
+      <c r="H84" s="21"/>
+      <c r="I84" s="35"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A85" s="21"/>
+      <c r="B85" s="21"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="F85" s="21"/>
+      <c r="G85" s="21"/>
+      <c r="H85" s="21"/>
+      <c r="I85" s="35"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A86" s="21"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D86" s="21"/>
+      <c r="E86" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="F86" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="G86" s="21"/>
+      <c r="H86" s="21"/>
+      <c r="I86" s="35"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A87" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B87" s="21"/>
+      <c r="C87" s="21"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F87" s="22"/>
+      <c r="G87" s="22"/>
+      <c r="H87" s="22"/>
+      <c r="I87" s="35"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A88" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B88" s="21"/>
+      <c r="C88" s="21"/>
+      <c r="D88" s="22"/>
+      <c r="E88" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F88" s="22"/>
+      <c r="G88" s="22"/>
+      <c r="H88" s="22"/>
+      <c r="I88" s="35"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A89" s="20"/>
+      <c r="B89" s="21"/>
+      <c r="C89" s="21"/>
+      <c r="D89" s="22"/>
+      <c r="E89" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="F89" s="22"/>
+      <c r="G89" s="22"/>
+      <c r="H89" s="22"/>
+      <c r="I89" s="35"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A90" s="21"/>
+      <c r="B90" s="21"/>
+      <c r="C90" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D90" s="22"/>
+      <c r="E90" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="F75" s="26"/>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A76" s="26"/>
-      <c r="B76" s="26"/>
-      <c r="C76" s="26"/>
-      <c r="D76" s="26"/>
-      <c r="E76" s="26"/>
-      <c r="F76" s="26"/>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A77" s="25"/>
-      <c r="B77" s="26"/>
-      <c r="C77" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="D77" s="26"/>
-      <c r="E77" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="F77" s="26"/>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A78" s="26"/>
-      <c r="B78" s="26"/>
-      <c r="C78" s="26"/>
-      <c r="D78" s="26"/>
-      <c r="E78" s="26"/>
-      <c r="F78" s="26"/>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A79" s="26"/>
-      <c r="B79" s="26"/>
-      <c r="C79" s="26"/>
-      <c r="D79" s="26"/>
-      <c r="E79" s="37" t="s">
-        <v>128</v>
-      </c>
-      <c r="F79" s="26"/>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A80" s="25"/>
-      <c r="B80" s="26"/>
-      <c r="C80" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="D80" s="27"/>
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="7"/>
-      <c r="H80" s="7"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A81" s="26"/>
-      <c r="B81" s="26"/>
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="F81" s="27"/>
-      <c r="G81" s="7"/>
-      <c r="H81" s="7"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A82" s="25"/>
-      <c r="B82" s="26"/>
-      <c r="C82" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="D82" s="27"/>
-      <c r="E82" s="26"/>
-      <c r="F82" s="27"/>
-      <c r="G82" s="7"/>
-      <c r="H82" s="7"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A83" s="26"/>
-      <c r="B83" s="26"/>
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="27"/>
-      <c r="F83" s="27"/>
-      <c r="G83" s="7"/>
-      <c r="H83" s="7"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A84" s="26"/>
-      <c r="B84" s="26"/>
-      <c r="C84" s="27"/>
-      <c r="D84" s="27"/>
-      <c r="E84" s="27"/>
-      <c r="F84" s="27"/>
-      <c r="G84" s="7"/>
-      <c r="H84" s="7"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C85" s="7"/>
-      <c r="D85" s="7"/>
-      <c r="E85" s="7"/>
-      <c r="F85" s="7"/>
-      <c r="G85" s="7"/>
-      <c r="H85" s="7"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C86" s="7"/>
-      <c r="D86" s="7"/>
-      <c r="E86" s="7"/>
-      <c r="F86" s="7"/>
-      <c r="G86" s="7"/>
-      <c r="H86" s="7"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C87" s="7"/>
-      <c r="D87" s="7"/>
-      <c r="E87" s="7"/>
-      <c r="F87" s="7"/>
-      <c r="G87" s="7"/>
-      <c r="H87" s="7"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C88" s="7"/>
-      <c r="D88" s="7"/>
-      <c r="E88" s="7"/>
-      <c r="F88" s="7"/>
-      <c r="G88" s="7"/>
-      <c r="H88" s="7"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C89" s="7"/>
-      <c r="D89" s="7"/>
-      <c r="E89" s="7"/>
-      <c r="F89" s="7"/>
-      <c r="G89" s="7"/>
-      <c r="H89" s="7"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C90" s="7"/>
-      <c r="D90" s="7"/>
-      <c r="E90" s="7"/>
-      <c r="F90" s="7"/>
-      <c r="G90" s="7"/>
-      <c r="H90" s="7"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C91" s="7"/>
-      <c r="D91" s="7"/>
-      <c r="E91" s="7"/>
-      <c r="F91" s="7"/>
-      <c r="G91" s="7"/>
-      <c r="H91" s="7"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C92" s="7"/>
-      <c r="D92" s="7"/>
-      <c r="E92" s="7"/>
-      <c r="F92" s="7"/>
-      <c r="G92" s="7"/>
-      <c r="H92" s="7"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C93" s="7"/>
-      <c r="D93" s="7"/>
-      <c r="E93" s="7"/>
-      <c r="F93" s="7"/>
-      <c r="G93" s="7"/>
-      <c r="H93" s="7"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F90" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="G90" s="22"/>
+      <c r="H90" s="22"/>
+      <c r="I90" s="35"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A91" s="20"/>
+      <c r="B91" s="21"/>
+      <c r="D91" s="22"/>
+      <c r="E91" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F91" s="22"/>
+      <c r="G91" s="22"/>
+      <c r="H91" s="22"/>
+      <c r="I91" s="35"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A92" s="20">
+        <v>42956</v>
+      </c>
+      <c r="B92" s="21"/>
+      <c r="C92" s="22"/>
+      <c r="D92" s="22"/>
+      <c r="E92" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F92" s="22"/>
+      <c r="G92" s="22"/>
+      <c r="H92" s="22"/>
+      <c r="I92" s="35"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A93" s="21"/>
+      <c r="B93" s="21"/>
+      <c r="C93" s="22"/>
+      <c r="D93" s="22"/>
+      <c r="E93" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="F93" s="22"/>
+      <c r="G93" s="22"/>
+      <c r="H93" s="22"/>
+      <c r="I93" s="35"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
@@ -3721,293 +3880,445 @@
       <c r="G94" s="7"/>
       <c r="H94" s="7"/>
     </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C95" s="7"/>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
+      <c r="F95" s="7"/>
+      <c r="G95" s="7"/>
+      <c r="H95" s="7"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C96" s="7"/>
+      <c r="D96" s="7"/>
+      <c r="E96" s="7"/>
+      <c r="F96" s="7"/>
+      <c r="G96" s="7"/>
+      <c r="H96" s="7"/>
+    </row>
+    <row r="97" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="C97" s="7"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7"/>
+      <c r="G97" s="7"/>
+      <c r="H97" s="7"/>
+    </row>
+    <row r="98" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="C98" s="7"/>
+      <c r="D98" s="7"/>
+      <c r="E98" s="7"/>
+      <c r="F98" s="7"/>
+      <c r="G98" s="7"/>
+      <c r="H98" s="7"/>
+    </row>
+    <row r="99" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="C99" s="7"/>
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="7"/>
+      <c r="G99" s="7"/>
+      <c r="H99" s="7"/>
+    </row>
+    <row r="100" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="C100" s="7"/>
+      <c r="D100" s="7"/>
+      <c r="E100" s="7"/>
+      <c r="F100" s="7"/>
+      <c r="G100" s="7"/>
+      <c r="H100" s="7"/>
+    </row>
+    <row r="101" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="C101" s="7"/>
+      <c r="D101" s="7"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="7"/>
+      <c r="G101" s="7"/>
+      <c r="H101" s="7"/>
+    </row>
+    <row r="102" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="C102" s="7"/>
+      <c r="D102" s="7"/>
+      <c r="E102" s="7"/>
+      <c r="F102" s="7"/>
+      <c r="G102" s="7"/>
+      <c r="H102" s="7"/>
+    </row>
+    <row r="103" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="C103" s="7"/>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="7"/>
+      <c r="G103" s="7"/>
+      <c r="H103" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:A7">
-    <cfRule type="notContainsBlanks" dxfId="84" priority="168">
+    <cfRule type="notContainsBlanks" dxfId="72" priority="201">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="62">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="60">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57">
+    <cfRule type="notContainsBlanks" dxfId="69" priority="77">
+      <formula>LEN(TRIM(A57))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52">
+    <cfRule type="notContainsBlanks" dxfId="68" priority="78">
+      <formula>LEN(TRIM(A52))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="74">
+      <formula>LEN(TRIM(A69))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60">
+    <cfRule type="notContainsBlanks" dxfId="66" priority="76">
+      <formula>LEN(TRIM(A60))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="59">
+      <formula>LEN(TRIM(A26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A78">
+    <cfRule type="notContainsBlanks" dxfId="64" priority="72">
+      <formula>LEN(TRIM(A78))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A73">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="73">
+      <formula>LEN(TRIM(A73))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="71">
+      <formula>LEN(TRIM(A82))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63">
+    <cfRule type="notContainsBlanks" dxfId="61" priority="75">
+      <formula>LEN(TRIM(A63))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="69">
+      <formula>LEN(TRIM(A91))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A89">
+    <cfRule type="notContainsBlanks" dxfId="59" priority="70">
+      <formula>LEN(TRIM(A89))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="42">
+      <formula>LEN(TRIM(A15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="41">
+      <formula>LEN(TRIM(A18))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="29">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="63">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="61">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="64">
+      <formula>LEN(TRIM(A8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="57">
+      <formula>LEN(TRIM(A43))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="55">
+      <formula>LEN(TRIM(A49))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="58">
+      <formula>LEN(TRIM(A41))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45">
+    <cfRule type="notContainsBlanks" dxfId="49" priority="56">
+      <formula>LEN(TRIM(A45))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="53">
+      <formula>LEN(TRIM(A61))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="54">
+      <formula>LEN(TRIM(A58))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="52">
+      <formula>LEN(TRIM(A64))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="51">
+      <formula>LEN(TRIM(A67))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="50">
+      <formula>LEN(TRIM(A71))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A75">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="49">
+      <formula>LEN(TRIM(A75))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="48">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="47">
+      <formula>LEN(TRIM(A12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="46">
+      <formula>LEN(TRIM(A35))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="45">
+      <formula>LEN(TRIM(A36))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="44">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="43">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="38">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21:A22">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="37">
+      <formula>LEN(TRIM(A21))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="40">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="39">
+      <formula>LEN(TRIM(A19))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="36">
+      <formula>LEN(TRIM(A24))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="35">
+      <formula>LEN(TRIM(A25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:A29">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="34">
+      <formula>LEN(TRIM(A27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="33">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="32">
+      <formula>LEN(TRIM(A31))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="31">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="30">
+      <formula>LEN(TRIM(A33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="25">
+      <formula>LEN(TRIM(A40))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="28">
+      <formula>LEN(TRIM(A37))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A39">
-    <cfRule type="notContainsBlanks" dxfId="72" priority="72">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="27">
       <formula>LEN(TRIM(A39))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
-    <cfRule type="notContainsBlanks" dxfId="58" priority="58">
-      <formula>LEN(TRIM(A30))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
-    <cfRule type="notContainsBlanks" dxfId="57" priority="57">
-      <formula>LEN(TRIM(A31))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="notContainsBlanks" dxfId="56" priority="56">
-      <formula>LEN(TRIM(A32))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="notContainsBlanks" dxfId="55" priority="55">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
-    <cfRule type="notContainsBlanks" dxfId="54" priority="54">
-      <formula>LEN(TRIM(A34))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
-    <cfRule type="notContainsBlanks" dxfId="53" priority="53">
-      <formula>LEN(TRIM(A37))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A38">
-    <cfRule type="notContainsBlanks" dxfId="52" priority="52">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="26">
       <formula>LEN(TRIM(A38))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
-    <cfRule type="notContainsBlanks" dxfId="51" priority="51">
-      <formula>LEN(TRIM(A40))&gt;0</formula>
+  <conditionalFormatting sqref="A44">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="23">
+      <formula>LEN(TRIM(A44))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="notContainsBlanks" dxfId="49" priority="49">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="24">
       <formula>LEN(TRIM(A42))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A44">
-    <cfRule type="notContainsBlanks" dxfId="47" priority="47">
-      <formula>LEN(TRIM(A44))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48 A50">
-    <cfRule type="notContainsBlanks" dxfId="46" priority="46">
+  <conditionalFormatting sqref="A47">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="22">
+      <formula>LEN(TRIM(A47))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:A56">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="21">
+      <formula>LEN(TRIM(A54))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="20">
+      <formula>LEN(TRIM(A65))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="19">
+      <formula>LEN(TRIM(A68))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="14">
       <formula>LEN(TRIM(A48))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A52">
-    <cfRule type="notContainsBlanks" dxfId="45" priority="45">
-      <formula>LEN(TRIM(A52))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55">
-    <cfRule type="notContainsBlanks" dxfId="44" priority="44">
-      <formula>LEN(TRIM(A55))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A58">
-    <cfRule type="notContainsBlanks" dxfId="43" priority="43">
-      <formula>LEN(TRIM(A58))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="42">
-      <formula>LEN(TRIM(A61))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="41">
-      <formula>LEN(TRIM(A67))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="40">
-      <formula>LEN(TRIM(A71))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A75">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="39">
-      <formula>LEN(TRIM(A75))&gt;0</formula>
+  <conditionalFormatting sqref="A46">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="17">
+      <formula>LEN(TRIM(A46))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="16">
+      <formula>LEN(TRIM(A50))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A80">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="12">
+      <formula>LEN(TRIM(A80))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A79">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="13">
+      <formula>LEN(TRIM(A79))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A83">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
+      <formula>LEN(TRIM(A83))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
+      <formula>LEN(TRIM(A87))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="38">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
       <formula>LEN(TRIM(A77))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A80">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="37">
-      <formula>LEN(TRIM(A80))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A82">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="36">
-      <formula>LEN(TRIM(A82))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="34">
-      <formula>LEN(TRIM(A46))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="33">
-      <formula>LEN(TRIM(A47))&gt;0</formula>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(A59))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(A62))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A72">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(A72))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A76">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(A76))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(A88))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A92">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(A92))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A84">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(A84))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="32">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A51))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="31">
-      <formula>LEN(TRIM(A8))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="30">
-      <formula>LEN(TRIM(A9))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="29">
-      <formula>LEN(TRIM(A10))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="28">
-      <formula>LEN(TRIM(A17))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="27">
-      <formula>LEN(TRIM(A23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="26">
-      <formula>LEN(TRIM(A26))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="25">
-      <formula>LEN(TRIM(A41))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A43">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="24">
-      <formula>LEN(TRIM(A43))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="23">
-      <formula>LEN(TRIM(A45))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A49">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="22">
-      <formula>LEN(TRIM(A49))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="21">
-      <formula>LEN(TRIM(A56))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="20">
-      <formula>LEN(TRIM(A59))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="19">
-      <formula>LEN(TRIM(A62))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="18">
-      <formula>LEN(TRIM(A65))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="17">
-      <formula>LEN(TRIM(A69))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A73">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="16">
-      <formula>LEN(TRIM(A73))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
-      <formula>LEN(TRIM(A11))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
-      <formula>LEN(TRIM(A12))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
-      <formula>LEN(TRIM(A35))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
-      <formula>LEN(TRIM(A36))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
-      <formula>LEN(TRIM(A13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
-      <formula>LEN(TRIM(A14))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
-      <formula>LEN(TRIM(A15))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
-      <formula>LEN(TRIM(A18))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
-      <formula>LEN(TRIM(A16))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(A19))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
-      <formula>LEN(TRIM(A20))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21:A22">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(A21))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(A24))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27:A29">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
scripting and doc edits
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="142">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -423,25 +423,31 @@
     <t>Child of prev</t>
   </si>
   <si>
-    <t>cdiscpilot01:HeightLengthOutcome_1</t>
-  </si>
-  <si>
-    <t>missing decimal. Email to AO 9 Aug17</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:PulseHROutcome_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:PulseHROutcome_2</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:PulseHROutcome_3</t>
-  </si>
-  <si>
     <t>BLOOD PRESSURE</t>
   </si>
   <si>
     <t>PULSE</t>
+  </si>
+  <si>
+    <t>WEIGHT</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:HeightOutcome_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:PulseOutcome_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:PulseOutcome_2</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:PulseOutcome_3</t>
+  </si>
+  <si>
+    <t>Pulse label minor error. Email to AO 14Aug</t>
+  </si>
+  <si>
+    <t>HEIGHT</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1061,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1119,7 +1125,6 @@
     <xf numFmtId="0" fontId="26" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1171,7 +1176,56 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="73">
+  <dxfs count="80">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1996,8 +2050,8 @@
   <dimension ref="A1:N103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
+      <pane ySplit="3" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2021,10 +2075,10 @@
       <c r="C1" t="s">
         <v>103</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="41"/>
+      <c r="K1" s="40"/>
       <c r="L1" s="10" t="s">
         <v>44</v>
       </c>
@@ -2995,7 +3049,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="20">
-        <v>42956</v>
+        <v>42961</v>
       </c>
       <c r="B44" s="22" t="s">
         <v>113</v>
@@ -3057,7 +3111,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="20">
-        <v>42956</v>
+        <v>42961</v>
       </c>
       <c r="B47" s="22" t="s">
         <v>113</v>
@@ -3077,7 +3131,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="20">
-        <v>42956</v>
+        <v>42961</v>
       </c>
       <c r="B48" s="22" t="s">
         <v>113</v>
@@ -3089,7 +3143,9 @@
       <c r="E48" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="F48" s="27"/>
+      <c r="F48" s="27" t="s">
+        <v>135</v>
+      </c>
       <c r="G48" s="27"/>
       <c r="H48" s="27"/>
       <c r="I48" s="35"/>
@@ -3115,7 +3171,7 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" s="20">
-        <v>42956</v>
+        <v>42961</v>
       </c>
       <c r="B50" s="22" t="s">
         <v>113</v>
@@ -3133,9 +3189,11 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" s="20">
-        <v>42956</v>
-      </c>
-      <c r="B51" s="21"/>
+        <v>42961</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>113</v>
+      </c>
       <c r="C51" s="22"/>
       <c r="D51" s="23"/>
       <c r="E51" s="22" t="s">
@@ -3158,7 +3216,7 @@
         <v>130</v>
       </c>
       <c r="F52" s="27" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G52" s="27"/>
       <c r="H52" s="27"/>
@@ -3252,7 +3310,7 @@
         <v>116</v>
       </c>
       <c r="F57" s="27" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G57" s="27"/>
       <c r="H57" s="27"/>
@@ -3308,7 +3366,7 @@
         <v>115</v>
       </c>
       <c r="F60" s="27" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G60" s="27"/>
       <c r="H60" s="27"/>
@@ -3366,7 +3424,7 @@
         <v>114</v>
       </c>
       <c r="F63" s="27" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G63" s="27"/>
       <c r="H63" s="27"/>
@@ -3474,7 +3532,7 @@
         <v>117</v>
       </c>
       <c r="F69" s="27" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G69" s="27"/>
       <c r="H69" s="27"/>
@@ -3554,7 +3612,7 @@
         <v>118</v>
       </c>
       <c r="F73" s="27" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G73" s="36"/>
       <c r="H73" s="36"/>
@@ -3635,7 +3693,7 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A78" s="20">
-        <v>42956</v>
+        <v>42961</v>
       </c>
       <c r="B78" s="21"/>
       <c r="C78" s="25" t="s">
@@ -3645,7 +3703,9 @@
       <c r="E78" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="F78" s="21"/>
+      <c r="F78" s="21" t="s">
+        <v>141</v>
+      </c>
       <c r="G78" s="21"/>
       <c r="H78" s="21"/>
       <c r="I78" s="35"/>
@@ -3681,16 +3741,16 @@
       <c r="I80" s="35"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A81" s="21"/>
+      <c r="A81" s="20">
+        <v>42961</v>
+      </c>
       <c r="B81" s="21"/>
       <c r="C81" s="21"/>
       <c r="D81" s="21"/>
-      <c r="E81" s="39" t="s">
-        <v>133</v>
-      </c>
-      <c r="F81" s="21" t="s">
-        <v>134</v>
-      </c>
+      <c r="E81" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="F81" s="21"/>
       <c r="G81" s="21"/>
       <c r="H81" s="21"/>
       <c r="I81" s="35"/>
@@ -3706,7 +3766,7 @@
         <v>124</v>
       </c>
       <c r="F82" s="21" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G82" s="21"/>
       <c r="H82" s="21"/>
@@ -3743,12 +3803,14 @@
       <c r="I84" s="35"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A85" s="21"/>
+      <c r="A85" s="20">
+        <v>42961</v>
+      </c>
       <c r="B85" s="21"/>
       <c r="C85" s="21"/>
       <c r="D85" s="21"/>
       <c r="E85" s="21" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F85" s="21"/>
       <c r="G85" s="21"/>
@@ -3762,11 +3824,11 @@
         <v>94</v>
       </c>
       <c r="D86" s="21"/>
-      <c r="E86" s="32" t="s">
+      <c r="E86" s="21" t="s">
         <v>125</v>
       </c>
       <c r="F86" s="21" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G86" s="21"/>
       <c r="H86" s="21"/>
@@ -3803,14 +3865,18 @@
       <c r="I88" s="35"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A89" s="20"/>
+      <c r="A89" s="20">
+        <v>42961</v>
+      </c>
       <c r="B89" s="21"/>
       <c r="C89" s="21"/>
       <c r="D89" s="22"/>
       <c r="E89" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="F89" s="22"/>
+        <v>138</v>
+      </c>
+      <c r="F89" s="21" t="s">
+        <v>140</v>
+      </c>
       <c r="G89" s="22"/>
       <c r="H89" s="22"/>
       <c r="I89" s="35"/>
@@ -3826,7 +3892,7 @@
         <v>126</v>
       </c>
       <c r="F90" s="21" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G90" s="22"/>
       <c r="H90" s="22"/>
@@ -3860,14 +3926,18 @@
       <c r="I92" s="35"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A93" s="21"/>
+      <c r="A93" s="20">
+        <v>42961</v>
+      </c>
       <c r="B93" s="21"/>
       <c r="C93" s="22"/>
       <c r="D93" s="22"/>
       <c r="E93" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="F93" s="22"/>
+        <v>139</v>
+      </c>
+      <c r="F93" s="21" t="s">
+        <v>140</v>
+      </c>
       <c r="G93" s="22"/>
       <c r="H93" s="22"/>
       <c r="I93" s="35"/>
@@ -3957,368 +4027,383 @@
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:A7">
-    <cfRule type="notContainsBlanks" dxfId="72" priority="201">
+    <cfRule type="notContainsBlanks" dxfId="79" priority="208">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="notContainsBlanks" dxfId="71" priority="62">
+    <cfRule type="notContainsBlanks" dxfId="78" priority="69">
       <formula>LEN(TRIM(A10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="notContainsBlanks" dxfId="70" priority="60">
+    <cfRule type="notContainsBlanks" dxfId="77" priority="67">
       <formula>LEN(TRIM(A23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57">
-    <cfRule type="notContainsBlanks" dxfId="69" priority="77">
+    <cfRule type="notContainsBlanks" dxfId="76" priority="84">
       <formula>LEN(TRIM(A57))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
-    <cfRule type="notContainsBlanks" dxfId="68" priority="78">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="85">
       <formula>LEN(TRIM(A52))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="notContainsBlanks" dxfId="67" priority="74">
+    <cfRule type="notContainsBlanks" dxfId="74" priority="81">
       <formula>LEN(TRIM(A69))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60">
-    <cfRule type="notContainsBlanks" dxfId="66" priority="76">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="83">
       <formula>LEN(TRIM(A60))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="notContainsBlanks" dxfId="65" priority="59">
+    <cfRule type="notContainsBlanks" dxfId="72" priority="66">
       <formula>LEN(TRIM(A26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78">
-    <cfRule type="notContainsBlanks" dxfId="64" priority="72">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="79">
       <formula>LEN(TRIM(A78))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A73">
-    <cfRule type="notContainsBlanks" dxfId="63" priority="73">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="80">
       <formula>LEN(TRIM(A73))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82">
-    <cfRule type="notContainsBlanks" dxfId="62" priority="71">
+    <cfRule type="notContainsBlanks" dxfId="69" priority="78">
       <formula>LEN(TRIM(A82))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63">
-    <cfRule type="notContainsBlanks" dxfId="61" priority="75">
+    <cfRule type="notContainsBlanks" dxfId="68" priority="82">
       <formula>LEN(TRIM(A63))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91">
-    <cfRule type="notContainsBlanks" dxfId="60" priority="69">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="76">
       <formula>LEN(TRIM(A91))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="49">
+      <formula>LEN(TRIM(A15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="notContainsBlanks" dxfId="64" priority="48">
+      <formula>LEN(TRIM(A18))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="36">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="70">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="notContainsBlanks" dxfId="61" priority="68">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="71">
+      <formula>LEN(TRIM(A8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43">
+    <cfRule type="notContainsBlanks" dxfId="59" priority="64">
+      <formula>LEN(TRIM(A43))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="62">
+      <formula>LEN(TRIM(A49))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="65">
+      <formula>LEN(TRIM(A41))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="63">
+      <formula>LEN(TRIM(A45))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="60">
+      <formula>LEN(TRIM(A61))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="61">
+      <formula>LEN(TRIM(A58))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="59">
+      <formula>LEN(TRIM(A64))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="58">
+      <formula>LEN(TRIM(A67))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="57">
+      <formula>LEN(TRIM(A71))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A75">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="56">
+      <formula>LEN(TRIM(A75))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="notContainsBlanks" dxfId="49" priority="55">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="54">
+      <formula>LEN(TRIM(A12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="53">
+      <formula>LEN(TRIM(A35))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="52">
+      <formula>LEN(TRIM(A36))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="51">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="50">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="45">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21:A22">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="44">
+      <formula>LEN(TRIM(A21))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="47">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="46">
+      <formula>LEN(TRIM(A19))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="43">
+      <formula>LEN(TRIM(A24))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="42">
+      <formula>LEN(TRIM(A25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:A29">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="41">
+      <formula>LEN(TRIM(A27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="40">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="39">
+      <formula>LEN(TRIM(A31))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="38">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="37">
+      <formula>LEN(TRIM(A33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="32">
+      <formula>LEN(TRIM(A40))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="35">
+      <formula>LEN(TRIM(A37))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="34">
+      <formula>LEN(TRIM(A39))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="33">
+      <formula>LEN(TRIM(A38))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="30">
+      <formula>LEN(TRIM(A44))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="31">
+      <formula>LEN(TRIM(A42))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:A56">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="28">
+      <formula>LEN(TRIM(A54))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="27">
+      <formula>LEN(TRIM(A65))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="26">
+      <formula>LEN(TRIM(A68))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="24">
+      <formula>LEN(TRIM(A46))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A80">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="19">
+      <formula>LEN(TRIM(A80))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A79">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="20">
+      <formula>LEN(TRIM(A79))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A83">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="18">
+      <formula>LEN(TRIM(A83))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="17">
+      <formula>LEN(TRIM(A87))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A77">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="16">
+      <formula>LEN(TRIM(A77))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
+      <formula>LEN(TRIM(A59))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
+      <formula>LEN(TRIM(A62))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A72">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
+      <formula>LEN(TRIM(A72))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A76">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
+      <formula>LEN(TRIM(A76))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
+      <formula>LEN(TRIM(A88))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A92">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
+      <formula>LEN(TRIM(A92))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A84">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
+      <formula>LEN(TRIM(A84))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(A51))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(A48))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(A50))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(A47))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A81">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(A81))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A85">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(A85))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A89">
-    <cfRule type="notContainsBlanks" dxfId="59" priority="70">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A89))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="notContainsBlanks" dxfId="58" priority="42">
-      <formula>LEN(TRIM(A15))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="notContainsBlanks" dxfId="57" priority="41">
-      <formula>LEN(TRIM(A18))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
-    <cfRule type="notContainsBlanks" dxfId="56" priority="29">
-      <formula>LEN(TRIM(A34))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="notContainsBlanks" dxfId="55" priority="63">
-      <formula>LEN(TRIM(A9))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="notContainsBlanks" dxfId="54" priority="61">
-      <formula>LEN(TRIM(A17))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="notContainsBlanks" dxfId="53" priority="64">
-      <formula>LEN(TRIM(A8))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A43">
-    <cfRule type="notContainsBlanks" dxfId="52" priority="57">
-      <formula>LEN(TRIM(A43))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A49">
-    <cfRule type="notContainsBlanks" dxfId="51" priority="55">
-      <formula>LEN(TRIM(A49))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41">
-    <cfRule type="notContainsBlanks" dxfId="50" priority="58">
-      <formula>LEN(TRIM(A41))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45">
-    <cfRule type="notContainsBlanks" dxfId="49" priority="56">
-      <formula>LEN(TRIM(A45))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61">
-    <cfRule type="notContainsBlanks" dxfId="48" priority="53">
-      <formula>LEN(TRIM(A61))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A58">
-    <cfRule type="notContainsBlanks" dxfId="47" priority="54">
-      <formula>LEN(TRIM(A58))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A64">
-    <cfRule type="notContainsBlanks" dxfId="46" priority="52">
-      <formula>LEN(TRIM(A64))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67">
-    <cfRule type="notContainsBlanks" dxfId="45" priority="51">
-      <formula>LEN(TRIM(A67))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71">
-    <cfRule type="notContainsBlanks" dxfId="44" priority="50">
-      <formula>LEN(TRIM(A71))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A75">
-    <cfRule type="notContainsBlanks" dxfId="43" priority="49">
-      <formula>LEN(TRIM(A75))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="48">
-      <formula>LEN(TRIM(A11))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="47">
-      <formula>LEN(TRIM(A12))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="46">
-      <formula>LEN(TRIM(A35))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="45">
-      <formula>LEN(TRIM(A36))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="44">
-      <formula>LEN(TRIM(A13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="43">
-      <formula>LEN(TRIM(A14))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="38">
-      <formula>LEN(TRIM(A20))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21:A22">
-    <cfRule type="notContainsBlanks" dxfId="35" priority="37">
-      <formula>LEN(TRIM(A21))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="40">
-      <formula>LEN(TRIM(A16))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="39">
-      <formula>LEN(TRIM(A19))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="36">
-      <formula>LEN(TRIM(A24))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="35">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27:A29">
-    <cfRule type="notContainsBlanks" dxfId="30" priority="34">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="33">
-      <formula>LEN(TRIM(A30))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="32">
-      <formula>LEN(TRIM(A31))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="31">
-      <formula>LEN(TRIM(A32))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="30">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="25">
-      <formula>LEN(TRIM(A40))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="28">
-      <formula>LEN(TRIM(A37))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A39">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="27">
-      <formula>LEN(TRIM(A39))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="26">
-      <formula>LEN(TRIM(A38))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A44">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="23">
-      <formula>LEN(TRIM(A44))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A42">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="24">
-      <formula>LEN(TRIM(A42))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="22">
-      <formula>LEN(TRIM(A47))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:A56">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="21">
-      <formula>LEN(TRIM(A54))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="20">
-      <formula>LEN(TRIM(A65))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="19">
-      <formula>LEN(TRIM(A68))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="14">
-      <formula>LEN(TRIM(A48))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="17">
-      <formula>LEN(TRIM(A46))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="16">
-      <formula>LEN(TRIM(A50))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A80">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="12">
-      <formula>LEN(TRIM(A80))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A79">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="13">
-      <formula>LEN(TRIM(A79))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A83">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
-      <formula>LEN(TRIM(A83))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A87">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
-      <formula>LEN(TRIM(A87))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A77">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
-      <formula>LEN(TRIM(A77))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
-      <formula>LEN(TRIM(A59))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
-      <formula>LEN(TRIM(A62))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(A72))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A76">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
-      <formula>LEN(TRIM(A76))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A88">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(A88))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A92">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(A92))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A84">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(A84))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51">
+  <conditionalFormatting sqref="A93">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A51))&gt;0</formula>
+      <formula>LEN(TRIM(A93))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
A step closer with BP based on row order of BP measures for the SDTM code frag. Kludges in createFrag_f need cleaned up.
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -2069,9 +2069,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
BP triples now created. Minor discrepancy with SysBP,  Several extra Ont triples for DiaBP requires clarification with AO
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945"/>
   </bookViews>
   <sheets>
     <sheet name="person_1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="128">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -360,9 +360,6 @@
     <t>cdiscpilot01:C67153.C25298_1</t>
   </si>
   <si>
-    <t>Child of prev</t>
-  </si>
-  <si>
     <t>BLOOD PRESSURE</t>
   </si>
   <si>
@@ -382,6 +379,84 @@
   </si>
   <si>
     <t>cdiscpilot01:WeightOutcome_1</t>
+  </si>
+  <si>
+    <r>
+      <t>Ontology:   study:hasCode  sdtmterm:C67153.C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>25299</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+R                : study:hasCode  sdtmterm:C67153.C25298
+Correct the ontology to point to the C67153.C25298 code</t>
+    </r>
+  </si>
+  <si>
+    <t>cdiscpilot01:BloodPressureOutcome_5</t>
+  </si>
+  <si>
+    <r>
+      <t>Ont: study:hasCode  sdtmterm:C67153.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C25299</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+R: study:hasCode  sdtmterm:C67153.C25298
+Correct ontology to point to  C67153.C25298
+Ont: study:bodyPosition  sdtmterm:C71148.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C62167</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+R: study:bodyPosition  sdtmterm:C71148.C62166
+This is a Standing BP, so change Ont to C71148.C62166</t>
+    </r>
   </si>
   <si>
     <r>
@@ -391,7 +466,6 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -401,7 +475,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -418,7 +491,6 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -428,7 +500,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -445,7 +516,6 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -455,7 +525,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -463,12 +532,21 @@
       <t xml:space="preserve"> 3"</t>
     </r>
   </si>
+  <si>
+    <t>BLOOD PRESSURE Diastolic</t>
+  </si>
+  <si>
+    <t>BLOOD PRESSURE  Diastolic</t>
+  </si>
+  <si>
+    <t>See RDMD notes about additional triples in the DBP measures that are not in the Systolic triples.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,14 +688,6 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color theme="0" tint="-0.34998626667073579"/>
@@ -660,14 +730,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -680,8 +742,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -885,6 +954,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1078,19 +1153,18 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1098,13 +1172,13 @@
     <xf numFmtId="0" fontId="14" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1114,15 +1188,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2067,35 +2142,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G103"/>
+  <dimension ref="A1:G104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
+      <pane ySplit="3" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.08984375" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="57.08984375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="57.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>66</v>
       </c>
@@ -2118,7 +2193,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>42989</v>
       </c>
@@ -2134,12 +2209,12 @@
       <c r="E4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="G4" s="27"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G4" s="26"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>42989</v>
       </c>
@@ -2150,15 +2225,15 @@
         <v>0</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="27"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F5" s="21"/>
+      <c r="G5" s="26"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>42989</v>
       </c>
@@ -2174,10 +2249,10 @@
       <c r="E6" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="27"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F6" s="21"/>
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>42989</v>
       </c>
@@ -2193,10 +2268,10 @@
       <c r="E7" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="27"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F7" s="21"/>
+      <c r="G7" s="26"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>42989</v>
       </c>
@@ -2212,10 +2287,10 @@
       <c r="E8" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="27"/>
-    </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F8" s="21"/>
+      <c r="G8" s="26"/>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>42989</v>
       </c>
@@ -2229,10 +2304,10 @@
       <c r="E9" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="31"/>
-    </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F9" s="21"/>
+      <c r="G9" s="29"/>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>42989</v>
       </c>
@@ -2246,10 +2321,10 @@
       <c r="E10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="31"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F10" s="21"/>
+      <c r="G10" s="29"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>42989</v>
       </c>
@@ -2265,10 +2340,10 @@
       <c r="E11" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="27"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F11" s="21"/>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>42989</v>
       </c>
@@ -2282,10 +2357,10 @@
       <c r="E12" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="22"/>
-      <c r="G12" s="27"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F12" s="21"/>
+      <c r="G12" s="26"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>42989</v>
       </c>
@@ -2299,10 +2374,10 @@
       <c r="E13" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="22"/>
-      <c r="G13" s="27"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F13" s="21"/>
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>42989</v>
       </c>
@@ -2318,10 +2393,10 @@
       <c r="E14" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="22"/>
-      <c r="G14" s="27"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F14" s="21"/>
+      <c r="G14" s="26"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>42989</v>
       </c>
@@ -2335,10 +2410,10 @@
       <c r="E15" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="27"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F15" s="21"/>
+      <c r="G15" s="26"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>42989</v>
       </c>
@@ -2354,10 +2429,10 @@
       <c r="E16" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="27"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F16" s="21"/>
+      <c r="G16" s="26"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>42989</v>
       </c>
@@ -2371,10 +2446,10 @@
       <c r="E17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="22"/>
-      <c r="G17" s="27"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F17" s="21"/>
+      <c r="G17" s="26"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>42989</v>
       </c>
@@ -2388,10 +2463,10 @@
       <c r="E18" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="22"/>
-      <c r="G18" s="27"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F18" s="21"/>
+      <c r="G18" s="26"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>42989</v>
       </c>
@@ -2407,10 +2482,10 @@
       <c r="E19" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="22"/>
-      <c r="G19" s="27"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F19" s="21"/>
+      <c r="G19" s="26"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>42989</v>
       </c>
@@ -2426,10 +2501,10 @@
       <c r="E20" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="22"/>
-      <c r="G20" s="27"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F20" s="21"/>
+      <c r="G20" s="26"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>42989</v>
       </c>
@@ -2445,10 +2520,10 @@
       <c r="E21" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="23"/>
-      <c r="G21" s="27"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F21" s="22"/>
+      <c r="G21" s="26"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>42989</v>
       </c>
@@ -2462,10 +2537,10 @@
       <c r="E22" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="27"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F22" s="21"/>
+      <c r="G22" s="26"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>42989</v>
       </c>
@@ -2479,10 +2554,10 @@
       <c r="E23" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="22"/>
-      <c r="G23" s="27"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F23" s="21"/>
+      <c r="G23" s="26"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>42989</v>
       </c>
@@ -2498,10 +2573,10 @@
       <c r="E24" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="22"/>
-      <c r="G24" s="31"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F24" s="21"/>
+      <c r="G24" s="29"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>42989</v>
       </c>
@@ -2515,10 +2590,10 @@
       <c r="E25" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F25" s="22"/>
-      <c r="G25" s="31"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F25" s="21"/>
+      <c r="G25" s="29"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>42989</v>
       </c>
@@ -2532,10 +2607,10 @@
       <c r="E26" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="22"/>
-      <c r="G26" s="31"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F26" s="21"/>
+      <c r="G26" s="29"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>42989</v>
       </c>
@@ -2551,10 +2626,10 @@
       <c r="E27" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F27" s="22"/>
-      <c r="G27" s="27"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F27" s="21"/>
+      <c r="G27" s="26"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>42989</v>
       </c>
@@ -2570,10 +2645,10 @@
       <c r="E28" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="F28" s="22"/>
-      <c r="G28" s="27"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F28" s="21"/>
+      <c r="G28" s="26"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>42989</v>
       </c>
@@ -2589,10 +2664,10 @@
       <c r="E29" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="F29" s="24"/>
-      <c r="G29" s="27"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F29" s="23"/>
+      <c r="G29" s="26"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>42989</v>
       </c>
@@ -2606,10 +2681,10 @@
       <c r="E30" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F30" s="24"/>
-      <c r="G30" s="31"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F30" s="23"/>
+      <c r="G30" s="29"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>42989</v>
       </c>
@@ -2621,10 +2696,10 @@
       <c r="E31" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F31" s="24"/>
-      <c r="G31" s="31"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F31" s="23"/>
+      <c r="G31" s="29"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>42989</v>
       </c>
@@ -2636,10 +2711,10 @@
       <c r="E32" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F32" s="24"/>
-      <c r="G32" s="31"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F32" s="23"/>
+      <c r="G32" s="29"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>42989</v>
       </c>
@@ -2655,10 +2730,10 @@
       <c r="E33" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F33" s="22"/>
-      <c r="G33" s="27"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F33" s="21"/>
+      <c r="G33" s="26"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>42989</v>
       </c>
@@ -2672,10 +2747,10 @@
       <c r="E34" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="F34" s="24"/>
-      <c r="G34" s="27"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F34" s="23"/>
+      <c r="G34" s="26"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>42989</v>
       </c>
@@ -2689,10 +2764,10 @@
       <c r="E35" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F35" s="22"/>
-      <c r="G35" s="27"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F35" s="21"/>
+      <c r="G35" s="26"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>42989</v>
       </c>
@@ -2706,10 +2781,10 @@
       <c r="E36" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F36" s="22"/>
-      <c r="G36" s="27"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F36" s="21"/>
+      <c r="G36" s="26"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>42989</v>
       </c>
@@ -2725,10 +2800,10 @@
       <c r="E37" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="F37" s="24"/>
-      <c r="G37" s="27"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F37" s="23"/>
+      <c r="G37" s="26"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>42989</v>
       </c>
@@ -2744,10 +2819,10 @@
       <c r="E38" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="F38" s="24"/>
-      <c r="G38" s="27"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F38" s="23"/>
+      <c r="G38" s="26"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>42989</v>
       </c>
@@ -2761,10 +2836,10 @@
       <c r="E39" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F39" s="22"/>
-      <c r="G39" s="27"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F39" s="21"/>
+      <c r="G39" s="26"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>42989</v>
       </c>
@@ -2780,10 +2855,10 @@
       <c r="E40" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="F40" s="25"/>
-      <c r="G40" s="27"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F40" s="24"/>
+      <c r="G40" s="26"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>42989</v>
       </c>
@@ -2797,10 +2872,10 @@
       <c r="E41" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F41" s="25"/>
-      <c r="G41" s="27"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F41" s="24"/>
+      <c r="G41" s="26"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>42989</v>
       </c>
@@ -2816,10 +2891,10 @@
       <c r="E42" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="F42" s="25"/>
-      <c r="G42" s="27"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F42" s="24"/>
+      <c r="G42" s="26"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>42989</v>
       </c>
@@ -2833,10 +2908,10 @@
       <c r="E43" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F43" s="25"/>
-      <c r="G43" s="27"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F43" s="24"/>
+      <c r="G43" s="26"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>42989</v>
       </c>
@@ -2852,10 +2927,10 @@
       <c r="E44" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="F44" s="26"/>
-      <c r="G44" s="27"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F44" s="25"/>
+      <c r="G44" s="26"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>42989</v>
       </c>
@@ -2869,10 +2944,10 @@
       <c r="E45" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F45" s="25"/>
-      <c r="G45" s="27"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F45" s="24"/>
+      <c r="G45" s="26"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>42989</v>
       </c>
@@ -2886,10 +2961,10 @@
       <c r="E46" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="F46" s="25"/>
-      <c r="G46" s="27"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F46" s="24"/>
+      <c r="G46" s="26"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>42989</v>
       </c>
@@ -2903,10 +2978,10 @@
       <c r="E47" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="F47" s="25"/>
-      <c r="G47" s="27"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F47" s="24"/>
+      <c r="G47" s="26"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>42989</v>
       </c>
@@ -2920,10 +2995,10 @@
       <c r="E48" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="F48" s="26"/>
-      <c r="G48" s="27"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F48" s="25"/>
+      <c r="G48" s="26"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>42989</v>
       </c>
@@ -2935,10 +3010,10 @@
       <c r="E49" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F49" s="25"/>
-      <c r="G49" s="27"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F49" s="24"/>
+      <c r="G49" s="26"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
         <v>42989</v>
       </c>
@@ -2950,10 +3025,10 @@
       <c r="E50" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="F50" s="25"/>
-      <c r="G50" s="27"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F50" s="24"/>
+      <c r="G50" s="26"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
         <v>42989</v>
       </c>
@@ -2963,27 +3038,29 @@
       <c r="C51" s="11"/>
       <c r="D51" s="12"/>
       <c r="E51" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="F51" s="25"/>
-      <c r="G51" s="27"/>
-    </row>
-    <row r="52" spans="1:7" s="5" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="21"/>
+        <v>118</v>
+      </c>
+      <c r="F51" s="24"/>
+      <c r="G51" s="26"/>
+    </row>
+    <row r="52" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="20"/>
       <c r="B52" s="12"/>
       <c r="C52" s="14" t="s">
         <v>77</v>
       </c>
       <c r="D52" s="12"/>
-      <c r="E52" s="20" t="s">
+      <c r="E52" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="F52" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="G52" s="22"/>
-    </row>
-    <row r="53" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F52" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="G52" s="30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
         <v>42989</v>
       </c>
@@ -2993,64 +3070,66 @@
       <c r="E53" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F53" s="25"/>
-      <c r="G53" s="22"/>
-    </row>
-    <row r="54" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="21"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="21"/>
+    </row>
+    <row r="54" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="9">
+        <v>42989</v>
+      </c>
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
       <c r="E54" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F54" s="25"/>
-      <c r="G54" s="22"/>
-    </row>
-    <row r="55" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="21"/>
+        <v>80</v>
+      </c>
+      <c r="F54" s="24"/>
+      <c r="G54" s="21"/>
+    </row>
+    <row r="55" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="9">
+        <v>42989</v>
+      </c>
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
-      <c r="D55" s="12" t="s">
+      <c r="D55" s="12"/>
+      <c r="E55" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F55" s="24"/>
+      <c r="G55" s="21"/>
+    </row>
+    <row r="56" spans="1:7" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A56" s="20"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" s="12"/>
+      <c r="E56" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F56" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="E55" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F55" s="25"/>
-      <c r="G55" s="22"/>
-    </row>
-    <row r="56" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="9">
-        <v>42989</v>
-      </c>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="E56" s="11" t="s">
+      <c r="G56" s="21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="9">
+        <v>42989</v>
+      </c>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F56" s="25"/>
-      <c r="G56" s="22"/>
-    </row>
-    <row r="57" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="9"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D57" s="12"/>
-      <c r="E57" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="F57" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="G57" s="22"/>
-    </row>
-    <row r="58" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F57" s="24"/>
+      <c r="G57" s="21"/>
+    </row>
+    <row r="58" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
         <v>42989</v>
       </c>
@@ -3058,303 +3137,311 @@
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
       <c r="E58" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F58" s="25"/>
-      <c r="G58" s="22"/>
-    </row>
-    <row r="59" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="9"/>
+        <v>81</v>
+      </c>
+      <c r="F58" s="24"/>
+      <c r="G58" s="21"/>
+    </row>
+    <row r="59" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="9">
+        <v>42989</v>
+      </c>
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
       <c r="D59" s="12"/>
       <c r="E59" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F59" s="25"/>
-      <c r="G59" s="22"/>
-    </row>
-    <row r="60" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="9"/>
+        <v>64</v>
+      </c>
+      <c r="F59" s="24"/>
+      <c r="G59" s="21"/>
+    </row>
+    <row r="60" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="9">
+        <v>42989</v>
+      </c>
       <c r="B60" s="12"/>
-      <c r="C60" s="14" t="s">
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F60" s="24"/>
+      <c r="G60" s="21"/>
+    </row>
+    <row r="61" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="32"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D60" s="12"/>
-      <c r="E60" s="18" t="s">
+      <c r="D61" s="12"/>
+      <c r="E61" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="F60" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="G60" s="22"/>
-    </row>
-    <row r="61" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="9">
-        <v>42989</v>
-      </c>
-      <c r="B61" s="12"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F61" s="25"/>
-      <c r="G61" s="22"/>
-    </row>
-    <row r="62" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="9"/>
+      <c r="F61" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="G61" s="21"/>
+    </row>
+    <row r="62" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="9">
+        <v>42989</v>
+      </c>
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
       <c r="D62" s="12"/>
       <c r="E62" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F62" s="24"/>
+      <c r="G62" s="21"/>
+    </row>
+    <row r="63" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="9"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="F62" s="25"/>
-      <c r="G62" s="22"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="9"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="14" t="s">
+      <c r="F63" s="24"/>
+      <c r="G63" s="21"/>
+    </row>
+    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="32"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D63" s="12" t="s">
+      <c r="D64" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E63" s="18" t="s">
+      <c r="E64" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F63" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="G63" s="27"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64" s="9">
-        <v>42989</v>
-      </c>
-      <c r="B64" s="10"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F64" s="24"/>
-      <c r="G64" s="27"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" s="9"/>
+      <c r="F64" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="G64" s="30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="9">
+        <v>42989</v>
+      </c>
       <c r="B65" s="10"/>
       <c r="C65" s="11"/>
       <c r="D65" s="12" t="s">
         <v>61</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F65" s="24"/>
-      <c r="G65" s="27"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A66" s="10"/>
+        <v>78</v>
+      </c>
+      <c r="F65" s="23"/>
+      <c r="G65" s="26"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="9"/>
       <c r="B66" s="10"/>
       <c r="C66" s="11"/>
       <c r="D66" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E66" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="F66" s="27"/>
-      <c r="G66" s="27"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A67" s="9">
-        <v>42989</v>
-      </c>
+      <c r="E66" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F66" s="23"/>
+      <c r="G66" s="26"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="10"/>
       <c r="B67" s="10"/>
       <c r="C67" s="11"/>
       <c r="D67" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E67" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F67" s="27"/>
-      <c r="G67" s="27"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" s="9"/>
+      <c r="E67" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F67" s="26"/>
+      <c r="G67" s="26"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="9">
+        <v>42989</v>
+      </c>
       <c r="B68" s="10"/>
       <c r="C68" s="11"/>
       <c r="D68" s="12" t="s">
         <v>61</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F68" s="27"/>
-      <c r="G68" s="27"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+      <c r="F68" s="26"/>
+      <c r="G68" s="26"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="9"/>
       <c r="B69" s="10"/>
-      <c r="C69" s="14" t="s">
+      <c r="C69" s="11"/>
+      <c r="D69" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F69" s="26"/>
+      <c r="G69" s="26"/>
+    </row>
+    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="32"/>
+      <c r="B70" s="10"/>
+      <c r="C70" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D69" s="12" t="s">
+      <c r="D70" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E69" s="18" t="s">
+      <c r="E70" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="F69" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="G69" s="27"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70" s="10"/>
-      <c r="B70" s="10"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E70" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="F70" s="27"/>
-      <c r="G70" s="27"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A71" s="9">
-        <v>42989</v>
-      </c>
+      <c r="F70" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G70" s="30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="10"/>
       <c r="B71" s="10"/>
       <c r="C71" s="11"/>
       <c r="D71" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E71" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F71" s="27"/>
-      <c r="G71" s="27"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A72" s="9"/>
+      <c r="E71" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F71" s="26"/>
+      <c r="G71" s="26"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="9">
+        <v>42989</v>
+      </c>
       <c r="B72" s="10"/>
       <c r="C72" s="11"/>
       <c r="D72" s="12" t="s">
         <v>61</v>
       </c>
       <c r="E72" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F72" s="26"/>
+      <c r="G72" s="26"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="9"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E73" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F72" s="27"/>
-      <c r="G72" s="27"/>
-    </row>
-    <row r="73" spans="1:7" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="9"/>
-      <c r="B73" s="16"/>
-      <c r="C73" s="14" t="s">
+      <c r="F73" s="26"/>
+      <c r="G73" s="26"/>
+    </row>
+    <row r="74" spans="1:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="32"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D73" s="17" t="s">
+      <c r="D74" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E73" s="18" t="s">
+      <c r="E74" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="F73" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="G73" s="32"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A74" s="10"/>
-      <c r="B74" s="10"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E74" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="F74" s="27"/>
-      <c r="G74" s="27"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75" s="9">
-        <v>42989</v>
-      </c>
+      <c r="F74" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G74" s="30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="10"/>
       <c r="B75" s="10"/>
       <c r="C75" s="11"/>
       <c r="D75" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E75" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F75" s="27"/>
-      <c r="G75" s="27"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A76" s="9"/>
+      <c r="E75" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F75" s="26"/>
+      <c r="G75" s="26"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="9">
+        <v>42989</v>
+      </c>
       <c r="B76" s="10"/>
       <c r="C76" s="11"/>
       <c r="D76" s="12" t="s">
         <v>61</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F76" s="27"/>
-      <c r="G76" s="27"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+      <c r="F76" s="26"/>
+      <c r="G76" s="26"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="9"/>
       <c r="B77" s="10"/>
       <c r="C77" s="11"/>
-      <c r="D77" s="12"/>
+      <c r="D77" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="E77" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F77" s="26"/>
+      <c r="G77" s="26"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="9"/>
+      <c r="B78" s="10"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F77" s="27"/>
-      <c r="G77" s="27"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A78" s="9">
-        <v>42989</v>
-      </c>
-      <c r="B78" s="10"/>
-      <c r="C78" s="14" t="s">
+      <c r="F78" s="26"/>
+      <c r="G78" s="26"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="9">
+        <v>42989</v>
+      </c>
+      <c r="B79" s="10"/>
+      <c r="C79" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D78" s="10"/>
-      <c r="E78" s="18" t="s">
+      <c r="D79" s="10"/>
+      <c r="E79" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F78" s="28"/>
-      <c r="G78" s="27"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A79" s="9">
-        <v>42989</v>
-      </c>
-      <c r="B79" s="10"/>
-      <c r="C79" s="10"/>
-      <c r="D79" s="10"/>
-      <c r="E79" s="10" t="s">
-        <v>25</v>
-      </c>
       <c r="F79" s="27"/>
-      <c r="G79" s="27"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G79" s="26"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
         <v>42989</v>
       </c>
@@ -3362,12 +3449,12 @@
       <c r="C80" s="10"/>
       <c r="D80" s="10"/>
       <c r="E80" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F80" s="27"/>
-      <c r="G80" s="27"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="F80" s="26"/>
+      <c r="G80" s="26"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
         <v>42989</v>
       </c>
@@ -3375,42 +3462,41 @@
       <c r="C81" s="10"/>
       <c r="D81" s="10"/>
       <c r="E81" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="F81" s="27"/>
-      <c r="G81" s="27"/>
-    </row>
-    <row r="82" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+      <c r="F81" s="26"/>
+      <c r="G81" s="26"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <v>42989</v>
       </c>
       <c r="B82" s="10"/>
-      <c r="C82" s="14" t="s">
+      <c r="C82" s="10"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F82" s="26"/>
+      <c r="G82" s="26"/>
+    </row>
+    <row r="83" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A83" s="9">
+        <v>42989</v>
+      </c>
+      <c r="B83" s="10"/>
+      <c r="C83" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D82" s="10"/>
-      <c r="E82" s="29" t="s">
+      <c r="D83" s="10"/>
+      <c r="E83" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="F82" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="G82" s="27"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83" s="9">
-        <v>42989</v>
-      </c>
-      <c r="B83" s="10"/>
-      <c r="C83" s="10"/>
-      <c r="D83" s="10"/>
-      <c r="E83" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F83" s="27"/>
-      <c r="G83" s="27"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G83" s="31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>42989</v>
       </c>
@@ -3418,12 +3504,12 @@
       <c r="C84" s="10"/>
       <c r="D84" s="10"/>
       <c r="E84" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F84" s="27"/>
-      <c r="G84" s="27"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="F84" s="26"/>
+      <c r="G84" s="31"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <v>42989</v>
       </c>
@@ -3431,42 +3517,41 @@
       <c r="C85" s="10"/>
       <c r="D85" s="10"/>
       <c r="E85" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="F85" s="27"/>
-      <c r="G85" s="27"/>
-    </row>
-    <row r="86" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+      <c r="F85" s="26"/>
+      <c r="G85" s="31"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="9">
         <v>42989</v>
       </c>
       <c r="B86" s="10"/>
-      <c r="C86" s="14" t="s">
+      <c r="C86" s="10"/>
+      <c r="D86" s="10"/>
+      <c r="E86" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F86" s="26"/>
+      <c r="G86" s="31"/>
+    </row>
+    <row r="87" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A87" s="9">
+        <v>42989</v>
+      </c>
+      <c r="B87" s="10"/>
+      <c r="C87" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D86" s="10"/>
-      <c r="E86" s="29" t="s">
+      <c r="D87" s="10"/>
+      <c r="E87" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="F86" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="G86" s="27"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A87" s="9">
-        <v>42989</v>
-      </c>
-      <c r="B87" s="10"/>
-      <c r="C87" s="10"/>
-      <c r="D87" s="11"/>
-      <c r="E87" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F87" s="22"/>
-      <c r="G87" s="27"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G87" s="31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="9">
         <v>42989</v>
       </c>
@@ -3474,12 +3559,12 @@
       <c r="C88" s="10"/>
       <c r="D88" s="11"/>
       <c r="E88" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F88" s="22"/>
-      <c r="G88" s="27"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="F88" s="21"/>
+      <c r="G88" s="31"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <v>42989</v>
       </c>
@@ -3487,54 +3572,53 @@
       <c r="C89" s="10"/>
       <c r="D89" s="11"/>
       <c r="E89" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="F89" s="27"/>
-      <c r="G89" s="27"/>
-    </row>
-    <row r="90" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+      <c r="F89" s="21"/>
+      <c r="G89" s="31"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>42989</v>
       </c>
       <c r="B90" s="10"/>
-      <c r="C90" s="14" t="s">
+      <c r="C90" s="10"/>
+      <c r="D90" s="11"/>
+      <c r="E90" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F90" s="26"/>
+      <c r="G90" s="31"/>
+    </row>
+    <row r="91" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A91" s="9">
+        <v>42989</v>
+      </c>
+      <c r="B91" s="10"/>
+      <c r="C91" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D90" s="11"/>
-      <c r="E90" s="29" t="s">
+      <c r="D91" s="11"/>
+      <c r="E91" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F90" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="G90" s="27"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A91" s="9">
-        <v>42989</v>
-      </c>
-      <c r="B91" s="10"/>
-      <c r="D91" s="11"/>
-      <c r="E91" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F91" s="22"/>
-      <c r="G91" s="27"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G91" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
         <v>42989</v>
       </c>
       <c r="B92" s="10"/>
-      <c r="C92" s="11"/>
       <c r="D92" s="11"/>
       <c r="E92" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F92" s="22"/>
-      <c r="G92" s="27"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="F92" s="21"/>
+      <c r="G92" s="26"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="9">
         <v>42989</v>
       </c>
@@ -3542,490 +3626,503 @@
       <c r="C93" s="11"/>
       <c r="D93" s="11"/>
       <c r="E93" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="F93" s="27"/>
-      <c r="G93" s="27"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="7"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+      <c r="F93" s="21"/>
+      <c r="G93" s="26"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="9">
+        <v>42989</v>
+      </c>
+      <c r="B94" s="10"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="11"/>
+      <c r="E94" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F94" s="26"/>
+      <c r="G94" s="26"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
       <c r="E95" s="5"/>
       <c r="F95" s="7"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
       <c r="E96" s="5"/>
       <c r="F96" s="7"/>
     </row>
-    <row r="97" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
       <c r="E97" s="5"/>
       <c r="F97" s="7"/>
     </row>
-    <row r="98" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
       <c r="E98" s="5"/>
       <c r="F98" s="7"/>
     </row>
-    <row r="99" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
       <c r="E99" s="5"/>
       <c r="F99" s="7"/>
     </row>
-    <row r="100" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
       <c r="E100" s="5"/>
       <c r="F100" s="7"/>
     </row>
-    <row r="101" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
       <c r="E101" s="5"/>
       <c r="F101" s="7"/>
     </row>
-    <row r="102" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
       <c r="E102" s="5"/>
       <c r="F102" s="7"/>
     </row>
-    <row r="103" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
       <c r="E103" s="5"/>
       <c r="F103" s="7"/>
     </row>
+    <row r="104" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="7"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A4:A7">
-    <cfRule type="notContainsBlanks" dxfId="83" priority="279">
+    <cfRule type="notContainsBlanks" dxfId="83" priority="283">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="notContainsBlanks" dxfId="82" priority="71">
+    <cfRule type="notContainsBlanks" dxfId="82" priority="75">
       <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A56">
+    <cfRule type="notContainsBlanks" dxfId="81" priority="159">
+      <formula>LEN(TRIM(A56))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52">
+    <cfRule type="notContainsBlanks" dxfId="80" priority="160">
+      <formula>LEN(TRIM(A52))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70">
+    <cfRule type="notContainsBlanks" dxfId="79" priority="156">
+      <formula>LEN(TRIM(A70))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61">
+    <cfRule type="notContainsBlanks" dxfId="78" priority="158">
+      <formula>LEN(TRIM(A61))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A74">
+    <cfRule type="notContainsBlanks" dxfId="77" priority="155">
+      <formula>LEN(TRIM(A74))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64">
+    <cfRule type="notContainsBlanks" dxfId="76" priority="157">
+      <formula>LEN(TRIM(A64))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="68">
+      <formula>LEN(TRIM(A36))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="notContainsBlanks" dxfId="74" priority="70">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="89">
+      <formula>LEN(TRIM(A63))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A73">
+    <cfRule type="notContainsBlanks" dxfId="72" priority="88">
+      <formula>LEN(TRIM(A73))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="62">
+      <formula>LEN(TRIM(A19))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="69">
+      <formula>LEN(TRIM(A35))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="notContainsBlanks" dxfId="69" priority="63">
+      <formula>LEN(TRIM(A18))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="notContainsBlanks" dxfId="68" priority="66">
+      <formula>LEN(TRIM(A15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="67">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20">
+    <cfRule type="notContainsBlanks" dxfId="66" priority="61">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A77">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="87">
+      <formula>LEN(TRIM(A77))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66">
+    <cfRule type="notContainsBlanks" dxfId="64" priority="102">
+      <formula>LEN(TRIM(A66))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="101">
+      <formula>LEN(TRIM(A69))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="59">
+      <formula>LEN(TRIM(A26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39">
+    <cfRule type="notContainsBlanks" dxfId="61" priority="58">
+      <formula>LEN(TRIM(A39))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A57">
-    <cfRule type="notContainsBlanks" dxfId="81" priority="155">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="52">
       <formula>LEN(TRIM(A57))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A52">
-    <cfRule type="notContainsBlanks" dxfId="80" priority="156">
-      <formula>LEN(TRIM(A52))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
-    <cfRule type="notContainsBlanks" dxfId="79" priority="152">
-      <formula>LEN(TRIM(A69))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60">
-    <cfRule type="notContainsBlanks" dxfId="78" priority="154">
-      <formula>LEN(TRIM(A60))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A73">
-    <cfRule type="notContainsBlanks" dxfId="77" priority="151">
-      <formula>LEN(TRIM(A73))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A63">
-    <cfRule type="notContainsBlanks" dxfId="76" priority="153">
-      <formula>LEN(TRIM(A63))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="notContainsBlanks" dxfId="75" priority="64">
-      <formula>LEN(TRIM(A36))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="notContainsBlanks" dxfId="74" priority="66">
-      <formula>LEN(TRIM(A13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59">
-    <cfRule type="notContainsBlanks" dxfId="73" priority="86">
+  <conditionalFormatting sqref="A78">
+    <cfRule type="notContainsBlanks" dxfId="59" priority="91">
+      <formula>LEN(TRIM(A78))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="74">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="71">
+      <formula>LEN(TRIM(A12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="65">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="72">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="73">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="64">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="60">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="55">
+      <formula>LEN(TRIM(A49))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="51">
+      <formula>LEN(TRIM(A62))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43">
+    <cfRule type="notContainsBlanks" dxfId="49" priority="57">
+      <formula>LEN(TRIM(A43))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="56">
+      <formula>LEN(TRIM(A45))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A53">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="54">
+      <formula>LEN(TRIM(A53))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="50">
+      <formula>LEN(TRIM(A65))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="49">
+      <formula>LEN(TRIM(A68))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A72">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="48">
+      <formula>LEN(TRIM(A72))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A76">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="47">
+      <formula>LEN(TRIM(A76))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A80">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="46">
+      <formula>LEN(TRIM(A80))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A84">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="45">
+      <formula>LEN(TRIM(A84))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="44">
+      <formula>LEN(TRIM(A88))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A92">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="43">
+      <formula>LEN(TRIM(A92))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="42">
+      <formula>LEN(TRIM(A21))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="41">
+      <formula>LEN(TRIM(A22))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="40">
+      <formula>LEN(TRIM(A24))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="39">
+      <formula>LEN(TRIM(A25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="38">
+      <formula>LEN(TRIM(A27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="37">
+      <formula>LEN(TRIM(A28))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="36">
+      <formula>LEN(TRIM(A29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="35">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="34">
+      <formula>LEN(TRIM(A31))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="33">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="32">
+      <formula>LEN(TRIM(A33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="31">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="30">
+      <formula>LEN(TRIM(A37))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="29">
+      <formula>LEN(TRIM(A38))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A85">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="12">
+      <formula>LEN(TRIM(A85))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="27">
+      <formula>LEN(TRIM(A40))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="26">
+      <formula>LEN(TRIM(A41))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="25">
+      <formula>LEN(TRIM(A42))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="24">
+      <formula>LEN(TRIM(A46))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="23">
+      <formula>LEN(TRIM(A47))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="22">
+      <formula>LEN(TRIM(A44))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="21">
+      <formula>LEN(TRIM(A48))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="20">
+      <formula>LEN(TRIM(A50))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="19">
+      <formula>LEN(TRIM(A51))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A79">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="16">
+      <formula>LEN(TRIM(A79))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A81">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="15">
+      <formula>LEN(TRIM(A81))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A86">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="11">
+      <formula>LEN(TRIM(A86))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="14">
+      <formula>LEN(TRIM(A82))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A83">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="13">
+      <formula>LEN(TRIM(A83))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="6">
+      <formula>LEN(TRIM(A87))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="5">
+      <formula>LEN(TRIM(A91))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A89">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="10">
+      <formula>LEN(TRIM(A89))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="9">
+      <formula>LEN(TRIM(A90))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A93">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="8">
+      <formula>LEN(TRIM(A93))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A94">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="7">
+      <formula>LEN(TRIM(A94))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(A54))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(A55))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(A58))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59:A60">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A59))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62">
-    <cfRule type="notContainsBlanks" dxfId="72" priority="85">
-      <formula>LEN(TRIM(A62))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
-    <cfRule type="notContainsBlanks" dxfId="71" priority="84">
-      <formula>LEN(TRIM(A72))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="notContainsBlanks" dxfId="70" priority="58">
-      <formula>LEN(TRIM(A19))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35">
-    <cfRule type="notContainsBlanks" dxfId="69" priority="65">
-      <formula>LEN(TRIM(A35))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="notContainsBlanks" dxfId="68" priority="59">
-      <formula>LEN(TRIM(A18))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="notContainsBlanks" dxfId="67" priority="62">
-      <formula>LEN(TRIM(A15))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="notContainsBlanks" dxfId="66" priority="63">
-      <formula>LEN(TRIM(A14))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
-    <cfRule type="notContainsBlanks" dxfId="65" priority="57">
-      <formula>LEN(TRIM(A20))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A76">
-    <cfRule type="notContainsBlanks" dxfId="64" priority="83">
-      <formula>LEN(TRIM(A76))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65">
-    <cfRule type="notContainsBlanks" dxfId="63" priority="98">
-      <formula>LEN(TRIM(A65))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68">
-    <cfRule type="notContainsBlanks" dxfId="62" priority="97">
-      <formula>LEN(TRIM(A68))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="notContainsBlanks" dxfId="61" priority="55">
-      <formula>LEN(TRIM(A26))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A39">
-    <cfRule type="notContainsBlanks" dxfId="60" priority="54">
-      <formula>LEN(TRIM(A39))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A58">
-    <cfRule type="notContainsBlanks" dxfId="59" priority="48">
-      <formula>LEN(TRIM(A58))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A77">
-    <cfRule type="notContainsBlanks" dxfId="58" priority="87">
-      <formula>LEN(TRIM(A77))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="notContainsBlanks" dxfId="57" priority="70">
-      <formula>LEN(TRIM(A9))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="notContainsBlanks" dxfId="56" priority="67">
-      <formula>LEN(TRIM(A12))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="notContainsBlanks" dxfId="55" priority="61">
-      <formula>LEN(TRIM(A16))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="notContainsBlanks" dxfId="54" priority="68">
-      <formula>LEN(TRIM(A11))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="notContainsBlanks" dxfId="53" priority="69">
-      <formula>LEN(TRIM(A10))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="notContainsBlanks" dxfId="52" priority="60">
-      <formula>LEN(TRIM(A17))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="notContainsBlanks" dxfId="51" priority="56">
-      <formula>LEN(TRIM(A23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A49">
-    <cfRule type="notContainsBlanks" dxfId="50" priority="51">
-      <formula>LEN(TRIM(A49))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56">
-    <cfRule type="notContainsBlanks" dxfId="49" priority="49">
-      <formula>LEN(TRIM(A56))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A43">
-    <cfRule type="notContainsBlanks" dxfId="48" priority="53">
-      <formula>LEN(TRIM(A43))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45">
-    <cfRule type="notContainsBlanks" dxfId="47" priority="52">
-      <formula>LEN(TRIM(A45))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
-    <cfRule type="notContainsBlanks" dxfId="46" priority="50">
-      <formula>LEN(TRIM(A53))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61">
-    <cfRule type="notContainsBlanks" dxfId="45" priority="47">
-      <formula>LEN(TRIM(A61))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A64">
-    <cfRule type="notContainsBlanks" dxfId="44" priority="46">
-      <formula>LEN(TRIM(A64))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67">
-    <cfRule type="notContainsBlanks" dxfId="43" priority="45">
-      <formula>LEN(TRIM(A67))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="44">
-      <formula>LEN(TRIM(A71))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A75">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="43">
-      <formula>LEN(TRIM(A75))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A79">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="42">
-      <formula>LEN(TRIM(A79))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A83">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="41">
-      <formula>LEN(TRIM(A83))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A87">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="40">
-      <formula>LEN(TRIM(A87))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A91">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="39">
-      <formula>LEN(TRIM(A91))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="38">
-      <formula>LEN(TRIM(A21))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="notContainsBlanks" dxfId="35" priority="37">
-      <formula>LEN(TRIM(A22))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="36">
-      <formula>LEN(TRIM(A24))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="35">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="34">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="33">
-      <formula>LEN(TRIM(A28))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29">
-    <cfRule type="notContainsBlanks" dxfId="30" priority="32">
-      <formula>LEN(TRIM(A29))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="31">
-      <formula>LEN(TRIM(A30))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="30">
-      <formula>LEN(TRIM(A31))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="29">
-      <formula>LEN(TRIM(A32))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="28">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="27">
-      <formula>LEN(TRIM(A34))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="26">
-      <formula>LEN(TRIM(A37))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="25">
-      <formula>LEN(TRIM(A38))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A84">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="8">
-      <formula>LEN(TRIM(A84))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="23">
-      <formula>LEN(TRIM(A40))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="22">
-      <formula>LEN(TRIM(A41))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A42">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="21">
-      <formula>LEN(TRIM(A42))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="20">
-      <formula>LEN(TRIM(A46))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="19">
-      <formula>LEN(TRIM(A47))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A44">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="18">
-      <formula>LEN(TRIM(A44))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="17">
-      <formula>LEN(TRIM(A48))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="16">
-      <formula>LEN(TRIM(A50))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="15">
-      <formula>LEN(TRIM(A51))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="14">
-      <formula>LEN(TRIM(A54))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="13">
-      <formula>LEN(TRIM(A55))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A85">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="7">
-      <formula>LEN(TRIM(A85))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A78">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="12">
-      <formula>LEN(TRIM(A78))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A80">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="11">
-      <formula>LEN(TRIM(A80))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A81">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="10">
-      <formula>LEN(TRIM(A81))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A82">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="9">
-      <formula>LEN(TRIM(A82))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A86">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="2">
-      <formula>LEN(TRIM(A86))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A90">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="1">
-      <formula>LEN(TRIM(A90))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A88">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="6">
-      <formula>LEN(TRIM(A88))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A89">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="5">
-      <formula>LEN(TRIM(A89))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A92">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="4">
-      <formula>LEN(TRIM(A92))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A93">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="3">
-      <formula>LEN(TRIM(A93))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4041,14 +4138,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -4059,7 +4156,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -4073,7 +4170,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -4087,7 +4184,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -4115,14 +4212,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -4130,7 +4227,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -4138,7 +4235,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
@@ -4146,7 +4243,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>35</v>
       </c>
@@ -4154,7 +4251,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4162,7 +4259,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -4170,7 +4267,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -4184,7 +4281,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -4198,7 +4295,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -4212,7 +4309,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -4226,16 +4323,16 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -4243,7 +4340,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -4257,7 +4354,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -4271,7 +4368,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -4285,7 +4382,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -4299,7 +4396,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
@@ -4312,7 +4409,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
@@ -4325,7 +4422,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>54</v>
       </c>
@@ -4336,11 +4433,11 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="3"/>
     </row>

</xml_diff>

<commit_message>
prior to new approach for select triples from AO
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="person_1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="129">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -540,6 +540,9 @@
   </si>
   <si>
     <t>See RDMD notes about additional triples in the DBP measures that are not in the Systolic triples.</t>
+  </si>
+  <si>
+    <t>emailed AO 14Sept17</t>
   </si>
 </sst>
 </file>
@@ -2142,35 +2145,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A93" sqref="A93"/>
+      <pane ySplit="3" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="57.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="49.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="57.1796875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>66</v>
       </c>
@@ -2193,7 +2196,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <v>42989</v>
       </c>
@@ -2214,7 +2217,7 @@
       </c>
       <c r="G4" s="26"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>42989</v>
       </c>
@@ -2233,7 +2236,7 @@
       <c r="F5" s="21"/>
       <c r="G5" s="26"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>42989</v>
       </c>
@@ -2252,7 +2255,7 @@
       <c r="F6" s="21"/>
       <c r="G6" s="26"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>42989</v>
       </c>
@@ -2271,7 +2274,7 @@
       <c r="F7" s="21"/>
       <c r="G7" s="26"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <v>42989</v>
       </c>
@@ -2290,7 +2293,7 @@
       <c r="F8" s="21"/>
       <c r="G8" s="26"/>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>42989</v>
       </c>
@@ -2307,7 +2310,7 @@
       <c r="F9" s="21"/>
       <c r="G9" s="29"/>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <v>42989</v>
       </c>
@@ -2324,7 +2327,7 @@
       <c r="F10" s="21"/>
       <c r="G10" s="29"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <v>42989</v>
       </c>
@@ -2343,7 +2346,7 @@
       <c r="F11" s="21"/>
       <c r="G11" s="26"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>42989</v>
       </c>
@@ -2360,7 +2363,7 @@
       <c r="F12" s="21"/>
       <c r="G12" s="26"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <v>42989</v>
       </c>
@@ -2377,7 +2380,7 @@
       <c r="F13" s="21"/>
       <c r="G13" s="26"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>42989</v>
       </c>
@@ -2396,7 +2399,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="26"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <v>42989</v>
       </c>
@@ -2413,7 +2416,7 @@
       <c r="F15" s="21"/>
       <c r="G15" s="26"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <v>42989</v>
       </c>
@@ -2432,7 +2435,7 @@
       <c r="F16" s="21"/>
       <c r="G16" s="26"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
         <v>42989</v>
       </c>
@@ -2449,7 +2452,7 @@
       <c r="F17" s="21"/>
       <c r="G17" s="26"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
         <v>42989</v>
       </c>
@@ -2466,7 +2469,7 @@
       <c r="F18" s="21"/>
       <c r="G18" s="26"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
         <v>42989</v>
       </c>
@@ -2485,7 +2488,7 @@
       <c r="F19" s="21"/>
       <c r="G19" s="26"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
         <v>42989</v>
       </c>
@@ -2504,7 +2507,7 @@
       <c r="F20" s="21"/>
       <c r="G20" s="26"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="9">
         <v>42989</v>
       </c>
@@ -2523,7 +2526,7 @@
       <c r="F21" s="22"/>
       <c r="G21" s="26"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
         <v>42989</v>
       </c>
@@ -2540,7 +2543,7 @@
       <c r="F22" s="21"/>
       <c r="G22" s="26"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="9">
         <v>42989</v>
       </c>
@@ -2557,7 +2560,7 @@
       <c r="F23" s="21"/>
       <c r="G23" s="26"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="9">
         <v>42989</v>
       </c>
@@ -2576,7 +2579,7 @@
       <c r="F24" s="21"/>
       <c r="G24" s="29"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="9">
         <v>42989</v>
       </c>
@@ -2593,7 +2596,7 @@
       <c r="F25" s="21"/>
       <c r="G25" s="29"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="9">
         <v>42989</v>
       </c>
@@ -2610,7 +2613,7 @@
       <c r="F26" s="21"/>
       <c r="G26" s="29"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="9">
         <v>42989</v>
       </c>
@@ -2629,7 +2632,7 @@
       <c r="F27" s="21"/>
       <c r="G27" s="26"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="9">
         <v>42989</v>
       </c>
@@ -2648,7 +2651,7 @@
       <c r="F28" s="21"/>
       <c r="G28" s="26"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="9">
         <v>42989</v>
       </c>
@@ -2667,7 +2670,7 @@
       <c r="F29" s="23"/>
       <c r="G29" s="26"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="9">
         <v>42989</v>
       </c>
@@ -2684,7 +2687,7 @@
       <c r="F30" s="23"/>
       <c r="G30" s="29"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="9">
         <v>42989</v>
       </c>
@@ -2699,7 +2702,7 @@
       <c r="F31" s="23"/>
       <c r="G31" s="29"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="9">
         <v>42989</v>
       </c>
@@ -2714,7 +2717,7 @@
       <c r="F32" s="23"/>
       <c r="G32" s="29"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="9">
         <v>42989</v>
       </c>
@@ -2733,7 +2736,7 @@
       <c r="F33" s="21"/>
       <c r="G33" s="26"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="9">
         <v>42989</v>
       </c>
@@ -2750,7 +2753,7 @@
       <c r="F34" s="23"/>
       <c r="G34" s="26"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="9">
         <v>42989</v>
       </c>
@@ -2767,7 +2770,7 @@
       <c r="F35" s="21"/>
       <c r="G35" s="26"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="9">
         <v>42989</v>
       </c>
@@ -2784,7 +2787,7 @@
       <c r="F36" s="21"/>
       <c r="G36" s="26"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="9">
         <v>42989</v>
       </c>
@@ -2803,7 +2806,7 @@
       <c r="F37" s="23"/>
       <c r="G37" s="26"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="9">
         <v>42989</v>
       </c>
@@ -2822,7 +2825,7 @@
       <c r="F38" s="23"/>
       <c r="G38" s="26"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="9">
         <v>42989</v>
       </c>
@@ -2839,7 +2842,7 @@
       <c r="F39" s="21"/>
       <c r="G39" s="26"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="9">
         <v>42989</v>
       </c>
@@ -2858,7 +2861,7 @@
       <c r="F40" s="24"/>
       <c r="G40" s="26"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="9">
         <v>42989</v>
       </c>
@@ -2875,7 +2878,7 @@
       <c r="F41" s="24"/>
       <c r="G41" s="26"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="9">
         <v>42989</v>
       </c>
@@ -2894,7 +2897,7 @@
       <c r="F42" s="24"/>
       <c r="G42" s="26"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="9">
         <v>42989</v>
       </c>
@@ -2911,7 +2914,7 @@
       <c r="F43" s="24"/>
       <c r="G43" s="26"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="9">
         <v>42989</v>
       </c>
@@ -2930,7 +2933,7 @@
       <c r="F44" s="25"/>
       <c r="G44" s="26"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="9">
         <v>42989</v>
       </c>
@@ -2947,7 +2950,7 @@
       <c r="F45" s="24"/>
       <c r="G45" s="26"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="9">
         <v>42989</v>
       </c>
@@ -2964,7 +2967,7 @@
       <c r="F46" s="24"/>
       <c r="G46" s="26"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="9">
         <v>42989</v>
       </c>
@@ -2981,7 +2984,7 @@
       <c r="F47" s="24"/>
       <c r="G47" s="26"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="9">
         <v>42989</v>
       </c>
@@ -2998,7 +3001,7 @@
       <c r="F48" s="25"/>
       <c r="G48" s="26"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="9">
         <v>42989</v>
       </c>
@@ -3013,7 +3016,7 @@
       <c r="F49" s="24"/>
       <c r="G49" s="26"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="9">
         <v>42989</v>
       </c>
@@ -3028,7 +3031,7 @@
       <c r="F50" s="24"/>
       <c r="G50" s="26"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="9">
         <v>42989</v>
       </c>
@@ -3043,7 +3046,7 @@
       <c r="F51" s="24"/>
       <c r="G51" s="26"/>
     </row>
-    <row r="52" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A52" s="20"/>
       <c r="B52" s="12"/>
       <c r="C52" s="14" t="s">
@@ -3059,8 +3062,11 @@
       <c r="G52" s="30" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H52" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="9">
         <v>42989</v>
       </c>
@@ -3073,7 +3079,7 @@
       <c r="F53" s="24"/>
       <c r="G53" s="21"/>
     </row>
-    <row r="54" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="9">
         <v>42989</v>
       </c>
@@ -3086,7 +3092,7 @@
       <c r="F54" s="24"/>
       <c r="G54" s="21"/>
     </row>
-    <row r="55" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9">
         <v>42989</v>
       </c>
@@ -3099,7 +3105,7 @@
       <c r="F55" s="24"/>
       <c r="G55" s="21"/>
     </row>
-    <row r="56" spans="1:7" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" s="5" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A56" s="20"/>
       <c r="B56" s="12"/>
       <c r="C56" s="14" t="s">
@@ -3115,8 +3121,11 @@
       <c r="G56" s="21" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H56" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9">
         <v>42989</v>
       </c>
@@ -3129,7 +3138,7 @@
       <c r="F57" s="24"/>
       <c r="G57" s="21"/>
     </row>
-    <row r="58" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9">
         <v>42989</v>
       </c>
@@ -3142,7 +3151,7 @@
       <c r="F58" s="24"/>
       <c r="G58" s="21"/>
     </row>
-    <row r="59" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="9">
         <v>42989</v>
       </c>
@@ -3155,7 +3164,7 @@
       <c r="F59" s="24"/>
       <c r="G59" s="21"/>
     </row>
-    <row r="60" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="9">
         <v>42989</v>
       </c>
@@ -3168,7 +3177,7 @@
       <c r="F60" s="24"/>
       <c r="G60" s="21"/>
     </row>
-    <row r="61" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="32"/>
       <c r="B61" s="12"/>
       <c r="C61" s="14" t="s">
@@ -3183,7 +3192,7 @@
       </c>
       <c r="G61" s="21"/>
     </row>
-    <row r="62" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="9">
         <v>42989</v>
       </c>
@@ -3196,7 +3205,7 @@
       <c r="F62" s="24"/>
       <c r="G62" s="21"/>
     </row>
-    <row r="63" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="9"/>
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
@@ -3207,7 +3216,7 @@
       <c r="F63" s="24"/>
       <c r="G63" s="21"/>
     </row>
-    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="32"/>
       <c r="B64" s="10"/>
       <c r="C64" s="14" t="s">
@@ -3226,7 +3235,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="9">
         <v>42989</v>
       </c>
@@ -3241,7 +3250,7 @@
       <c r="F65" s="23"/>
       <c r="G65" s="26"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="9"/>
       <c r="B66" s="10"/>
       <c r="C66" s="11"/>
@@ -3254,7 +3263,7 @@
       <c r="F66" s="23"/>
       <c r="G66" s="26"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="10"/>
       <c r="B67" s="10"/>
       <c r="C67" s="11"/>
@@ -3267,7 +3276,7 @@
       <c r="F67" s="26"/>
       <c r="G67" s="26"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="9">
         <v>42989</v>
       </c>
@@ -3282,7 +3291,7 @@
       <c r="F68" s="26"/>
       <c r="G68" s="26"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="9"/>
       <c r="B69" s="10"/>
       <c r="C69" s="11"/>
@@ -3295,7 +3304,7 @@
       <c r="F69" s="26"/>
       <c r="G69" s="26"/>
     </row>
-    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="32"/>
       <c r="B70" s="10"/>
       <c r="C70" s="14" t="s">
@@ -3314,7 +3323,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="10"/>
       <c r="B71" s="10"/>
       <c r="C71" s="11"/>
@@ -3327,7 +3336,7 @@
       <c r="F71" s="26"/>
       <c r="G71" s="26"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="9">
         <v>42989</v>
       </c>
@@ -3342,7 +3351,7 @@
       <c r="F72" s="26"/>
       <c r="G72" s="26"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="9"/>
       <c r="B73" s="10"/>
       <c r="C73" s="11"/>
@@ -3355,7 +3364,7 @@
       <c r="F73" s="26"/>
       <c r="G73" s="26"/>
     </row>
-    <row r="74" spans="1:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="32"/>
       <c r="B74" s="16"/>
       <c r="C74" s="14" t="s">
@@ -3374,7 +3383,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="10"/>
       <c r="B75" s="10"/>
       <c r="C75" s="11"/>
@@ -3387,7 +3396,7 @@
       <c r="F75" s="26"/>
       <c r="G75" s="26"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="9">
         <v>42989</v>
       </c>
@@ -3402,7 +3411,7 @@
       <c r="F76" s="26"/>
       <c r="G76" s="26"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="9"/>
       <c r="B77" s="10"/>
       <c r="C77" s="11"/>
@@ -3415,7 +3424,7 @@
       <c r="F77" s="26"/>
       <c r="G77" s="26"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="9"/>
       <c r="B78" s="10"/>
       <c r="C78" s="11"/>
@@ -3426,7 +3435,7 @@
       <c r="F78" s="26"/>
       <c r="G78" s="26"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="9">
         <v>42989</v>
       </c>
@@ -3441,7 +3450,7 @@
       <c r="F79" s="27"/>
       <c r="G79" s="26"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="9">
         <v>42989</v>
       </c>
@@ -3454,7 +3463,7 @@
       <c r="F80" s="26"/>
       <c r="G80" s="26"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="9">
         <v>42989</v>
       </c>
@@ -3467,7 +3476,7 @@
       <c r="F81" s="26"/>
       <c r="G81" s="26"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="9">
         <v>42989</v>
       </c>
@@ -3480,7 +3489,7 @@
       <c r="F82" s="26"/>
       <c r="G82" s="26"/>
     </row>
-    <row r="83" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A83" s="9">
         <v>42989</v>
       </c>
@@ -3496,7 +3505,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="9">
         <v>42989</v>
       </c>
@@ -3509,7 +3518,7 @@
       <c r="F84" s="26"/>
       <c r="G84" s="31"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="9">
         <v>42989</v>
       </c>
@@ -3522,7 +3531,7 @@
       <c r="F85" s="26"/>
       <c r="G85" s="31"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="9">
         <v>42989</v>
       </c>
@@ -3535,7 +3544,7 @@
       <c r="F86" s="26"/>
       <c r="G86" s="31"/>
     </row>
-    <row r="87" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A87" s="9">
         <v>42989</v>
       </c>
@@ -3551,7 +3560,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="9">
         <v>42989</v>
       </c>
@@ -3564,7 +3573,7 @@
       <c r="F88" s="21"/>
       <c r="G88" s="31"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="9">
         <v>42989</v>
       </c>
@@ -3577,7 +3586,7 @@
       <c r="F89" s="21"/>
       <c r="G89" s="31"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="9">
         <v>42989</v>
       </c>
@@ -3590,7 +3599,7 @@
       <c r="F90" s="26"/>
       <c r="G90" s="31"/>
     </row>
-    <row r="91" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A91" s="9">
         <v>42989</v>
       </c>
@@ -3606,7 +3615,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="9">
         <v>42989</v>
       </c>
@@ -3618,7 +3627,7 @@
       <c r="F92" s="21"/>
       <c r="G92" s="26"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="9">
         <v>42989</v>
       </c>
@@ -3631,7 +3640,7 @@
       <c r="F93" s="21"/>
       <c r="G93" s="26"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="9">
         <v>42989</v>
       </c>
@@ -3644,61 +3653,61 @@
       <c r="F94" s="26"/>
       <c r="G94" s="26"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
       <c r="E95" s="5"/>
       <c r="F95" s="7"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
       <c r="E96" s="5"/>
       <c r="F96" s="7"/>
     </row>
-    <row r="97" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
       <c r="E97" s="5"/>
       <c r="F97" s="7"/>
     </row>
-    <row r="98" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
       <c r="E98" s="5"/>
       <c r="F98" s="7"/>
     </row>
-    <row r="99" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
       <c r="E99" s="5"/>
       <c r="F99" s="7"/>
     </row>
-    <row r="100" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
       <c r="E100" s="5"/>
       <c r="F100" s="7"/>
     </row>
-    <row r="101" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
       <c r="E101" s="5"/>
       <c r="F101" s="7"/>
     </row>
-    <row r="102" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
       <c r="E102" s="5"/>
       <c r="F102" s="7"/>
     </row>
-    <row r="103" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
       <c r="E103" s="5"/>
       <c r="F103" s="7"/>
     </row>
-    <row r="104" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
       <c r="E104" s="5"/>
@@ -4138,14 +4147,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -4156,7 +4165,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -4170,7 +4179,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -4184,7 +4193,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -4212,14 +4221,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -4227,7 +4236,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -4235,7 +4244,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
@@ -4243,7 +4252,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>35</v>
       </c>
@@ -4251,7 +4260,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4259,7 +4268,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -4267,7 +4276,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -4281,7 +4290,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -4295,7 +4304,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -4309,7 +4318,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -4323,16 +4332,16 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -4340,7 +4349,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -4354,7 +4363,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -4368,7 +4377,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -4382,7 +4391,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -4396,7 +4405,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
@@ -4409,7 +4418,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
@@ -4422,7 +4431,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>54</v>
       </c>
@@ -4433,11 +4442,11 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="3"/>
     </row>

</xml_diff>

<commit_message>
working on the final BP issues.
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="132">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -334,9 +334,6 @@
   </si>
   <si>
     <t>cdiscpilot01:C67153.C49676_3</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:StartRuleNone_1</t>
   </si>
   <si>
     <t>cdiscpilot01:TemperatureOutcome_1</t>
@@ -438,9 +435,6 @@
     <t>cd01p:Site_1</t>
   </si>
   <si>
-    <t>email to AO. Can't find in any current TTL files!</t>
-  </si>
-  <si>
     <t>CHILD-CHILD-CHILD</t>
   </si>
   <si>
@@ -450,77 +444,25 @@
     <t>cdiscpilot01:BloodPressureOutcome_6</t>
   </si>
   <si>
-    <t>derived flags in R need removed</t>
-  </si>
-  <si>
-    <t>StartRuleNone not in TTL files as Subject. Email to AO 18Sept17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remove derived flag from R ?  </t>
-  </si>
-  <si>
-    <t>Email to AO 18Sept17</t>
-  </si>
-  <si>
-    <t>See above for errors</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Email re. flat to AO 18 Sept. Addtional: NOT EMAILED YET: CHange label in Ont : "P1 Screening 1 Pulse </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Rate </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Email to AO 18Sept17:  NOT EMAILED: Change label to: "P1 Screening 1 Pulse </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Rate </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3"</t>
-    </r>
-  </si>
-  <si>
-    <t>remove derived flag from R ?  . Derived flag IS present in Ont.</t>
-  </si>
-  <si>
     <t>BLOOD PRESSURE Systolic</t>
+  </si>
+  <si>
+    <t>PENDING: Derived flag being added to Ont</t>
+  </si>
+  <si>
+    <t>AO email 19SEpt</t>
+  </si>
+  <si>
+    <t>Email to AO 18Sept17, 19 sept</t>
+  </si>
+  <si>
+    <t>sdtmterm:C74456.CC12421</t>
+  </si>
+  <si>
+    <t>Oral cavity for vsloc in original data. Missing in Ont</t>
+  </si>
+  <si>
+    <t>AO email 19Sept17</t>
   </si>
 </sst>
 </file>
@@ -712,19 +654,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -934,6 +877,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1110,7 +1059,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1150,9 +1099,6 @@
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1171,7 +1117,11 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1217,98 +1167,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="133">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="120">
     <dxf>
       <fill>
         <patternFill>
@@ -2459,11 +2318,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H119"/>
+  <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C74" sqref="C74"/>
+      <pane ySplit="3" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2529,7 +2388,7 @@
       <c r="F4" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
@@ -2542,13 +2401,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>60</v>
       </c>
       <c r="F5" s="19"/>
-      <c r="G5" s="24"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -2567,7 +2426,7 @@
         <v>80</v>
       </c>
       <c r="F6" s="19"/>
-      <c r="G6" s="24"/>
+      <c r="G6" s="23"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
@@ -2586,7 +2445,7 @@
         <v>61</v>
       </c>
       <c r="F7" s="19"/>
-      <c r="G7" s="24"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -2605,7 +2464,7 @@
         <v>65</v>
       </c>
       <c r="F8" s="19"/>
-      <c r="G8" s="24"/>
+      <c r="G8" s="23"/>
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
@@ -2622,7 +2481,7 @@
         <v>54</v>
       </c>
       <c r="F9" s="19"/>
-      <c r="G9" s="27"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -2639,7 +2498,7 @@
         <v>23</v>
       </c>
       <c r="F10" s="19"/>
-      <c r="G10" s="27"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
@@ -2658,7 +2517,7 @@
         <v>66</v>
       </c>
       <c r="F11" s="19"/>
-      <c r="G11" s="24"/>
+      <c r="G11" s="23"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -2675,7 +2534,7 @@
         <v>55</v>
       </c>
       <c r="F12" s="19"/>
-      <c r="G12" s="24"/>
+      <c r="G12" s="23"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
@@ -2692,7 +2551,7 @@
         <v>56</v>
       </c>
       <c r="F13" s="19"/>
-      <c r="G13" s="24"/>
+      <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -2708,10 +2567,10 @@
         <v>9</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F14" s="19"/>
-      <c r="G14" s="24"/>
+      <c r="G14" s="23"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
@@ -2730,7 +2589,7 @@
         <v>67</v>
       </c>
       <c r="F15" s="19"/>
-      <c r="G15" s="24"/>
+      <c r="G15" s="23"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
@@ -2747,7 +2606,7 @@
         <v>23</v>
       </c>
       <c r="F16" s="19"/>
-      <c r="G16" s="24"/>
+      <c r="G16" s="23"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
@@ -2764,7 +2623,7 @@
         <v>57</v>
       </c>
       <c r="F17" s="19"/>
-      <c r="G17" s="24"/>
+      <c r="G17" s="23"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
@@ -2780,10 +2639,10 @@
         <v>11</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F18" s="19"/>
-      <c r="G18" s="24"/>
+      <c r="G18" s="23"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
@@ -2799,10 +2658,10 @@
         <v>12</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F19" s="19"/>
-      <c r="G19" s="24"/>
+      <c r="G19" s="23"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
@@ -2821,7 +2680,7 @@
         <v>14</v>
       </c>
       <c r="F20" s="20"/>
-      <c r="G20" s="24"/>
+      <c r="G20" s="23"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
@@ -2838,7 +2697,7 @@
         <v>69</v>
       </c>
       <c r="F21" s="19"/>
-      <c r="G21" s="24"/>
+      <c r="G21" s="23"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
@@ -2855,7 +2714,7 @@
         <v>23</v>
       </c>
       <c r="F22" s="19"/>
-      <c r="G22" s="24"/>
+      <c r="G22" s="23"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
@@ -2874,7 +2733,7 @@
         <v>68</v>
       </c>
       <c r="F23" s="19"/>
-      <c r="G23" s="27"/>
+      <c r="G23" s="26"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
@@ -2891,7 +2750,7 @@
         <v>70</v>
       </c>
       <c r="F24" s="19"/>
-      <c r="G24" s="27"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
@@ -2908,7 +2767,7 @@
         <v>23</v>
       </c>
       <c r="F25" s="19"/>
-      <c r="G25" s="27"/>
+      <c r="G25" s="26"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
@@ -2927,7 +2786,7 @@
         <v>83</v>
       </c>
       <c r="F26" s="19"/>
-      <c r="G26" s="24"/>
+      <c r="G26" s="23"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
@@ -2946,7 +2805,7 @@
         <v>84</v>
       </c>
       <c r="F27" s="19"/>
-      <c r="G27" s="24"/>
+      <c r="G27" s="23"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
@@ -2965,7 +2824,7 @@
         <v>85</v>
       </c>
       <c r="F28" s="21"/>
-      <c r="G28" s="24"/>
+      <c r="G28" s="23"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
@@ -2982,7 +2841,7 @@
         <v>86</v>
       </c>
       <c r="F29" s="21"/>
-      <c r="G29" s="27"/>
+      <c r="G29" s="26"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
@@ -2997,7 +2856,7 @@
         <v>87</v>
       </c>
       <c r="F30" s="21"/>
-      <c r="G30" s="27"/>
+      <c r="G30" s="26"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
@@ -3012,7 +2871,7 @@
         <v>88</v>
       </c>
       <c r="F31" s="21"/>
-      <c r="G31" s="27"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
@@ -3031,7 +2890,7 @@
         <v>15</v>
       </c>
       <c r="F32" s="19"/>
-      <c r="G32" s="24"/>
+      <c r="G32" s="23"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
@@ -3048,7 +2907,7 @@
         <v>71</v>
       </c>
       <c r="F33" s="21"/>
-      <c r="G33" s="24"/>
+      <c r="G33" s="23"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
@@ -3065,7 +2924,7 @@
         <v>55</v>
       </c>
       <c r="F34" s="19"/>
-      <c r="G34" s="24"/>
+      <c r="G34" s="23"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
@@ -3082,7 +2941,7 @@
         <v>56</v>
       </c>
       <c r="F35" s="19"/>
-      <c r="G35" s="24"/>
+      <c r="G35" s="23"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
@@ -3101,7 +2960,7 @@
         <v>72</v>
       </c>
       <c r="F36" s="21"/>
-      <c r="G36" s="24"/>
+      <c r="G36" s="23"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
@@ -3120,7 +2979,7 @@
         <v>73</v>
       </c>
       <c r="F37" s="21"/>
-      <c r="G37" s="24"/>
+      <c r="G37" s="23"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
@@ -3137,7 +2996,7 @@
         <v>23</v>
       </c>
       <c r="F38" s="19"/>
-      <c r="G38" s="24"/>
+      <c r="G38" s="23"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
@@ -3156,7 +3015,7 @@
         <v>62</v>
       </c>
       <c r="F39" s="22"/>
-      <c r="G39" s="24"/>
+      <c r="G39" s="23"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
@@ -3173,7 +3032,7 @@
         <v>74</v>
       </c>
       <c r="F40" s="22"/>
-      <c r="G40" s="24"/>
+      <c r="G40" s="23"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
@@ -3192,7 +3051,7 @@
         <v>63</v>
       </c>
       <c r="F41" s="22"/>
-      <c r="G41" s="24"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
@@ -3209,7 +3068,7 @@
         <v>74</v>
       </c>
       <c r="F42" s="22"/>
-      <c r="G42" s="24"/>
+      <c r="G42" s="23"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
@@ -3220,15 +3079,17 @@
         <v>73</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="E43" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E43" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="F43" s="23" t="s">
+      <c r="F43" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G43" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
@@ -3245,25 +3106,21 @@
         <v>23</v>
       </c>
       <c r="F44" s="22"/>
-      <c r="G44" s="24"/>
-    </row>
-    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G44" s="23"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
-      <c r="B45" s="11" t="s">
-        <v>90</v>
-      </c>
+      <c r="B45" s="11"/>
       <c r="C45" s="11"/>
-      <c r="D45" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E45" s="32" t="s">
-        <v>104</v>
+      <c r="D45" s="12"/>
+      <c r="E45" s="33" t="s">
+        <v>129</v>
       </c>
       <c r="F45" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="G45" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
+      </c>
+      <c r="G45" s="23" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3278,13 +3135,15 @@
         <v>58</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F46" s="22"/>
-      <c r="G46" s="24"/>
+      <c r="G46" s="23"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="9"/>
+      <c r="A47" s="9">
+        <v>42997</v>
+      </c>
       <c r="B47" s="11" t="s">
         <v>90</v>
       </c>
@@ -3292,13 +3151,11 @@
         <v>73</v>
       </c>
       <c r="D47" s="12"/>
-      <c r="E47" s="31" t="s">
+      <c r="E47" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="F47" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="G47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="23"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
@@ -3313,63 +3170,63 @@
         <v>23</v>
       </c>
       <c r="F48" s="22"/>
-      <c r="G48" s="24"/>
-    </row>
-    <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="9"/>
-      <c r="B49" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C49" s="14"/>
+      <c r="G48" s="23"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="9">
+        <v>42996</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="11"/>
       <c r="D49" s="12"/>
-      <c r="E49" s="32" t="s">
-        <v>104</v>
+      <c r="E49" s="11" t="s">
+        <v>112</v>
       </c>
       <c r="F49" s="22"/>
-      <c r="G49" s="24" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G49" s="23"/>
+    </row>
+    <row r="50" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C50" s="11"/>
+      <c r="C50" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D50" s="12"/>
-      <c r="E50" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F50" s="22"/>
-      <c r="G50" s="24"/>
+      <c r="E50" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="F50" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="G50" s="27"/>
+      <c r="H50" s="5" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="51" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B51" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C51" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="C51" s="12"/>
       <c r="D51" s="12"/>
-      <c r="E51" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="F51" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="G51" s="28"/>
-      <c r="H51" s="5" t="s">
-        <v>119</v>
-      </c>
+      <c r="E51" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F51" s="22"/>
+      <c r="G51" s="19"/>
     </row>
     <row r="52" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B52" s="10" t="s">
         <v>90</v>
@@ -3377,102 +3234,102 @@
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
       <c r="E52" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F52" s="22"/>
       <c r="G52" s="19"/>
     </row>
     <row r="53" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B53" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
+      <c r="D53" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="E53" s="11" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="F53" s="22"/>
       <c r="G53" s="19"/>
     </row>
     <row r="54" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C54" s="12"/>
       <c r="D54" s="12" t="s">
-        <v>59</v>
+        <v>122</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="F54" s="22"/>
       <c r="G54" s="19"/>
     </row>
     <row r="55" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C55" s="12"/>
-      <c r="D55" s="12" t="s">
-        <v>124</v>
-      </c>
+      <c r="D55" s="12"/>
       <c r="E55" s="11" t="s">
-        <v>23</v>
+        <v>113</v>
       </c>
       <c r="F55" s="22"/>
       <c r="G55" s="19"/>
     </row>
-    <row r="56" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C56" s="12"/>
+      <c r="C56" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D56" s="12"/>
-      <c r="E56" s="11" t="s">
+      <c r="E56" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F56" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="G56" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F56" s="22"/>
-      <c r="G56" s="19"/>
-    </row>
-    <row r="57" spans="1:8" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="H56" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C57" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="C57" s="12"/>
       <c r="D57" s="12"/>
-      <c r="E57" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F57" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="G57" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>119</v>
-      </c>
+      <c r="E57" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F57" s="22"/>
+      <c r="G57" s="19"/>
     </row>
     <row r="58" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B58" s="10" t="s">
         <v>90</v>
@@ -3480,97 +3337,97 @@
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
       <c r="E58" s="11" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F58" s="22"/>
       <c r="G58" s="19"/>
     </row>
     <row r="59" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B59" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
+      <c r="D59" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="E59" s="11" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="F59" s="22"/>
       <c r="G59" s="19"/>
     </row>
     <row r="60" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B60" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C60" s="12"/>
       <c r="D60" s="12" t="s">
-        <v>59</v>
+        <v>122</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="F60" s="22"/>
       <c r="G60" s="19"/>
     </row>
     <row r="61" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B61" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C61" s="12"/>
-      <c r="D61" s="12" t="s">
-        <v>124</v>
-      </c>
+      <c r="D61" s="12"/>
       <c r="E61" s="11" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="F61" s="22"/>
       <c r="G61" s="19"/>
     </row>
     <row r="62" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B62" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C62" s="12"/>
+      <c r="C62" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D62" s="12"/>
-      <c r="E62" s="11" t="s">
+      <c r="E62" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F62" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="F62" s="22"/>
       <c r="G62" s="19"/>
     </row>
     <row r="63" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B63" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C63" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="C63" s="12"/>
       <c r="D63" s="12"/>
-      <c r="E63" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="F63" s="22" t="s">
-        <v>135</v>
-      </c>
+      <c r="E63" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F63" s="22"/>
       <c r="G63" s="19"/>
     </row>
     <row r="64" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B64" s="10" t="s">
         <v>90</v>
@@ -3578,100 +3435,98 @@
       <c r="C64" s="12"/>
       <c r="D64" s="12"/>
       <c r="E64" s="11" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F64" s="22"/>
       <c r="G64" s="19"/>
     </row>
     <row r="65" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B65" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
+      <c r="D65" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="E65" s="11" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="F65" s="22"/>
       <c r="G65" s="19"/>
     </row>
     <row r="66" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B66" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C66" s="12"/>
       <c r="D66" s="12" t="s">
-        <v>59</v>
+        <v>122</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="F66" s="22"/>
       <c r="G66" s="19"/>
     </row>
     <row r="67" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B67" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C67" s="12"/>
-      <c r="D67" s="12" t="s">
+      <c r="D67" s="12"/>
+      <c r="E67" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="E67" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="F67" s="22"/>
       <c r="G67" s="19"/>
     </row>
-    <row r="68" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="9">
-        <v>42996</v>
-      </c>
+    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="29"/>
       <c r="B68" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="F68" s="22"/>
-      <c r="G68" s="19"/>
-    </row>
-    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="30"/>
+      <c r="C68" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E68" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F68" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="G68" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="9"/>
       <c r="B69" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C69" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="C69" s="11"/>
       <c r="D69" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E69" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="F69" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G69" s="28" t="s">
-        <v>118</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F69" s="21"/>
+      <c r="G69" s="23"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="9">
-        <v>42996</v>
-      </c>
+      <c r="A70" s="9"/>
       <c r="B70" s="10" t="s">
         <v>90</v>
       </c>
@@ -3680,13 +3535,13 @@
         <v>59</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F70" s="21"/>
-      <c r="G70" s="24"/>
+      <c r="G70" s="23"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="9"/>
+      <c r="A71" s="10"/>
       <c r="B71" s="10" t="s">
         <v>90</v>
       </c>
@@ -3694,14 +3549,14 @@
       <c r="D71" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E71" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F71" s="21"/>
-      <c r="G71" s="24"/>
+      <c r="E71" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F71" s="23"/>
+      <c r="G71" s="23"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="10"/>
+      <c r="A72" s="9"/>
       <c r="B72" s="10" t="s">
         <v>90</v>
       </c>
@@ -3709,16 +3564,14 @@
       <c r="D72" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E72" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F72" s="24"/>
-      <c r="G72" s="24"/>
+      <c r="E72" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F72" s="23"/>
+      <c r="G72" s="23"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="9">
-        <v>42996</v>
-      </c>
+      <c r="A73" s="9"/>
       <c r="B73" s="10" t="s">
         <v>90</v>
       </c>
@@ -3727,10 +3580,10 @@
         <v>59</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F73" s="24"/>
-      <c r="G73" s="24"/>
+        <v>76</v>
+      </c>
+      <c r="F73" s="23"/>
+      <c r="G73" s="23"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="9"/>
@@ -3738,14 +3591,10 @@
         <v>90</v>
       </c>
       <c r="C74" s="11"/>
-      <c r="D74" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E74" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F74" s="24"/>
-      <c r="G74" s="24"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="23"/>
+      <c r="G74" s="23"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="9"/>
@@ -3755,43 +3604,47 @@
       <c r="C75" s="11"/>
       <c r="D75" s="12"/>
       <c r="E75" s="11"/>
-      <c r="F75" s="24"/>
-      <c r="G75" s="24"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="9"/>
+      <c r="F75" s="23"/>
+      <c r="G75" s="23"/>
+    </row>
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="29"/>
       <c r="B76" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C76" s="11"/>
-      <c r="D76" s="12"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="24"/>
-      <c r="G76" s="24"/>
-    </row>
-    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="30"/>
+      <c r="C76" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E76" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="F76" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G76" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="10"/>
       <c r="B77" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C77" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="C77" s="11"/>
       <c r="D77" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E77" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="F77" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="G77" s="28" t="s">
-        <v>118</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E77" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F77" s="23"/>
+      <c r="G77" s="23"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="10"/>
+      <c r="A78" s="9"/>
       <c r="B78" s="10" t="s">
         <v>90</v>
       </c>
@@ -3799,16 +3652,14 @@
       <c r="D78" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E78" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F78" s="24"/>
-      <c r="G78" s="24"/>
+      <c r="E78" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F78" s="23"/>
+      <c r="G78" s="23"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="9">
-        <v>42996</v>
-      </c>
+      <c r="A79" s="9"/>
       <c r="B79" s="10" t="s">
         <v>90</v>
       </c>
@@ -3817,10 +3668,10 @@
         <v>59</v>
       </c>
       <c r="E79" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="F79" s="24"/>
-      <c r="G79" s="24"/>
+        <v>77</v>
+      </c>
+      <c r="F79" s="23"/>
+      <c r="G79" s="23"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="9"/>
@@ -3828,14 +3679,10 @@
         <v>90</v>
       </c>
       <c r="C80" s="11"/>
-      <c r="D80" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="F80" s="24"/>
-      <c r="G80" s="24"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="23"/>
+      <c r="G80" s="23"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="9"/>
@@ -3845,43 +3692,47 @@
       <c r="C81" s="11"/>
       <c r="D81" s="12"/>
       <c r="E81" s="10"/>
-      <c r="F81" s="24"/>
-      <c r="G81" s="24"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="9"/>
+      <c r="F81" s="23"/>
+      <c r="G81" s="23"/>
+    </row>
+    <row r="82" spans="1:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="29"/>
       <c r="B82" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C82" s="11"/>
-      <c r="D82" s="12"/>
-      <c r="E82" s="10"/>
-      <c r="F82" s="24"/>
-      <c r="G82" s="24"/>
-    </row>
-    <row r="83" spans="1:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="30"/>
+      <c r="C82" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D82" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E82" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="F82" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G82" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="10"/>
       <c r="B83" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C83" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D83" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E83" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="F83" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="G83" s="28" t="s">
-        <v>118</v>
-      </c>
+      <c r="C83" s="11"/>
+      <c r="D83" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E83" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F83" s="23"/>
+      <c r="G83" s="23"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="10"/>
+      <c r="A84" s="9"/>
       <c r="B84" s="10" t="s">
         <v>90</v>
       </c>
@@ -3889,16 +3740,14 @@
       <c r="D84" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E84" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F84" s="24"/>
-      <c r="G84" s="24"/>
+      <c r="E84" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F84" s="23"/>
+      <c r="G84" s="23"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="9">
-        <v>42996</v>
-      </c>
+      <c r="A85" s="9"/>
       <c r="B85" s="10" t="s">
         <v>90</v>
       </c>
@@ -3907,10 +3756,10 @@
         <v>59</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="F85" s="24"/>
-      <c r="G85" s="24"/>
+        <v>78</v>
+      </c>
+      <c r="F85" s="23"/>
+      <c r="G85" s="23"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="9"/>
@@ -3918,168 +3767,168 @@
         <v>90</v>
       </c>
       <c r="C86" s="11"/>
-      <c r="D86" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="D86" s="12"/>
       <c r="E86" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F86" s="24"/>
-      <c r="G86" s="24"/>
+        <v>62</v>
+      </c>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="9"/>
       <c r="B87" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C87" s="11"/>
-      <c r="D87" s="12"/>
-      <c r="E87" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F87" s="24"/>
-      <c r="G87" s="24"/>
+      <c r="C87" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D87" s="10"/>
+      <c r="E87" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F87" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G87" s="23" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="9"/>
       <c r="B88" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C88" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="C88" s="10"/>
       <c r="D88" s="10"/>
-      <c r="E88" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="F88" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="G88" s="24" t="s">
-        <v>130</v>
-      </c>
+      <c r="E88" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F88" s="23"/>
+      <c r="G88" s="23"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="9">
-        <v>42996</v>
-      </c>
+      <c r="A89" s="9"/>
       <c r="B89" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C89" s="10"/>
       <c r="D89" s="10"/>
       <c r="E89" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F89" s="24"/>
-      <c r="G89" s="24"/>
+        <v>107</v>
+      </c>
+      <c r="F89" s="23"/>
+      <c r="G89" s="23"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="9"/>
       <c r="B90" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C90" s="10"/>
+      <c r="C90" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D90" s="10"/>
-      <c r="E90" s="32" t="s">
-        <v>104</v>
+      <c r="E90" s="25" t="s">
+        <v>101</v>
       </c>
       <c r="F90" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="G90" s="24"/>
+        <v>126</v>
+      </c>
+      <c r="G90" s="23" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="9"/>
+      <c r="A91" s="9">
+        <v>42996</v>
+      </c>
       <c r="B91" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C91" s="10"/>
       <c r="D91" s="10"/>
       <c r="E91" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F91" s="24"/>
-      <c r="G91" s="24"/>
+        <v>23</v>
+      </c>
+      <c r="F91" s="23"/>
+      <c r="G91" s="28"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="9"/>
+      <c r="A92" s="9">
+        <v>42996</v>
+      </c>
       <c r="B92" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C92" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="C92" s="10"/>
       <c r="D92" s="10"/>
-      <c r="E92" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="F92" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="G92" s="24" t="s">
-        <v>130</v>
-      </c>
+      <c r="E92" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F92" s="23"/>
+      <c r="G92" s="28"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="9">
         <v>42996</v>
       </c>
-      <c r="B93" s="10" t="s">
-        <v>90</v>
-      </c>
+      <c r="B93" s="10"/>
       <c r="C93" s="10"/>
-      <c r="D93" s="10"/>
+      <c r="D93" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="E93" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F93" s="24"/>
-      <c r="G93" s="29"/>
+        <v>63</v>
+      </c>
+      <c r="F93" s="23"/>
+      <c r="G93" s="28"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="9">
         <v>42996</v>
       </c>
-      <c r="B94" s="10" t="s">
-        <v>90</v>
-      </c>
+      <c r="B94" s="10"/>
       <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
+      <c r="D94" s="12" t="s">
+        <v>122</v>
+      </c>
       <c r="E94" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F94" s="24"/>
-      <c r="G94" s="29"/>
+        <v>23</v>
+      </c>
+      <c r="F94" s="23"/>
+      <c r="G94" s="28"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="9">
         <v>42996</v>
       </c>
-      <c r="B95" s="10"/>
+      <c r="B95" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="C95" s="10"/>
-      <c r="D95" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="D95" s="10"/>
       <c r="E95" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F95" s="24"/>
-      <c r="G95" s="29"/>
+        <v>108</v>
+      </c>
+      <c r="F95" s="23"/>
+      <c r="G95" s="28"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
-        <v>42996</v>
-      </c>
-      <c r="B96" s="10"/>
-      <c r="C96" s="10"/>
-      <c r="D96" s="12" t="s">
-        <v>124</v>
-      </c>
+        <v>42997</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D96" s="10"/>
       <c r="E96" s="10" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="F96" s="24"/>
-      <c r="G96" s="29"/>
+      <c r="G96" s="23"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="9">
@@ -4089,89 +3938,87 @@
         <v>90</v>
       </c>
       <c r="C97" s="10"/>
-      <c r="D97" s="10"/>
+      <c r="D97" s="11"/>
       <c r="E97" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F97" s="24"/>
-      <c r="G97" s="29"/>
-    </row>
-    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="F97" s="19"/>
+      <c r="G97" s="28"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="9">
+        <v>42997</v>
+      </c>
       <c r="B98" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C98" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D98" s="10"/>
-      <c r="E98" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="F98" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="G98" s="24" t="s">
-        <v>132</v>
-      </c>
+      <c r="C98" s="10"/>
+      <c r="D98" s="11"/>
+      <c r="E98" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F98" s="19"/>
+      <c r="G98" s="28"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="9">
-        <v>42996</v>
-      </c>
-      <c r="B99" s="10" t="s">
-        <v>90</v>
-      </c>
+        <v>42997</v>
+      </c>
+      <c r="B99" s="10"/>
       <c r="C99" s="10"/>
       <c r="D99" s="11"/>
       <c r="E99" s="10" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="F99" s="19"/>
-      <c r="G99" s="29"/>
+      <c r="G99" s="28"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="9">
         <v>42996</v>
       </c>
-      <c r="B100" s="10" t="s">
-        <v>90</v>
-      </c>
+      <c r="B100" s="10"/>
       <c r="C100" s="10"/>
-      <c r="D100" s="11"/>
+      <c r="D100" s="12" t="s">
+        <v>122</v>
+      </c>
       <c r="E100" s="10" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="F100" s="19"/>
-      <c r="G100" s="29"/>
+      <c r="G100" s="28"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="9">
-        <v>42996</v>
-      </c>
-      <c r="B101" s="10"/>
+        <v>42997</v>
+      </c>
+      <c r="B101" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="C101" s="10"/>
       <c r="D101" s="11"/>
       <c r="E101" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F101" s="19"/>
-      <c r="G101" s="29"/>
+        <v>109</v>
+      </c>
+      <c r="F101" s="23"/>
+      <c r="G101" s="28"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="9">
-        <v>42996</v>
-      </c>
-      <c r="B102" s="10"/>
-      <c r="C102" s="10"/>
-      <c r="D102" s="12" t="s">
-        <v>124</v>
-      </c>
+        <v>42997</v>
+      </c>
+      <c r="B102" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C102" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D102" s="11"/>
       <c r="E102" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F102" s="19"/>
-      <c r="G102" s="29"/>
+        <v>103</v>
+      </c>
+      <c r="F102" s="24"/>
+      <c r="G102" s="23"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="9">
@@ -4180,104 +4027,82 @@
       <c r="B103" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C103" s="10"/>
       <c r="D103" s="11"/>
       <c r="E103" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="F103" s="24"/>
-      <c r="G103" s="29"/>
-    </row>
-    <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="F103" s="19"/>
+      <c r="G103" s="23"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="9">
+        <v>42996</v>
+      </c>
       <c r="B104" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C104" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="C104" s="11"/>
       <c r="D104" s="11"/>
-      <c r="E104" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="F104" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="G104" s="24" t="s">
-        <v>133</v>
-      </c>
+      <c r="E104" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F104" s="19"/>
+      <c r="G104" s="23"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="9">
         <v>42996</v>
       </c>
-      <c r="B105" s="10" t="s">
-        <v>90</v>
-      </c>
+      <c r="B105" s="10"/>
+      <c r="C105" s="11"/>
       <c r="D105" s="11"/>
       <c r="E105" s="10" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="F105" s="19"/>
-      <c r="G105" s="24"/>
+      <c r="G105" s="23"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="9">
         <v>42996</v>
       </c>
-      <c r="B106" s="10" t="s">
-        <v>90</v>
-      </c>
+      <c r="B106" s="10"/>
       <c r="C106" s="11"/>
-      <c r="D106" s="11"/>
+      <c r="D106" s="12" t="s">
+        <v>122</v>
+      </c>
       <c r="E106" s="10" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="F106" s="19"/>
-      <c r="G106" s="24"/>
+      <c r="G106" s="23"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="9">
         <v>42996</v>
       </c>
-      <c r="B107" s="10"/>
+      <c r="B107" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="C107" s="11"/>
       <c r="D107" s="11"/>
       <c r="E107" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F107" s="19"/>
-      <c r="G107" s="24"/>
+        <v>110</v>
+      </c>
+      <c r="F107" s="23"/>
+      <c r="G107" s="23"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="9">
-        <v>42996</v>
-      </c>
-      <c r="B108" s="10"/>
-      <c r="C108" s="11"/>
-      <c r="D108" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="E108" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F108" s="19"/>
-      <c r="G108" s="24"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="7"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="9">
-        <v>42996</v>
-      </c>
-      <c r="B109" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C109" s="11"/>
-      <c r="D109" s="11"/>
-      <c r="E109" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="F109" s="24"/>
-      <c r="G109" s="24"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="7"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C110" s="5"/>
@@ -4327,482 +4152,460 @@
       <c r="E117" s="5"/>
       <c r="F117" s="7"/>
     </row>
-    <row r="118" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
-      <c r="E118" s="5"/>
-      <c r="F118" s="7"/>
-    </row>
-    <row r="119" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
-      <c r="E119" s="5"/>
-      <c r="F119" s="7"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="A4:A7">
-    <cfRule type="notContainsBlanks" dxfId="132" priority="358">
+    <cfRule type="notContainsBlanks" dxfId="119" priority="384">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A77">
-    <cfRule type="notContainsBlanks" dxfId="131" priority="231">
-      <formula>LEN(TRIM(A77))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A83">
-    <cfRule type="notContainsBlanks" dxfId="127" priority="230">
-      <formula>LEN(TRIM(A83))&gt;0</formula>
+  <conditionalFormatting sqref="A76">
+    <cfRule type="notContainsBlanks" dxfId="118" priority="257">
+      <formula>LEN(TRIM(A76))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82">
+    <cfRule type="notContainsBlanks" dxfId="117" priority="256">
+      <formula>LEN(TRIM(A82))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68">
+    <cfRule type="notContainsBlanks" dxfId="116" priority="258">
+      <formula>LEN(TRIM(A68))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="notContainsBlanks" dxfId="115" priority="114">
+      <formula>LEN(TRIM(A90))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A79:A81">
+    <cfRule type="notContainsBlanks" dxfId="114" priority="189">
+      <formula>LEN(TRIM(A79))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43">
+    <cfRule type="notContainsBlanks" dxfId="113" priority="123">
+      <formula>LEN(TRIM(A43))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="notContainsBlanks" dxfId="112" priority="122">
+      <formula>LEN(TRIM(A47))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A85">
+    <cfRule type="notContainsBlanks" dxfId="111" priority="188">
+      <formula>LEN(TRIM(A85))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70">
+    <cfRule type="notContainsBlanks" dxfId="110" priority="203">
+      <formula>LEN(TRIM(A70))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A73:A75">
+    <cfRule type="notContainsBlanks" dxfId="109" priority="202">
+      <formula>LEN(TRIM(A73))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="notContainsBlanks" dxfId="108" priority="117">
+      <formula>LEN(TRIM(A87))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A86">
+    <cfRule type="notContainsBlanks" dxfId="107" priority="192">
+      <formula>LEN(TRIM(A86))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A89">
+    <cfRule type="notContainsBlanks" dxfId="106" priority="115">
+      <formula>LEN(TRIM(A89))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A96">
+    <cfRule type="notContainsBlanks" dxfId="105" priority="107">
+      <formula>LEN(TRIM(A96))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48">
+    <cfRule type="notContainsBlanks" dxfId="103" priority="94">
+      <formula>LEN(TRIM(A48))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="notContainsBlanks" dxfId="100" priority="98">
+      <formula>LEN(TRIM(A25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:A10">
+    <cfRule type="notContainsBlanks" dxfId="99" priority="101">
+      <formula>LEN(TRIM(A8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="notContainsBlanks" dxfId="98" priority="100">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="notContainsBlanks" dxfId="97" priority="99">
+      <formula>LEN(TRIM(A22))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44:A45">
+    <cfRule type="notContainsBlanks" dxfId="96" priority="95">
+      <formula>LEN(TRIM(A44))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="notContainsBlanks" dxfId="126" priority="232">
+    <cfRule type="notContainsBlanks" dxfId="93" priority="90">
       <formula>LEN(TRIM(A69))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A45">
-    <cfRule type="notContainsBlanks" dxfId="125" priority="99">
-      <formula>LEN(TRIM(A45))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A80:A82">
-    <cfRule type="notContainsBlanks" dxfId="124" priority="163">
-      <formula>LEN(TRIM(A80))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A43">
-    <cfRule type="notContainsBlanks" dxfId="122" priority="97">
-      <formula>LEN(TRIM(A43))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
-    <cfRule type="notContainsBlanks" dxfId="119" priority="96">
-      <formula>LEN(TRIM(A47))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A86">
-    <cfRule type="notContainsBlanks" dxfId="118" priority="162">
-      <formula>LEN(TRIM(A86))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71">
-    <cfRule type="notContainsBlanks" dxfId="117" priority="177">
-      <formula>LEN(TRIM(A71))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A74:A76">
-    <cfRule type="notContainsBlanks" dxfId="116" priority="176">
-      <formula>LEN(TRIM(A74))&gt;0</formula>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="notContainsBlanks" dxfId="92" priority="97">
+      <formula>LEN(TRIM(A40))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42">
+    <cfRule type="notContainsBlanks" dxfId="91" priority="96">
+      <formula>LEN(TRIM(A42))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A84">
+    <cfRule type="notContainsBlanks" dxfId="90" priority="87">
+      <formula>LEN(TRIM(A84))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A103">
+    <cfRule type="notContainsBlanks" dxfId="89" priority="82">
+      <formula>LEN(TRIM(A103))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A72">
+    <cfRule type="notContainsBlanks" dxfId="87" priority="89">
+      <formula>LEN(TRIM(A72))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A78">
+    <cfRule type="notContainsBlanks" dxfId="86" priority="88">
+      <formula>LEN(TRIM(A78))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
+    <cfRule type="notContainsBlanks" dxfId="85" priority="77">
+      <formula>LEN(TRIM(A35))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="notContainsBlanks" dxfId="113" priority="91">
+    <cfRule type="notContainsBlanks" dxfId="84" priority="85">
       <formula>LEN(TRIM(A88))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A87">
-    <cfRule type="notContainsBlanks" dxfId="112" priority="166">
-      <formula>LEN(TRIM(A87))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A91">
-    <cfRule type="notContainsBlanks" dxfId="108" priority="89">
+    <cfRule type="notContainsBlanks" dxfId="83" priority="84">
       <formula>LEN(TRIM(A91))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A97">
+    <cfRule type="notContainsBlanks" dxfId="82" priority="83">
+      <formula>LEN(TRIM(A97))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="notContainsBlanks" dxfId="80" priority="81">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="notContainsBlanks" dxfId="79" priority="80">
+      <formula>LEN(TRIM(A12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="notContainsBlanks" dxfId="78" priority="79">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="notContainsBlanks" dxfId="77" priority="78">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="notContainsBlanks" dxfId="76" priority="76">
+      <formula>LEN(TRIM(A18))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="75">
+      <formula>LEN(TRIM(A19))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="notContainsBlanks" dxfId="74" priority="74">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="73">
+      <formula>LEN(TRIM(A15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="notContainsBlanks" dxfId="72" priority="72">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="71">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="70">
+      <formula>LEN(TRIM(A21))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="notContainsBlanks" dxfId="69" priority="69">
+      <formula>LEN(TRIM(A24))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="notContainsBlanks" dxfId="68" priority="68">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="67">
+      <formula>LEN(TRIM(A26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27">
+    <cfRule type="notContainsBlanks" dxfId="66" priority="66">
+      <formula>LEN(TRIM(A27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="65">
+      <formula>LEN(TRIM(A28))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29">
+    <cfRule type="notContainsBlanks" dxfId="64" priority="64">
+      <formula>LEN(TRIM(A29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="63">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="62">
+      <formula>LEN(TRIM(A31))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="notContainsBlanks" dxfId="61" priority="61">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="60">
+      <formula>LEN(TRIM(A33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="notContainsBlanks" dxfId="59" priority="59">
+      <formula>LEN(TRIM(A36))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="58">
+      <formula>LEN(TRIM(A38))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="57">
+      <formula>LEN(TRIM(A37))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="56">
+      <formula>LEN(TRIM(A39))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="55">
+      <formula>LEN(TRIM(A41))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="54">
+      <formula>LEN(TRIM(A46))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="53">
+      <formula>LEN(TRIM(A49))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="48">
+      <formula>LEN(TRIM(A56))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A94">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="39">
+      <formula>LEN(TRIM(A94))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A93">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="38">
+      <formula>LEN(TRIM(A93))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A92">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="37">
+      <formula>LEN(TRIM(A92))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A95">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="36">
+      <formula>LEN(TRIM(A95))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A104">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="31">
+      <formula>LEN(TRIM(A104))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A100">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="33">
+      <formula>LEN(TRIM(A100))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A105">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="30">
+      <formula>LEN(TRIM(A105))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A106">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="29">
+      <formula>LEN(TRIM(A106))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A107">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="28">
+      <formula>LEN(TRIM(A107))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A98">
-    <cfRule type="notContainsBlanks" dxfId="106" priority="81">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="26">
       <formula>LEN(TRIM(A98))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A49">
-    <cfRule type="notContainsBlanks" dxfId="98" priority="95">
-      <formula>LEN(TRIM(A49))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A104">
-    <cfRule type="notContainsBlanks" dxfId="95" priority="80">
-      <formula>LEN(TRIM(A104))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A90">
-    <cfRule type="notContainsBlanks" dxfId="93" priority="90">
-      <formula>LEN(TRIM(A90))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A92">
-    <cfRule type="notContainsBlanks" dxfId="91" priority="88">
-      <formula>LEN(TRIM(A92))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="80" priority="72">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8:A10">
-    <cfRule type="notContainsBlanks" dxfId="79" priority="75">
-      <formula>LEN(TRIM(A8))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="notContainsBlanks" dxfId="76" priority="74">
-      <formula>LEN(TRIM(A16))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="notContainsBlanks" dxfId="74" priority="73">
-      <formula>LEN(TRIM(A22))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A44">
-    <cfRule type="notContainsBlanks" dxfId="73" priority="69">
-      <formula>LEN(TRIM(A44))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
-    <cfRule type="notContainsBlanks" dxfId="72" priority="68">
-      <formula>LEN(TRIM(A48))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61:A62">
-    <cfRule type="notContainsBlanks" dxfId="71" priority="65">
+  <conditionalFormatting sqref="A99">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="25">
+      <formula>LEN(TRIM(A99))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A101">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="24">
+      <formula>LEN(TRIM(A101))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A102">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="23">
+      <formula>LEN(TRIM(A102))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="16">
+      <formula>LEN(TRIM(A51))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="18">
+      <formula>LEN(TRIM(A50))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="15">
+      <formula>LEN(TRIM(A52))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="12">
+      <formula>LEN(TRIM(A55))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A53">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
+      <formula>LEN(TRIM(A53))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
+      <formula>LEN(TRIM(A54))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
+      <formula>LEN(TRIM(A57))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
+      <formula>LEN(TRIM(A58))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
+      <formula>LEN(TRIM(A59))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(A60))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
       <formula>LEN(TRIM(A61))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A70">
-    <cfRule type="notContainsBlanks" dxfId="70" priority="64">
-      <formula>LEN(TRIM(A70))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
-    <cfRule type="notContainsBlanks" dxfId="69" priority="71">
-      <formula>LEN(TRIM(A40))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A42">
-    <cfRule type="notContainsBlanks" dxfId="68" priority="70">
-      <formula>LEN(TRIM(A42))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A85">
-    <cfRule type="notContainsBlanks" dxfId="67" priority="61">
-      <formula>LEN(TRIM(A85))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A52">
-    <cfRule type="notContainsBlanks" dxfId="65" priority="67">
-      <formula>LEN(TRIM(A52))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A58">
-    <cfRule type="notContainsBlanks" dxfId="64" priority="66">
-      <formula>LEN(TRIM(A58))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A73">
-    <cfRule type="notContainsBlanks" dxfId="61" priority="63">
-      <formula>LEN(TRIM(A73))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A79">
-    <cfRule type="notContainsBlanks" dxfId="60" priority="62">
-      <formula>LEN(TRIM(A79))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35">
-    <cfRule type="notContainsBlanks" dxfId="58" priority="51">
-      <formula>LEN(TRIM(A35))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A89">
-    <cfRule type="notContainsBlanks" dxfId="57" priority="59">
-      <formula>LEN(TRIM(A89))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A93">
-    <cfRule type="notContainsBlanks" dxfId="56" priority="58">
-      <formula>LEN(TRIM(A93))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A99">
-    <cfRule type="notContainsBlanks" dxfId="55" priority="57">
-      <formula>LEN(TRIM(A99))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A105">
-    <cfRule type="notContainsBlanks" dxfId="54" priority="56">
-      <formula>LEN(TRIM(A105))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="notContainsBlanks" dxfId="53" priority="55">
-      <formula>LEN(TRIM(A11))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="notContainsBlanks" dxfId="52" priority="54">
-      <formula>LEN(TRIM(A12))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="notContainsBlanks" dxfId="51" priority="53">
-      <formula>LEN(TRIM(A13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
-    <cfRule type="notContainsBlanks" dxfId="50" priority="52">
-      <formula>LEN(TRIM(A34))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="notContainsBlanks" dxfId="49" priority="50">
-      <formula>LEN(TRIM(A18))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="notContainsBlanks" dxfId="48" priority="49">
-      <formula>LEN(TRIM(A19))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="notContainsBlanks" dxfId="47" priority="48">
-      <formula>LEN(TRIM(A14))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="notContainsBlanks" dxfId="46" priority="47">
-      <formula>LEN(TRIM(A15))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="notContainsBlanks" dxfId="45" priority="46">
-      <formula>LEN(TRIM(A17))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
-    <cfRule type="notContainsBlanks" dxfId="44" priority="45">
-      <formula>LEN(TRIM(A20))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="notContainsBlanks" dxfId="43" priority="44">
-      <formula>LEN(TRIM(A21))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="43">
-      <formula>LEN(TRIM(A24))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="42">
-      <formula>LEN(TRIM(A23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="41">
-      <formula>LEN(TRIM(A26))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="40">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="39">
-      <formula>LEN(TRIM(A28))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="38">
-      <formula>LEN(TRIM(A29))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="37">
-      <formula>LEN(TRIM(A30))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
-    <cfRule type="notContainsBlanks" dxfId="35" priority="36">
-      <formula>LEN(TRIM(A31))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="35">
-      <formula>LEN(TRIM(A32))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="34">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="33">
-      <formula>LEN(TRIM(A36))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="32">
-      <formula>LEN(TRIM(A38))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
-    <cfRule type="notContainsBlanks" dxfId="30" priority="31">
-      <formula>LEN(TRIM(A37))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A39">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="30">
-      <formula>LEN(TRIM(A39))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="29">
-      <formula>LEN(TRIM(A41))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="28">
-      <formula>LEN(TRIM(A46))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="27">
-      <formula>LEN(TRIM(A50))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="26">
-      <formula>LEN(TRIM(A53))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="25">
-      <formula>LEN(TRIM(A54))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="24">
-      <formula>LEN(TRIM(A55))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="23">
-      <formula>LEN(TRIM(A56))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A57">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="22">
-      <formula>LEN(TRIM(A57))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="21">
-      <formula>LEN(TRIM(A59))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="20">
-      <formula>LEN(TRIM(A60))&gt;0</formula>
+  <conditionalFormatting sqref="A62">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(A62))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="19">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(A63))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(A64))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="17">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(A65))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A66))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A67))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
-      <formula>LEN(TRIM(A68))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A96">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
-      <formula>LEN(TRIM(A96))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A95">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
-      <formula>LEN(TRIM(A95))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A94">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
-      <formula>LEN(TRIM(A94))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A97">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
-      <formula>LEN(TRIM(A97))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A100">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
-      <formula>LEN(TRIM(A100))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A101">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
-      <formula>LEN(TRIM(A101))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A102">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
-      <formula>LEN(TRIM(A102))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A103">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(A103))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A106">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
-      <formula>LEN(TRIM(A106))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A107">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(A107))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A108">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(A108))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A109">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(A109))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A51))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
more data reconcilation + viz for Person_1
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="person_1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="133">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -366,66 +366,12 @@
     <t>cdiscpilot01:BloodPressureOutcome_5</t>
   </si>
   <si>
-    <r>
-      <t>Ont: study:hasCode  sdtmterm:C67153.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C25299</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-R: study:hasCode  sdtmterm:C67153.C25298
-Correct ontology to point to  C67153.C25298
-Ont: study:bodyPosition  sdtmterm:C71148.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C62167</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-R: study:bodyPosition  sdtmterm:C71148.C62166
-This is a Standing BP, so change Ont to C71148.C62166</t>
-    </r>
-  </si>
-  <si>
     <t>BLOOD PRESSURE Diastolic</t>
   </si>
   <si>
     <t>BLOOD PRESSURE  Diastolic</t>
   </si>
   <si>
-    <t>See RDMD notes about additional triples in the DBP measures that are not in the Systolic triples.</t>
-  </si>
-  <si>
-    <t>emailed AO 14Sept17</t>
-  </si>
-  <si>
     <t>cdiscpilot01:SubjectIdentifier_1</t>
   </si>
   <si>
@@ -447,29 +393,41 @@
     <t>BLOOD PRESSURE Systolic</t>
   </si>
   <si>
-    <t>PENDING: Derived flag being added to Ont</t>
-  </si>
-  <si>
     <t>AO email 19SEpt</t>
   </si>
   <si>
-    <t>Email to AO 18Sept17, 19 sept</t>
-  </si>
-  <si>
-    <t>sdtmterm:C74456.CC12421</t>
-  </si>
-  <si>
-    <t>Oral cavity for vsloc in original data. Missing in Ont</t>
-  </si>
-  <si>
-    <t>AO email 19Sept17</t>
+    <t>sdtmterm:C74456.C12421</t>
+  </si>
+  <si>
+    <t>custom: prefix issue. Email to AO 20 SEPT</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:BloodPressureOutcome_2</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:BloodPressureOutcome_3</t>
+  </si>
+  <si>
+    <t>PENDING: Derived flag MISSING IN R! &gt; Present in Ont.</t>
+  </si>
+  <si>
+    <t>missing study:sponsordefinedID value in Onotology. Emailed AO 20 sept.</t>
+  </si>
+  <si>
+    <t>From FullTripleComp.R</t>
+  </si>
+  <si>
+    <t>dm</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Investigator_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -653,21 +611,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
+      <sz val="7"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -855,18 +805,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -883,8 +821,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1014,6 +958,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1059,7 +1012,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1086,7 +1039,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1105,23 +1057,23 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1167,154 +1119,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="120">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="99">
     <dxf>
       <fill>
         <patternFill>
@@ -2318,35 +2123,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H117"/>
+  <dimension ref="A1:H116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
+      <pane ySplit="3" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.81640625" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="57.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="49.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="57.1796875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>64</v>
       </c>
@@ -2369,7 +2174,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <v>42996</v>
       </c>
@@ -2385,12 +2190,12 @@
       <c r="E4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="G4" s="23"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>42996</v>
       </c>
@@ -2406,10 +2211,10 @@
       <c r="E5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="23"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="18"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>42996</v>
       </c>
@@ -2425,10 +2230,10 @@
       <c r="E6" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="23"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="18"/>
+      <c r="G6" s="22"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>42996</v>
       </c>
@@ -2444,10 +2249,10 @@
       <c r="E7" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="23"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="18"/>
+      <c r="G7" s="22"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <v>42996</v>
       </c>
@@ -2463,10 +2268,10 @@
       <c r="E8" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="23"/>
-    </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="18"/>
+      <c r="G8" s="22"/>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>42996</v>
       </c>
@@ -2480,10 +2285,10 @@
       <c r="E9" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="26"/>
-    </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="18"/>
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <v>42996</v>
       </c>
@@ -2497,10 +2302,10 @@
       <c r="E10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="26"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F10" s="18"/>
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <v>42996</v>
       </c>
@@ -2516,10 +2321,10 @@
       <c r="E11" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="23"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11" s="18"/>
+      <c r="G11" s="22"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>42996</v>
       </c>
@@ -2533,10 +2338,10 @@
       <c r="E12" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="23"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="18"/>
+      <c r="G12" s="22"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <v>42996</v>
       </c>
@@ -2550,10 +2355,10 @@
       <c r="E13" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="23"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" s="18"/>
+      <c r="G13" s="22"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>42996</v>
       </c>
@@ -2567,12 +2372,12 @@
         <v>9</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="23"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="22"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <v>42996</v>
       </c>
@@ -2588,10 +2393,10 @@
       <c r="E15" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="23"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F15" s="18"/>
+      <c r="G15" s="22"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <v>42996</v>
       </c>
@@ -2605,10 +2410,10 @@
       <c r="E16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="23"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16" s="18"/>
+      <c r="G16" s="22"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
         <v>42996</v>
       </c>
@@ -2622,10 +2427,10 @@
       <c r="E17" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="23"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="18"/>
+      <c r="G17" s="22"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
         <v>42996</v>
       </c>
@@ -2639,12 +2444,12 @@
         <v>11</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="23"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="22"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
         <v>42996</v>
       </c>
@@ -2658,12 +2463,12 @@
         <v>12</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="F19" s="19"/>
-      <c r="G19" s="23"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="22"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
         <v>42996</v>
       </c>
@@ -2679,10 +2484,10 @@
       <c r="E20" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="23"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F20" s="19"/>
+      <c r="G20" s="22"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="9">
         <v>42996</v>
       </c>
@@ -2696,10 +2501,10 @@
       <c r="E21" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="23"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="18"/>
+      <c r="G21" s="22"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
         <v>42996</v>
       </c>
@@ -2713,10 +2518,10 @@
       <c r="E22" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="23"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F22" s="18"/>
+      <c r="G22" s="22"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="9">
         <v>42996</v>
       </c>
@@ -2732,10 +2537,10 @@
       <c r="E23" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="26"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F23" s="18"/>
+      <c r="G23" s="25"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="9">
         <v>42996</v>
       </c>
@@ -2749,10 +2554,10 @@
       <c r="E24" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="26"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="18"/>
+      <c r="G24" s="25"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="9">
         <v>42996</v>
       </c>
@@ -2766,12 +2571,12 @@
       <c r="E25" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="26"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="18"/>
+      <c r="G25" s="25"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="9">
-        <v>42996</v>
+        <v>42998</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>53</v>
@@ -2785,12 +2590,14 @@
       <c r="E26" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="F26" s="19"/>
-      <c r="G26" s="23"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="G26" s="22"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="9">
-        <v>42996</v>
+        <v>42998</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>53</v>
@@ -2804,12 +2611,14 @@
       <c r="E27" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="23"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="G27" s="22"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="9">
-        <v>42996</v>
+        <v>42998</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>53</v>
@@ -2823,12 +2632,14 @@
       <c r="E28" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="23"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="G28" s="22"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="9">
-        <v>42996</v>
+        <v>42998</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="15" t="s">
@@ -2840,12 +2651,14 @@
       <c r="E29" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="26"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F29" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="G29" s="25"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="9">
-        <v>42996</v>
+        <v>42998</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="11"/>
@@ -2855,12 +2668,14 @@
       <c r="E30" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F30" s="21"/>
-      <c r="G30" s="26"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F30" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="G30" s="25"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="9">
-        <v>42996</v>
+        <v>42998</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="11"/>
@@ -2870,10 +2685,12 @@
       <c r="E31" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F31" s="21"/>
-      <c r="G31" s="26"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F31" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="G31" s="25"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="9">
         <v>42996</v>
       </c>
@@ -2889,10 +2706,10 @@
       <c r="E32" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F32" s="19"/>
-      <c r="G32" s="23"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F32" s="18"/>
+      <c r="G32" s="22"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="9">
         <v>42996</v>
       </c>
@@ -2906,10 +2723,10 @@
       <c r="E33" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="F33" s="21"/>
-      <c r="G33" s="23"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F33" s="20"/>
+      <c r="G33" s="22"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="9">
         <v>42996</v>
       </c>
@@ -2923,10 +2740,10 @@
       <c r="E34" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="F34" s="19"/>
-      <c r="G34" s="23"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F34" s="18"/>
+      <c r="G34" s="22"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="9">
         <v>42996</v>
       </c>
@@ -2940,10 +2757,10 @@
       <c r="E35" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F35" s="19"/>
-      <c r="G35" s="23"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F35" s="18"/>
+      <c r="G35" s="22"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="9">
         <v>42996</v>
       </c>
@@ -2959,13 +2776,11 @@
       <c r="E36" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F36" s="21"/>
-      <c r="G36" s="23"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
-        <v>42996</v>
-      </c>
+      <c r="F36" s="20"/>
+      <c r="G36" s="22"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="27"/>
       <c r="B37" s="11" t="s">
         <v>90</v>
       </c>
@@ -2975,13 +2790,13 @@
       <c r="D37" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="E37" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="F37" s="21"/>
-      <c r="G37" s="23"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F37" s="20"/>
+      <c r="G37" s="22"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="9">
         <v>42996</v>
       </c>
@@ -2995,10 +2810,10 @@
       <c r="E38" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F38" s="19"/>
-      <c r="G38" s="23"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F38" s="18"/>
+      <c r="G38" s="22"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="9">
         <v>42996</v>
       </c>
@@ -3014,10 +2829,10 @@
       <c r="E39" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="F39" s="22"/>
-      <c r="G39" s="23"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F39" s="21"/>
+      <c r="G39" s="22"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="9">
         <v>42996</v>
       </c>
@@ -3031,10 +2846,10 @@
       <c r="E40" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F40" s="22"/>
-      <c r="G40" s="23"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F40" s="21"/>
+      <c r="G40" s="22"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="9">
         <v>42996</v>
       </c>
@@ -3050,10 +2865,10 @@
       <c r="E41" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="F41" s="22"/>
-      <c r="G41" s="23"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F41" s="21"/>
+      <c r="G41" s="22"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="9">
         <v>42996</v>
       </c>
@@ -3067,11 +2882,13 @@
       <c r="E42" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F42" s="22"/>
-      <c r="G42" s="23"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="22"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="9">
+        <v>42998</v>
+      </c>
       <c r="B43" s="11" t="s">
         <v>90</v>
       </c>
@@ -3081,17 +2898,15 @@
       <c r="D43" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="E43" s="30" t="s">
+      <c r="E43" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="F43" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="G43" s="23" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F43" s="23"/>
+      <c r="G43" s="22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="9">
         <v>42996</v>
       </c>
@@ -3105,25 +2920,23 @@
       <c r="E44" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F44" s="22"/>
-      <c r="G44" s="23"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="22"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="9">
+        <v>42998</v>
+      </c>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
       <c r="D45" s="12"/>
-      <c r="E45" s="33" t="s">
-        <v>129</v>
-      </c>
-      <c r="F45" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G45" s="23" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E45" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F45" s="21"/>
+      <c r="G45" s="22"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="9">
         <v>42996</v>
       </c>
@@ -3137,10 +2950,10 @@
       <c r="E46" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="F46" s="22"/>
-      <c r="G46" s="23"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F46" s="21"/>
+      <c r="G46" s="22"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="9">
         <v>42997</v>
       </c>
@@ -3154,10 +2967,10 @@
       <c r="E47" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="F47" s="24"/>
-      <c r="G47" s="23"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F47" s="23"/>
+      <c r="G47" s="22"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="9">
         <v>42996</v>
       </c>
@@ -3169,10 +2982,10 @@
       <c r="E48" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F48" s="22"/>
-      <c r="G48" s="23"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F48" s="21"/>
+      <c r="G48" s="22"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="9">
         <v>42996</v>
       </c>
@@ -3184,10 +2997,10 @@
       <c r="E49" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="F49" s="22"/>
-      <c r="G49" s="23"/>
-    </row>
-    <row r="50" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F49" s="21"/>
+      <c r="G49" s="22"/>
+    </row>
+    <row r="50" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="9">
         <v>42997</v>
       </c>
@@ -3198,18 +3011,15 @@
         <v>73</v>
       </c>
       <c r="D50" s="12"/>
-      <c r="E50" s="32" t="s">
+      <c r="E50" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="F50" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="G50" s="27"/>
-      <c r="H50" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F50" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="G50" s="22"/>
+    </row>
+    <row r="51" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="9">
         <v>42997</v>
       </c>
@@ -3221,10 +3031,10 @@
       <c r="E51" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F51" s="22"/>
-      <c r="G51" s="19"/>
-    </row>
-    <row r="52" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F51" s="21"/>
+      <c r="G51" s="22"/>
+    </row>
+    <row r="52" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="9">
         <v>42997</v>
       </c>
@@ -3236,10 +3046,10 @@
       <c r="E52" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="F52" s="22"/>
-      <c r="G52" s="19"/>
-    </row>
-    <row r="53" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F52" s="21"/>
+      <c r="G52" s="22"/>
+    </row>
+    <row r="53" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="9">
         <v>42997</v>
       </c>
@@ -3253,10 +3063,10 @@
       <c r="E53" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F53" s="22"/>
-      <c r="G53" s="19"/>
-    </row>
-    <row r="54" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F53" s="21"/>
+      <c r="G53" s="22"/>
+    </row>
+    <row r="54" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="9">
         <v>42997</v>
       </c>
@@ -3265,15 +3075,15 @@
       </c>
       <c r="C54" s="12"/>
       <c r="D54" s="12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E54" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F54" s="22"/>
-      <c r="G54" s="19"/>
-    </row>
-    <row r="55" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F54" s="21"/>
+      <c r="G54" s="22"/>
+    </row>
+    <row r="55" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9">
         <v>42997</v>
       </c>
@@ -3285,10 +3095,10 @@
       <c r="E55" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F55" s="22"/>
-      <c r="G55" s="19"/>
-    </row>
-    <row r="56" spans="1:8" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="F55" s="21"/>
+      <c r="G55" s="22"/>
+    </row>
+    <row r="56" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="9">
         <v>42997</v>
       </c>
@@ -3302,17 +3112,12 @@
       <c r="E56" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="F56" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="G56" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="H56" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F56" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="G56" s="22"/>
+    </row>
+    <row r="57" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9">
         <v>42997</v>
       </c>
@@ -3324,10 +3129,10 @@
       <c r="E57" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F57" s="22"/>
-      <c r="G57" s="19"/>
-    </row>
-    <row r="58" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F57" s="21"/>
+      <c r="G57" s="22"/>
+    </row>
+    <row r="58" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9">
         <v>42997</v>
       </c>
@@ -3339,10 +3144,10 @@
       <c r="E58" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F58" s="22"/>
-      <c r="G58" s="19"/>
-    </row>
-    <row r="59" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F58" s="21"/>
+      <c r="G58" s="22"/>
+    </row>
+    <row r="59" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="9">
         <v>42997</v>
       </c>
@@ -3356,10 +3161,10 @@
       <c r="E59" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F59" s="22"/>
-      <c r="G59" s="19"/>
-    </row>
-    <row r="60" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F59" s="21"/>
+      <c r="G59" s="22"/>
+    </row>
+    <row r="60" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="9">
         <v>42997</v>
       </c>
@@ -3368,15 +3173,15 @@
       </c>
       <c r="C60" s="12"/>
       <c r="D60" s="12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E60" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F60" s="22"/>
-      <c r="G60" s="19"/>
-    </row>
-    <row r="61" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F60" s="21"/>
+      <c r="G60" s="22"/>
+    </row>
+    <row r="61" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="9">
         <v>42997</v>
       </c>
@@ -3386,12 +3191,12 @@
       <c r="C61" s="12"/>
       <c r="D61" s="12"/>
       <c r="E61" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="F61" s="22"/>
-      <c r="G61" s="19"/>
-    </row>
-    <row r="62" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="F61" s="21"/>
+      <c r="G61" s="22"/>
+    </row>
+    <row r="62" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="9">
         <v>42997</v>
       </c>
@@ -3405,12 +3210,12 @@
       <c r="E62" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="F62" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="G62" s="19"/>
-    </row>
-    <row r="63" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F62" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="G62" s="22"/>
+    </row>
+    <row r="63" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="9">
         <v>42997</v>
       </c>
@@ -3422,10 +3227,10 @@
       <c r="E63" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F63" s="22"/>
-      <c r="G63" s="19"/>
-    </row>
-    <row r="64" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F63" s="21"/>
+      <c r="G63" s="22"/>
+    </row>
+    <row r="64" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="9">
         <v>42997</v>
       </c>
@@ -3437,10 +3242,10 @@
       <c r="E64" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F64" s="22"/>
-      <c r="G64" s="19"/>
-    </row>
-    <row r="65" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F64" s="21"/>
+      <c r="G64" s="22"/>
+    </row>
+    <row r="65" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="9">
         <v>42997</v>
       </c>
@@ -3454,10 +3259,10 @@
       <c r="E65" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F65" s="22"/>
-      <c r="G65" s="19"/>
-    </row>
-    <row r="66" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F65" s="21"/>
+      <c r="G65" s="22"/>
+    </row>
+    <row r="66" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9">
         <v>42997</v>
       </c>
@@ -3466,15 +3271,15 @@
       </c>
       <c r="C66" s="12"/>
       <c r="D66" s="12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F66" s="22"/>
-      <c r="G66" s="19"/>
-    </row>
-    <row r="67" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F66" s="21"/>
+      <c r="G66" s="22"/>
+    </row>
+    <row r="67" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="9">
         <v>42997</v>
       </c>
@@ -3484,64 +3289,68 @@
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
       <c r="E67" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F67" s="22"/>
-      <c r="G67" s="19"/>
-    </row>
-    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="29"/>
+        <v>121</v>
+      </c>
+      <c r="F67" s="21"/>
+      <c r="G67" s="22"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A68" s="27">
+        <v>42998</v>
+      </c>
       <c r="B68" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C68" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D68" s="12" t="s">
-        <v>58</v>
-      </c>
+      <c r="D68" s="12"/>
       <c r="E68" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="F68" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="G68" s="27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="9"/>
+      <c r="F68" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G68" s="22"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A69" s="27">
+        <v>42998</v>
+      </c>
       <c r="B69" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C69" s="11"/>
       <c r="D69" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E69" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F69" s="21"/>
-      <c r="G69" s="23"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="9"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="22"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A70" s="27">
+        <v>42998</v>
+      </c>
       <c r="B70" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E70" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="F70" s="21"/>
-      <c r="G70" s="23"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="10"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="22"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A71" s="27">
+        <v>42998</v>
+      </c>
       <c r="B71" s="10" t="s">
         <v>90</v>
       </c>
@@ -3549,175 +3358,205 @@
       <c r="D71" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E71" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F71" s="23"/>
-      <c r="G71" s="23"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="9"/>
+      <c r="E71" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F71" s="20"/>
+      <c r="G71" s="22"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A72" s="27">
+        <v>42998</v>
+      </c>
       <c r="B72" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="12" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
       <c r="E72" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F72" s="23"/>
-      <c r="G72" s="23"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="9"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="22"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A73" s="27">
+        <v>42998</v>
+      </c>
       <c r="B73" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F73" s="23"/>
-      <c r="G73" s="23"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="9"/>
+        <v>126</v>
+      </c>
+      <c r="F73" s="22"/>
+      <c r="G73" s="22"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A74" s="27">
+        <v>42998</v>
+      </c>
       <c r="B74" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C74" s="11"/>
+      <c r="C74" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D74" s="12"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="23"/>
-      <c r="G74" s="23"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="9"/>
+      <c r="E74" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="F74" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="G74" s="18"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A75" s="27">
+        <v>42998</v>
+      </c>
       <c r="B75" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C75" s="11"/>
-      <c r="D75" s="12"/>
-      <c r="E75" s="11"/>
-      <c r="F75" s="23"/>
-      <c r="G75" s="23"/>
-    </row>
-    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="29"/>
+      <c r="D75" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F75" s="22"/>
+      <c r="G75" s="18"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A76" s="27">
+        <v>42998</v>
+      </c>
       <c r="B76" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C76" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="C76" s="11"/>
       <c r="D76" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E76" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="F76" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G76" s="27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="10"/>
+      <c r="E76" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F76" s="22"/>
+      <c r="G76" s="18"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A77" s="27">
+        <v>42998</v>
+      </c>
       <c r="B77" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C77" s="11"/>
+      <c r="C77" s="14"/>
       <c r="D77" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E77" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F77" s="23"/>
-      <c r="G77" s="23"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="9"/>
+      <c r="E77" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F77" s="21"/>
+      <c r="G77" s="18"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A78" s="27">
+        <v>42998</v>
+      </c>
       <c r="B78" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C78" s="11"/>
       <c r="D78" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E78" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E78" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F78" s="23"/>
-      <c r="G78" s="23"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="9"/>
+      <c r="G78" s="7"/>
+    </row>
+    <row r="79" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="27">
+        <v>42998</v>
+      </c>
       <c r="B79" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C79" s="11"/>
       <c r="D79" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E79" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="F79" s="23"/>
-      <c r="G79" s="23"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="9"/>
+        <v>58</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F79" s="22"/>
+      <c r="G79" s="18"/>
+    </row>
+    <row r="80" spans="1:8" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A80" s="27"/>
       <c r="B80" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C80" s="11"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="10"/>
-      <c r="F80" s="23"/>
-      <c r="G80" s="23"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="9"/>
+      <c r="C80" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E80" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="F80" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="G80" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="H80" s="32"/>
+    </row>
+    <row r="81" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A81" s="27">
+        <v>42998</v>
+      </c>
       <c r="B81" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C81" s="11"/>
-      <c r="D81" s="12"/>
-      <c r="E81" s="10"/>
-      <c r="F81" s="23"/>
-      <c r="G81" s="23"/>
-    </row>
-    <row r="82" spans="1:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="29"/>
+      <c r="D81" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F81" s="22"/>
+      <c r="G81" s="18"/>
+    </row>
+    <row r="82" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A82" s="27">
+        <v>42998</v>
+      </c>
       <c r="B82" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C82" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="C82" s="11"/>
       <c r="D82" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E82" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="F82" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G82" s="27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="10"/>
+      <c r="E82" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F82" s="22"/>
+      <c r="G82" s="18"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" s="27">
+        <v>42998</v>
+      </c>
       <c r="B83" s="10" t="s">
         <v>90</v>
       </c>
@@ -3725,120 +3564,126 @@
       <c r="D83" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E83" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F83" s="23"/>
-      <c r="G83" s="23"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="9"/>
+      <c r="E83" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F83" s="22"/>
+      <c r="G83" s="22"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" s="27">
+        <v>42998</v>
+      </c>
       <c r="B84" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C84" s="11"/>
       <c r="D84" s="12" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
       <c r="E84" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F84" s="23"/>
-      <c r="G84" s="23"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="9"/>
+      <c r="F84" s="22"/>
+      <c r="G84" s="22"/>
+    </row>
+    <row r="85" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="27">
+        <v>42998</v>
+      </c>
       <c r="B85" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C85" s="11"/>
       <c r="D85" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F85" s="23"/>
-      <c r="G85" s="23"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="9"/>
+        <v>75</v>
+      </c>
+      <c r="F85" s="22"/>
+      <c r="G85" s="22"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86" s="27">
+        <v>42998</v>
+      </c>
       <c r="B86" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C86" s="11"/>
-      <c r="D86" s="12"/>
-      <c r="E86" s="10" t="s">
-        <v>62</v>
+      <c r="C86" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D86" s="10"/>
+      <c r="E86" s="17" t="s">
+        <v>100</v>
       </c>
       <c r="F86" s="23"/>
-      <c r="G86" s="23"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="9"/>
+      <c r="G86" s="22"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" s="27">
+        <v>42998</v>
+      </c>
       <c r="B87" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C87" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="C87" s="10"/>
       <c r="D87" s="10"/>
-      <c r="E87" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="F87" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="G87" s="23" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="9"/>
+      <c r="E87" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F87" s="22"/>
+      <c r="G87" s="22"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" s="27">
+        <v>42998</v>
+      </c>
       <c r="B88" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C88" s="10"/>
       <c r="D88" s="10"/>
       <c r="E88" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F88" s="23"/>
-      <c r="G88" s="23"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="F88" s="22"/>
+      <c r="G88" s="22"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="9"/>
       <c r="B89" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C89" s="10"/>
+      <c r="C89" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D89" s="10"/>
-      <c r="E89" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F89" s="23"/>
-      <c r="G89" s="23"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="9"/>
+      <c r="E89" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F89" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="G89" s="22"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" s="9">
+        <v>42996</v>
+      </c>
       <c r="B90" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C90" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="C90" s="10"/>
       <c r="D90" s="10"/>
-      <c r="E90" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="F90" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="G90" s="23" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E90" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F90" s="22"/>
+      <c r="G90" s="26"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="9">
         <v>42996</v>
       </c>
@@ -3848,91 +3693,91 @@
       <c r="C91" s="10"/>
       <c r="D91" s="10"/>
       <c r="E91" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F91" s="23"/>
-      <c r="G91" s="28"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="F91" s="22"/>
+      <c r="G91" s="26"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="9">
         <v>42996</v>
       </c>
-      <c r="B92" s="10" t="s">
-        <v>90</v>
-      </c>
+      <c r="B92" s="10"/>
       <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
+      <c r="D92" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="E92" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F92" s="23"/>
-      <c r="G92" s="28"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="F92" s="22"/>
+      <c r="G92" s="26"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="9">
         <v>42996</v>
       </c>
       <c r="B93" s="10"/>
       <c r="C93" s="10"/>
       <c r="D93" s="12" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F93" s="23"/>
-      <c r="G93" s="28"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F93" s="22"/>
+      <c r="G93" s="26"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="9">
         <v>42996</v>
       </c>
-      <c r="B94" s="10"/>
+      <c r="B94" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="C94" s="10"/>
-      <c r="D94" s="12" t="s">
-        <v>122</v>
-      </c>
+      <c r="D94" s="10"/>
       <c r="E94" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F94" s="23"/>
-      <c r="G94" s="28"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="F94" s="22"/>
+      <c r="G94" s="26"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="9">
-        <v>42996</v>
+        <v>42997</v>
       </c>
       <c r="B95" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C95" s="10"/>
+      <c r="C95" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D95" s="10"/>
       <c r="E95" s="10" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F95" s="23"/>
-      <c r="G95" s="28"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G95" s="22"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="9">
+        <v>42996</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C96" s="10"/>
+      <c r="D96" s="11"/>
+      <c r="E96" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F96" s="18"/>
+      <c r="G96" s="26"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A97" s="9">
         <v>42997</v>
-      </c>
-      <c r="B96" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C96" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D96" s="10"/>
-      <c r="E96" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="F96" s="24"/>
-      <c r="G96" s="23"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="9">
-        <v>42996</v>
       </c>
       <c r="B97" s="10" t="s">
         <v>90</v>
@@ -3940,672 +3785,673 @@
       <c r="C97" s="10"/>
       <c r="D97" s="11"/>
       <c r="E97" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F97" s="19"/>
-      <c r="G97" s="28"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="F97" s="18"/>
+      <c r="G97" s="26"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" s="9">
         <v>42997</v>
       </c>
-      <c r="B98" s="10" t="s">
-        <v>90</v>
-      </c>
+      <c r="B98" s="10"/>
       <c r="C98" s="10"/>
       <c r="D98" s="11"/>
       <c r="E98" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="F98" s="19"/>
-      <c r="G98" s="28"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="F98" s="18"/>
+      <c r="G98" s="26"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" s="9">
-        <v>42997</v>
+        <v>42996</v>
       </c>
       <c r="B99" s="10"/>
       <c r="C99" s="10"/>
-      <c r="D99" s="11"/>
+      <c r="D99" s="12" t="s">
+        <v>119</v>
+      </c>
       <c r="E99" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F99" s="19"/>
-      <c r="G99" s="28"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F99" s="18"/>
+      <c r="G99" s="26"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" s="9">
-        <v>42996</v>
-      </c>
-      <c r="B100" s="10"/>
+        <v>42997</v>
+      </c>
+      <c r="B100" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="C100" s="10"/>
-      <c r="D100" s="12" t="s">
-        <v>122</v>
-      </c>
+      <c r="D100" s="11"/>
       <c r="E100" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F100" s="19"/>
-      <c r="G100" s="28"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="F100" s="22"/>
+      <c r="G100" s="26"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101" s="9">
         <v>42997</v>
       </c>
       <c r="B101" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C101" s="10"/>
+      <c r="C101" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D101" s="11"/>
       <c r="E101" s="10" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F101" s="23"/>
-      <c r="G101" s="28"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G101" s="22"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" s="9">
-        <v>42997</v>
+        <v>42996</v>
       </c>
       <c r="B102" s="10" t="s">
         <v>90</v>
-      </c>
-      <c r="C102" s="14" t="s">
-        <v>73</v>
       </c>
       <c r="D102" s="11"/>
       <c r="E102" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="F102" s="24"/>
-      <c r="G102" s="23"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F102" s="18"/>
+      <c r="G102" s="22"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" s="9">
         <v>42996</v>
       </c>
       <c r="B103" s="10" t="s">
         <v>90</v>
       </c>
+      <c r="C103" s="11"/>
       <c r="D103" s="11"/>
       <c r="E103" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F103" s="19"/>
-      <c r="G103" s="23"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="F103" s="18"/>
+      <c r="G103" s="22"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" s="9">
         <v>42996</v>
       </c>
-      <c r="B104" s="10" t="s">
-        <v>90</v>
-      </c>
+      <c r="B104" s="10"/>
       <c r="C104" s="11"/>
       <c r="D104" s="11"/>
       <c r="E104" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F104" s="19"/>
-      <c r="G104" s="23"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="F104" s="18"/>
+      <c r="G104" s="22"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" s="9">
         <v>42996</v>
       </c>
       <c r="B105" s="10"/>
       <c r="C105" s="11"/>
-      <c r="D105" s="11"/>
+      <c r="D105" s="12" t="s">
+        <v>119</v>
+      </c>
       <c r="E105" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F105" s="19"/>
-      <c r="G105" s="23"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F105" s="18"/>
+      <c r="G105" s="22"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" s="9">
         <v>42996</v>
       </c>
-      <c r="B106" s="10"/>
+      <c r="B106" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="C106" s="11"/>
-      <c r="D106" s="12" t="s">
-        <v>122</v>
-      </c>
+      <c r="D106" s="11"/>
       <c r="E106" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F106" s="19"/>
-      <c r="G106" s="23"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="9">
-        <v>42996</v>
-      </c>
-      <c r="B107" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
-      <c r="E107" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="F107" s="23"/>
-      <c r="G107" s="23"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F106" s="22"/>
+      <c r="G106" s="22"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="7"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>130</v>
+      </c>
       <c r="C108" s="5"/>
       <c r="D108" s="5"/>
       <c r="E108" s="5"/>
       <c r="F108" s="7"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C109" s="5"/>
-      <c r="D109" s="5"/>
-      <c r="E109" s="5"/>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B109" t="s">
+        <v>131</v>
+      </c>
+      <c r="C109" t="s">
+        <v>118</v>
+      </c>
+      <c r="E109" t="s">
+        <v>132</v>
+      </c>
       <c r="F109" s="7"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C110" s="5"/>
-      <c r="D110" s="5"/>
-      <c r="E110" s="5"/>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F110" s="7"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
       <c r="E111" s="5"/>
       <c r="F111" s="7"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C112" s="5"/>
       <c r="D112" s="5"/>
       <c r="E112" s="5"/>
       <c r="F112" s="7"/>
     </row>
-    <row r="113" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
       <c r="E113" s="5"/>
       <c r="F113" s="7"/>
     </row>
-    <row r="114" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C114" s="5"/>
       <c r="D114" s="5"/>
       <c r="E114" s="5"/>
       <c r="F114" s="7"/>
     </row>
-    <row r="115" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C115" s="5"/>
       <c r="D115" s="5"/>
       <c r="E115" s="5"/>
       <c r="F115" s="7"/>
     </row>
-    <row r="116" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C116" s="5"/>
       <c r="D116" s="5"/>
       <c r="E116" s="5"/>
       <c r="F116" s="7"/>
     </row>
-    <row r="117" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C117" s="5"/>
-      <c r="D117" s="5"/>
-      <c r="E117" s="5"/>
-      <c r="F117" s="7"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="A4:A7">
-    <cfRule type="notContainsBlanks" dxfId="119" priority="384">
+    <cfRule type="notContainsBlanks" dxfId="98" priority="417">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A80">
+    <cfRule type="notContainsBlanks" dxfId="97" priority="289">
+      <formula>LEN(TRIM(A80))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68">
+    <cfRule type="notContainsBlanks" dxfId="96" priority="291">
+      <formula>LEN(TRIM(A68))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A89">
+    <cfRule type="notContainsBlanks" dxfId="95" priority="147">
+      <formula>LEN(TRIM(A89))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="notContainsBlanks" dxfId="93" priority="155">
+      <formula>LEN(TRIM(A47))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A95">
+    <cfRule type="notContainsBlanks" dxfId="90" priority="140">
+      <formula>LEN(TRIM(A95))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48">
+    <cfRule type="notContainsBlanks" dxfId="89" priority="127">
+      <formula>LEN(TRIM(A48))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="notContainsBlanks" dxfId="88" priority="131">
+      <formula>LEN(TRIM(A25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:A10">
+    <cfRule type="notContainsBlanks" dxfId="87" priority="134">
+      <formula>LEN(TRIM(A8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="notContainsBlanks" dxfId="86" priority="133">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="notContainsBlanks" dxfId="85" priority="132">
+      <formula>LEN(TRIM(A22))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44:A45">
+    <cfRule type="notContainsBlanks" dxfId="84" priority="128">
+      <formula>LEN(TRIM(A44))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A102">
+    <cfRule type="notContainsBlanks" dxfId="83" priority="115">
+      <formula>LEN(TRIM(A102))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="notContainsBlanks" dxfId="82" priority="130">
+      <formula>LEN(TRIM(A40))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42">
+    <cfRule type="notContainsBlanks" dxfId="81" priority="129">
+      <formula>LEN(TRIM(A42))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="notContainsBlanks" dxfId="79" priority="117">
+      <formula>LEN(TRIM(A90))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
+    <cfRule type="notContainsBlanks" dxfId="78" priority="110">
+      <formula>LEN(TRIM(A35))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="notContainsBlanks" dxfId="76" priority="112">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A96">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="116">
+      <formula>LEN(TRIM(A96))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="notContainsBlanks" dxfId="74" priority="114">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="113">
+      <formula>LEN(TRIM(A12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="notContainsBlanks" dxfId="72" priority="111">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="109">
+      <formula>LEN(TRIM(A18))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="108">
+      <formula>LEN(TRIM(A19))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="notContainsBlanks" dxfId="69" priority="107">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="notContainsBlanks" dxfId="68" priority="106">
+      <formula>LEN(TRIM(A15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="105">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20">
+    <cfRule type="notContainsBlanks" dxfId="66" priority="104">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="103">
+      <formula>LEN(TRIM(A21))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="notContainsBlanks" dxfId="64" priority="102">
+      <formula>LEN(TRIM(A24))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="101">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="94">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="notContainsBlanks" dxfId="61" priority="90">
+      <formula>LEN(TRIM(A37))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="92">
+      <formula>LEN(TRIM(A36))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39">
+    <cfRule type="notContainsBlanks" dxfId="59" priority="89">
+      <formula>LEN(TRIM(A39))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="93">
+      <formula>LEN(TRIM(A33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="88">
+      <formula>LEN(TRIM(A41))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="91">
+      <formula>LEN(TRIM(A38))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="87">
+      <formula>LEN(TRIM(A46))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="86">
+      <formula>LEN(TRIM(A49))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="81">
+      <formula>LEN(TRIM(A56))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A93">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="72">
+      <formula>LEN(TRIM(A93))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A92">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="71">
+      <formula>LEN(TRIM(A92))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="70">
+      <formula>LEN(TRIM(A91))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A94">
+    <cfRule type="notContainsBlanks" dxfId="49" priority="69">
+      <formula>LEN(TRIM(A94))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A103">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="64">
+      <formula>LEN(TRIM(A103))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A99">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="66">
+      <formula>LEN(TRIM(A99))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A104">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="63">
+      <formula>LEN(TRIM(A104))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A105">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="62">
+      <formula>LEN(TRIM(A105))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A106">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="61">
+      <formula>LEN(TRIM(A106))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A97">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="59">
+      <formula>LEN(TRIM(A97))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A98">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="58">
+      <formula>LEN(TRIM(A98))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A100">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="57">
+      <formula>LEN(TRIM(A100))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A101">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="56">
+      <formula>LEN(TRIM(A101))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="49">
+      <formula>LEN(TRIM(A51))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="51">
+      <formula>LEN(TRIM(A50))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="48">
+      <formula>LEN(TRIM(A52))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="45">
+      <formula>LEN(TRIM(A55))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A53">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="47">
+      <formula>LEN(TRIM(A53))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="46">
+      <formula>LEN(TRIM(A54))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="44">
+      <formula>LEN(TRIM(A57))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="43">
+      <formula>LEN(TRIM(A58))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="42">
+      <formula>LEN(TRIM(A59))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="41">
+      <formula>LEN(TRIM(A60))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="40">
+      <formula>LEN(TRIM(A61))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="39">
+      <formula>LEN(TRIM(A62))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="38">
+      <formula>LEN(TRIM(A63))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="37">
+      <formula>LEN(TRIM(A64))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="36">
+      <formula>LEN(TRIM(A65))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="35">
+      <formula>LEN(TRIM(A66))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="34">
+      <formula>LEN(TRIM(A67))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="33">
+      <formula>LEN(TRIM(A43))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="28">
+      <formula>LEN(TRIM(A26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:A31">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="27">
+      <formula>LEN(TRIM(A27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A72">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="17">
+      <formula>LEN(TRIM(A72))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="20">
+      <formula>LEN(TRIM(A69))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="19">
+      <formula>LEN(TRIM(A70))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="18">
+      <formula>LEN(TRIM(A71))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A73">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="16">
+      <formula>LEN(TRIM(A73))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A74">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
+      <formula>LEN(TRIM(A74))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A75">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
+      <formula>LEN(TRIM(A75))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A76">
-    <cfRule type="notContainsBlanks" dxfId="118" priority="257">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
       <formula>LEN(TRIM(A76))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A77">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
+      <formula>LEN(TRIM(A77))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A78">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
+      <formula>LEN(TRIM(A78))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A79">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
+      <formula>LEN(TRIM(A79))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A84">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="6">
+      <formula>LEN(TRIM(A84))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A81">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(A81))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A82">
-    <cfRule type="notContainsBlanks" dxfId="117" priority="256">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
       <formula>LEN(TRIM(A82))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A68">
-    <cfRule type="notContainsBlanks" dxfId="116" priority="258">
-      <formula>LEN(TRIM(A68))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A90">
-    <cfRule type="notContainsBlanks" dxfId="115" priority="114">
-      <formula>LEN(TRIM(A90))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A79:A81">
-    <cfRule type="notContainsBlanks" dxfId="114" priority="189">
-      <formula>LEN(TRIM(A79))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A43">
-    <cfRule type="notContainsBlanks" dxfId="113" priority="123">
-      <formula>LEN(TRIM(A43))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
-    <cfRule type="notContainsBlanks" dxfId="112" priority="122">
-      <formula>LEN(TRIM(A47))&gt;0</formula>
+  <conditionalFormatting sqref="A83">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(A83))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85">
-    <cfRule type="notContainsBlanks" dxfId="111" priority="188">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(A85))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A70">
-    <cfRule type="notContainsBlanks" dxfId="110" priority="203">
-      <formula>LEN(TRIM(A70))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A73:A75">
-    <cfRule type="notContainsBlanks" dxfId="109" priority="202">
-      <formula>LEN(TRIM(A73))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A87">
-    <cfRule type="notContainsBlanks" dxfId="108" priority="117">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(A87))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86">
-    <cfRule type="notContainsBlanks" dxfId="107" priority="192">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A86))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A89">
-    <cfRule type="notContainsBlanks" dxfId="106" priority="115">
-      <formula>LEN(TRIM(A89))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A96">
-    <cfRule type="notContainsBlanks" dxfId="105" priority="107">
-      <formula>LEN(TRIM(A96))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
-    <cfRule type="notContainsBlanks" dxfId="103" priority="94">
-      <formula>LEN(TRIM(A48))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="100" priority="98">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8:A10">
-    <cfRule type="notContainsBlanks" dxfId="99" priority="101">
-      <formula>LEN(TRIM(A8))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="notContainsBlanks" dxfId="98" priority="100">
-      <formula>LEN(TRIM(A16))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="notContainsBlanks" dxfId="97" priority="99">
-      <formula>LEN(TRIM(A22))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A44:A45">
-    <cfRule type="notContainsBlanks" dxfId="96" priority="95">
-      <formula>LEN(TRIM(A44))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
-    <cfRule type="notContainsBlanks" dxfId="93" priority="90">
-      <formula>LEN(TRIM(A69))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
-    <cfRule type="notContainsBlanks" dxfId="92" priority="97">
-      <formula>LEN(TRIM(A40))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A42">
-    <cfRule type="notContainsBlanks" dxfId="91" priority="96">
-      <formula>LEN(TRIM(A42))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A84">
-    <cfRule type="notContainsBlanks" dxfId="90" priority="87">
-      <formula>LEN(TRIM(A84))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A103">
-    <cfRule type="notContainsBlanks" dxfId="89" priority="82">
-      <formula>LEN(TRIM(A103))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
-    <cfRule type="notContainsBlanks" dxfId="87" priority="89">
-      <formula>LEN(TRIM(A72))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A78">
-    <cfRule type="notContainsBlanks" dxfId="86" priority="88">
-      <formula>LEN(TRIM(A78))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35">
-    <cfRule type="notContainsBlanks" dxfId="85" priority="77">
-      <formula>LEN(TRIM(A35))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="notContainsBlanks" dxfId="84" priority="85">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A88))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A91">
-    <cfRule type="notContainsBlanks" dxfId="83" priority="84">
-      <formula>LEN(TRIM(A91))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A97">
-    <cfRule type="notContainsBlanks" dxfId="82" priority="83">
-      <formula>LEN(TRIM(A97))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="notContainsBlanks" dxfId="80" priority="81">
-      <formula>LEN(TRIM(A11))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="notContainsBlanks" dxfId="79" priority="80">
-      <formula>LEN(TRIM(A12))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="notContainsBlanks" dxfId="78" priority="79">
-      <formula>LEN(TRIM(A13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
-    <cfRule type="notContainsBlanks" dxfId="77" priority="78">
-      <formula>LEN(TRIM(A34))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="notContainsBlanks" dxfId="76" priority="76">
-      <formula>LEN(TRIM(A18))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="notContainsBlanks" dxfId="75" priority="75">
-      <formula>LEN(TRIM(A19))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="notContainsBlanks" dxfId="74" priority="74">
-      <formula>LEN(TRIM(A14))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="notContainsBlanks" dxfId="73" priority="73">
-      <formula>LEN(TRIM(A15))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="notContainsBlanks" dxfId="72" priority="72">
-      <formula>LEN(TRIM(A17))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
-    <cfRule type="notContainsBlanks" dxfId="71" priority="71">
-      <formula>LEN(TRIM(A20))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="notContainsBlanks" dxfId="70" priority="70">
-      <formula>LEN(TRIM(A21))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24">
-    <cfRule type="notContainsBlanks" dxfId="69" priority="69">
-      <formula>LEN(TRIM(A24))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="notContainsBlanks" dxfId="68" priority="68">
-      <formula>LEN(TRIM(A23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="notContainsBlanks" dxfId="67" priority="67">
-      <formula>LEN(TRIM(A26))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="notContainsBlanks" dxfId="66" priority="66">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
-    <cfRule type="notContainsBlanks" dxfId="65" priority="65">
-      <formula>LEN(TRIM(A28))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29">
-    <cfRule type="notContainsBlanks" dxfId="64" priority="64">
-      <formula>LEN(TRIM(A29))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
-    <cfRule type="notContainsBlanks" dxfId="63" priority="63">
-      <formula>LEN(TRIM(A30))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
-    <cfRule type="notContainsBlanks" dxfId="62" priority="62">
-      <formula>LEN(TRIM(A31))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="notContainsBlanks" dxfId="61" priority="61">
-      <formula>LEN(TRIM(A32))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="notContainsBlanks" dxfId="60" priority="60">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="notContainsBlanks" dxfId="59" priority="59">
-      <formula>LEN(TRIM(A36))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
-    <cfRule type="notContainsBlanks" dxfId="58" priority="58">
-      <formula>LEN(TRIM(A38))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
-    <cfRule type="notContainsBlanks" dxfId="57" priority="57">
-      <formula>LEN(TRIM(A37))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A39">
-    <cfRule type="notContainsBlanks" dxfId="56" priority="56">
-      <formula>LEN(TRIM(A39))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41">
-    <cfRule type="notContainsBlanks" dxfId="55" priority="55">
-      <formula>LEN(TRIM(A41))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46">
-    <cfRule type="notContainsBlanks" dxfId="54" priority="54">
-      <formula>LEN(TRIM(A46))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A49">
-    <cfRule type="notContainsBlanks" dxfId="53" priority="53">
-      <formula>LEN(TRIM(A49))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56">
-    <cfRule type="notContainsBlanks" dxfId="48" priority="48">
-      <formula>LEN(TRIM(A56))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A94">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="39">
-      <formula>LEN(TRIM(A94))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A93">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="38">
-      <formula>LEN(TRIM(A93))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A92">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="37">
-      <formula>LEN(TRIM(A92))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A95">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="36">
-      <formula>LEN(TRIM(A95))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A104">
-    <cfRule type="notContainsBlanks" dxfId="35" priority="31">
-      <formula>LEN(TRIM(A104))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A100">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="33">
-      <formula>LEN(TRIM(A100))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A105">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="30">
-      <formula>LEN(TRIM(A105))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A106">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="29">
-      <formula>LEN(TRIM(A106))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A107">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="28">
-      <formula>LEN(TRIM(A107))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A98">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="26">
-      <formula>LEN(TRIM(A98))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A99">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="25">
-      <formula>LEN(TRIM(A99))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A101">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="24">
-      <formula>LEN(TRIM(A101))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A102">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="23">
-      <formula>LEN(TRIM(A102))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="16">
-      <formula>LEN(TRIM(A51))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="18">
-      <formula>LEN(TRIM(A50))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A52">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="15">
-      <formula>LEN(TRIM(A52))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="12">
-      <formula>LEN(TRIM(A55))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
-      <formula>LEN(TRIM(A53))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
-      <formula>LEN(TRIM(A54))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A57">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
-      <formula>LEN(TRIM(A57))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A58">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
-      <formula>LEN(TRIM(A58))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
-      <formula>LEN(TRIM(A59))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
-      <formula>LEN(TRIM(A60))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
-      <formula>LEN(TRIM(A61))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(A62))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A63">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
-      <formula>LEN(TRIM(A63))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A64">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(A64))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(A65))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A66">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(A66))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A67))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4621,14 +4467,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -4639,7 +4485,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -4653,7 +4499,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -4667,7 +4513,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -4695,14 +4541,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>30</v>
       </c>
@@ -4710,7 +4556,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -4718,7 +4564,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -4726,7 +4572,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
@@ -4734,7 +4580,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -4742,7 +4588,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -4750,7 +4596,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -4764,7 +4610,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -4778,7 +4624,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -4792,7 +4638,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -4806,16 +4652,16 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -4823,7 +4669,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -4837,7 +4683,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -4851,7 +4697,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -4865,7 +4711,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -4879,7 +4725,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
@@ -4892,7 +4738,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
@@ -4905,7 +4751,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>52</v>
       </c>
@@ -4916,11 +4762,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="3"/>
     </row>

</xml_diff>

<commit_message>
Match Ont --> R. Commit prior to branching for switch from rrdf to redland
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -1119,49 +1119,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="99">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="93">
     <dxf>
       <fill>
         <patternFill>
@@ -2126,8 +2084,8 @@
   <dimension ref="A1:H116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B112" sqref="B112"/>
+      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2254,7 +2212,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
-        <v>42996</v>
+        <v>43005</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>79</v>
@@ -2887,7 +2845,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="9">
-        <v>42998</v>
+        <v>43005</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>90</v>
@@ -3990,442 +3948,442 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:A7">
-    <cfRule type="notContainsBlanks" dxfId="98" priority="417">
+    <cfRule type="notContainsBlanks" dxfId="92" priority="417">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A80">
-    <cfRule type="notContainsBlanks" dxfId="97" priority="289">
+    <cfRule type="notContainsBlanks" dxfId="91" priority="289">
       <formula>LEN(TRIM(A80))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68">
-    <cfRule type="notContainsBlanks" dxfId="96" priority="291">
+    <cfRule type="notContainsBlanks" dxfId="90" priority="291">
       <formula>LEN(TRIM(A68))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89">
-    <cfRule type="notContainsBlanks" dxfId="95" priority="147">
+    <cfRule type="notContainsBlanks" dxfId="89" priority="147">
       <formula>LEN(TRIM(A89))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="notContainsBlanks" dxfId="93" priority="155">
+    <cfRule type="notContainsBlanks" dxfId="88" priority="155">
       <formula>LEN(TRIM(A47))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95">
-    <cfRule type="notContainsBlanks" dxfId="90" priority="140">
+    <cfRule type="notContainsBlanks" dxfId="87" priority="140">
       <formula>LEN(TRIM(A95))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48">
-    <cfRule type="notContainsBlanks" dxfId="89" priority="127">
+    <cfRule type="notContainsBlanks" dxfId="86" priority="127">
       <formula>LEN(TRIM(A48))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="88" priority="131">
+    <cfRule type="notContainsBlanks" dxfId="85" priority="131">
       <formula>LEN(TRIM(A25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A10">
-    <cfRule type="notContainsBlanks" dxfId="87" priority="134">
+    <cfRule type="notContainsBlanks" dxfId="84" priority="134">
       <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="notContainsBlanks" dxfId="86" priority="133">
+    <cfRule type="notContainsBlanks" dxfId="83" priority="133">
       <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="notContainsBlanks" dxfId="85" priority="132">
+    <cfRule type="notContainsBlanks" dxfId="82" priority="132">
       <formula>LEN(TRIM(A22))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44:A45">
-    <cfRule type="notContainsBlanks" dxfId="84" priority="128">
+    <cfRule type="notContainsBlanks" dxfId="81" priority="128">
       <formula>LEN(TRIM(A44))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102">
-    <cfRule type="notContainsBlanks" dxfId="83" priority="115">
+    <cfRule type="notContainsBlanks" dxfId="80" priority="115">
       <formula>LEN(TRIM(A102))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="notContainsBlanks" dxfId="82" priority="130">
+    <cfRule type="notContainsBlanks" dxfId="79" priority="130">
       <formula>LEN(TRIM(A40))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="notContainsBlanks" dxfId="81" priority="129">
+    <cfRule type="notContainsBlanks" dxfId="78" priority="129">
       <formula>LEN(TRIM(A42))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90">
-    <cfRule type="notContainsBlanks" dxfId="79" priority="117">
+    <cfRule type="notContainsBlanks" dxfId="77" priority="117">
       <formula>LEN(TRIM(A90))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="notContainsBlanks" dxfId="78" priority="110">
+    <cfRule type="notContainsBlanks" dxfId="76" priority="110">
       <formula>LEN(TRIM(A35))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="notContainsBlanks" dxfId="76" priority="112">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="112">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="notContainsBlanks" dxfId="75" priority="116">
+    <cfRule type="notContainsBlanks" dxfId="74" priority="116">
       <formula>LEN(TRIM(A96))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="notContainsBlanks" dxfId="74" priority="114">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="114">
       <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="notContainsBlanks" dxfId="73" priority="113">
+    <cfRule type="notContainsBlanks" dxfId="72" priority="113">
       <formula>LEN(TRIM(A12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="notContainsBlanks" dxfId="72" priority="111">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="111">
       <formula>LEN(TRIM(A34))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18">
-    <cfRule type="notContainsBlanks" dxfId="71" priority="109">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="109">
       <formula>LEN(TRIM(A18))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19">
-    <cfRule type="notContainsBlanks" dxfId="70" priority="108">
+    <cfRule type="notContainsBlanks" dxfId="69" priority="108">
       <formula>LEN(TRIM(A19))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="notContainsBlanks" dxfId="69" priority="107">
+    <cfRule type="notContainsBlanks" dxfId="68" priority="107">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="notContainsBlanks" dxfId="68" priority="106">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="106">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="notContainsBlanks" dxfId="67" priority="105">
+    <cfRule type="notContainsBlanks" dxfId="66" priority="105">
       <formula>LEN(TRIM(A17))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="notContainsBlanks" dxfId="66" priority="104">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="104">
       <formula>LEN(TRIM(A20))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="notContainsBlanks" dxfId="65" priority="103">
+    <cfRule type="notContainsBlanks" dxfId="64" priority="103">
       <formula>LEN(TRIM(A21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="notContainsBlanks" dxfId="64" priority="102">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="102">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="notContainsBlanks" dxfId="63" priority="101">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="101">
       <formula>LEN(TRIM(A23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="notContainsBlanks" dxfId="62" priority="94">
+    <cfRule type="notContainsBlanks" dxfId="61" priority="94">
       <formula>LEN(TRIM(A32))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="notContainsBlanks" dxfId="61" priority="90">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="90">
       <formula>LEN(TRIM(A37))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="notContainsBlanks" dxfId="60" priority="92">
+    <cfRule type="notContainsBlanks" dxfId="59" priority="92">
       <formula>LEN(TRIM(A36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39">
-    <cfRule type="notContainsBlanks" dxfId="59" priority="89">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="89">
       <formula>LEN(TRIM(A39))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33">
-    <cfRule type="notContainsBlanks" dxfId="58" priority="93">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="93">
       <formula>LEN(TRIM(A33))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41">
-    <cfRule type="notContainsBlanks" dxfId="57" priority="88">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="88">
       <formula>LEN(TRIM(A41))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38">
-    <cfRule type="notContainsBlanks" dxfId="56" priority="91">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="91">
       <formula>LEN(TRIM(A38))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="notContainsBlanks" dxfId="55" priority="87">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="87">
       <formula>LEN(TRIM(A46))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49">
-    <cfRule type="notContainsBlanks" dxfId="54" priority="86">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="86">
       <formula>LEN(TRIM(A49))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56">
-    <cfRule type="notContainsBlanks" dxfId="53" priority="81">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="81">
       <formula>LEN(TRIM(A56))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93">
-    <cfRule type="notContainsBlanks" dxfId="52" priority="72">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="72">
       <formula>LEN(TRIM(A93))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92">
-    <cfRule type="notContainsBlanks" dxfId="51" priority="71">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="71">
       <formula>LEN(TRIM(A92))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91">
-    <cfRule type="notContainsBlanks" dxfId="50" priority="70">
+    <cfRule type="notContainsBlanks" dxfId="49" priority="70">
       <formula>LEN(TRIM(A91))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94">
-    <cfRule type="notContainsBlanks" dxfId="49" priority="69">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="69">
       <formula>LEN(TRIM(A94))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="notContainsBlanks" dxfId="48" priority="64">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="64">
       <formula>LEN(TRIM(A103))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99">
-    <cfRule type="notContainsBlanks" dxfId="47" priority="66">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="66">
       <formula>LEN(TRIM(A99))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104">
-    <cfRule type="notContainsBlanks" dxfId="46" priority="63">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="63">
       <formula>LEN(TRIM(A104))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105">
-    <cfRule type="notContainsBlanks" dxfId="45" priority="62">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="62">
       <formula>LEN(TRIM(A105))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A106">
-    <cfRule type="notContainsBlanks" dxfId="44" priority="61">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="61">
       <formula>LEN(TRIM(A106))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97">
-    <cfRule type="notContainsBlanks" dxfId="43" priority="59">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="59">
       <formula>LEN(TRIM(A97))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="58">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="58">
       <formula>LEN(TRIM(A98))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="57">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="57">
       <formula>LEN(TRIM(A100))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="56">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="56">
       <formula>LEN(TRIM(A101))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="49">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="49">
       <formula>LEN(TRIM(A51))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="51">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="51">
       <formula>LEN(TRIM(A50))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="48">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="48">
       <formula>LEN(TRIM(A52))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="45">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="45">
       <formula>LEN(TRIM(A55))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="notContainsBlanks" dxfId="35" priority="47">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="47">
       <formula>LEN(TRIM(A53))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="46">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="46">
       <formula>LEN(TRIM(A54))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="44">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="44">
       <formula>LEN(TRIM(A57))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="43">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="43">
       <formula>LEN(TRIM(A58))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="42">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="42">
       <formula>LEN(TRIM(A59))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60">
-    <cfRule type="notContainsBlanks" dxfId="30" priority="41">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="41">
       <formula>LEN(TRIM(A60))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="40">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="40">
       <formula>LEN(TRIM(A61))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="39">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="39">
       <formula>LEN(TRIM(A62))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="38">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="38">
       <formula>LEN(TRIM(A63))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="37">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="37">
       <formula>LEN(TRIM(A64))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="36">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="36">
       <formula>LEN(TRIM(A65))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="35">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="35">
       <formula>LEN(TRIM(A66))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="34">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="34">
       <formula>LEN(TRIM(A67))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="33">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="33">
       <formula>LEN(TRIM(A43))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="28">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="28">
       <formula>LEN(TRIM(A26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:A31">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="27">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="27">
       <formula>LEN(TRIM(A27))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="17">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="17">
       <formula>LEN(TRIM(A72))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="20">
       <formula>LEN(TRIM(A69))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="19">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="19">
       <formula>LEN(TRIM(A70))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="18">
       <formula>LEN(TRIM(A71))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A73">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="16">
       <formula>LEN(TRIM(A73))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="15">
       <formula>LEN(TRIM(A74))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A75">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="14">
       <formula>LEN(TRIM(A75))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A76">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="13">
       <formula>LEN(TRIM(A76))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="12">
       <formula>LEN(TRIM(A77))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="11">
       <formula>LEN(TRIM(A78))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A79">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="10">
       <formula>LEN(TRIM(A79))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="6">
       <formula>LEN(TRIM(A84))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="8">
       <formula>LEN(TRIM(A81))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="7">
       <formula>LEN(TRIM(A82))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
synched with exception of adding new visit data for Person1: Baseline, Wk2, Wk24 for match with AO
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_gitHub\CTDasRDF\r\validation\"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="139">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -396,12 +396,6 @@
     <t>AO email 19SEpt</t>
   </si>
   <si>
-    <t>sdtmterm:C74456.C12421</t>
-  </si>
-  <si>
-    <t>custom: prefix issue. Email to AO 20 SEPT</t>
-  </si>
-  <si>
     <t>cdiscpilot01:BloodPressureOutcome_2</t>
   </si>
   <si>
@@ -421,13 +415,37 @@
   </si>
   <si>
     <t>cdiscpilot01:Investigator_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:VisitBaseline_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:VisitWk2_1</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:VisitWk24_1</t>
+  </si>
+  <si>
+    <t>need to add: study:FixedDoseIntervalBegin</t>
+  </si>
+  <si>
+    <t>need to add: study:FixedDoseIntervalEnd</t>
+  </si>
+  <si>
+    <t>HERE</t>
+  </si>
+  <si>
+    <t>Need to move</t>
+  </si>
+  <si>
+    <t>Not present in new Ont version</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -616,8 +634,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -800,12 +826,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1012,7 +1032,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1057,23 +1077,25 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1119,7 +1141,343 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="93">
+  <dxfs count="141">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2081,11 +2439,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H116"/>
+  <dimension ref="A1:H119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
+      <pane ySplit="3" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2134,7 +2492,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>79</v>
@@ -2155,7 +2513,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>79</v>
@@ -2174,7 +2532,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>79</v>
@@ -2193,7 +2551,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>79</v>
@@ -2212,7 +2570,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
-        <v>43005</v>
+        <v>43027</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>79</v>
@@ -2231,7 +2589,7 @@
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>79</v>
@@ -2244,11 +2602,11 @@
         <v>54</v>
       </c>
       <c r="F9" s="18"/>
-      <c r="G9" s="25"/>
+      <c r="G9" s="24"/>
     </row>
     <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>79</v>
@@ -2261,11 +2619,11 @@
         <v>23</v>
       </c>
       <c r="F10" s="18"/>
-      <c r="G10" s="25"/>
+      <c r="G10" s="24"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>79</v>
@@ -2283,9 +2641,7 @@
       <c r="G11" s="22"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="9">
-        <v>42996</v>
-      </c>
+      <c r="A12" s="26"/>
       <c r="B12" s="10" t="s">
         <v>79</v>
       </c>
@@ -2293,16 +2649,16 @@
       <c r="D12" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="18"/>
+      <c r="F12" s="19" t="s">
+        <v>134</v>
+      </c>
       <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="9">
-        <v>42996</v>
-      </c>
+      <c r="A13" s="26"/>
       <c r="B13" s="10" t="s">
         <v>79</v>
       </c>
@@ -2310,15 +2666,17 @@
       <c r="D13" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="18"/>
+      <c r="F13" s="19" t="s">
+        <v>135</v>
+      </c>
       <c r="G13" s="22"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>79</v>
@@ -2337,7 +2695,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>79</v>
@@ -2356,7 +2714,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>79</v>
@@ -2373,7 +2731,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>79</v>
@@ -2390,7 +2748,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>79</v>
@@ -2409,7 +2767,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>79</v>
@@ -2428,7 +2786,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>79</v>
@@ -2442,12 +2800,14 @@
       <c r="E20" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="19"/>
+      <c r="F20" s="19" t="s">
+        <v>136</v>
+      </c>
       <c r="G20" s="22"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>79</v>
@@ -2464,7 +2824,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>79</v>
@@ -2481,7 +2841,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>79</v>
@@ -2496,11 +2856,11 @@
         <v>68</v>
       </c>
       <c r="F23" s="18"/>
-      <c r="G23" s="25"/>
+      <c r="G23" s="24"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>79</v>
@@ -2513,11 +2873,11 @@
         <v>70</v>
       </c>
       <c r="F24" s="18"/>
-      <c r="G24" s="25"/>
+      <c r="G24" s="24"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>79</v>
@@ -2530,11 +2890,11 @@
         <v>23</v>
       </c>
       <c r="F25" s="18"/>
-      <c r="G25" s="25"/>
+      <c r="G25" s="24"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="9">
-        <v>42998</v>
+        <v>43027</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>53</v>
@@ -2548,14 +2908,12 @@
       <c r="E26" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="F26" s="18" t="s">
-        <v>125</v>
-      </c>
+      <c r="F26" s="18"/>
       <c r="G26" s="22"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="9">
-        <v>42998</v>
+        <v>43027</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>53</v>
@@ -2569,14 +2927,12 @@
       <c r="E27" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="F27" s="18" t="s">
-        <v>125</v>
-      </c>
+      <c r="F27" s="18"/>
       <c r="G27" s="22"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="9">
-        <v>42998</v>
+        <v>43027</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>53</v>
@@ -2590,14 +2946,12 @@
       <c r="E28" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F28" s="18" t="s">
-        <v>125</v>
-      </c>
+      <c r="F28" s="18"/>
       <c r="G28" s="22"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="9">
-        <v>42998</v>
+        <v>43027</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="15" t="s">
@@ -2609,14 +2963,12 @@
       <c r="E29" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="F29" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="G29" s="25"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="24"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="9">
-        <v>42998</v>
+        <v>43027</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="11"/>
@@ -2626,14 +2978,12 @@
       <c r="E30" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F30" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="G30" s="25"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="24"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="9">
-        <v>42998</v>
+        <v>43027</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="11"/>
@@ -2643,14 +2993,12 @@
       <c r="E31" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F31" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="G31" s="25"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="24"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>79</v>
@@ -2669,7 +3017,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>79</v>
@@ -2685,9 +3033,7 @@
       <c r="G33" s="22"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="9">
-        <v>42996</v>
-      </c>
+      <c r="A34" s="26"/>
       <c r="B34" s="10" t="s">
         <v>79</v>
       </c>
@@ -2695,16 +3041,16 @@
       <c r="D34" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="F34" s="18"/>
+      <c r="F34" s="19" t="s">
+        <v>137</v>
+      </c>
       <c r="G34" s="22"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="9">
-        <v>42996</v>
-      </c>
+      <c r="A35" s="26"/>
       <c r="B35" s="10" t="s">
         <v>79</v>
       </c>
@@ -2712,15 +3058,17 @@
       <c r="D35" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F35" s="18"/>
+      <c r="F35" s="19" t="s">
+        <v>137</v>
+      </c>
       <c r="G35" s="22"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>79</v>
@@ -2738,42 +3086,44 @@
       <c r="G36" s="22"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="27"/>
-      <c r="B37" s="11" t="s">
-        <v>90</v>
-      </c>
+      <c r="A37" s="26"/>
+      <c r="B37" s="10"/>
       <c r="C37" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F37" s="20"/>
+      <c r="E37" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>138</v>
+      </c>
       <c r="G37" s="22"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="12" t="s">
-        <v>58</v>
+      <c r="C38" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="18"/>
+        <v>73</v>
+      </c>
+      <c r="F38" s="20"/>
       <c r="G38" s="22"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>90</v>
@@ -2784,68 +3134,70 @@
       <c r="D39" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="F39" s="21"/>
+      <c r="E39" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="18"/>
       <c r="G39" s="22"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="11"/>
+      <c r="C40" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D40" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>74</v>
+        <v>58</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>62</v>
       </c>
       <c r="F40" s="21"/>
       <c r="G40" s="22"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="C41" s="11"/>
       <c r="D41" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>63</v>
+        <v>59</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="F41" s="21"/>
       <c r="G41" s="22"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C42" s="11"/>
+      <c r="C42" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D42" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>74</v>
+        <v>58</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="F42" s="21"/>
       <c r="G42" s="22"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="9">
-        <v>43005</v>
+        <v>43027</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>90</v>
@@ -2853,55 +3205,65 @@
       <c r="C43" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D43" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="F43" s="23"/>
-      <c r="G43" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="D43" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43" s="21"/>
+      <c r="G43" s="22"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F44" s="21"/>
-      <c r="G44" s="22"/>
+      <c r="C44" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F44" s="23"/>
+      <c r="G44" s="22" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="9">
-        <v>42998</v>
-      </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="12"/>
+        <v>43027</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>58</v>
+      </c>
       <c r="E45" s="11" t="s">
-        <v>124</v>
+        <v>23</v>
       </c>
       <c r="F45" s="21"/>
       <c r="G45" s="22"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="11"/>
+      <c r="C46" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D46" s="12" t="s">
         <v>58</v>
       </c>
@@ -2913,7 +3275,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B47" s="11" t="s">
         <v>90</v>
@@ -2930,12 +3292,14 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B48" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C48" s="14"/>
+      <c r="C48" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D48" s="12"/>
       <c r="E48" s="11" t="s">
         <v>23</v>
@@ -2945,12 +3309,14 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B49" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="11"/>
+      <c r="C49" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D49" s="12"/>
       <c r="E49" s="11" t="s">
         <v>112</v>
@@ -2960,7 +3326,7 @@
     </row>
     <row r="50" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>90</v>
@@ -2968,23 +3334,27 @@
       <c r="C50" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D50" s="12"/>
-      <c r="E50" s="29" t="s">
+      <c r="D50" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E50" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="F50" s="28" t="s">
+      <c r="F50" s="27" t="s">
         <v>122</v>
       </c>
       <c r="G50" s="22"/>
     </row>
     <row r="51" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B51" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C51" s="12"/>
+      <c r="C51" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D51" s="12"/>
       <c r="E51" s="11" t="s">
         <v>74</v>
@@ -2994,12 +3364,14 @@
     </row>
     <row r="52" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B52" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C52" s="12"/>
+      <c r="C52" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D52" s="12"/>
       <c r="E52" s="11" t="s">
         <v>76</v>
@@ -3009,15 +3381,15 @@
     </row>
     <row r="53" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B53" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="C53" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="12"/>
       <c r="E53" s="11" t="s">
         <v>63</v>
       </c>
@@ -3026,15 +3398,15 @@
     </row>
     <row r="54" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12" t="s">
-        <v>119</v>
-      </c>
+      <c r="C54" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D54" s="12"/>
       <c r="E54" s="11" t="s">
         <v>23</v>
       </c>
@@ -3043,12 +3415,14 @@
     </row>
     <row r="55" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C55" s="12"/>
+      <c r="C55" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D55" s="12"/>
       <c r="E55" s="11" t="s">
         <v>113</v>
@@ -3058,7 +3432,7 @@
     </row>
     <row r="56" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>90</v>
@@ -3077,12 +3451,14 @@
     </row>
     <row r="57" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C57" s="12"/>
+      <c r="C57" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="D57" s="12"/>
       <c r="E57" s="11" t="s">
         <v>74</v>
@@ -3092,12 +3468,14 @@
     </row>
     <row r="58" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B58" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C58" s="12"/>
+      <c r="C58" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="D58" s="12"/>
       <c r="E58" s="11" t="s">
         <v>77</v>
@@ -3107,15 +3485,15 @@
     </row>
     <row r="59" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B59" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="C59" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D59" s="12"/>
       <c r="E59" s="11" t="s">
         <v>62</v>
       </c>
@@ -3124,15 +3502,13 @@
     </row>
     <row r="60" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B60" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C60" s="12"/>
-      <c r="D60" s="12" t="s">
-        <v>119</v>
-      </c>
+      <c r="D60" s="12"/>
       <c r="E60" s="11" t="s">
         <v>74</v>
       </c>
@@ -3141,7 +3517,7 @@
     </row>
     <row r="61" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B61" s="10" t="s">
         <v>90</v>
@@ -3156,7 +3532,7 @@
     </row>
     <row r="62" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B62" s="10" t="s">
         <v>90</v>
@@ -3175,13 +3551,17 @@
     </row>
     <row r="63" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B63" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
+      <c r="C63" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>58</v>
+      </c>
       <c r="E63" s="11" t="s">
         <v>74</v>
       </c>
@@ -3190,7 +3570,7 @@
     </row>
     <row r="64" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B64" s="10" t="s">
         <v>90</v>
@@ -3205,7 +3585,7 @@
     </row>
     <row r="65" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B65" s="10" t="s">
         <v>90</v>
@@ -3222,7 +3602,7 @@
     </row>
     <row r="66" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B66" s="10" t="s">
         <v>90</v>
@@ -3239,7 +3619,7 @@
     </row>
     <row r="67" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="9">
-        <v>42997</v>
+        <v>43027</v>
       </c>
       <c r="B67" s="10" t="s">
         <v>90</v>
@@ -3253,8 +3633,8 @@
       <c r="G67" s="22"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A68" s="27">
-        <v>42998</v>
+      <c r="A68" s="9">
+        <v>43027</v>
       </c>
       <c r="B68" s="10" t="s">
         <v>90</v>
@@ -3272,8 +3652,8 @@
       <c r="G68" s="22"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A69" s="27">
-        <v>42998</v>
+      <c r="A69" s="9">
+        <v>43027</v>
       </c>
       <c r="B69" s="10" t="s">
         <v>90</v>
@@ -3289,8 +3669,8 @@
       <c r="G69" s="22"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A70" s="27">
-        <v>42998</v>
+      <c r="A70" s="9">
+        <v>43027</v>
       </c>
       <c r="B70" s="10" t="s">
         <v>90</v>
@@ -3306,8 +3686,8 @@
       <c r="G70" s="22"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A71" s="27">
-        <v>42998</v>
+      <c r="A71" s="9">
+        <v>43027</v>
       </c>
       <c r="B71" s="10" t="s">
         <v>90</v>
@@ -3323,8 +3703,8 @@
       <c r="G71" s="22"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A72" s="27">
-        <v>42998</v>
+      <c r="A72" s="9">
+        <v>43027</v>
       </c>
       <c r="B72" s="10" t="s">
         <v>90</v>
@@ -3340,8 +3720,8 @@
       <c r="G72" s="22"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A73" s="27">
-        <v>42998</v>
+      <c r="A73" s="9">
+        <v>43027</v>
       </c>
       <c r="B73" s="10" t="s">
         <v>90</v>
@@ -3351,14 +3731,14 @@
         <v>58</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F73" s="22"/>
       <c r="G73" s="22"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A74" s="27">
-        <v>42998</v>
+      <c r="A74" s="9">
+        <v>43027</v>
       </c>
       <c r="B74" s="10" t="s">
         <v>90</v>
@@ -3376,8 +3756,8 @@
       <c r="G74" s="18"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A75" s="27">
-        <v>42998</v>
+      <c r="A75" s="9">
+        <v>43027</v>
       </c>
       <c r="B75" s="10" t="s">
         <v>90</v>
@@ -3393,8 +3773,8 @@
       <c r="G75" s="18"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A76" s="27">
-        <v>42998</v>
+      <c r="A76" s="9">
+        <v>43027</v>
       </c>
       <c r="B76" s="10" t="s">
         <v>90</v>
@@ -3410,8 +3790,8 @@
       <c r="G76" s="18"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A77" s="27">
-        <v>42998</v>
+      <c r="A77" s="9">
+        <v>43027</v>
       </c>
       <c r="B77" s="10" t="s">
         <v>90</v>
@@ -3427,8 +3807,8 @@
       <c r="G77" s="18"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A78" s="27">
-        <v>42998</v>
+      <c r="A78" s="9">
+        <v>43027</v>
       </c>
       <c r="B78" s="10" t="s">
         <v>90</v>
@@ -3442,8 +3822,8 @@
       <c r="G78" s="7"/>
     </row>
     <row r="79" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="27">
-        <v>42998</v>
+      <c r="A79" s="9">
+        <v>43027</v>
       </c>
       <c r="B79" s="10" t="s">
         <v>90</v>
@@ -3453,33 +3833,35 @@
         <v>58</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F79" s="22"/>
       <c r="G79" s="18"/>
     </row>
     <row r="80" spans="1:8" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A80" s="27"/>
+      <c r="A80" s="9">
+        <v>43027</v>
+      </c>
       <c r="B80" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C80" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="E80" s="31" t="s">
+      <c r="E80" s="17" t="s">
         <v>95</v>
       </c>
       <c r="F80" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="G80" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="H80" s="32"/>
+      <c r="G80" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="H80" s="30"/>
     </row>
     <row r="81" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A81" s="27">
-        <v>42998</v>
+      <c r="A81" s="9">
+        <v>43027</v>
       </c>
       <c r="B81" s="10" t="s">
         <v>90</v>
@@ -3495,8 +3877,8 @@
       <c r="G81" s="18"/>
     </row>
     <row r="82" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A82" s="27">
-        <v>42998</v>
+      <c r="A82" s="9">
+        <v>43027</v>
       </c>
       <c r="B82" s="10" t="s">
         <v>90</v>
@@ -3512,8 +3894,8 @@
       <c r="G82" s="18"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83" s="27">
-        <v>42998</v>
+      <c r="A83" s="9">
+        <v>43027</v>
       </c>
       <c r="B83" s="10" t="s">
         <v>90</v>
@@ -3529,8 +3911,8 @@
       <c r="G83" s="22"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A84" s="27">
-        <v>42998</v>
+      <c r="A84" s="9">
+        <v>43027</v>
       </c>
       <c r="B84" s="10" t="s">
         <v>90</v>
@@ -3546,8 +3928,8 @@
       <c r="G84" s="22"/>
     </row>
     <row r="85" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="27">
-        <v>42998</v>
+      <c r="A85" s="9">
+        <v>43027</v>
       </c>
       <c r="B85" s="10" t="s">
         <v>90</v>
@@ -3563,9 +3945,7 @@
       <c r="G85" s="22"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A86" s="27">
-        <v>42998</v>
-      </c>
+      <c r="A86" s="31"/>
       <c r="B86" s="10" t="s">
         <v>90</v>
       </c>
@@ -3580,8 +3960,8 @@
       <c r="G86" s="22"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A87" s="27">
-        <v>42998</v>
+      <c r="A87" s="9">
+        <v>43027</v>
       </c>
       <c r="B87" s="10" t="s">
         <v>90</v>
@@ -3595,9 +3975,7 @@
       <c r="G87" s="22"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A88" s="27">
-        <v>42998</v>
-      </c>
+      <c r="A88" s="31"/>
       <c r="B88" s="10" t="s">
         <v>90</v>
       </c>
@@ -3610,7 +3988,7 @@
       <c r="G88" s="22"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A89" s="9"/>
+      <c r="A89" s="31"/>
       <c r="B89" s="10" t="s">
         <v>90</v>
       </c>
@@ -3618,17 +3996,17 @@
         <v>73</v>
       </c>
       <c r="D89" s="10"/>
-      <c r="E89" s="24" t="s">
+      <c r="E89" s="17" t="s">
         <v>101</v>
       </c>
       <c r="F89" s="23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G89" s="22"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B90" s="10" t="s">
         <v>90</v>
@@ -3639,12 +4017,10 @@
         <v>23</v>
       </c>
       <c r="F90" s="22"/>
-      <c r="G90" s="26"/>
+      <c r="G90" s="25"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A91" s="9">
-        <v>42996</v>
-      </c>
+      <c r="A91" s="31"/>
       <c r="B91" s="10" t="s">
         <v>90</v>
       </c>
@@ -3654,12 +4030,10 @@
         <v>76</v>
       </c>
       <c r="F91" s="22"/>
-      <c r="G91" s="26"/>
+      <c r="G91" s="25"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A92" s="9">
-        <v>42996</v>
-      </c>
+      <c r="A92" s="31"/>
       <c r="B92" s="10"/>
       <c r="C92" s="10"/>
       <c r="D92" s="12" t="s">
@@ -3669,11 +4043,11 @@
         <v>63</v>
       </c>
       <c r="F92" s="22"/>
-      <c r="G92" s="26"/>
+      <c r="G92" s="25"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B93" s="10"/>
       <c r="C93" s="10"/>
@@ -3684,12 +4058,10 @@
         <v>23</v>
       </c>
       <c r="F93" s="22"/>
-      <c r="G93" s="26"/>
+      <c r="G93" s="25"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A94" s="9">
-        <v>42996</v>
-      </c>
+      <c r="A94" s="9"/>
       <c r="B94" s="10" t="s">
         <v>90</v>
       </c>
@@ -3699,12 +4071,10 @@
         <v>108</v>
       </c>
       <c r="F94" s="22"/>
-      <c r="G94" s="26"/>
+      <c r="G94" s="25"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A95" s="9">
-        <v>42997</v>
-      </c>
+      <c r="A95" s="9"/>
       <c r="B95" s="10" t="s">
         <v>90</v>
       </c>
@@ -3712,7 +4082,7 @@
         <v>73</v>
       </c>
       <c r="D95" s="10"/>
-      <c r="E95" s="10" t="s">
+      <c r="E95" s="33" t="s">
         <v>102</v>
       </c>
       <c r="F95" s="23"/>
@@ -3720,7 +4090,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B96" s="10" t="s">
         <v>90</v>
@@ -3731,12 +4101,10 @@
         <v>23</v>
       </c>
       <c r="F96" s="18"/>
-      <c r="G96" s="26"/>
+      <c r="G96" s="25"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A97" s="9">
-        <v>42997</v>
-      </c>
+      <c r="A97" s="9"/>
       <c r="B97" s="10" t="s">
         <v>90</v>
       </c>
@@ -3746,12 +4114,10 @@
         <v>77</v>
       </c>
       <c r="F97" s="18"/>
-      <c r="G97" s="26"/>
+      <c r="G97" s="25"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A98" s="9">
-        <v>42997</v>
-      </c>
+      <c r="A98" s="9"/>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
       <c r="D98" s="11"/>
@@ -3759,11 +4125,11 @@
         <v>62</v>
       </c>
       <c r="F98" s="18"/>
-      <c r="G98" s="26"/>
+      <c r="G98" s="25"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B99" s="10"/>
       <c r="C99" s="10"/>
@@ -3774,12 +4140,10 @@
         <v>23</v>
       </c>
       <c r="F99" s="18"/>
-      <c r="G99" s="26"/>
+      <c r="G99" s="25"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A100" s="9">
-        <v>42997</v>
-      </c>
+      <c r="A100" s="9"/>
       <c r="B100" s="10" t="s">
         <v>90</v>
       </c>
@@ -3789,12 +4153,10 @@
         <v>109</v>
       </c>
       <c r="F100" s="22"/>
-      <c r="G100" s="26"/>
+      <c r="G100" s="25"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A101" s="9">
-        <v>42997</v>
-      </c>
+      <c r="A101" s="9"/>
       <c r="B101" s="10" t="s">
         <v>90</v>
       </c>
@@ -3802,7 +4164,7 @@
         <v>73</v>
       </c>
       <c r="D101" s="11"/>
-      <c r="E101" s="10" t="s">
+      <c r="E101" s="33" t="s">
         <v>103</v>
       </c>
       <c r="F101" s="23"/>
@@ -3810,7 +4172,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B102" s="10" t="s">
         <v>90</v>
@@ -3823,9 +4185,7 @@
       <c r="G102" s="22"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A103" s="9">
-        <v>42996</v>
-      </c>
+      <c r="A103" s="9"/>
       <c r="B103" s="10" t="s">
         <v>90</v>
       </c>
@@ -3838,9 +4198,7 @@
       <c r="G103" s="22"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A104" s="9">
-        <v>42996</v>
-      </c>
+      <c r="A104" s="9"/>
       <c r="B104" s="10"/>
       <c r="C104" s="11"/>
       <c r="D104" s="11"/>
@@ -3852,7 +4210,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" s="9">
-        <v>42996</v>
+        <v>43027</v>
       </c>
       <c r="B105" s="10"/>
       <c r="C105" s="11"/>
@@ -3866,9 +4224,7 @@
       <c r="G105" s="22"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A106" s="9">
-        <v>42996</v>
-      </c>
+      <c r="A106" s="9"/>
       <c r="B106" s="10" t="s">
         <v>90</v>
       </c>
@@ -3877,55 +4233,68 @@
       <c r="E106" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="F106" s="22"/>
+      <c r="F106" s="18"/>
       <c r="G106" s="22"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C107" s="5"/>
-      <c r="D107" s="5"/>
-      <c r="E107" s="5"/>
-      <c r="F107" s="7"/>
+      <c r="A107" s="9"/>
+      <c r="B107" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
+      <c r="E107" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="F107" s="18"/>
+      <c r="G107" s="22"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
-        <v>130</v>
-      </c>
-      <c r="C108" s="5"/>
-      <c r="D108" s="5"/>
-      <c r="E108" s="5"/>
-      <c r="F108" s="7"/>
+      <c r="A108" s="9"/>
+      <c r="B108" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C108" s="11"/>
+      <c r="D108" s="12"/>
+      <c r="E108" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="F108" s="18"/>
+      <c r="G108" s="22"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B109" t="s">
-        <v>131</v>
-      </c>
-      <c r="C109" t="s">
-        <v>118</v>
-      </c>
-      <c r="E109" t="s">
-        <v>132</v>
-      </c>
-      <c r="F109" s="7"/>
+      <c r="A109" s="9"/>
+      <c r="F109" s="22"/>
+      <c r="G109" s="22"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
       <c r="F110" s="7"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>128</v>
+      </c>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
       <c r="E111" s="5"/>
       <c r="F111" s="7"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C112" s="5"/>
-      <c r="D112" s="5"/>
-      <c r="E112" s="5"/>
+      <c r="B112" t="s">
+        <v>129</v>
+      </c>
+      <c r="C112" t="s">
+        <v>118</v>
+      </c>
+      <c r="E112" t="s">
+        <v>130</v>
+      </c>
       <c r="F112" s="7"/>
     </row>
     <row r="113" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
-      <c r="E113" s="5"/>
       <c r="F113" s="7"/>
     </row>
     <row r="114" spans="3:6" x14ac:dyDescent="0.35">
@@ -3946,470 +4315,518 @@
       <c r="E116" s="5"/>
       <c r="F116" s="7"/>
     </row>
+    <row r="117" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C117" s="5"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="5"/>
+      <c r="F117" s="7"/>
+    </row>
+    <row r="118" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C118" s="5"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="5"/>
+      <c r="F118" s="7"/>
+    </row>
+    <row r="119" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C119" s="5"/>
+      <c r="D119" s="5"/>
+      <c r="E119" s="5"/>
+      <c r="F119" s="7"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A4:A7">
-    <cfRule type="notContainsBlanks" dxfId="92" priority="417">
+    <cfRule type="notContainsBlanks" dxfId="140" priority="495">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A89">
+    <cfRule type="notContainsBlanks" dxfId="137" priority="225">
+      <formula>LEN(TRIM(A89))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A95">
+    <cfRule type="notContainsBlanks" dxfId="135" priority="218">
+      <formula>LEN(TRIM(A95))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="notContainsBlanks" dxfId="134" priority="211">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
+    <cfRule type="notContainsBlanks" dxfId="132" priority="188">
+      <formula>LEN(TRIM(A35))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="notContainsBlanks" dxfId="131" priority="190">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="notContainsBlanks" dxfId="130" priority="191">
+      <formula>LEN(TRIM(A12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="notContainsBlanks" dxfId="129" priority="189">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="notContainsBlanks" dxfId="122" priority="170">
+      <formula>LEN(TRIM(A37))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A92">
+    <cfRule type="notContainsBlanks" dxfId="115" priority="149">
+      <formula>LEN(TRIM(A92))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="notContainsBlanks" dxfId="114" priority="148">
+      <formula>LEN(TRIM(A91))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A94">
+    <cfRule type="notContainsBlanks" dxfId="113" priority="147">
+      <formula>LEN(TRIM(A94))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A103">
+    <cfRule type="notContainsBlanks" dxfId="112" priority="142">
+      <formula>LEN(TRIM(A103))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A104">
+    <cfRule type="notContainsBlanks" dxfId="111" priority="141">
+      <formula>LEN(TRIM(A104))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A106:A108">
+    <cfRule type="notContainsBlanks" dxfId="110" priority="140">
+      <formula>LEN(TRIM(A106))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A109">
+    <cfRule type="notContainsBlanks" dxfId="109" priority="139">
+      <formula>LEN(TRIM(A109))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A97">
+    <cfRule type="notContainsBlanks" dxfId="108" priority="137">
+      <formula>LEN(TRIM(A97))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A98">
+    <cfRule type="notContainsBlanks" dxfId="107" priority="136">
+      <formula>LEN(TRIM(A98))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A100">
+    <cfRule type="notContainsBlanks" dxfId="106" priority="135">
+      <formula>LEN(TRIM(A100))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A101">
+    <cfRule type="notContainsBlanks" dxfId="105" priority="134">
+      <formula>LEN(TRIM(A101))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A86">
+    <cfRule type="notContainsBlanks" dxfId="80" priority="80">
+      <formula>LEN(TRIM(A86))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88">
+    <cfRule type="notContainsBlanks" dxfId="79" priority="79">
+      <formula>LEN(TRIM(A88))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="notContainsBlanks" dxfId="78" priority="78">
+      <formula>LEN(TRIM(A8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="notContainsBlanks" dxfId="77" priority="77">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="notContainsBlanks" dxfId="76" priority="76">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="75">
+      <formula>LEN(TRIM(A22))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="notContainsBlanks" dxfId="74" priority="74">
+      <formula>LEN(TRIM(A25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="73">
+      <formula>LEN(TRIM(A39))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41">
+    <cfRule type="notContainsBlanks" dxfId="72" priority="72">
+      <formula>LEN(TRIM(A41))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="71">
+      <formula>LEN(TRIM(A43))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="70">
+      <formula>LEN(TRIM(A45))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48">
+    <cfRule type="notContainsBlanks" dxfId="69" priority="69">
+      <formula>LEN(TRIM(A48))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51">
+    <cfRule type="notContainsBlanks" dxfId="68" priority="68">
+      <formula>LEN(TRIM(A51))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="67">
+      <formula>LEN(TRIM(A54))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57">
+    <cfRule type="notContainsBlanks" dxfId="66" priority="66">
+      <formula>LEN(TRIM(A57))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="65">
+      <formula>LEN(TRIM(A60))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63">
+    <cfRule type="notContainsBlanks" dxfId="64" priority="64">
+      <formula>LEN(TRIM(A63))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="63">
+      <formula>LEN(TRIM(A66))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="62">
+      <formula>LEN(TRIM(A69))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A72">
+    <cfRule type="notContainsBlanks" dxfId="61" priority="61">
+      <formula>LEN(TRIM(A72))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A75">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="60">
+      <formula>LEN(TRIM(A75))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A78">
+    <cfRule type="notContainsBlanks" dxfId="59" priority="59">
+      <formula>LEN(TRIM(A78))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A81">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="58">
+      <formula>LEN(TRIM(A81))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A84">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="57">
+      <formula>LEN(TRIM(A84))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="56">
+      <formula>LEN(TRIM(A87))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="55">
+      <formula>LEN(TRIM(A90))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A93">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="54">
+      <formula>LEN(TRIM(A93))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A96">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="53">
+      <formula>LEN(TRIM(A96))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A99">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="52">
+      <formula>LEN(TRIM(A99))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A102">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="51">
+      <formula>LEN(TRIM(A102))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A105">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="50">
+      <formula>LEN(TRIM(A105))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="notContainsBlanks" dxfId="49" priority="49">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="48">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="47">
+      <formula>LEN(TRIM(A15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="46">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="45">
+      <formula>LEN(TRIM(A18))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="44">
+      <formula>LEN(TRIM(A19))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="43">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="42">
+      <formula>LEN(TRIM(A21))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="41">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="40">
+      <formula>LEN(TRIM(A24))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="39">
+      <formula>LEN(TRIM(A26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="38">
+      <formula>LEN(TRIM(A27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="37">
+      <formula>LEN(TRIM(A28))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:A31">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="36">
+      <formula>LEN(TRIM(A29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="35">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="34">
+      <formula>LEN(TRIM(A33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="33">
+      <formula>LEN(TRIM(A36))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="29">
+      <formula>LEN(TRIM(A42))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="31">
+      <formula>LEN(TRIM(A38))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="30">
+      <formula>LEN(TRIM(A40))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="28">
+      <formula>LEN(TRIM(A44))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="27">
+      <formula>LEN(TRIM(A46))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="26">
+      <formula>LEN(TRIM(A47))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="25">
+      <formula>LEN(TRIM(A49))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="24">
+      <formula>LEN(TRIM(A50))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="23">
+      <formula>LEN(TRIM(A52))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A53">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="22">
+      <formula>LEN(TRIM(A53))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="21">
+      <formula>LEN(TRIM(A55))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="20">
+      <formula>LEN(TRIM(A59))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="19">
+      <formula>LEN(TRIM(A58))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="18">
+      <formula>LEN(TRIM(A56))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="17">
+      <formula>LEN(TRIM(A61))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="16">
+      <formula>LEN(TRIM(A64))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
+      <formula>LEN(TRIM(A62))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
+      <formula>LEN(TRIM(A65))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
+      <formula>LEN(TRIM(A67))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
+      <formula>LEN(TRIM(A68))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
+      <formula>LEN(TRIM(A71))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
+      <formula>LEN(TRIM(A70))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A73">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
+      <formula>LEN(TRIM(A73))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A74">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(A74))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A76">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(A76))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A77">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(A77))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A79">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(A79))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A80">
-    <cfRule type="notContainsBlanks" dxfId="91" priority="289">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(A80))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A68">
-    <cfRule type="notContainsBlanks" dxfId="90" priority="291">
-      <formula>LEN(TRIM(A68))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A89">
-    <cfRule type="notContainsBlanks" dxfId="89" priority="147">
-      <formula>LEN(TRIM(A89))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
-    <cfRule type="notContainsBlanks" dxfId="88" priority="155">
-      <formula>LEN(TRIM(A47))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A95">
-    <cfRule type="notContainsBlanks" dxfId="87" priority="140">
-      <formula>LEN(TRIM(A95))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
-    <cfRule type="notContainsBlanks" dxfId="86" priority="127">
-      <formula>LEN(TRIM(A48))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="85" priority="131">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8:A10">
-    <cfRule type="notContainsBlanks" dxfId="84" priority="134">
-      <formula>LEN(TRIM(A8))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="notContainsBlanks" dxfId="83" priority="133">
-      <formula>LEN(TRIM(A16))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="notContainsBlanks" dxfId="82" priority="132">
-      <formula>LEN(TRIM(A22))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A44:A45">
-    <cfRule type="notContainsBlanks" dxfId="81" priority="128">
-      <formula>LEN(TRIM(A44))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A102">
-    <cfRule type="notContainsBlanks" dxfId="80" priority="115">
-      <formula>LEN(TRIM(A102))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
-    <cfRule type="notContainsBlanks" dxfId="79" priority="130">
-      <formula>LEN(TRIM(A40))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A42">
-    <cfRule type="notContainsBlanks" dxfId="78" priority="129">
-      <formula>LEN(TRIM(A42))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A90">
-    <cfRule type="notContainsBlanks" dxfId="77" priority="117">
-      <formula>LEN(TRIM(A90))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35">
-    <cfRule type="notContainsBlanks" dxfId="76" priority="110">
-      <formula>LEN(TRIM(A35))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="notContainsBlanks" dxfId="75" priority="112">
-      <formula>LEN(TRIM(A13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A96">
-    <cfRule type="notContainsBlanks" dxfId="74" priority="116">
-      <formula>LEN(TRIM(A96))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="notContainsBlanks" dxfId="73" priority="114">
-      <formula>LEN(TRIM(A11))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="notContainsBlanks" dxfId="72" priority="113">
-      <formula>LEN(TRIM(A12))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
-    <cfRule type="notContainsBlanks" dxfId="71" priority="111">
-      <formula>LEN(TRIM(A34))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="notContainsBlanks" dxfId="70" priority="109">
-      <formula>LEN(TRIM(A18))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="notContainsBlanks" dxfId="69" priority="108">
-      <formula>LEN(TRIM(A19))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="notContainsBlanks" dxfId="68" priority="107">
-      <formula>LEN(TRIM(A14))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="notContainsBlanks" dxfId="67" priority="106">
-      <formula>LEN(TRIM(A15))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="notContainsBlanks" dxfId="66" priority="105">
-      <formula>LEN(TRIM(A17))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
-    <cfRule type="notContainsBlanks" dxfId="65" priority="104">
-      <formula>LEN(TRIM(A20))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="notContainsBlanks" dxfId="64" priority="103">
-      <formula>LEN(TRIM(A21))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24">
-    <cfRule type="notContainsBlanks" dxfId="63" priority="102">
-      <formula>LEN(TRIM(A24))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="notContainsBlanks" dxfId="62" priority="101">
-      <formula>LEN(TRIM(A23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="notContainsBlanks" dxfId="61" priority="94">
-      <formula>LEN(TRIM(A32))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
-    <cfRule type="notContainsBlanks" dxfId="60" priority="90">
-      <formula>LEN(TRIM(A37))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="notContainsBlanks" dxfId="59" priority="92">
-      <formula>LEN(TRIM(A36))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A39">
-    <cfRule type="notContainsBlanks" dxfId="58" priority="89">
-      <formula>LEN(TRIM(A39))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="notContainsBlanks" dxfId="57" priority="93">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41">
-    <cfRule type="notContainsBlanks" dxfId="56" priority="88">
-      <formula>LEN(TRIM(A41))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
-    <cfRule type="notContainsBlanks" dxfId="55" priority="91">
-      <formula>LEN(TRIM(A38))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46">
-    <cfRule type="notContainsBlanks" dxfId="54" priority="87">
-      <formula>LEN(TRIM(A46))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A49">
-    <cfRule type="notContainsBlanks" dxfId="53" priority="86">
-      <formula>LEN(TRIM(A49))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56">
-    <cfRule type="notContainsBlanks" dxfId="52" priority="81">
-      <formula>LEN(TRIM(A56))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A93">
-    <cfRule type="notContainsBlanks" dxfId="51" priority="72">
-      <formula>LEN(TRIM(A93))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A92">
-    <cfRule type="notContainsBlanks" dxfId="50" priority="71">
-      <formula>LEN(TRIM(A92))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A91">
-    <cfRule type="notContainsBlanks" dxfId="49" priority="70">
-      <formula>LEN(TRIM(A91))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A94">
-    <cfRule type="notContainsBlanks" dxfId="48" priority="69">
-      <formula>LEN(TRIM(A94))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A103">
-    <cfRule type="notContainsBlanks" dxfId="47" priority="64">
-      <formula>LEN(TRIM(A103))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A99">
-    <cfRule type="notContainsBlanks" dxfId="46" priority="66">
-      <formula>LEN(TRIM(A99))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A104">
-    <cfRule type="notContainsBlanks" dxfId="45" priority="63">
-      <formula>LEN(TRIM(A104))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A105">
-    <cfRule type="notContainsBlanks" dxfId="44" priority="62">
-      <formula>LEN(TRIM(A105))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A106">
-    <cfRule type="notContainsBlanks" dxfId="43" priority="61">
-      <formula>LEN(TRIM(A106))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A97">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="59">
-      <formula>LEN(TRIM(A97))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A98">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="58">
-      <formula>LEN(TRIM(A98))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A100">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="57">
-      <formula>LEN(TRIM(A100))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A101">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="56">
-      <formula>LEN(TRIM(A101))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="49">
-      <formula>LEN(TRIM(A51))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="51">
-      <formula>LEN(TRIM(A50))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A52">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="48">
-      <formula>LEN(TRIM(A52))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55">
-    <cfRule type="notContainsBlanks" dxfId="35" priority="45">
-      <formula>LEN(TRIM(A55))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="47">
-      <formula>LEN(TRIM(A53))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="46">
-      <formula>LEN(TRIM(A54))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A57">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="44">
-      <formula>LEN(TRIM(A57))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A58">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="43">
-      <formula>LEN(TRIM(A58))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59">
-    <cfRule type="notContainsBlanks" dxfId="30" priority="42">
-      <formula>LEN(TRIM(A59))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="41">
-      <formula>LEN(TRIM(A60))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="40">
-      <formula>LEN(TRIM(A61))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="39">
-      <formula>LEN(TRIM(A62))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A63">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="38">
-      <formula>LEN(TRIM(A63))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A64">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="37">
-      <formula>LEN(TRIM(A64))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="36">
-      <formula>LEN(TRIM(A65))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A66">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="35">
-      <formula>LEN(TRIM(A66))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="34">
-      <formula>LEN(TRIM(A67))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A43">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="33">
-      <formula>LEN(TRIM(A43))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="28">
-      <formula>LEN(TRIM(A26))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27:A31">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="27">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="17">
-      <formula>LEN(TRIM(A72))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="20">
-      <formula>LEN(TRIM(A69))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="19">
-      <formula>LEN(TRIM(A70))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="18">
-      <formula>LEN(TRIM(A71))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A73">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="16">
-      <formula>LEN(TRIM(A73))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A74">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="15">
-      <formula>LEN(TRIM(A74))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A75">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="14">
-      <formula>LEN(TRIM(A75))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A76">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="13">
-      <formula>LEN(TRIM(A76))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A77">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="12">
-      <formula>LEN(TRIM(A77))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A78">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="11">
-      <formula>LEN(TRIM(A78))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A79">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="10">
-      <formula>LEN(TRIM(A79))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A84">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="6">
-      <formula>LEN(TRIM(A84))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A81">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="8">
-      <formula>LEN(TRIM(A81))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A82">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="7">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(A82))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A83))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A85))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A87">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(A87))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A86">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(A86))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A88">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A88))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
start rule 5_1 assigned to AssumeBodyPositionStanding_1 as per email with AO 2017-11-02
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -17,6 +17,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -857,7 +858,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Need to change preflabel to match other visit types</t>
+      <t>Preflabel as all uppercase is inconsistent with other later visits that use mixed case. - email to AO 01Nov17
+Incorrect assign of tirples under AssumeBodyPositionStanding - email to AO 01Nov17</t>
     </r>
     <r>
       <rPr>
@@ -1123,7 +1125,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1306,12 +1308,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1529,7 +1525,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1567,11 +1563,10 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1616,7 +1611,7 @@
     <xf numFmtId="49" fontId="32" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="33" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="33" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="32" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1624,7 +1619,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1670,322 +1664,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="129">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="84">
     <dxf>
       <fill>
         <patternFill>
@@ -2886,9 +2565,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2898,8 +2577,8 @@
     <col min="3" max="3" width="29.81640625" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.81640625" style="38" customWidth="1"/>
+    <col min="6" max="6" width="7.7265625" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.81640625" style="37" customWidth="1"/>
     <col min="8" max="8" width="57.1796875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2929,10 +2608,10 @@
       <c r="E3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="37" t="s">
         <v>69</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -2955,10 +2634,10 @@
       <c r="E4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="30">
         <v>0</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="38" t="s">
         <v>77</v>
       </c>
       <c r="H4" s="18"/>
@@ -2979,10 +2658,10 @@
       <c r="E5" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="30">
         <v>0</v>
       </c>
-      <c r="G5" s="39"/>
+      <c r="G5" s="38"/>
       <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -3001,10 +2680,10 @@
       <c r="E6" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="30">
         <v>0</v>
       </c>
-      <c r="G6" s="39"/>
+      <c r="G6" s="38"/>
       <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -3023,10 +2702,10 @@
       <c r="E7" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F7" s="30">
         <v>0</v>
       </c>
-      <c r="G7" s="39"/>
+      <c r="G7" s="38"/>
       <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -3045,10 +2724,10 @@
       <c r="E8" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="30">
         <v>0</v>
       </c>
-      <c r="G8" s="39"/>
+      <c r="G8" s="38"/>
       <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3065,10 +2744,10 @@
       <c r="E9" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="F9" s="31">
+      <c r="F9" s="30">
         <v>1</v>
       </c>
-      <c r="G9" s="39"/>
+      <c r="G9" s="38"/>
       <c r="H9" s="19"/>
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3085,10 +2764,10 @@
       <c r="E10" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="30">
         <v>1</v>
       </c>
-      <c r="G10" s="39"/>
+      <c r="G10" s="38"/>
       <c r="H10" s="19"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -3107,10 +2786,10 @@
       <c r="E11" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="F11" s="31">
+      <c r="F11" s="30">
         <v>0</v>
       </c>
-      <c r="G11" s="39"/>
+      <c r="G11" s="38"/>
       <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -3124,13 +2803,13 @@
       <c r="D12" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="32">
+      <c r="F12" s="31">
         <v>1</v>
       </c>
-      <c r="G12" s="39"/>
+      <c r="G12" s="38"/>
       <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -3144,13 +2823,13 @@
       <c r="D13" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="31">
         <v>1</v>
       </c>
-      <c r="G13" s="39" t="s">
+      <c r="G13" s="38" t="s">
         <v>119</v>
       </c>
       <c r="H13" s="18"/>
@@ -3171,10 +2850,10 @@
       <c r="E14" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="F14" s="31">
+      <c r="F14" s="30">
         <v>0</v>
       </c>
-      <c r="G14" s="39"/>
+      <c r="G14" s="38"/>
       <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -3193,10 +2872,10 @@
       <c r="E15" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="31">
+      <c r="F15" s="30">
         <v>0</v>
       </c>
-      <c r="G15" s="39"/>
+      <c r="G15" s="38"/>
       <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -3213,10 +2892,10 @@
       <c r="E16" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F16" s="31">
+      <c r="F16" s="30">
         <v>1</v>
       </c>
-      <c r="G16" s="39"/>
+      <c r="G16" s="38"/>
       <c r="H16" s="18"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -3233,10 +2912,10 @@
       <c r="E17" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="30">
         <v>1</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="G17" s="38" t="s">
         <v>120</v>
       </c>
       <c r="H17" s="18"/>
@@ -3257,10 +2936,10 @@
       <c r="E18" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="F18" s="31">
+      <c r="F18" s="30">
         <v>0</v>
       </c>
-      <c r="G18" s="39"/>
+      <c r="G18" s="38"/>
       <c r="H18" s="18"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -3279,10 +2958,10 @@
       <c r="E19" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="F19" s="31">
+      <c r="F19" s="30">
         <v>0</v>
       </c>
-      <c r="G19" s="39"/>
+      <c r="G19" s="38"/>
       <c r="H19" s="18"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -3301,10 +2980,10 @@
       <c r="E20" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F20" s="31">
+      <c r="F20" s="30">
         <v>0</v>
       </c>
-      <c r="G20" s="39"/>
+      <c r="G20" s="38"/>
       <c r="H20" s="18"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -3321,10 +3000,10 @@
       <c r="E21" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="F21" s="31">
+      <c r="F21" s="30">
         <v>1</v>
       </c>
-      <c r="G21" s="39"/>
+      <c r="G21" s="38"/>
       <c r="H21" s="18"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -3341,10 +3020,10 @@
       <c r="E22" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F22" s="31">
+      <c r="F22" s="30">
         <v>1</v>
       </c>
-      <c r="G22" s="39"/>
+      <c r="G22" s="38"/>
       <c r="H22" s="18"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -3363,10 +3042,10 @@
       <c r="E23" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="F23" s="31">
+      <c r="F23" s="30">
         <v>0</v>
       </c>
-      <c r="G23" s="39"/>
+      <c r="G23" s="38"/>
       <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -3383,10 +3062,10 @@
       <c r="E24" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="F24" s="31">
+      <c r="F24" s="30">
         <v>1</v>
       </c>
-      <c r="G24" s="39"/>
+      <c r="G24" s="38"/>
       <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -3403,10 +3082,10 @@
       <c r="E25" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F25" s="31">
+      <c r="F25" s="30">
         <v>1</v>
       </c>
-      <c r="G25" s="39"/>
+      <c r="G25" s="38"/>
       <c r="H25" s="19"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -3425,10 +3104,10 @@
       <c r="E26" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="F26" s="31">
+      <c r="F26" s="30">
         <v>0</v>
       </c>
-      <c r="G26" s="39"/>
+      <c r="G26" s="38"/>
       <c r="H26" s="18"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -3447,10 +3126,10 @@
       <c r="E27" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="F27" s="31">
+      <c r="F27" s="30">
         <v>0</v>
       </c>
-      <c r="G27" s="39"/>
+      <c r="G27" s="38"/>
       <c r="H27" s="18"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -3466,13 +3145,13 @@
       <c r="D28" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="F28" s="33">
+      <c r="F28" s="32">
         <v>0</v>
       </c>
-      <c r="G28" s="39"/>
+      <c r="G28" s="38"/>
       <c r="H28" s="18"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -3486,13 +3165,13 @@
       <c r="D29" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="27" t="s">
+      <c r="E29" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="F29" s="33">
+      <c r="F29" s="32">
         <v>0</v>
       </c>
-      <c r="G29" s="39"/>
+      <c r="G29" s="38"/>
       <c r="H29" s="19"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -3504,13 +3183,13 @@
       <c r="D30" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="27" t="s">
+      <c r="E30" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="F30" s="33">
+      <c r="F30" s="32">
         <v>0</v>
       </c>
-      <c r="G30" s="39"/>
+      <c r="G30" s="38"/>
       <c r="H30" s="19"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -3522,13 +3201,13 @@
       <c r="D31" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="27" t="s">
+      <c r="E31" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="F31" s="33">
+      <c r="F31" s="32">
         <v>0</v>
       </c>
-      <c r="G31" s="39"/>
+      <c r="G31" s="38"/>
       <c r="H31" s="19"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -3547,10 +3226,10 @@
       <c r="E32" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F32" s="31">
+      <c r="F32" s="30">
         <v>0</v>
       </c>
-      <c r="G32" s="39"/>
+      <c r="G32" s="38"/>
       <c r="H32" s="18"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -3567,10 +3246,10 @@
       <c r="E33" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="F33" s="31">
+      <c r="F33" s="30">
         <v>1</v>
       </c>
-      <c r="G33" s="39"/>
+      <c r="G33" s="38"/>
       <c r="H33" s="18"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -3589,10 +3268,10 @@
       <c r="E34" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="F34" s="31">
+      <c r="F34" s="30">
         <v>0</v>
       </c>
-      <c r="G34" s="39"/>
+      <c r="G34" s="38"/>
       <c r="H34" s="18"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -3607,10 +3286,10 @@
       <c r="E35" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="F35" s="31">
+      <c r="F35" s="30">
         <v>0</v>
       </c>
-      <c r="G35" s="39"/>
+      <c r="G35" s="38"/>
       <c r="H35" s="18"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -3618,87 +3297,89 @@
       <c r="B36" s="10"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
-      <c r="E36" s="16" t="s">
+      <c r="E36" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="F36" s="31">
+      <c r="F36" s="30">
         <v>1</v>
       </c>
-      <c r="G36" s="39"/>
+      <c r="G36" s="38"/>
       <c r="H36" s="18"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="45"/>
+      <c r="A37" s="44"/>
       <c r="B37" s="10"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
       <c r="E37" s="16"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="39"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="38"/>
       <c r="H37" s="18"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="45"/>
+      <c r="A38" s="44"/>
       <c r="B38" s="10"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
       <c r="E38" s="16"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="39"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="38"/>
       <c r="H38" s="18"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="45"/>
+      <c r="A39" s="44"/>
       <c r="B39" s="10"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
       <c r="E39" s="16"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="39"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="38"/>
       <c r="H39" s="18"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="45"/>
+      <c r="A40" s="44"/>
       <c r="B40" s="10"/>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="16"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="39"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="38"/>
       <c r="H40" s="18"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="45"/>
+      <c r="A41" s="44"/>
       <c r="B41" s="10"/>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
       <c r="E41" s="16"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="39"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="38"/>
       <c r="H41" s="18"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="45"/>
+      <c r="A42" s="44"/>
       <c r="B42" s="10"/>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
       <c r="E42" s="16"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="39"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="38"/>
       <c r="H42" s="18"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="45"/>
+      <c r="A43" s="44"/>
       <c r="B43" s="10"/>
       <c r="C43" s="11"/>
       <c r="D43" s="11"/>
       <c r="E43" s="16"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="39"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="38"/>
       <c r="H43" s="18"/>
     </row>
-    <row r="44" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A44" s="23"/>
+    <row r="44" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="9">
+        <v>43040</v>
+      </c>
       <c r="B44" s="11" t="s">
         <v>71</v>
       </c>
@@ -3708,13 +3389,13 @@
       <c r="D44" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E44" s="46" t="s">
+      <c r="E44" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F44" s="31">
+      <c r="F44" s="30">
         <v>0</v>
       </c>
-      <c r="G44" s="39" t="s">
+      <c r="G44" s="38" t="s">
         <v>139</v>
       </c>
       <c r="H44" s="18"/>
@@ -3735,8 +3416,10 @@
       <c r="E45" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F45" s="31"/>
-      <c r="G45" s="39"/>
+      <c r="F45" s="30">
+        <v>1</v>
+      </c>
+      <c r="G45" s="38"/>
       <c r="H45" s="18"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
@@ -3750,11 +3433,13 @@
       <c r="D46" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E46" s="28" t="s">
+      <c r="E46" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F46" s="34"/>
-      <c r="G46" s="40"/>
+      <c r="F46" s="33">
+        <v>1</v>
+      </c>
+      <c r="G46" s="39"/>
       <c r="H46" s="18"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
@@ -3771,8 +3456,10 @@
       <c r="E47" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F47" s="31"/>
-      <c r="G47" s="40"/>
+      <c r="F47" s="30">
+        <v>2</v>
+      </c>
+      <c r="G47" s="39"/>
       <c r="H47" s="18"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
@@ -3789,8 +3476,10 @@
       <c r="E48" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F48" s="31"/>
-      <c r="G48" s="40"/>
+      <c r="F48" s="30">
+        <v>1</v>
+      </c>
+      <c r="G48" s="39"/>
       <c r="H48" s="18"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
@@ -3809,8 +3498,10 @@
       <c r="E49" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F49" s="31"/>
-      <c r="G49" s="40"/>
+      <c r="F49" s="30">
+        <v>2</v>
+      </c>
+      <c r="G49" s="39"/>
       <c r="H49" s="18"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
@@ -3824,11 +3515,13 @@
       <c r="D50" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E50" s="28" t="s">
+      <c r="E50" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="F50" s="34"/>
-      <c r="G50" s="41"/>
+      <c r="F50" s="33">
+        <v>1</v>
+      </c>
+      <c r="G50" s="40"/>
       <c r="H50" s="18" t="s">
         <v>102</v>
       </c>
@@ -3849,8 +3542,8 @@
       <c r="E51" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F51" s="31"/>
-      <c r="G51" s="40"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="39"/>
       <c r="H51" s="18"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
@@ -3867,8 +3560,8 @@
       <c r="E52" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="F52" s="31"/>
-      <c r="G52" s="40"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="39"/>
       <c r="H52" s="18"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
@@ -3880,11 +3573,13 @@
         <v>61</v>
       </c>
       <c r="D53" s="12"/>
-      <c r="E53" s="28" t="s">
+      <c r="E53" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="F53" s="34"/>
-      <c r="G53" s="41"/>
+      <c r="F53" s="33">
+        <v>1</v>
+      </c>
+      <c r="G53" s="40"/>
       <c r="H53" s="18"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
@@ -3901,8 +3596,8 @@
       <c r="E54" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F54" s="31"/>
-      <c r="G54" s="40"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="39"/>
       <c r="H54" s="18"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
@@ -3917,8 +3612,8 @@
       <c r="E55" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F55" s="31"/>
-      <c r="G55" s="40"/>
+      <c r="F55" s="30"/>
+      <c r="G55" s="39"/>
       <c r="H55" s="18"/>
     </row>
     <row r="56" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -3932,11 +3627,13 @@
       <c r="D56" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E56" s="28" t="s">
+      <c r="E56" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="F56" s="34"/>
-      <c r="G56" s="42" t="s">
+      <c r="F56" s="33">
+        <v>1</v>
+      </c>
+      <c r="G56" s="41" t="s">
         <v>101</v>
       </c>
       <c r="H56" s="18"/>
@@ -3955,8 +3652,8 @@
       <c r="E57" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F57" s="31"/>
-      <c r="G57" s="40"/>
+      <c r="F57" s="30"/>
+      <c r="G57" s="39"/>
       <c r="H57" s="18"/>
     </row>
     <row r="58" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -3971,8 +3668,8 @@
       <c r="E58" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F58" s="31"/>
-      <c r="G58" s="40"/>
+      <c r="F58" s="30"/>
+      <c r="G58" s="39"/>
       <c r="H58" s="18"/>
     </row>
     <row r="59" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -3980,15 +3677,15 @@
       <c r="B59" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C59" s="25" t="s">
+      <c r="C59" s="24" t="s">
         <v>63</v>
       </c>
       <c r="D59" s="12"/>
       <c r="E59" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F59" s="31"/>
-      <c r="G59" s="40"/>
+      <c r="F59" s="30"/>
+      <c r="G59" s="39"/>
       <c r="H59" s="18"/>
     </row>
     <row r="60" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -4005,8 +3702,8 @@
       <c r="E60" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F60" s="31"/>
-      <c r="G60" s="40"/>
+      <c r="F60" s="30"/>
+      <c r="G60" s="39"/>
       <c r="H60" s="18"/>
     </row>
     <row r="61" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -4021,8 +3718,8 @@
       <c r="E61" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="F61" s="31"/>
-      <c r="G61" s="40"/>
+      <c r="F61" s="30"/>
+      <c r="G61" s="39"/>
       <c r="H61" s="18"/>
     </row>
     <row r="62" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -4034,11 +3731,13 @@
         <v>61</v>
       </c>
       <c r="D62" s="12"/>
-      <c r="E62" s="28" t="s">
+      <c r="E62" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="F62" s="34"/>
-      <c r="G62" s="40" t="s">
+      <c r="F62" s="33">
+        <v>1</v>
+      </c>
+      <c r="G62" s="39" t="s">
         <v>101</v>
       </c>
       <c r="H62" s="18"/>
@@ -4057,8 +3756,8 @@
       <c r="E63" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F63" s="31"/>
-      <c r="G63" s="40"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="39"/>
       <c r="H63" s="18"/>
     </row>
     <row r="64" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -4073,8 +3772,8 @@
       <c r="E64" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F64" s="31"/>
-      <c r="G64" s="40"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="39"/>
       <c r="H64" s="18"/>
     </row>
     <row r="65" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -4089,8 +3788,8 @@
       <c r="E65" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F65" s="31"/>
-      <c r="G65" s="40"/>
+      <c r="F65" s="30"/>
+      <c r="G65" s="39"/>
       <c r="H65" s="18"/>
     </row>
     <row r="66" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -4105,8 +3804,8 @@
       <c r="E66" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F66" s="31"/>
-      <c r="G66" s="40"/>
+      <c r="F66" s="30"/>
+      <c r="G66" s="39"/>
       <c r="H66" s="18"/>
     </row>
     <row r="67" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -4119,8 +3818,8 @@
       <c r="E67" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="F67" s="31"/>
-      <c r="G67" s="40"/>
+      <c r="F67" s="30"/>
+      <c r="G67" s="39"/>
       <c r="H67" s="18"/>
     </row>
     <row r="68" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -4132,11 +3831,13 @@
         <v>61</v>
       </c>
       <c r="D68" s="12"/>
-      <c r="E68" s="28" t="s">
+      <c r="E68" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="F68" s="34"/>
-      <c r="G68" s="40" t="s">
+      <c r="F68" s="33">
+        <v>1</v>
+      </c>
+      <c r="G68" s="39" t="s">
         <v>101</v>
       </c>
       <c r="H68" s="18"/>
@@ -4157,8 +3858,8 @@
       <c r="E69" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F69" s="31"/>
-      <c r="G69" s="40"/>
+      <c r="F69" s="30"/>
+      <c r="G69" s="39"/>
       <c r="H69" s="18"/>
     </row>
     <row r="70" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -4171,8 +3872,8 @@
       <c r="E70" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="F70" s="31"/>
-      <c r="G70" s="40"/>
+      <c r="F70" s="30"/>
+      <c r="G70" s="39"/>
       <c r="H70" s="18"/>
     </row>
     <row r="71" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -4187,8 +3888,8 @@
       <c r="E71" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F71" s="31"/>
-      <c r="G71" s="40"/>
+      <c r="F71" s="30"/>
+      <c r="G71" s="39"/>
       <c r="H71" s="18"/>
     </row>
     <row r="72" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -4205,8 +3906,8 @@
       <c r="E72" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F72" s="31"/>
-      <c r="G72" s="40"/>
+      <c r="F72" s="30"/>
+      <c r="G72" s="39"/>
       <c r="H72" s="18"/>
     </row>
     <row r="73" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -4219,8 +3920,8 @@
       <c r="E73" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="F73" s="31"/>
-      <c r="G73" s="40"/>
+      <c r="F73" s="30"/>
+      <c r="G73" s="39"/>
       <c r="H73" s="18"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
@@ -4232,11 +3933,13 @@
         <v>61</v>
       </c>
       <c r="D74" s="12"/>
-      <c r="E74" s="28" t="s">
+      <c r="E74" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="F74" s="34"/>
-      <c r="G74" s="40" t="s">
+      <c r="F74" s="33">
+        <v>1</v>
+      </c>
+      <c r="G74" s="39" t="s">
         <v>95</v>
       </c>
       <c r="H74" s="18"/>
@@ -4255,8 +3958,8 @@
       <c r="E75" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F75" s="31"/>
-      <c r="G75" s="39"/>
+      <c r="F75" s="30"/>
+      <c r="G75" s="38"/>
       <c r="H75" s="18"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.35">
@@ -4271,8 +3974,8 @@
       <c r="E76" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F76" s="31"/>
-      <c r="G76" s="39"/>
+      <c r="F76" s="30"/>
+      <c r="G76" s="38"/>
       <c r="H76" s="18"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.35">
@@ -4287,8 +3990,8 @@
       <c r="E77" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F77" s="31"/>
-      <c r="G77" s="39"/>
+      <c r="F77" s="30"/>
+      <c r="G77" s="38"/>
       <c r="H77" s="18"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.35">
@@ -4305,8 +4008,8 @@
       <c r="E78" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F78" s="31"/>
-      <c r="G78" s="39"/>
+      <c r="F78" s="30"/>
+      <c r="G78" s="38"/>
       <c r="H78" s="18"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
@@ -4321,8 +4024,8 @@
       <c r="E79" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="F79" s="31"/>
-      <c r="G79" s="41"/>
+      <c r="F79" s="30"/>
+      <c r="G79" s="40"/>
       <c r="H79" s="18"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.35">
@@ -4334,11 +4037,13 @@
         <v>61</v>
       </c>
       <c r="D80" s="12"/>
-      <c r="E80" s="28" t="s">
+      <c r="E80" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="F80" s="34"/>
-      <c r="G80" s="40" t="s">
+      <c r="F80" s="33">
+        <v>1</v>
+      </c>
+      <c r="G80" s="39" t="s">
         <v>96</v>
       </c>
       <c r="H80" s="17"/>
@@ -4357,8 +4062,8 @@
       <c r="E81" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F81" s="35"/>
-      <c r="G81" s="41"/>
+      <c r="F81" s="34"/>
+      <c r="G81" s="40"/>
       <c r="H81" s="17"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
@@ -4373,8 +4078,8 @@
       <c r="E82" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F82" s="35"/>
-      <c r="G82" s="41"/>
+      <c r="F82" s="34"/>
+      <c r="G82" s="40"/>
       <c r="H82" s="17"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
@@ -4389,8 +4094,8 @@
       <c r="E83" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F83" s="31"/>
-      <c r="G83" s="40"/>
+      <c r="F83" s="30"/>
+      <c r="G83" s="39"/>
       <c r="H83" s="17"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
@@ -4406,7 +4111,7 @@
       <c r="E84" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F84" s="36"/>
+      <c r="F84" s="35"/>
       <c r="H84" s="7"/>
     </row>
     <row r="85" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4421,8 +4126,8 @@
       <c r="E85" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="F85" s="31"/>
-      <c r="G85" s="41"/>
+      <c r="F85" s="30"/>
+      <c r="G85" s="40"/>
       <c r="H85" s="17"/>
     </row>
     <row r="86" spans="1:9" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
@@ -4433,11 +4138,13 @@
       <c r="C86" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E86" s="28" t="s">
+      <c r="E86" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="F86" s="34"/>
-      <c r="G86" s="40" t="s">
+      <c r="F86" s="33">
+        <v>1</v>
+      </c>
+      <c r="G86" s="39" t="s">
         <v>96</v>
       </c>
       <c r="H86" s="22" t="s">
@@ -4459,8 +4166,8 @@
       <c r="E87" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F87" s="35"/>
-      <c r="G87" s="41"/>
+      <c r="F87" s="34"/>
+      <c r="G87" s="40"/>
       <c r="H87" s="17"/>
     </row>
     <row r="88" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
@@ -4475,8 +4182,8 @@
       <c r="E88" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F88" s="35"/>
-      <c r="G88" s="41"/>
+      <c r="F88" s="34"/>
+      <c r="G88" s="40"/>
       <c r="H88" s="17"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
@@ -4491,8 +4198,8 @@
       <c r="E89" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F89" s="35"/>
-      <c r="G89" s="41"/>
+      <c r="F89" s="34"/>
+      <c r="G89" s="40"/>
       <c r="H89" s="18"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
@@ -4509,8 +4216,8 @@
       <c r="E90" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F90" s="35"/>
-      <c r="G90" s="41"/>
+      <c r="F90" s="34"/>
+      <c r="G90" s="40"/>
       <c r="H90" s="18"/>
     </row>
     <row r="91" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.35">
@@ -4525,8 +4232,8 @@
       <c r="E91" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="F91" s="35"/>
-      <c r="G91" s="41"/>
+      <c r="F91" s="34"/>
+      <c r="G91" s="40"/>
       <c r="H91" s="18"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
@@ -4538,11 +4245,13 @@
         <v>61</v>
       </c>
       <c r="D92" s="10"/>
-      <c r="E92" s="28" t="s">
+      <c r="E92" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="F92" s="34"/>
-      <c r="G92" s="41"/>
+      <c r="F92" s="33">
+        <v>1</v>
+      </c>
+      <c r="G92" s="40"/>
       <c r="H92" s="18"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
@@ -4557,8 +4266,8 @@
       <c r="E93" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F93" s="35"/>
-      <c r="G93" s="41"/>
+      <c r="F93" s="34"/>
+      <c r="G93" s="40"/>
       <c r="H93" s="18"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
@@ -4571,8 +4280,8 @@
       <c r="E94" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F94" s="35"/>
-      <c r="G94" s="41"/>
+      <c r="F94" s="34"/>
+      <c r="G94" s="40"/>
       <c r="H94" s="18"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
@@ -4584,11 +4293,13 @@
         <v>61</v>
       </c>
       <c r="D95" s="10"/>
-      <c r="E95" s="28" t="s">
+      <c r="E95" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="F95" s="34"/>
-      <c r="G95" s="41"/>
+      <c r="F95" s="33">
+        <v>1</v>
+      </c>
+      <c r="G95" s="40"/>
       <c r="H95" s="18"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
@@ -4603,8 +4314,8 @@
       <c r="E96" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F96" s="35"/>
-      <c r="G96" s="41"/>
+      <c r="F96" s="34"/>
+      <c r="G96" s="40"/>
       <c r="H96" s="20"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.35">
@@ -4617,8 +4328,8 @@
       <c r="E97" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F97" s="35"/>
-      <c r="G97" s="41"/>
+      <c r="F97" s="34"/>
+      <c r="G97" s="40"/>
       <c r="H97" s="20"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.35">
@@ -4631,8 +4342,8 @@
       <c r="E98" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F98" s="35"/>
-      <c r="G98" s="41"/>
+      <c r="F98" s="34"/>
+      <c r="G98" s="40"/>
       <c r="H98" s="20"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.35">
@@ -4647,8 +4358,8 @@
       <c r="E99" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F99" s="35"/>
-      <c r="G99" s="41"/>
+      <c r="F99" s="34"/>
+      <c r="G99" s="40"/>
       <c r="H99" s="20"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.35">
@@ -4663,8 +4374,8 @@
       <c r="E100" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F100" s="35"/>
-      <c r="G100" s="41"/>
+      <c r="F100" s="34"/>
+      <c r="G100" s="40"/>
       <c r="H100" s="20"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.35">
@@ -4676,11 +4387,13 @@
         <v>61</v>
       </c>
       <c r="D101" s="10"/>
-      <c r="E101" s="28" t="s">
+      <c r="E101" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="F101" s="34"/>
-      <c r="G101" s="41"/>
+      <c r="F101" s="33">
+        <v>1</v>
+      </c>
+      <c r="G101" s="40"/>
       <c r="H101" s="18"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.35">
@@ -4695,8 +4408,8 @@
       <c r="E102" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F102" s="35"/>
-      <c r="G102" s="39"/>
+      <c r="F102" s="34"/>
+      <c r="G102" s="38"/>
       <c r="H102" s="20"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.35">
@@ -4709,8 +4422,8 @@
       <c r="E103" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F103" s="35"/>
-      <c r="G103" s="39"/>
+      <c r="F103" s="34"/>
+      <c r="G103" s="38"/>
       <c r="H103" s="20"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.35">
@@ -4721,8 +4434,8 @@
       <c r="E104" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F104" s="35"/>
-      <c r="G104" s="39"/>
+      <c r="F104" s="34"/>
+      <c r="G104" s="38"/>
       <c r="H104" s="20"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.35">
@@ -4737,8 +4450,8 @@
       <c r="E105" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F105" s="35"/>
-      <c r="G105" s="39"/>
+      <c r="F105" s="34"/>
+      <c r="G105" s="38"/>
       <c r="H105" s="20"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.35">
@@ -4751,8 +4464,8 @@
       <c r="E106" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F106" s="35"/>
-      <c r="G106" s="41"/>
+      <c r="F106" s="34"/>
+      <c r="G106" s="40"/>
       <c r="H106" s="20"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.35">
@@ -4764,11 +4477,13 @@
         <v>61</v>
       </c>
       <c r="D107" s="11"/>
-      <c r="E107" s="28" t="s">
+      <c r="E107" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="F107" s="34"/>
-      <c r="G107" s="41"/>
+      <c r="F107" s="33">
+        <v>1</v>
+      </c>
+      <c r="G107" s="40"/>
       <c r="H107" s="18"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.35">
@@ -4782,8 +4497,8 @@
       <c r="E108" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F108" s="35"/>
-      <c r="G108" s="39"/>
+      <c r="F108" s="34"/>
+      <c r="G108" s="38"/>
       <c r="H108" s="18"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.35">
@@ -4796,8 +4511,8 @@
       <c r="E109" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F109" s="35"/>
-      <c r="G109" s="39"/>
+      <c r="F109" s="34"/>
+      <c r="G109" s="38"/>
       <c r="H109" s="18"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.35">
@@ -4808,8 +4523,8 @@
       <c r="E110" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F110" s="35"/>
-      <c r="G110" s="39"/>
+      <c r="F110" s="34"/>
+      <c r="G110" s="38"/>
       <c r="H110" s="18"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.35">
@@ -4824,8 +4539,8 @@
       <c r="E111" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F111" s="35"/>
-      <c r="G111" s="39"/>
+      <c r="F111" s="34"/>
+      <c r="G111" s="38"/>
       <c r="H111" s="18"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.35">
@@ -4838,8 +4553,8 @@
       <c r="E112" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F112" s="35"/>
-      <c r="G112" s="39"/>
+      <c r="F112" s="34"/>
+      <c r="G112" s="38"/>
       <c r="H112" s="18"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.35">
@@ -4849,13 +4564,13 @@
       </c>
       <c r="C113" s="11"/>
       <c r="D113" s="12"/>
-      <c r="E113" s="24" t="s">
+      <c r="E113" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="F113" s="35">
+      <c r="F113" s="34">
         <v>0</v>
       </c>
-      <c r="G113" s="39" t="s">
+      <c r="G113" s="38" t="s">
         <v>112</v>
       </c>
       <c r="H113" s="18"/>
@@ -4867,13 +4582,13 @@
       </c>
       <c r="C114" s="11"/>
       <c r="D114" s="11"/>
-      <c r="E114" s="24" t="s">
+      <c r="E114" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="F114" s="35">
+      <c r="F114" s="34">
         <v>0</v>
       </c>
-      <c r="G114" s="39" t="s">
+      <c r="G114" s="38" t="s">
         <v>112</v>
       </c>
       <c r="H114" s="18"/>
@@ -4883,21 +4598,21 @@
         <f>ROUND(COUNTA(A4:A114)/ROWS(A4:A114)*100,0)</f>
         <v>50</v>
       </c>
-      <c r="B115" s="44" t="s">
+      <c r="B115" s="43" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="9"/>
-      <c r="G116" s="41"/>
+      <c r="G116" s="40"/>
       <c r="H116" s="18"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
       <c r="E117" s="5"/>
-      <c r="F117" s="37"/>
-      <c r="G117" s="43"/>
+      <c r="F117" s="36"/>
+      <c r="G117" s="42"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
@@ -4906,8 +4621,8 @@
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
       <c r="E118" s="5"/>
-      <c r="F118" s="37"/>
-      <c r="G118" s="43"/>
+      <c r="F118" s="36"/>
+      <c r="G118" s="42"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
@@ -4919,467 +4634,467 @@
       <c r="E119" t="s">
         <v>108</v>
       </c>
-      <c r="G119" s="43"/>
+      <c r="G119" s="42"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G120" s="43"/>
+      <c r="G120" s="42"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C121" s="5"/>
       <c r="D121" s="5"/>
       <c r="E121" s="5"/>
-      <c r="F121" s="37"/>
-      <c r="G121" s="43"/>
+      <c r="F121" s="36"/>
+      <c r="G121" s="42"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C122" s="5"/>
       <c r="D122" s="5"/>
       <c r="E122" s="5"/>
-      <c r="F122" s="37"/>
-      <c r="G122" s="43"/>
+      <c r="F122" s="36"/>
+      <c r="G122" s="42"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C123" s="5"/>
       <c r="D123" s="5"/>
       <c r="E123" s="5"/>
-      <c r="F123" s="37"/>
-      <c r="G123" s="43"/>
+      <c r="F123" s="36"/>
+      <c r="G123" s="42"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C124" s="5"/>
       <c r="D124" s="5"/>
       <c r="E124" s="5"/>
-      <c r="F124" s="37"/>
-      <c r="G124" s="43"/>
+      <c r="F124" s="36"/>
+      <c r="G124" s="42"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C125" s="5"/>
       <c r="D125" s="5"/>
       <c r="E125" s="5"/>
-      <c r="F125" s="37"/>
-      <c r="G125" s="43"/>
+      <c r="F125" s="36"/>
+      <c r="G125" s="42"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C126" s="5"/>
       <c r="D126" s="5"/>
       <c r="E126" s="5"/>
-      <c r="F126" s="37"/>
-      <c r="G126" s="43"/>
+      <c r="F126" s="36"/>
+      <c r="G126" s="42"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A116">
-    <cfRule type="notContainsBlanks" dxfId="126" priority="204">
+    <cfRule type="notContainsBlanks" dxfId="83" priority="205">
       <formula>LEN(TRIM(A116))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70">
-    <cfRule type="notContainsBlanks" dxfId="124" priority="81">
+    <cfRule type="notContainsBlanks" dxfId="82" priority="82">
       <formula>LEN(TRIM(A70))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62">
-    <cfRule type="notContainsBlanks" dxfId="122" priority="83">
+    <cfRule type="notContainsBlanks" dxfId="81" priority="84">
       <formula>LEN(TRIM(A62))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="notContainsBlanks" dxfId="116" priority="143">
+    <cfRule type="notContainsBlanks" dxfId="80" priority="144">
       <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48">
-    <cfRule type="notContainsBlanks" dxfId="102" priority="94">
+    <cfRule type="notContainsBlanks" dxfId="79" priority="95">
       <formula>LEN(TRIM(A48))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55">
-    <cfRule type="notContainsBlanks" dxfId="101" priority="90">
+    <cfRule type="notContainsBlanks" dxfId="78" priority="91">
       <formula>LEN(TRIM(A55))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64">
-    <cfRule type="notContainsBlanks" dxfId="100" priority="84">
+    <cfRule type="notContainsBlanks" dxfId="77" priority="85">
       <formula>LEN(TRIM(A64))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67">
-    <cfRule type="notContainsBlanks" dxfId="99" priority="82">
+    <cfRule type="notContainsBlanks" dxfId="76" priority="83">
       <formula>LEN(TRIM(A67))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="notContainsBlanks" dxfId="92" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="19">
       <formula>LEN(TRIM(A45))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="notContainsBlanks" dxfId="91" priority="95">
+    <cfRule type="notContainsBlanks" dxfId="74" priority="96">
       <formula>LEN(TRIM(A46))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="notContainsBlanks" dxfId="90" priority="39">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="40">
       <formula>LEN(TRIM(A20))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50">
-    <cfRule type="notContainsBlanks" dxfId="89" priority="93">
+    <cfRule type="notContainsBlanks" dxfId="72" priority="94">
       <formula>LEN(TRIM(A50))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
-    <cfRule type="notContainsBlanks" dxfId="88" priority="92">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="93">
       <formula>LEN(TRIM(A52))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="notContainsBlanks" dxfId="87" priority="91">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="92">
       <formula>LEN(TRIM(A53))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56">
-    <cfRule type="notContainsBlanks" dxfId="85" priority="89">
+    <cfRule type="notContainsBlanks" dxfId="69" priority="90">
       <formula>LEN(TRIM(A56))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="notContainsBlanks" dxfId="84" priority="88">
+    <cfRule type="notContainsBlanks" dxfId="68" priority="89">
       <formula>LEN(TRIM(A58))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59">
-    <cfRule type="notContainsBlanks" dxfId="83" priority="87">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="88">
       <formula>LEN(TRIM(A59))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61">
-    <cfRule type="notContainsBlanks" dxfId="82" priority="86">
+    <cfRule type="notContainsBlanks" dxfId="66" priority="87">
       <formula>LEN(TRIM(A61))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="notContainsBlanks" dxfId="81" priority="85">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="86">
       <formula>LEN(TRIM(A65))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68">
-    <cfRule type="notContainsBlanks" dxfId="76" priority="80">
+    <cfRule type="notContainsBlanks" dxfId="64" priority="81">
       <formula>LEN(TRIM(A68))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71">
-    <cfRule type="notContainsBlanks" dxfId="75" priority="79">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="80">
       <formula>LEN(TRIM(A71))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A73">
-    <cfRule type="notContainsBlanks" dxfId="74" priority="78">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="79">
       <formula>LEN(TRIM(A73))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74">
-    <cfRule type="notContainsBlanks" dxfId="73" priority="77">
+    <cfRule type="notContainsBlanks" dxfId="61" priority="78">
       <formula>LEN(TRIM(A74))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77">
-    <cfRule type="notContainsBlanks" dxfId="72" priority="76">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="77">
       <formula>LEN(TRIM(A77))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A76">
-    <cfRule type="notContainsBlanks" dxfId="71" priority="75">
+    <cfRule type="notContainsBlanks" dxfId="59" priority="76">
       <formula>LEN(TRIM(A76))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A79">
-    <cfRule type="notContainsBlanks" dxfId="70" priority="74">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="75">
       <formula>LEN(TRIM(A79))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A80">
-    <cfRule type="notContainsBlanks" dxfId="69" priority="73">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="74">
       <formula>LEN(TRIM(A80))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82">
-    <cfRule type="notContainsBlanks" dxfId="68" priority="72">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="73">
       <formula>LEN(TRIM(A82))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83">
-    <cfRule type="notContainsBlanks" dxfId="67" priority="71">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="72">
       <formula>LEN(TRIM(A83))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85">
-    <cfRule type="notContainsBlanks" dxfId="66" priority="70">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="71">
       <formula>LEN(TRIM(A85))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86">
-    <cfRule type="notContainsBlanks" dxfId="65" priority="69">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="70">
       <formula>LEN(TRIM(A86))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="notContainsBlanks" dxfId="64" priority="68">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="69">
       <formula>LEN(TRIM(A88))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89">
-    <cfRule type="notContainsBlanks" dxfId="63" priority="67">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="68">
       <formula>LEN(TRIM(A89))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91">
-    <cfRule type="notContainsBlanks" dxfId="62" priority="66">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="67">
       <formula>LEN(TRIM(A91))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="notContainsBlanks" dxfId="61" priority="36">
+    <cfRule type="notContainsBlanks" dxfId="49" priority="37">
       <formula>LEN(TRIM(A34))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92">
-    <cfRule type="notContainsBlanks" dxfId="60" priority="64">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="65">
       <formula>LEN(TRIM(A92))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94">
-    <cfRule type="notContainsBlanks" dxfId="59" priority="63">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="64">
       <formula>LEN(TRIM(A94))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95">
-    <cfRule type="notContainsBlanks" dxfId="58" priority="62">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="63">
       <formula>LEN(TRIM(A95))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97:A98">
-    <cfRule type="notContainsBlanks" dxfId="57" priority="61">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="62">
       <formula>LEN(TRIM(A97))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63">
-    <cfRule type="notContainsBlanks" dxfId="56" priority="26">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="27">
       <formula>LEN(TRIM(A63))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66">
-    <cfRule type="notContainsBlanks" dxfId="55" priority="25">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="26">
       <formula>LEN(TRIM(A66))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="notContainsBlanks" dxfId="54" priority="24">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="25">
       <formula>LEN(TRIM(A69))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72">
-    <cfRule type="notContainsBlanks" dxfId="53" priority="23">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="24">
       <formula>LEN(TRIM(A72))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A75">
-    <cfRule type="notContainsBlanks" dxfId="52" priority="22">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="23">
       <formula>LEN(TRIM(A75))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78">
-    <cfRule type="notContainsBlanks" dxfId="51" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="22">
       <formula>LEN(TRIM(A78))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81">
-    <cfRule type="notContainsBlanks" dxfId="50" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="21">
       <formula>LEN(TRIM(A81))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="notContainsBlanks" dxfId="49" priority="19">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="20">
       <formula>LEN(TRIM(A84))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:A19">
-    <cfRule type="notContainsBlanks" dxfId="48" priority="40">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="41">
       <formula>LEN(TRIM(A18))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:A43">
-    <cfRule type="notContainsBlanks" dxfId="47" priority="48">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="49">
       <formula>LEN(TRIM(A35))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="notContainsBlanks" dxfId="46" priority="47">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="48">
       <formula>LEN(TRIM(A7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="notContainsBlanks" dxfId="45" priority="46">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="47">
       <formula>LEN(TRIM(A6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="notContainsBlanks" dxfId="44" priority="45">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="46">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="notContainsBlanks" dxfId="43" priority="44">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="45">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="43">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="44">
       <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="42">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="43">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="41">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="42">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="38">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="39">
       <formula>LEN(TRIM(A23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:A31">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="37">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="38">
       <formula>LEN(TRIM(A26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A100:A114">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="35">
+      <formula>LEN(TRIM(A100))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="34">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="33">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A99">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="32">
+      <formula>LEN(TRIM(A99))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A96">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="31">
+      <formula>LEN(TRIM(A96))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A93">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="30">
+      <formula>LEN(TRIM(A93))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="29">
+      <formula>LEN(TRIM(A90))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="28">
+      <formula>LEN(TRIM(A87))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="18">
+      <formula>LEN(TRIM(A47))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="17">
+      <formula>LEN(TRIM(A49))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="16">
+      <formula>LEN(TRIM(A51))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="15">
+      <formula>LEN(TRIM(A54))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="14">
+      <formula>LEN(TRIM(A57))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="13">
+      <formula>LEN(TRIM(A60))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="12">
+      <formula>LEN(TRIM(A12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="11">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="10">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="6">
+      <formula>LEN(TRIM(A24))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="8">
+      <formula>LEN(TRIM(A22))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="7">
+      <formula>LEN(TRIM(A21))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(A25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(A33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A44">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="35">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A44))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A100:A114">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="34">
-      <formula>LEN(TRIM(A100))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="33">
-      <formula>LEN(TRIM(A9))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="32">
-      <formula>LEN(TRIM(A10))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A99">
-    <cfRule type="notContainsBlanks" dxfId="30" priority="31">
-      <formula>LEN(TRIM(A99))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A96">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="30">
-      <formula>LEN(TRIM(A96))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A93">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="29">
-      <formula>LEN(TRIM(A93))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A90">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="28">
-      <formula>LEN(TRIM(A90))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A87">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="27">
-      <formula>LEN(TRIM(A87))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="17">
-      <formula>LEN(TRIM(A47))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A49">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="16">
-      <formula>LEN(TRIM(A49))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
-      <formula>LEN(TRIM(A51))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
-      <formula>LEN(TRIM(A54))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A57">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
-      <formula>LEN(TRIM(A57))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
-      <formula>LEN(TRIM(A60))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
-      <formula>LEN(TRIM(A12))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
-      <formula>LEN(TRIM(A13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
-      <formula>LEN(TRIM(A16))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="5">
-      <formula>LEN(TRIM(A24))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
-      <formula>LEN(TRIM(A22))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(A21))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(A17))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(A32))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Match on child triples for cdiscpilot01:VisitBaseline_1
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -17,12 +17,11 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="151">
   <si>
     <t>cdiscpilot01:Person_1</t>
   </si>
@@ -178,9 +177,6 @@
   </si>
   <si>
     <t>SUPPDM</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Date_20</t>
   </si>
   <si>
     <t>CHILD</t>
@@ -462,9 +458,6 @@
     </r>
   </si>
   <si>
-    <t>cdiscpilot01:Date_29/31</t>
-  </si>
-  <si>
     <t>"2014-07-02"</t>
   </si>
   <si>
@@ -872,6 +865,185 @@
       <t xml:space="preserve">
 subtriples are off in numbering by 1 due to inclusion of additional data. Ontology _1, is R _2. Need to look at sort during creation of the subtriples</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cdiscpilot01</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:VisitScreening1_1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cdiscpilot01</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:VisitWk2_1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cdiscpilot01:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>VisitWk24_1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cdiscpilot01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:Date_19/23</t>
+    </r>
+  </si>
+  <si>
+    <t>cdiscpilot01:Date_20/24</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Date_29/39</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cdiscpilot01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:DrugAdministration_1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cdiscpilot01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:DrugAdministration_2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cdiscpilot01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:DrugAdministration_3</t>
+    </r>
+  </si>
+  <si>
+    <t>EX?</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:FixedDoseInterval_1</t>
+  </si>
+  <si>
+    <t>looks good</t>
+  </si>
+  <si>
+    <t>looks crap</t>
   </si>
 </sst>
 </file>
@@ -1125,7 +1297,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1329,6 +1501,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -1525,7 +1709,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1619,6 +1803,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1664,7 +1851,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="85">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2563,11 +2757,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I126"/>
+  <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2584,20 +2778,20 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -2609,10 +2803,10 @@
         <v>26</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G3" s="37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>27</v>
@@ -2620,10 +2814,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>0</v>
@@ -2638,25 +2832,25 @@
         <v>0</v>
       </c>
       <c r="G4" s="38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5" s="30">
         <v>0</v>
@@ -2666,10 +2860,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>0</v>
@@ -2678,7 +2872,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F6" s="30">
         <v>0</v>
@@ -2688,10 +2882,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>0</v>
@@ -2700,7 +2894,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" s="30">
         <v>0</v>
@@ -2710,10 +2904,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>0</v>
@@ -2722,7 +2916,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F8" s="30">
         <v>0</v>
@@ -2732,17 +2926,17 @@
     </row>
     <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F9" s="30">
         <v>1</v>
@@ -2752,17 +2946,17 @@
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="F10" s="30">
         <v>1</v>
@@ -2772,10 +2966,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>0</v>
@@ -2784,7 +2978,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F11" s="30">
         <v>0</v>
@@ -2793,18 +2987,16 @@
       <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="9">
-        <v>43040</v>
-      </c>
+      <c r="A12" s="45"/>
       <c r="B12" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="F12" s="31">
         <v>1</v>
@@ -2813,33 +3005,31 @@
       <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="9">
-        <v>43040</v>
-      </c>
+      <c r="A13" s="45"/>
       <c r="B13" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="F13" s="31">
         <v>1</v>
       </c>
       <c r="G13" s="38" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>0</v>
@@ -2848,7 +3038,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F14" s="30">
         <v>0</v>
@@ -2858,10 +3048,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>0</v>
@@ -2870,7 +3060,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F15" s="30">
         <v>0</v>
@@ -2879,18 +3069,16 @@
       <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="9">
-        <v>43040</v>
-      </c>
+      <c r="A16" s="45"/>
       <c r="B16" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F16" s="30">
         <v>1</v>
@@ -2899,33 +3087,31 @@
       <c r="H16" s="18"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="9">
-        <v>43040</v>
-      </c>
+      <c r="A17" s="45"/>
       <c r="B17" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F17" s="30">
         <v>1</v>
       </c>
       <c r="G17" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>0</v>
@@ -2934,7 +3120,7 @@
         <v>11</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F18" s="30">
         <v>0</v>
@@ -2944,10 +3130,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>0</v>
@@ -2956,7 +3142,7 @@
         <v>12</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F19" s="30">
         <v>0</v>
@@ -2966,10 +3152,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>0</v>
@@ -2978,7 +3164,7 @@
         <v>13</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F20" s="30">
         <v>0</v>
@@ -2988,17 +3174,17 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F21" s="30">
         <v>1</v>
@@ -3008,17 +3194,17 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F22" s="30">
         <v>1</v>
@@ -3028,10 +3214,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>0</v>
@@ -3040,7 +3226,7 @@
         <v>13</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F23" s="30">
         <v>0</v>
@@ -3050,17 +3236,17 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F24" s="30">
         <v>1</v>
@@ -3070,17 +3256,17 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F25" s="30">
         <v>1</v>
@@ -3090,7 +3276,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>51</v>
@@ -3102,7 +3288,7 @@
         <v>13</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F26" s="30">
         <v>0</v>
@@ -3112,7 +3298,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>51</v>
@@ -3124,7 +3310,7 @@
         <v>13</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F27" s="30">
         <v>0</v>
@@ -3134,7 +3320,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>51</v>
@@ -3146,7 +3332,7 @@
         <v>13</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F28" s="32">
         <v>0</v>
@@ -3156,7 +3342,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="14" t="s">
@@ -3166,7 +3352,7 @@
         <v>13</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F29" s="32">
         <v>0</v>
@@ -3176,7 +3362,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="11"/>
@@ -3184,7 +3370,7 @@
         <v>13</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F30" s="32">
         <v>0</v>
@@ -3194,7 +3380,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="11"/>
@@ -3202,7 +3388,7 @@
         <v>13</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F31" s="32">
         <v>0</v>
@@ -3212,10 +3398,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>0</v>
@@ -3224,7 +3410,7 @@
         <v>13</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F32" s="30">
         <v>0</v>
@@ -3234,17 +3420,17 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="9">
-        <v>43040</v>
+        <v>43045</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F33" s="30">
         <v>1</v>
@@ -3253,136 +3439,170 @@
       <c r="H33" s="18"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="9">
-        <v>43040</v>
-      </c>
+      <c r="A34" s="9"/>
       <c r="B34" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>138</v>
+        <v>147</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>144</v>
       </c>
       <c r="F34" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="38"/>
       <c r="H34" s="18"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="21"/>
+      <c r="A35" s="9"/>
       <c r="B35" s="10"/>
-      <c r="C35" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>109</v>
+      <c r="C35" s="11"/>
+      <c r="D35" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="47" t="s">
+        <v>108</v>
       </c>
       <c r="F35" s="30">
-        <v>0</v>
-      </c>
-      <c r="G35" s="38"/>
+        <v>2</v>
+      </c>
+      <c r="G35" s="37" t="s">
+        <v>150</v>
+      </c>
       <c r="H35" s="18"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="21"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="10"/>
       <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="F36" s="30">
-        <v>1</v>
-      </c>
-      <c r="G36" s="38"/>
+      <c r="D36" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="F36" s="30"/>
+      <c r="G36" s="38" t="s">
+        <v>149</v>
+      </c>
       <c r="H36" s="18"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="44"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="10"/>
       <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="16"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="11"/>
       <c r="F37" s="30"/>
       <c r="G37" s="38"/>
       <c r="H37" s="18"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="44"/>
-      <c r="B38" s="10"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="10" t="s">
+        <v>147</v>
+      </c>
       <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="30"/>
+      <c r="D38" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="F38" s="30">
+        <v>1</v>
+      </c>
       <c r="G38" s="38"/>
       <c r="H38" s="18"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="44"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="10"/>
       <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="30"/>
+      <c r="D39" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="F39" s="30">
+        <v>2</v>
+      </c>
       <c r="G39" s="38"/>
       <c r="H39" s="18"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="44"/>
-      <c r="B40" s="10"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="10" t="s">
+        <v>147</v>
+      </c>
       <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="30"/>
+      <c r="D40" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F40" s="30">
+        <v>1</v>
+      </c>
       <c r="G40" s="38"/>
       <c r="H40" s="18"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="44"/>
+      <c r="A41" s="9"/>
       <c r="B41" s="10"/>
       <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="16"/>
+      <c r="D41" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E41" s="46" t="s">
+        <v>110</v>
+      </c>
       <c r="F41" s="30"/>
       <c r="G41" s="38"/>
       <c r="H41" s="18"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="44"/>
+      <c r="A42" s="9"/>
       <c r="B42" s="10"/>
       <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="16"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="11"/>
       <c r="F42" s="30"/>
       <c r="G42" s="38"/>
       <c r="H42" s="18"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="44"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="30"/>
+      <c r="A43" s="9">
+        <v>43045</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="F43" s="30">
+        <v>0</v>
+      </c>
       <c r="G43" s="38"/>
       <c r="H43" s="18"/>
     </row>
-    <row r="44" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="9">
-        <v>43040</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>71</v>
-      </c>
+        <v>43045</v>
+      </c>
+      <c r="B44" s="10"/>
       <c r="C44" s="11" t="s">
         <v>0</v>
       </c>
@@ -3390,31 +3610,21 @@
         <v>13</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="F44" s="30">
         <v>0</v>
       </c>
-      <c r="G44" s="38" t="s">
-        <v>139</v>
-      </c>
+      <c r="G44" s="38"/>
       <c r="H44" s="18"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" s="9">
-        <v>43040</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>116</v>
+      <c r="A45" s="21"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="27" t="s">
+        <v>135</v>
       </c>
       <c r="F45" s="30">
         <v>1</v>
@@ -3423,354 +3633,300 @@
       <c r="H45" s="18"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46" s="21"/>
-      <c r="B46" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E46" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="F46" s="33">
+      <c r="A46" s="44"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="18"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" s="44"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="18"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" s="44"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="18"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="44"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="38"/>
+      <c r="H49" s="18"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" s="44"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="18"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" s="44"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="38"/>
+      <c r="H51" s="18"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" s="44"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="38"/>
+      <c r="H52" s="18"/>
+    </row>
+    <row r="53" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="9">
+        <v>43045</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="F53" s="30">
+        <v>0</v>
+      </c>
+      <c r="G53" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="H53" s="18"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" s="9"/>
+      <c r="B54" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F54" s="30">
         <v>1</v>
       </c>
-      <c r="G46" s="39"/>
-      <c r="H46" s="18"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A47" s="9">
-        <v>43040</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F47" s="30">
-        <v>2</v>
-      </c>
-      <c r="G47" s="39"/>
-      <c r="H47" s="18"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" s="9"/>
-      <c r="B48" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="F48" s="30">
+      <c r="G54" s="38"/>
+      <c r="H54" s="18"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" s="21"/>
+      <c r="B55" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E55" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="F55" s="33">
         <v>1</v>
       </c>
-      <c r="G48" s="39"/>
-      <c r="H48" s="18"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A49" s="9">
-        <v>43040</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F49" s="30">
-        <v>2</v>
-      </c>
-      <c r="G49" s="39"/>
-      <c r="H49" s="18"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A50" s="9"/>
-      <c r="B50" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E50" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="F50" s="33">
-        <v>1</v>
-      </c>
-      <c r="G50" s="40"/>
-      <c r="H50" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A51" s="9">
-        <v>43040</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F51" s="30"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="18"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A52" s="9"/>
-      <c r="B52" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="F52" s="30"/>
-      <c r="G52" s="39"/>
-      <c r="H52" s="18"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A53" s="9"/>
-      <c r="B53" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D53" s="12"/>
-      <c r="E53" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="F53" s="33">
-        <v>1</v>
-      </c>
-      <c r="G53" s="40"/>
-      <c r="H53" s="18"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A54" s="9">
-        <v>43040</v>
-      </c>
-      <c r="B54" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D54" s="12"/>
-      <c r="E54" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F54" s="30"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="18"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A55" s="9"/>
-      <c r="B55" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D55" s="12"/>
-      <c r="E55" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F55" s="30"/>
       <c r="G55" s="39"/>
       <c r="H55" s="18"/>
     </row>
-    <row r="56" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="9"/>
-      <c r="B56" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C56" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E56" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="F56" s="33">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" s="45"/>
+      <c r="B56" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="11"/>
+      <c r="D56" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F56" s="30">
+        <v>2</v>
+      </c>
+      <c r="G56" s="39"/>
+      <c r="H56" s="18"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" s="9"/>
+      <c r="B57" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F57" s="30">
         <v>1</v>
       </c>
-      <c r="G56" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="H56" s="18"/>
-    </row>
-    <row r="57" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="9">
-        <v>43040</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D57" s="12"/>
-      <c r="E57" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F57" s="30"/>
       <c r="G57" s="39"/>
       <c r="H57" s="18"/>
     </row>
-    <row r="58" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="9"/>
-      <c r="B58" s="10" t="s">
-        <v>71</v>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" s="45"/>
+      <c r="B58" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D58" s="12"/>
+        <v>60</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="E58" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="F58" s="30"/>
+        <v>115</v>
+      </c>
+      <c r="F58" s="30">
+        <v>2</v>
+      </c>
       <c r="G58" s="39"/>
       <c r="H58" s="18"/>
     </row>
-    <row r="59" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="9"/>
-      <c r="B59" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C59" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="D59" s="12"/>
-      <c r="E59" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F59" s="30"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="18"/>
-    </row>
-    <row r="60" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="9">
-        <v>43040</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>71</v>
+      <c r="B59" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E59" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="F59" s="33">
+        <v>1</v>
+      </c>
+      <c r="G59" s="40"/>
+      <c r="H59" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60" s="45"/>
+      <c r="B60" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D60" s="12"/>
+        <v>60</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="E60" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F60" s="30"/>
       <c r="G60" s="39"/>
       <c r="H60" s="18"/>
     </row>
-    <row r="61" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="9"/>
-      <c r="B61" s="10" t="s">
-        <v>71</v>
+      <c r="B61" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D61" s="12"/>
+        <v>60</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="E61" s="11" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F61" s="30"/>
       <c r="G61" s="39"/>
       <c r="H61" s="18"/>
     </row>
-    <row r="62" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="9"/>
-      <c r="B62" s="10" t="s">
-        <v>71</v>
+      <c r="B62" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D62" s="12"/>
       <c r="E62" s="27" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F62" s="33">
         <v>1</v>
       </c>
-      <c r="G62" s="39" t="s">
-        <v>101</v>
-      </c>
+      <c r="G62" s="40"/>
       <c r="H62" s="18"/>
     </row>
-    <row r="63" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="9">
-        <v>43040</v>
-      </c>
-      <c r="B63" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C63" s="14" t="s">
-        <v>74</v>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" s="45"/>
+      <c r="B63" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="D63" s="12"/>
       <c r="E63" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F63" s="30"/>
       <c r="G63" s="39"/>
       <c r="H63" s="18"/>
     </row>
-    <row r="64" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="9"/>
       <c r="B64" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C64" s="14" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="D64" s="12"/>
       <c r="E64" s="11" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="F64" s="30"/>
       <c r="G64" s="39"/>
@@ -3779,30 +3935,36 @@
     <row r="65" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="9"/>
       <c r="B65" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C65" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D65" s="12"/>
-      <c r="E65" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F65" s="30"/>
-      <c r="G65" s="39"/>
+        <v>70</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E65" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F65" s="33">
+        <v>1</v>
+      </c>
+      <c r="G65" s="41" t="s">
+        <v>100</v>
+      </c>
       <c r="H65" s="18"/>
     </row>
     <row r="66" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="9">
-        <v>43040</v>
-      </c>
+      <c r="A66" s="45"/>
       <c r="B66" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C66" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>60</v>
+      </c>
       <c r="D66" s="12"/>
       <c r="E66" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F66" s="30"/>
       <c r="G66" s="39"/>
@@ -3811,12 +3973,14 @@
     <row r="67" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="9"/>
       <c r="B67" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C67" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>60</v>
+      </c>
       <c r="D67" s="12"/>
       <c r="E67" s="11" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="F67" s="30"/>
       <c r="G67" s="39"/>
@@ -3825,38 +3989,30 @@
     <row r="68" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="9"/>
       <c r="B68" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C68" s="13" t="s">
-        <v>61</v>
+        <v>70</v>
+      </c>
+      <c r="C68" s="24" t="s">
+        <v>62</v>
       </c>
       <c r="D68" s="12"/>
-      <c r="E68" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="F68" s="33">
-        <v>1</v>
-      </c>
-      <c r="G68" s="39" t="s">
-        <v>101</v>
-      </c>
+      <c r="E68" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F68" s="30"/>
+      <c r="G68" s="39"/>
       <c r="H68" s="18"/>
     </row>
     <row r="69" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="9">
-        <v>43040</v>
-      </c>
+      <c r="A69" s="45"/>
       <c r="B69" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C69" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D69" s="12" t="s">
-        <v>53</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D69" s="12"/>
       <c r="E69" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F69" s="30"/>
       <c r="G69" s="39"/>
@@ -3865,12 +4021,14 @@
     <row r="70" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="9"/>
       <c r="B70" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C70" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>60</v>
+      </c>
       <c r="D70" s="12"/>
       <c r="E70" s="11" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="F70" s="30"/>
       <c r="G70" s="39"/>
@@ -3879,32 +4037,34 @@
     <row r="71" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="9"/>
       <c r="B71" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E71" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F71" s="30"/>
-      <c r="G71" s="39"/>
+        <v>70</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D71" s="12"/>
+      <c r="E71" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F71" s="33">
+        <v>1</v>
+      </c>
+      <c r="G71" s="39" t="s">
+        <v>100</v>
+      </c>
       <c r="H71" s="18"/>
     </row>
     <row r="72" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="9">
-        <v>43040</v>
-      </c>
+      <c r="A72" s="45"/>
       <c r="B72" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12" t="s">
-        <v>98</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D72" s="12"/>
       <c r="E72" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F72" s="30"/>
       <c r="G72" s="39"/>
@@ -3913,482 +4073,472 @@
     <row r="73" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="9"/>
       <c r="B73" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C73" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D73" s="12"/>
       <c r="E73" s="11" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="F73" s="30"/>
       <c r="G73" s="39"/>
       <c r="H73" s="18"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="9"/>
       <c r="B74" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C74" s="13" t="s">
-        <v>61</v>
+        <v>70</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="D74" s="12"/>
-      <c r="E74" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="F74" s="33">
-        <v>1</v>
-      </c>
-      <c r="G74" s="39" t="s">
-        <v>95</v>
-      </c>
+      <c r="E74" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F74" s="30"/>
+      <c r="G74" s="39"/>
       <c r="H74" s="18"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A75" s="9">
-        <v>43040</v>
-      </c>
+    <row r="75" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="45"/>
       <c r="B75" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C75" s="11"/>
-      <c r="D75" s="12" t="s">
-        <v>53</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
       <c r="E75" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F75" s="30"/>
-      <c r="G75" s="38"/>
+      <c r="G75" s="39"/>
       <c r="H75" s="18"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76" s="9"/>
       <c r="B76" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C76" s="11"/>
-      <c r="D76" s="12" t="s">
-        <v>53</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
       <c r="E76" s="11" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="F76" s="30"/>
-      <c r="G76" s="38"/>
+      <c r="G76" s="39"/>
       <c r="H76" s="18"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77" s="9"/>
       <c r="B77" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C77" s="11"/>
-      <c r="D77" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E77" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F77" s="30"/>
-      <c r="G77" s="38"/>
+        <v>70</v>
+      </c>
+      <c r="C77" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D77" s="12"/>
+      <c r="E77" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="F77" s="33">
+        <v>1</v>
+      </c>
+      <c r="G77" s="39" t="s">
+        <v>100</v>
+      </c>
       <c r="H77" s="18"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A78" s="9">
-        <v>43040</v>
-      </c>
+    <row r="78" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="45"/>
       <c r="B78" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C78" s="11"/>
+        <v>70</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>72</v>
+      </c>
       <c r="D78" s="12" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F78" s="30"/>
-      <c r="G78" s="38"/>
+      <c r="G78" s="39"/>
       <c r="H78" s="18"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="9"/>
       <c r="B79" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C79" s="11"/>
-      <c r="D79" s="12" t="s">
-        <v>53</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
       <c r="E79" s="11" t="s">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="F79" s="30"/>
-      <c r="G79" s="40"/>
+      <c r="G79" s="39"/>
       <c r="H79" s="18"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A80" s="9"/>
       <c r="B80" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C80" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D80" s="12"/>
-      <c r="E80" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="F80" s="33">
-        <v>1</v>
-      </c>
-      <c r="G80" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="H80" s="17"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A81" s="9">
-        <v>43040</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E80" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F80" s="30"/>
+      <c r="G80" s="39"/>
+      <c r="H80" s="18"/>
+    </row>
+    <row r="81" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="45"/>
       <c r="B81" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C81" s="11"/>
+        <v>70</v>
+      </c>
+      <c r="C81" s="12"/>
       <c r="D81" s="12" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F81" s="34"/>
-      <c r="G81" s="40"/>
-      <c r="H81" s="17"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+      <c r="F81" s="30"/>
+      <c r="G81" s="39"/>
+      <c r="H81" s="18"/>
+    </row>
+    <row r="82" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82" s="9"/>
       <c r="B82" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C82" s="11"/>
-      <c r="D82" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E82" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F82" s="34"/>
-      <c r="G82" s="40"/>
-      <c r="H82" s="17"/>
+        <v>70</v>
+      </c>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F82" s="30"/>
+      <c r="G82" s="39"/>
+      <c r="H82" s="18"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="9"/>
       <c r="B83" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D83" s="12"/>
+      <c r="E83" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C83" s="13"/>
-      <c r="D83" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E83" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F83" s="30"/>
-      <c r="G83" s="39"/>
-      <c r="H83" s="17"/>
+      <c r="F83" s="33">
+        <v>1</v>
+      </c>
+      <c r="G83" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="H83" s="18"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A84" s="9">
-        <v>43040</v>
-      </c>
+      <c r="A84" s="45"/>
       <c r="B84" s="10" t="s">
-        <v>71</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C84" s="11"/>
       <c r="D84" s="12" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F84" s="35"/>
-      <c r="H84" s="7"/>
-    </row>
-    <row r="85" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>115</v>
+      </c>
+      <c r="F84" s="30"/>
+      <c r="G84" s="38"/>
+      <c r="H84" s="18"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="9"/>
       <c r="B85" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C85" s="11"/>
       <c r="D85" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="F85" s="30"/>
-      <c r="G85" s="40"/>
-      <c r="H85" s="17"/>
-    </row>
-    <row r="86" spans="1:9" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="G85" s="38"/>
+      <c r="H85" s="18"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="9"/>
       <c r="B86" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C86" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E86" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="F86" s="33">
-        <v>1</v>
-      </c>
-      <c r="G86" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="H86" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="I86" s="22"/>
-    </row>
-    <row r="87" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A87" s="9">
-        <v>43040</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C86" s="11"/>
+      <c r="D86" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E86" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F86" s="30"/>
+      <c r="G86" s="38"/>
+      <c r="H86" s="18"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A87" s="45"/>
       <c r="B87" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C87" s="11"/>
-      <c r="D87" s="15" t="s">
-        <v>53</v>
+      <c r="D87" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F87" s="34"/>
-      <c r="G87" s="40"/>
-      <c r="H87" s="17"/>
-    </row>
-    <row r="88" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+      <c r="F87" s="30"/>
+      <c r="G87" s="38"/>
+      <c r="H87" s="18"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="9"/>
       <c r="B88" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C88" s="11"/>
-      <c r="D88" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E88" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F88" s="34"/>
+      <c r="D88" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E88" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F88" s="30"/>
       <c r="G88" s="40"/>
-      <c r="H88" s="17"/>
+      <c r="H88" s="18"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="9"/>
       <c r="B89" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C89" s="11"/>
-      <c r="D89" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E89" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F89" s="34"/>
-      <c r="G89" s="40"/>
-      <c r="H89" s="18"/>
+        <v>70</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D89" s="12"/>
+      <c r="E89" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F89" s="33">
+        <v>1</v>
+      </c>
+      <c r="G89" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="H89" s="17"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A90" s="9">
-        <v>43040</v>
-      </c>
+      <c r="A90" s="45"/>
       <c r="B90" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C90" s="11"/>
       <c r="D90" s="12" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F90" s="34"/>
       <c r="G90" s="40"/>
-      <c r="H90" s="18"/>
-    </row>
-    <row r="91" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H90" s="17"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="9"/>
       <c r="B91" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C91" s="11"/>
       <c r="D91" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F91" s="34"/>
       <c r="G91" s="40"/>
-      <c r="H91" s="18"/>
+      <c r="H91" s="17"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="9"/>
       <c r="B92" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C92" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D92" s="10"/>
-      <c r="E92" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F92" s="33">
-        <v>1</v>
-      </c>
-      <c r="G92" s="40"/>
-      <c r="H92" s="18"/>
+        <v>70</v>
+      </c>
+      <c r="C92" s="13"/>
+      <c r="D92" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E92" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F92" s="30"/>
+      <c r="G92" s="39"/>
+      <c r="H92" s="17"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A93" s="9">
-        <v>43040</v>
-      </c>
+      <c r="A93" s="45"/>
       <c r="B93" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C93" s="10"/>
-      <c r="D93" s="10"/>
+        <v>70</v>
+      </c>
+      <c r="D93" s="12" t="s">
+        <v>97</v>
+      </c>
       <c r="E93" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F93" s="34"/>
-      <c r="G93" s="40"/>
-      <c r="H93" s="18"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+      <c r="F93" s="35"/>
+      <c r="H93" s="7"/>
+    </row>
+    <row r="94" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="9"/>
       <c r="B94" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
-      <c r="E94" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F94" s="34"/>
+        <v>70</v>
+      </c>
+      <c r="C94" s="11"/>
+      <c r="D94" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E94" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F94" s="30"/>
       <c r="G94" s="40"/>
-      <c r="H94" s="18"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H94" s="17"/>
+    </row>
+    <row r="95" spans="1:9" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A95" s="9"/>
       <c r="B95" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C95" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D95" s="10"/>
+        <v>60</v>
+      </c>
       <c r="E95" s="27" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F95" s="33">
         <v>1</v>
       </c>
-      <c r="G95" s="40"/>
-      <c r="H95" s="18"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A96" s="9">
-        <v>43040</v>
-      </c>
+      <c r="G95" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="H95" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="I95" s="22"/>
+    </row>
+    <row r="96" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A96" s="45"/>
       <c r="B96" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C96" s="10"/>
-      <c r="D96" s="10"/>
+        <v>70</v>
+      </c>
+      <c r="C96" s="11"/>
+      <c r="D96" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="E96" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F96" s="34"/>
       <c r="G96" s="40"/>
-      <c r="H96" s="20"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H96" s="17"/>
+    </row>
+    <row r="97" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A97" s="9"/>
       <c r="B97" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C97" s="10"/>
-      <c r="D97" s="10"/>
+        <v>70</v>
+      </c>
+      <c r="C97" s="11"/>
+      <c r="D97" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="E97" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F97" s="34"/>
       <c r="G97" s="40"/>
-      <c r="H97" s="20"/>
+      <c r="H97" s="17"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="9"/>
-      <c r="B98" s="10"/>
-      <c r="C98" s="10"/>
+      <c r="B98" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C98" s="11"/>
       <c r="D98" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E98" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F98" s="34"/>
       <c r="G98" s="40"/>
-      <c r="H98" s="20"/>
+      <c r="H98" s="18"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A99" s="9">
-        <v>43040</v>
-      </c>
-      <c r="B99" s="10"/>
-      <c r="C99" s="10"/>
+      <c r="A99" s="45"/>
+      <c r="B99" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C99" s="11"/>
       <c r="D99" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E99" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F99" s="34"/>
       <c r="G99" s="40"/>
-      <c r="H99" s="20"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H99" s="18"/>
+    </row>
+    <row r="100" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="9"/>
       <c r="B100" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C100" s="10"/>
+        <v>70</v>
+      </c>
+      <c r="C100" s="11"/>
       <c r="D100" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E100" s="10" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="F100" s="34"/>
       <c r="G100" s="40"/>
-      <c r="H100" s="20"/>
+      <c r="H100" s="18"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" s="9"/>
       <c r="B101" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D101" s="10"/>
       <c r="E101" s="27" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F101" s="33">
         <v>1</v>
@@ -4397,72 +4547,74 @@
       <c r="H101" s="18"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A102" s="9">
-        <v>43040</v>
-      </c>
+      <c r="A102" s="45"/>
       <c r="B102" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C102" s="10"/>
-      <c r="D102" s="11"/>
+      <c r="D102" s="10"/>
       <c r="E102" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F102" s="34"/>
-      <c r="G102" s="38"/>
-      <c r="H102" s="20"/>
+      <c r="G102" s="40"/>
+      <c r="H102" s="18"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="9"/>
       <c r="B103" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C103" s="10"/>
-      <c r="D103" s="11"/>
+      <c r="D103" s="10"/>
       <c r="E103" s="10" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="F103" s="34"/>
-      <c r="G103" s="38"/>
-      <c r="H103" s="20"/>
+      <c r="G103" s="40"/>
+      <c r="H103" s="18"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="9"/>
-      <c r="B104" s="10"/>
-      <c r="C104" s="10"/>
-      <c r="D104" s="11"/>
-      <c r="E104" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F104" s="34"/>
-      <c r="G104" s="38"/>
-      <c r="H104" s="20"/>
+      <c r="B104" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C104" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D104" s="10"/>
+      <c r="E104" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="F104" s="33">
+        <v>1</v>
+      </c>
+      <c r="G104" s="40"/>
+      <c r="H104" s="18"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A105" s="9">
-        <v>43040</v>
-      </c>
-      <c r="B105" s="10"/>
+      <c r="A105" s="45"/>
+      <c r="B105" s="10" t="s">
+        <v>70</v>
+      </c>
       <c r="C105" s="10"/>
-      <c r="D105" s="12" t="s">
-        <v>98</v>
-      </c>
+      <c r="D105" s="10"/>
       <c r="E105" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F105" s="34"/>
-      <c r="G105" s="38"/>
+      <c r="G105" s="40"/>
       <c r="H105" s="20"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="9"/>
       <c r="B106" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C106" s="10"/>
-      <c r="D106" s="11"/>
+      <c r="D106" s="10"/>
       <c r="E106" s="10" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="F106" s="34"/>
       <c r="G106" s="40"/>
@@ -4470,209 +4622,272 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="9"/>
-      <c r="B107" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C107" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D107" s="11"/>
-      <c r="E107" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="F107" s="33">
-        <v>1</v>
-      </c>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E107" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F107" s="34"/>
       <c r="G107" s="40"/>
-      <c r="H107" s="18"/>
+      <c r="H107" s="20"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A108" s="9">
-        <v>43040</v>
-      </c>
-      <c r="B108" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D108" s="11"/>
+      <c r="A108" s="45"/>
+      <c r="B108" s="10"/>
+      <c r="C108" s="10"/>
+      <c r="D108" s="12" t="s">
+        <v>97</v>
+      </c>
       <c r="E108" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F108" s="34"/>
-      <c r="G108" s="38"/>
-      <c r="H108" s="18"/>
+      <c r="G108" s="40"/>
+      <c r="H108" s="20"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="9"/>
       <c r="B109" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C109" s="11"/>
-      <c r="D109" s="11"/>
+        <v>70</v>
+      </c>
+      <c r="C109" s="10"/>
+      <c r="D109" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="E109" s="10" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="F109" s="34"/>
-      <c r="G109" s="38"/>
-      <c r="H109" s="18"/>
+      <c r="G109" s="40"/>
+      <c r="H109" s="20"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" s="9"/>
-      <c r="B110" s="10"/>
-      <c r="C110" s="11"/>
-      <c r="D110" s="11"/>
-      <c r="E110" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F110" s="34"/>
-      <c r="G110" s="38"/>
+      <c r="B110" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C110" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D110" s="10"/>
+      <c r="E110" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="F110" s="33">
+        <v>1</v>
+      </c>
+      <c r="G110" s="40"/>
       <c r="H110" s="18"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A111" s="9">
-        <v>43040</v>
-      </c>
-      <c r="B111" s="10"/>
-      <c r="C111" s="11"/>
-      <c r="D111" s="12" t="s">
-        <v>98</v>
-      </c>
+      <c r="A111" s="9"/>
+      <c r="B111" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C111" s="10"/>
+      <c r="D111" s="11"/>
       <c r="E111" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F111" s="34"/>
       <c r="G111" s="38"/>
-      <c r="H111" s="18"/>
+      <c r="H111" s="20"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" s="9"/>
       <c r="B112" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C112" s="11"/>
+        <v>70</v>
+      </c>
+      <c r="C112" s="10"/>
       <c r="D112" s="11"/>
       <c r="E112" s="10" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="F112" s="34"/>
       <c r="G112" s="38"/>
-      <c r="H112" s="18"/>
+      <c r="H112" s="20"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="9"/>
-      <c r="B113" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C113" s="11"/>
-      <c r="D113" s="12"/>
-      <c r="E113" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="F113" s="34">
-        <v>0</v>
-      </c>
-      <c r="G113" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="H113" s="18"/>
+      <c r="B113" s="10"/>
+      <c r="C113" s="10"/>
+      <c r="D113" s="11"/>
+      <c r="E113" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F113" s="34"/>
+      <c r="G113" s="38"/>
+      <c r="H113" s="20"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A114" s="9"/>
-      <c r="B114" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C114" s="11"/>
-      <c r="D114" s="11"/>
-      <c r="E114" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="F114" s="34">
-        <v>0</v>
-      </c>
-      <c r="G114" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="H114" s="18"/>
+      <c r="A114" s="45"/>
+      <c r="B114" s="10"/>
+      <c r="C114" s="10"/>
+      <c r="D114" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E114" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F114" s="34"/>
+      <c r="G114" s="38"/>
+      <c r="H114" s="20"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A115">
-        <f>ROUND(COUNTA(A4:A114)/ROWS(A4:A114)*100,0)</f>
-        <v>50</v>
-      </c>
-      <c r="B115" s="43" t="s">
-        <v>126</v>
-      </c>
+      <c r="A115" s="9"/>
+      <c r="B115" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C115" s="10"/>
+      <c r="D115" s="11"/>
+      <c r="E115" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F115" s="34"/>
+      <c r="G115" s="40"/>
+      <c r="H115" s="20"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="9"/>
+      <c r="B116" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C116" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D116" s="11"/>
+      <c r="E116" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="F116" s="33">
+        <v>1</v>
+      </c>
       <c r="G116" s="40"/>
       <c r="H116" s="18"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C117" s="5"/>
-      <c r="D117" s="5"/>
-      <c r="E117" s="5"/>
-      <c r="F117" s="36"/>
-      <c r="G117" s="42"/>
+      <c r="A117" s="45"/>
+      <c r="B117" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D117" s="11"/>
+      <c r="E117" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F117" s="34"/>
+      <c r="G117" s="38"/>
+      <c r="H117" s="18"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A118" t="s">
-        <v>106</v>
-      </c>
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
-      <c r="E118" s="5"/>
-      <c r="F118" s="36"/>
-      <c r="G118" s="42"/>
+      <c r="A118" s="9"/>
+      <c r="B118" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C118" s="11"/>
+      <c r="D118" s="11"/>
+      <c r="E118" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F118" s="34"/>
+      <c r="G118" s="38"/>
+      <c r="H118" s="18"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B119" t="s">
-        <v>107</v>
-      </c>
-      <c r="C119" t="s">
+      <c r="A119" s="9"/>
+      <c r="B119" s="10"/>
+      <c r="C119" s="11"/>
+      <c r="D119" s="11"/>
+      <c r="E119" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F119" s="34"/>
+      <c r="G119" s="38"/>
+      <c r="H119" s="18"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A120" s="45"/>
+      <c r="B120" s="10"/>
+      <c r="C120" s="11"/>
+      <c r="D120" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="E119" t="s">
-        <v>108</v>
-      </c>
-      <c r="G119" s="42"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G120" s="42"/>
+      <c r="E120" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F120" s="34"/>
+      <c r="G120" s="38"/>
+      <c r="H120" s="18"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C121" s="5"/>
-      <c r="D121" s="5"/>
-      <c r="E121" s="5"/>
-      <c r="F121" s="36"/>
-      <c r="G121" s="42"/>
+      <c r="A121" s="9"/>
+      <c r="B121" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C121" s="11"/>
+      <c r="D121" s="11"/>
+      <c r="E121" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F121" s="34"/>
+      <c r="G121" s="38"/>
+      <c r="H121" s="18"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C122" s="5"/>
-      <c r="D122" s="5"/>
-      <c r="E122" s="5"/>
-      <c r="F122" s="36"/>
-      <c r="G122" s="42"/>
+      <c r="A122" s="9">
+        <v>43045</v>
+      </c>
+      <c r="B122" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C122" s="11"/>
+      <c r="D122" s="12"/>
+      <c r="E122" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="F122" s="34">
+        <v>0</v>
+      </c>
+      <c r="G122" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="H122" s="18"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C123" s="5"/>
-      <c r="D123" s="5"/>
-      <c r="E123" s="5"/>
-      <c r="F123" s="36"/>
-      <c r="G123" s="42"/>
+      <c r="A123" s="9">
+        <v>43045</v>
+      </c>
+      <c r="B123" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C123" s="11"/>
+      <c r="D123" s="11"/>
+      <c r="E123" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="F123" s="34">
+        <v>0</v>
+      </c>
+      <c r="G123" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="H123" s="18"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C124" s="5"/>
-      <c r="D124" s="5"/>
-      <c r="E124" s="5"/>
-      <c r="F124" s="36"/>
-      <c r="G124" s="42"/>
+      <c r="A124">
+        <f>ROUND(COUNTA(A4:A123)/ROWS(A4:A123)*100,0)</f>
+        <v>26</v>
+      </c>
+      <c r="B124" s="43" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C125" s="5"/>
-      <c r="D125" s="5"/>
-      <c r="E125" s="5"/>
-      <c r="F125" s="36"/>
-      <c r="G125" s="42"/>
+      <c r="A125" s="9"/>
+      <c r="G125" s="40"/>
+      <c r="H125" s="18"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C126" s="5"/>
@@ -4681,420 +4896,497 @@
       <c r="F126" s="36"/>
       <c r="G126" s="42"/>
     </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>105</v>
+      </c>
+      <c r="C127" s="5"/>
+      <c r="D127" s="5"/>
+      <c r="E127" s="5"/>
+      <c r="F127" s="36"/>
+      <c r="G127" s="42"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B128" t="s">
+        <v>106</v>
+      </c>
+      <c r="C128" t="s">
+        <v>96</v>
+      </c>
+      <c r="E128" t="s">
+        <v>107</v>
+      </c>
+      <c r="G128" s="42"/>
+    </row>
+    <row r="129" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="G129" s="42"/>
+    </row>
+    <row r="130" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C130" s="5"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="5"/>
+      <c r="F130" s="36"/>
+      <c r="G130" s="42"/>
+    </row>
+    <row r="131" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C131" s="5"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="36"/>
+      <c r="G131" s="42"/>
+    </row>
+    <row r="132" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="36"/>
+      <c r="G132" s="42"/>
+    </row>
+    <row r="133" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C133" s="5"/>
+      <c r="D133" s="5"/>
+      <c r="E133" s="5"/>
+      <c r="F133" s="36"/>
+      <c r="G133" s="42"/>
+    </row>
+    <row r="134" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C134" s="5"/>
+      <c r="D134" s="5"/>
+      <c r="E134" s="5"/>
+      <c r="F134" s="36"/>
+      <c r="G134" s="42"/>
+    </row>
+    <row r="135" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C135" s="5"/>
+      <c r="D135" s="5"/>
+      <c r="E135" s="5"/>
+      <c r="F135" s="36"/>
+      <c r="G135" s="42"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A116">
-    <cfRule type="notContainsBlanks" dxfId="83" priority="205">
-      <formula>LEN(TRIM(A116))&gt;0</formula>
+  <conditionalFormatting sqref="A125 A34:A42">
+    <cfRule type="notContainsBlanks" dxfId="84" priority="254">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A79">
+    <cfRule type="notContainsBlanks" dxfId="83" priority="131">
+      <formula>LEN(TRIM(A79))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71">
+    <cfRule type="notContainsBlanks" dxfId="82" priority="133">
+      <formula>LEN(TRIM(A71))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57">
+    <cfRule type="notContainsBlanks" dxfId="81" priority="144">
+      <formula>LEN(TRIM(A57))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64">
+    <cfRule type="notContainsBlanks" dxfId="80" priority="140">
+      <formula>LEN(TRIM(A64))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A73">
+    <cfRule type="notContainsBlanks" dxfId="79" priority="134">
+      <formula>LEN(TRIM(A73))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A76">
+    <cfRule type="notContainsBlanks" dxfId="78" priority="132">
+      <formula>LEN(TRIM(A76))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54">
+    <cfRule type="notContainsBlanks" dxfId="77" priority="68">
+      <formula>LEN(TRIM(A54))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55">
+    <cfRule type="notContainsBlanks" dxfId="76" priority="145">
+      <formula>LEN(TRIM(A55))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="47">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="notContainsBlanks" dxfId="74" priority="143">
+      <formula>LEN(TRIM(A59))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="142">
+      <formula>LEN(TRIM(A61))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62">
+    <cfRule type="notContainsBlanks" dxfId="72" priority="141">
+      <formula>LEN(TRIM(A62))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="139">
+      <formula>LEN(TRIM(A65))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="138">
+      <formula>LEN(TRIM(A67))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68">
+    <cfRule type="notContainsBlanks" dxfId="69" priority="137">
+      <formula>LEN(TRIM(A68))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70">
-    <cfRule type="notContainsBlanks" dxfId="82" priority="82">
+    <cfRule type="notContainsBlanks" dxfId="68" priority="136">
       <formula>LEN(TRIM(A70))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A62">
-    <cfRule type="notContainsBlanks" dxfId="81" priority="84">
-      <formula>LEN(TRIM(A62))&gt;0</formula>
+  <conditionalFormatting sqref="A74">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="135">
+      <formula>LEN(TRIM(A74))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A77">
+    <cfRule type="notContainsBlanks" dxfId="66" priority="130">
+      <formula>LEN(TRIM(A77))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A80">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="129">
+      <formula>LEN(TRIM(A80))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82">
+    <cfRule type="notContainsBlanks" dxfId="64" priority="128">
+      <formula>LEN(TRIM(A82))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A83">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="127">
+      <formula>LEN(TRIM(A83))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A86">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="126">
+      <formula>LEN(TRIM(A86))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A85">
+    <cfRule type="notContainsBlanks" dxfId="61" priority="125">
+      <formula>LEN(TRIM(A85))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="124">
+      <formula>LEN(TRIM(A88))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A89">
+    <cfRule type="notContainsBlanks" dxfId="59" priority="123">
+      <formula>LEN(TRIM(A89))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="122">
+      <formula>LEN(TRIM(A91))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A92">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="121">
+      <formula>LEN(TRIM(A92))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A94">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="120">
+      <formula>LEN(TRIM(A94))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A95">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="119">
+      <formula>LEN(TRIM(A95))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A97">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="118">
+      <formula>LEN(TRIM(A97))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A98">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="117">
+      <formula>LEN(TRIM(A98))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A100">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="116">
+      <formula>LEN(TRIM(A100))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:A7">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="49">
+      <formula>LEN(TRIM(A5))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A101">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="114">
+      <formula>LEN(TRIM(A101))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A104">
+    <cfRule type="notContainsBlanks" dxfId="49" priority="112">
+      <formula>LEN(TRIM(A104))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A106:A107">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="111">
+      <formula>LEN(TRIM(A106))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="notContainsBlanks" dxfId="80" priority="144">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="48">
       <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
-    <cfRule type="notContainsBlanks" dxfId="79" priority="95">
-      <formula>LEN(TRIM(A48))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55">
-    <cfRule type="notContainsBlanks" dxfId="78" priority="91">
-      <formula>LEN(TRIM(A55))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A64">
-    <cfRule type="notContainsBlanks" dxfId="77" priority="85">
-      <formula>LEN(TRIM(A64))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67">
-    <cfRule type="notContainsBlanks" dxfId="76" priority="83">
-      <formula>LEN(TRIM(A67))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45">
-    <cfRule type="notContainsBlanks" dxfId="75" priority="19">
+  <conditionalFormatting sqref="A45:A52">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="98">
       <formula>LEN(TRIM(A45))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A46">
-    <cfRule type="notContainsBlanks" dxfId="74" priority="96">
-      <formula>LEN(TRIM(A46))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
-    <cfRule type="notContainsBlanks" dxfId="73" priority="40">
-      <formula>LEN(TRIM(A20))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50">
-    <cfRule type="notContainsBlanks" dxfId="72" priority="94">
-      <formula>LEN(TRIM(A50))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A52">
-    <cfRule type="notContainsBlanks" dxfId="71" priority="93">
-      <formula>LEN(TRIM(A52))&gt;0</formula>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="94">
+      <formula>LEN(TRIM(A4))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A109:A113 A115:A116 A118:A119 A121">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="84">
+      <formula>LEN(TRIM(A109))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="39">
+      <formula>LEN(TRIM(A43))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="61">
+      <formula>LEN(TRIM(A12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="60">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="28">
+      <formula>LEN(TRIM(A60))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="27">
+      <formula>LEN(TRIM(A63))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="25">
+      <formula>LEN(TRIM(A69))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A78">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="22">
+      <formula>LEN(TRIM(A78))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A99">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="15">
+      <formula>LEN(TRIM(A99))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="46">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="45">
+      <formula>LEN(TRIM(A15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18:A20">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="44">
+      <formula>LEN(TRIM(A18))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="43">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:A28">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="42">
+      <formula>LEN(TRIM(A26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:A31">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="41">
+      <formula>LEN(TRIM(A29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="38">
+      <formula>LEN(TRIM(A44))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="notContainsBlanks" dxfId="70" priority="92">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="37">
       <formula>LEN(TRIM(A53))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A122:A123">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="36">
+      <formula>LEN(TRIM(A122))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="35">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="34">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16:A17">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="33">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="29">
+      <formula>LEN(TRIM(A58))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A56">
-    <cfRule type="notContainsBlanks" dxfId="69" priority="90">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="30">
       <formula>LEN(TRIM(A56))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A58">
-    <cfRule type="notContainsBlanks" dxfId="68" priority="89">
-      <formula>LEN(TRIM(A58))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59">
-    <cfRule type="notContainsBlanks" dxfId="67" priority="88">
-      <formula>LEN(TRIM(A59))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61">
-    <cfRule type="notContainsBlanks" dxfId="66" priority="87">
-      <formula>LEN(TRIM(A61))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65">
-    <cfRule type="notContainsBlanks" dxfId="65" priority="86">
-      <formula>LEN(TRIM(A65))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68">
-    <cfRule type="notContainsBlanks" dxfId="64" priority="81">
-      <formula>LEN(TRIM(A68))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71">
-    <cfRule type="notContainsBlanks" dxfId="63" priority="80">
-      <formula>LEN(TRIM(A71))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A73">
-    <cfRule type="notContainsBlanks" dxfId="62" priority="79">
-      <formula>LEN(TRIM(A73))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A74">
-    <cfRule type="notContainsBlanks" dxfId="61" priority="78">
-      <formula>LEN(TRIM(A74))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A77">
-    <cfRule type="notContainsBlanks" dxfId="60" priority="77">
-      <formula>LEN(TRIM(A77))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A76">
-    <cfRule type="notContainsBlanks" dxfId="59" priority="76">
-      <formula>LEN(TRIM(A76))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A79">
-    <cfRule type="notContainsBlanks" dxfId="58" priority="75">
-      <formula>LEN(TRIM(A79))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A80">
-    <cfRule type="notContainsBlanks" dxfId="57" priority="74">
-      <formula>LEN(TRIM(A80))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A82">
-    <cfRule type="notContainsBlanks" dxfId="56" priority="73">
-      <formula>LEN(TRIM(A82))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A83">
-    <cfRule type="notContainsBlanks" dxfId="55" priority="72">
-      <formula>LEN(TRIM(A83))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A85">
-    <cfRule type="notContainsBlanks" dxfId="54" priority="71">
-      <formula>LEN(TRIM(A85))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A86">
-    <cfRule type="notContainsBlanks" dxfId="53" priority="70">
-      <formula>LEN(TRIM(A86))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A88">
-    <cfRule type="notContainsBlanks" dxfId="52" priority="69">
-      <formula>LEN(TRIM(A88))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A89">
-    <cfRule type="notContainsBlanks" dxfId="51" priority="68">
-      <formula>LEN(TRIM(A89))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A91">
-    <cfRule type="notContainsBlanks" dxfId="50" priority="67">
-      <formula>LEN(TRIM(A91))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
-    <cfRule type="notContainsBlanks" dxfId="49" priority="37">
-      <formula>LEN(TRIM(A34))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A92">
-    <cfRule type="notContainsBlanks" dxfId="48" priority="65">
-      <formula>LEN(TRIM(A92))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A94">
-    <cfRule type="notContainsBlanks" dxfId="47" priority="64">
-      <formula>LEN(TRIM(A94))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A95">
-    <cfRule type="notContainsBlanks" dxfId="46" priority="63">
-      <formula>LEN(TRIM(A95))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A97:A98">
-    <cfRule type="notContainsBlanks" dxfId="45" priority="62">
-      <formula>LEN(TRIM(A97))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A63">
-    <cfRule type="notContainsBlanks" dxfId="44" priority="27">
-      <formula>LEN(TRIM(A63))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A66">
-    <cfRule type="notContainsBlanks" dxfId="43" priority="26">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="26">
       <formula>LEN(TRIM(A66))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="25">
-      <formula>LEN(TRIM(A69))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A72">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="24">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="24">
       <formula>LEN(TRIM(A72))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A75">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="23">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="23">
       <formula>LEN(TRIM(A75))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A78">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="22">
-      <formula>LEN(TRIM(A78))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A81">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="21">
       <formula>LEN(TRIM(A81))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="20">
       <formula>LEN(TRIM(A84))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A18:A19">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="41">
-      <formula>LEN(TRIM(A18))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35:A43">
-    <cfRule type="notContainsBlanks" dxfId="35" priority="49">
-      <formula>LEN(TRIM(A35))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="48">
-      <formula>LEN(TRIM(A7))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A6">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="47">
-      <formula>LEN(TRIM(A6))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="46">
-      <formula>LEN(TRIM(A5))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="45">
-      <formula>LEN(TRIM(A4))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="notContainsBlanks" dxfId="30" priority="44">
-      <formula>LEN(TRIM(A11))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="43">
-      <formula>LEN(TRIM(A14))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="42">
-      <formula>LEN(TRIM(A15))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="39">
-      <formula>LEN(TRIM(A23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26:A31">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="38">
-      <formula>LEN(TRIM(A26))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A100:A114">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="35">
-      <formula>LEN(TRIM(A100))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="34">
-      <formula>LEN(TRIM(A9))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="33">
-      <formula>LEN(TRIM(A10))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A99">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="32">
-      <formula>LEN(TRIM(A99))&gt;0</formula>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="19">
+      <formula>LEN(TRIM(A87))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="18">
+      <formula>LEN(TRIM(A90))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A93">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="17">
+      <formula>LEN(TRIM(A93))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="31">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="16">
       <formula>LEN(TRIM(A96))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A93">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="30">
-      <formula>LEN(TRIM(A93))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A90">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="29">
-      <formula>LEN(TRIM(A90))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A87">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="28">
-      <formula>LEN(TRIM(A87))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="18">
-      <formula>LEN(TRIM(A47))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A49">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="17">
-      <formula>LEN(TRIM(A49))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="16">
-      <formula>LEN(TRIM(A51))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="15">
-      <formula>LEN(TRIM(A54))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A57">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="14">
-      <formula>LEN(TRIM(A57))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60">
+  <conditionalFormatting sqref="A117">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="9">
+      <formula>LEN(TRIM(A117))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A102">
     <cfRule type="notContainsBlanks" dxfId="11" priority="13">
-      <formula>LEN(TRIM(A60))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
+      <formula>LEN(TRIM(A102))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A105">
     <cfRule type="notContainsBlanks" dxfId="10" priority="12">
-      <formula>LEN(TRIM(A12))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
+      <formula>LEN(TRIM(A105))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A108">
     <cfRule type="notContainsBlanks" dxfId="9" priority="11">
-      <formula>LEN(TRIM(A13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
+      <formula>LEN(TRIM(A108))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A114">
     <cfRule type="notContainsBlanks" dxfId="8" priority="10">
-      <formula>LEN(TRIM(A16))&gt;0</formula>
+      <formula>LEN(TRIM(A114))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A120">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(A120))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A103">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(A103))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(A21))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(A22))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="8">
-      <formula>LEN(TRIM(A22))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="7">
-      <formula>LEN(TRIM(A21))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(A25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(A17))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A32))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A44">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A44))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
DM SMS conversion early dev
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -20,8 +20,284 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Williams Tim</author>
+  </authors>
+  <commentList>
+    <comment ref="C4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Williams Tim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+cdiscpilot01:Person_v29eedorsh9a5vr65uc1iob3mvn9blbb</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Williams Tim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+&lt;https://raw.githubusercontent.com/phuse-org/CTDasRDF/master/data/rdf/cdiscpilot01.ttl#ReferenceInterval_8v92vil0roc4ceo0b14jj7i633hiui9g_35vav5nu799ueqq90kuvhd6o487fkisl&gt;</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Williams Tim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+https://raw.githubusercontent.com/phuse-org/CTDasRDF/master/data/rdf/cdiscpilot01.ttl#Date_8v92vil0roc4ceo0b14jj7i633hiui9g</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Williams Tim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+https://raw.githubusercontent.com/phuse-org/CTDasRDF/master/data/rdf/cdiscpilot01.ttl#Date_35vav5nu799ueqq90kuvhd6o487fkisl
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C24" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Williams Tim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+cdiscpilot01:StudyParticipationInterval_prshbja29v1mj7t24e6hhfg6ar6tno4i_k78l4og87v61q51vabbketftn59735lb</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E26" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Williams Tim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+cdiscpilot01:Date_prshbja29v1mj7t24e6hhfg6ar6tno4i</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E27" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Williams Tim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+cdiscpilot01:Date_k78l4og87v61q51vabbketftn59735lb
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E29" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Williams Tim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+study:SubjectIdentifier_dasu7n9q16a5m9e4lc2ae2627c47vpv6</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C30" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Williams Tim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+study:SubjectIdentifier_dasu7n9q16a5m9e4lc2ae2627c47vpv6</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E33" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Williams Tim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+cdiscpilot01:UniqueSubjectIdentifier_v29eedorsh9a5vr65uc1iob3mvn9blbb</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C34" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Williams Tim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+cdiscpilot01:UniqueSubjectIdentifier_v29eedorsh9a5vr65uc1iob3mvn9blbb</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="237">
   <si>
     <t>rdf:type</t>
   </si>
@@ -1146,18 +1422,12 @@
     <t>cdiscpilot01:StudyParticipationInterval_#_#</t>
   </si>
   <si>
-    <t>study:StudyParticipationInterval ;</t>
-  </si>
-  <si>
     <t>Study Participation Interval 1</t>
   </si>
   <si>
     <t>AO: Change from Date_30</t>
   </si>
   <si>
-    <t>has T11:45 in source data. Not present in R version  - TW ?? 13Mar18</t>
-  </si>
-  <si>
     <t xml:space="preserve">cdiscpilot01:AgeOutcome_1 </t>
   </si>
   <si>
@@ -1213,9 +1483,6 @@
   </si>
   <si>
     <t>coded</t>
-  </si>
-  <si>
-    <t>cd01p:VisitScreening1DemogDataColl ;</t>
   </si>
   <si>
     <t>cdiscpilot01:VisitScreening1Activity_1 ;</t>
@@ -1249,9 +1516,6 @@
   #  triples for a specific person. Person_{#usubjid} --&gt;  DemographicDataCollection_{#usubjid}</t>
   </si>
   <si>
-    <t>AO: Change from VisitScreening1Activity_1</t>
-  </si>
-  <si>
     <t>Subject</t>
   </si>
   <si>
@@ -1270,9 +1534,6 @@
     </r>
   </si>
   <si>
-    <t>cdiscpilot01:VisitScreening1Activity_{#usubjid}</t>
-  </si>
-  <si>
     <t>owl:Class</t>
   </si>
   <si>
@@ -1283,13 +1544,86 @@
   </si>
   <si>
     <t>Visit Screening 1 Person {_ROW_}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cdiscpilot01:ReferenceInterval_#_#
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">study:StudyParticipationInterval </t>
+  </si>
+  <si>
+    <t>todo: Check date triples</t>
+  </si>
+  <si>
+    <t>code:DemographicDataCollection</t>
+  </si>
+  <si>
+    <t>cd01p:VisitScreening1DemogDataColl</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:VisitScreening1Activity_????</t>
+  </si>
+  <si>
+    <t>From: VisitScreening1Activity_1</t>
+  </si>
+  <si>
+    <t>What should ??? be based on?</t>
+  </si>
+  <si>
+    <t>"P {_ROW_} Screening {????} Demographic data collection</t>
+  </si>
+  <si>
+    <t>Again, ?? = what? there are _2, _3 in the data set</t>
+  </si>
+  <si>
+    <t>code:hasAge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AO: was AgeOutcome_1 .  </t>
+  </si>
+  <si>
+    <t>cdiscpilot01:AgeOutcome_{#age}</t>
+  </si>
+  <si>
+    <t>study:activityStatus</t>
+  </si>
+  <si>
+    <r>
+      <t>code:ActivityStatus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_1</t>
+    </r>
+  </si>
+  <si>
+    <t>KEEP AS-IS. ActivityStatus_1 is "complete"  and was hard coded.  Check R code to confirm</t>
+  </si>
+  <si>
+    <t>study:ethnicity</t>
+  </si>
+  <si>
+    <t>study:hasDate</t>
+  </si>
+  <si>
+    <t>study:race</t>
+  </si>
+  <si>
+    <t>study:sex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1488,12 +1822,30 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="39">
@@ -1702,13 +2054,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1881,7 +2233,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1924,9 +2276,8 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2005,25 +2356,23 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="21" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="21" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="21" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="25" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2044,9 +2393,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="10" xfId="42" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -2080,7 +2432,6 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2091,7 +2442,98 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="78">
+  <dxfs count="91">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2947,19 +3389,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G169"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44:D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.26953125" style="2" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="49.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49.81640625" style="19" customWidth="1"/>
@@ -2984,7 +3426,7 @@
         <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
@@ -3001,13 +3443,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="37">
-        <v>43171</v>
+        <v>43173</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>211</v>
+      <c r="C4" s="28" t="s">
+        <v>208</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>0</v>
@@ -3021,14 +3463,14 @@
       <c r="G4" s="14"/>
     </row>
     <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="38">
-        <v>43171</v>
+      <c r="A5" s="37">
+        <v>43173</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>75</v>
@@ -3043,13 +3485,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="37">
-        <v>43171</v>
+        <v>43173</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>2</v>
@@ -3062,13 +3504,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="37">
-        <v>43171</v>
+        <v>43173</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>3</v>
@@ -3080,28 +3522,28 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="40"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="42"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="40"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="37">
-        <v>43171</v>
+        <v>43173</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="43" t="s">
         <v>175</v>
       </c>
       <c r="F9" s="20" t="s">
@@ -3116,10 +3558,10 @@
       <c r="B10" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D10" s="49" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="10" t="s">
@@ -3134,10 +3576,10 @@
       <c r="B11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D11" s="49" t="s">
         <v>170</v>
       </c>
       <c r="E11" s="10" t="s">
@@ -3155,10 +3597,10 @@
       <c r="B12" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="49" t="s">
         <v>171</v>
       </c>
       <c r="E12" s="10" t="s">
@@ -3178,10 +3620,10 @@
       <c r="B13" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="D13" s="51" t="s">
+      <c r="D13" s="49" t="s">
         <v>172</v>
       </c>
       <c r="E13" s="10" t="s">
@@ -3195,23 +3637,23 @@
       </c>
     </row>
     <row r="14" spans="1:7" s="3" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="46"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="37">
-        <v>43172</v>
+        <v>43173</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>6</v>
@@ -3224,15 +3666,15 @@
       </c>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="37">
-        <v>43172</v>
+        <v>43173</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="45" t="s">
-        <v>177</v>
+      <c r="C16" s="28" t="s">
+        <v>217</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>0</v>
@@ -3245,18 +3687,18 @@
     </row>
     <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="37">
-        <v>43172</v>
+        <v>43173</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="43" t="s">
         <v>177</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="E17" s="45" t="s">
+      <c r="E17" s="43" t="s">
         <v>176</v>
       </c>
       <c r="F17" s="20"/>
@@ -3266,18 +3708,18 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="37">
-        <v>43172</v>
+        <v>43173</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="43" t="s">
         <v>177</v>
       </c>
-      <c r="D18" s="52" t="s">
+      <c r="D18" s="50" t="s">
         <v>171</v>
       </c>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="28" t="s">
         <v>178</v>
       </c>
       <c r="F18" s="20" t="s">
@@ -3289,18 +3731,18 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="37">
-        <v>43172</v>
+        <v>43173</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="43" t="s">
         <v>177</v>
       </c>
-      <c r="D19" s="52" t="s">
+      <c r="D19" s="50" t="s">
         <v>172</v>
       </c>
-      <c r="E19" s="39" t="s">
+      <c r="E19" s="28" t="s">
         <v>178</v>
       </c>
       <c r="F19" s="20" t="s">
@@ -3311,23 +3753,23 @@
       </c>
     </row>
     <row r="20" spans="1:7" s="3" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="46"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="50"/>
+      <c r="A20" s="44"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="48"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="37">
-        <v>43172</v>
+        <v>43173</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>8</v>
@@ -3343,28 +3785,28 @@
       </c>
     </row>
     <row r="22" spans="1:7" s="3" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="46"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="50"/>
+      <c r="A22" s="44"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="48"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="37" t="s">
-        <v>206</v>
+      <c r="A23" s="37">
+        <v>43173</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="45" t="s">
+      <c r="E23" s="43" t="s">
         <v>183</v>
       </c>
       <c r="F23" s="20" t="s">
@@ -3373,669 +3815,621 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="37" t="s">
-        <v>206</v>
+      <c r="A24" s="37">
+        <v>43173</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="45" t="s">
+      <c r="C24" s="28" t="s">
         <v>183</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>184</v>
+        <v>218</v>
       </c>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="37" t="s">
-        <v>206</v>
+      <c r="A25" s="37">
+        <v>43173</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="45" t="s">
+      <c r="C25" s="43" t="s">
         <v>183</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>170</v>
       </c>
       <c r="E25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="37" t="s">
-        <v>206</v>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="37">
+        <v>43173</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="45" t="s">
+      <c r="C26" s="43" t="s">
         <v>183</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E26" s="45" t="s">
+      <c r="E26" s="28" t="s">
         <v>178</v>
       </c>
       <c r="F26" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="G26" s="20" t="s">
-        <v>187</v>
-      </c>
+      <c r="G26" s="20"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="37" t="s">
-        <v>206</v>
+      <c r="A27" s="37">
+        <v>43173</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="45" t="s">
+      <c r="C27" s="43" t="s">
         <v>183</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E27" s="45" t="s">
+      <c r="E27" s="28" t="s">
         <v>178</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="G27" s="14"/>
+        <v>185</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="28" spans="1:7" s="3" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="46"/>
-      <c r="B28" s="47"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="50"/>
+      <c r="A28" s="44"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="48"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="37" t="s">
-        <v>206</v>
+      <c r="A29" s="37">
+        <v>43173</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="45" t="s">
-        <v>198</v>
+      <c r="E29" s="59" t="s">
+        <v>196</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="37" t="s">
-        <v>206</v>
+      <c r="A30" s="37">
+        <v>43173</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="45" t="s">
-        <v>198</v>
+      <c r="C30" s="59" t="s">
+        <v>196</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E30" s="45" t="s">
-        <v>199</v>
+      <c r="E30" s="43" t="s">
+        <v>197</v>
       </c>
       <c r="F30" s="20"/>
       <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="37" t="s">
-        <v>206</v>
+      <c r="A31" s="37">
+        <v>43173</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="45" t="s">
-        <v>198</v>
+      <c r="C31" s="43" t="s">
+        <v>196</v>
       </c>
       <c r="D31" t="s">
         <v>75</v>
       </c>
-      <c r="E31" s="45" t="s">
-        <v>204</v>
+      <c r="E31" s="43" t="s">
+        <v>202</v>
       </c>
       <c r="F31" s="20"/>
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" s="3" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="46"/>
-      <c r="B32" s="47"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="50"/>
+      <c r="A32" s="44"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="48"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="37" t="s">
-        <v>206</v>
+      <c r="A33" s="37">
+        <v>43173</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="45" t="s">
-        <v>205</v>
+      <c r="E33" s="59" t="s">
+        <v>203</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G33" s="14"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="37" t="s">
-        <v>206</v>
+      <c r="A34" s="37">
+        <v>43173</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="45" t="s">
-        <v>205</v>
+      <c r="C34" s="59" t="s">
+        <v>203</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E34" s="45" t="s">
-        <v>202</v>
+      <c r="E34" s="43" t="s">
+        <v>200</v>
       </c>
       <c r="F34" s="20"/>
       <c r="G34" s="14"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="37" t="s">
-        <v>206</v>
+      <c r="A35" s="37">
+        <v>43173</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="45" t="s">
-        <v>205</v>
+      <c r="C35" s="43" t="s">
+        <v>203</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E35" s="45" t="s">
-        <v>203</v>
+      <c r="E35" s="43" t="s">
+        <v>201</v>
       </c>
       <c r="F35" s="20"/>
       <c r="G35" s="14"/>
     </row>
     <row r="36" spans="1:7" s="3" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="46"/>
-      <c r="B36" s="47"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="48"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="50"/>
+      <c r="A36" s="44"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="48"/>
     </row>
     <row r="37" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="45" t="s">
+      <c r="E37" s="43" t="s">
+        <v>207</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="G37" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="F37" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>213</v>
-      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="8" t="s">
-        <v>206</v>
-      </c>
+      <c r="A38" s="8"/>
       <c r="B38" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="45" t="s">
-        <v>210</v>
+      <c r="C38" s="43" t="s">
+        <v>207</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E38" s="45" t="s">
-        <v>207</v>
+      <c r="E38" s="43" t="s">
+        <v>220</v>
       </c>
       <c r="F38" s="20"/>
       <c r="G38" s="14"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="8" t="s">
-        <v>206</v>
-      </c>
+      <c r="A39" s="8"/>
       <c r="B39" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="45" t="s">
-        <v>210</v>
+      <c r="C39" s="43" t="s">
+        <v>207</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E39" s="61" t="s">
-        <v>217</v>
-      </c>
-      <c r="F39" s="20" t="s">
-        <v>214</v>
-      </c>
+      <c r="E39" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="F39" s="20"/>
       <c r="G39" s="14"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="60"/>
-      <c r="B40" s="53"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="55"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="57"/>
-      <c r="G40" s="59"/>
+      <c r="A40" s="58"/>
+      <c r="B40" s="51"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" s="54" t="s">
+        <v>222</v>
+      </c>
+      <c r="F40" s="60" t="s">
+        <v>224</v>
+      </c>
+      <c r="G40" s="57" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="8"/>
-      <c r="B41" s="53"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="55"/>
-      <c r="E41" s="56"/>
-      <c r="F41" s="57"/>
+      <c r="B41" s="51"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="E41" s="54" t="s">
+        <v>225</v>
+      </c>
+      <c r="F41" s="55" t="s">
+        <v>226</v>
+      </c>
       <c r="G41" s="14"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="8"/>
-      <c r="B42" s="53"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="55"/>
-      <c r="E42" s="56"/>
-      <c r="F42" s="57"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="53" t="s">
+        <v>227</v>
+      </c>
+      <c r="E42" s="54" t="s">
+        <v>229</v>
+      </c>
+      <c r="F42" s="55" t="s">
+        <v>228</v>
+      </c>
       <c r="G42" s="14"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="8"/>
-      <c r="B43" s="53"/>
-      <c r="C43" s="56"/>
-      <c r="D43" s="55"/>
-      <c r="E43" s="56"/>
-      <c r="F43" s="57"/>
-      <c r="G43" s="58"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="54"/>
+      <c r="D43" s="53" t="s">
+        <v>230</v>
+      </c>
+      <c r="E43" s="54" t="s">
+        <v>231</v>
+      </c>
+      <c r="F43" s="55" t="s">
+        <v>232</v>
+      </c>
+      <c r="G43" s="56"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C44" s="45" t="s">
-        <v>216</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E44" s="45" t="s">
-        <v>218</v>
-      </c>
-      <c r="F44" s="20"/>
-      <c r="G44" s="14"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="51"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="53" t="s">
+        <v>233</v>
+      </c>
+      <c r="E44" s="54"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="56"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" s="45" t="s">
-        <v>216</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="F45" s="20"/>
-      <c r="G45" s="14"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="51"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="53" t="s">
+        <v>234</v>
+      </c>
+      <c r="E45" s="54"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="56"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C46" s="45" t="s">
-        <v>216</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="F46" s="20"/>
-      <c r="G46" s="14"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="51"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="53" t="s">
+        <v>235</v>
+      </c>
+      <c r="E46" s="54"/>
+      <c r="F46" s="55"/>
+      <c r="G46" s="56"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="8"/>
-      <c r="B47" s="53"/>
+      <c r="B47" s="51"/>
       <c r="C47" s="54"/>
-      <c r="D47" s="55"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="57"/>
-      <c r="G47" s="59"/>
+      <c r="D47" s="53" t="s">
+        <v>236</v>
+      </c>
+      <c r="E47" s="54"/>
+      <c r="F47" s="55"/>
+      <c r="G47" s="56"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="8"/>
-      <c r="B48" s="53"/>
+      <c r="B48" s="51"/>
       <c r="C48" s="54"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="56"/>
-      <c r="F48" s="57"/>
-      <c r="G48" s="14"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="54"/>
+      <c r="F48" s="55"/>
+      <c r="G48" s="56"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="8"/>
-      <c r="B49" s="53"/>
+      <c r="B49" s="51"/>
       <c r="C49" s="54"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="56"/>
-      <c r="F49" s="57"/>
-      <c r="G49" s="14"/>
+      <c r="D49" s="53"/>
+      <c r="E49" s="54"/>
+      <c r="F49" s="55"/>
+      <c r="G49" s="56"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="8"/>
-      <c r="B50" s="53"/>
+      <c r="B50" s="51"/>
       <c r="C50" s="54"/>
-      <c r="D50" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="E50" s="56" t="s">
-        <v>208</v>
-      </c>
-      <c r="F50" s="57"/>
-      <c r="G50" s="14"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="55"/>
+      <c r="G50" s="56"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="8"/>
-      <c r="B51" s="53"/>
+      <c r="B51" s="51"/>
       <c r="C51" s="54"/>
-      <c r="D51" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="E51" s="56" t="s">
-        <v>209</v>
-      </c>
-      <c r="F51" s="57"/>
-      <c r="G51" s="14"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="54"/>
+      <c r="F51" s="55"/>
+      <c r="G51" s="56"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="8"/>
-      <c r="B52" s="53"/>
+      <c r="B52" s="51"/>
       <c r="C52" s="54"/>
-      <c r="D52" s="55"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="57"/>
-      <c r="G52" s="14"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="54"/>
+      <c r="F52" s="55"/>
+      <c r="G52" s="56"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="8"/>
-      <c r="B53" s="53"/>
-      <c r="C53" s="54"/>
-      <c r="D53" s="55"/>
-      <c r="E53" s="56"/>
-      <c r="F53" s="57"/>
+      <c r="A53" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" s="43" t="s">
+        <v>212</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="43" t="s">
+        <v>213</v>
+      </c>
+      <c r="F53" s="20"/>
       <c r="G53" s="14"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" s="8"/>
-      <c r="B54" s="53"/>
-      <c r="C54" s="54"/>
-      <c r="D54" s="55"/>
-      <c r="E54" s="56"/>
-      <c r="F54" s="57"/>
+      <c r="A54" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="43" t="s">
+        <v>212</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="F54" s="20"/>
       <c r="G54" s="14"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A55" s="8"/>
-      <c r="B55" s="53"/>
-      <c r="C55" s="54"/>
-      <c r="D55" s="55"/>
-      <c r="E55" s="56"/>
-      <c r="F55" s="57"/>
+      <c r="A55" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" s="43" t="s">
+        <v>212</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="F55" s="20"/>
       <c r="G55" s="14"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="8"/>
-      <c r="G56" s="14"/>
+      <c r="B56" s="51"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="54"/>
+      <c r="F56" s="55"/>
+      <c r="G56" s="57"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="8"/>
-      <c r="B57" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C57" s="13"/>
-      <c r="D57" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E57" s="45" t="s">
-        <v>188</v>
-      </c>
-      <c r="F57" s="20" t="s">
-        <v>146</v>
-      </c>
+      <c r="B57" s="51"/>
+      <c r="C57" s="52"/>
+      <c r="D57" s="53"/>
+      <c r="E57" s="54"/>
+      <c r="F57" s="55"/>
       <c r="G57" s="14"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="8"/>
-      <c r="B58" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C58" s="13"/>
-      <c r="D58" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E58" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="F58" s="20" t="s">
-        <v>145</v>
-      </c>
+      <c r="B58" s="51"/>
+      <c r="C58" s="52"/>
+      <c r="D58" s="53"/>
+      <c r="E58" s="54"/>
+      <c r="F58" s="55"/>
       <c r="G58" s="14"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="8"/>
-      <c r="B59" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C59" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="D59" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E59" s="45" t="s">
-        <v>189</v>
-      </c>
-      <c r="F59" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="G59" s="15"/>
+      <c r="B59" s="51"/>
+      <c r="C59" s="52"/>
+      <c r="D59" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="54" t="s">
+        <v>205</v>
+      </c>
+      <c r="F59" s="55"/>
+      <c r="G59" s="14"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="8"/>
-      <c r="B60" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C60" s="13"/>
-      <c r="D60" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E60" s="45" t="s">
-        <v>190</v>
-      </c>
-      <c r="F60" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="G60" s="15"/>
+      <c r="B60" s="51"/>
+      <c r="C60" s="52"/>
+      <c r="D60" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="54" t="s">
+        <v>206</v>
+      </c>
+      <c r="F60" s="55"/>
+      <c r="G60" s="14"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="8"/>
-      <c r="B61" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C61" s="13"/>
-      <c r="D61" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E61" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="F61" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="G61" s="15"/>
+      <c r="B61" s="51"/>
+      <c r="C61" s="52"/>
+      <c r="D61" s="53"/>
+      <c r="E61" s="54"/>
+      <c r="F61" s="55"/>
+      <c r="G61" s="14"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="8"/>
-      <c r="B62" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E62" s="45" t="s">
-        <v>191</v>
-      </c>
-      <c r="F62" s="20" t="s">
-        <v>149</v>
-      </c>
+      <c r="B62" s="51"/>
+      <c r="C62" s="52"/>
+      <c r="D62" s="53"/>
+      <c r="E62" s="54"/>
+      <c r="F62" s="55"/>
       <c r="G62" s="14"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="8"/>
-      <c r="B63" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C63" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E63" s="45" t="s">
-        <v>192</v>
-      </c>
-      <c r="F63" s="20" t="s">
-        <v>150</v>
-      </c>
+      <c r="B63" s="51"/>
+      <c r="C63" s="52"/>
+      <c r="D63" s="53"/>
+      <c r="E63" s="54"/>
+      <c r="F63" s="55"/>
       <c r="G63" s="14"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="8"/>
-      <c r="B64" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C64" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E64" s="45" t="s">
-        <v>193</v>
-      </c>
-      <c r="F64" s="20" t="s">
-        <v>151</v>
-      </c>
+      <c r="B64" s="51"/>
+      <c r="C64" s="52"/>
+      <c r="D64" s="53"/>
+      <c r="E64" s="54"/>
+      <c r="F64" s="55"/>
       <c r="G64" s="14"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="8"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E65" s="45" t="s">
-        <v>194</v>
-      </c>
-      <c r="F65" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="G65" s="15"/>
+      <c r="G65" s="14"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="8"/>
-      <c r="B66" s="9"/>
+      <c r="B66" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="C66" s="13"/>
-      <c r="D66" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E66" s="45" t="s">
-        <v>195</v>
+      <c r="D66" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E66" s="43" t="s">
+        <v>186</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="G66" s="15"/>
+        <v>146</v>
+      </c>
+      <c r="G66" s="14"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="8"/>
-      <c r="B67" s="9"/>
+      <c r="B67" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="C67" s="13"/>
-      <c r="D67" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E67" s="45" t="s">
-        <v>196</v>
+      <c r="D67" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E67" s="43" t="s">
+        <v>20</v>
       </c>
       <c r="F67" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="G67" s="15"/>
+        <v>145</v>
+      </c>
+      <c r="G67" s="14"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="8"/>
@@ -4043,18 +4437,18 @@
         <v>62</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D68" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E68" s="45" t="s">
-        <v>197</v>
+      <c r="E68" s="43" t="s">
+        <v>187</v>
       </c>
       <c r="F68" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="G68" s="14"/>
+        <v>147</v>
+      </c>
+      <c r="G68" s="15"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="8"/>
@@ -4065,162 +4459,200 @@
       <c r="D69" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E69" s="10" t="s">
-        <v>90</v>
+      <c r="E69" s="43" t="s">
+        <v>188</v>
       </c>
       <c r="F69" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="G69" s="14"/>
+        <v>148</v>
+      </c>
+      <c r="G69" s="15"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="8"/>
       <c r="B70" s="9" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="C70" s="13"/>
       <c r="D70" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E70" s="10" t="s">
-        <v>95</v>
+      <c r="E70" s="43" t="s">
+        <v>20</v>
       </c>
       <c r="F70" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="G70" s="14"/>
+        <v>145</v>
+      </c>
+      <c r="G70" s="15"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="8"/>
-      <c r="B71" s="9"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E71" s="10" t="s">
-        <v>105</v>
+      <c r="B71" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E71" s="43" t="s">
+        <v>189</v>
       </c>
       <c r="F71" s="20" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="G71" s="14"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="8"/>
-      <c r="B72" s="9"/>
-      <c r="C72" s="13"/>
-      <c r="D72" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E72" s="10" t="s">
-        <v>99</v>
+      <c r="B72" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E72" s="43" t="s">
+        <v>190</v>
       </c>
       <c r="F72" s="20" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="G72" s="14"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="8"/>
-      <c r="B73" s="9"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="F73" s="20"/>
+      <c r="B73" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E73" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="F73" s="20" t="s">
+        <v>151</v>
+      </c>
       <c r="G73" s="14"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="8"/>
-      <c r="B74" s="9"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="F74" s="20"/>
-      <c r="G74" s="14"/>
+      <c r="B74" s="10"/>
+      <c r="C74" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E74" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="F74" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="G74" s="15"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="8"/>
-      <c r="B75" s="9" t="s">
-        <v>103</v>
-      </c>
+      <c r="B75" s="9"/>
       <c r="C75" s="13"/>
-      <c r="D75" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E75" s="10" t="s">
-        <v>96</v>
+      <c r="D75" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E75" s="43" t="s">
+        <v>193</v>
       </c>
       <c r="F75" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="G75" s="14"/>
+        <v>153</v>
+      </c>
+      <c r="G75" s="15"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="8"/>
       <c r="B76" s="9"/>
       <c r="C76" s="13"/>
-      <c r="D76" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E76" s="10" t="s">
-        <v>100</v>
+      <c r="D76" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E76" s="43" t="s">
+        <v>194</v>
       </c>
       <c r="F76" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="G76" s="14"/>
+        <v>154</v>
+      </c>
+      <c r="G76" s="15"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="8"/>
-      <c r="B77" s="9"/>
-      <c r="C77" s="13"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="F77" s="20"/>
+      <c r="B77" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C77" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E77" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="F77" s="20" t="s">
+        <v>155</v>
+      </c>
       <c r="G77" s="14"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="8"/>
-      <c r="B78" s="9"/>
+      <c r="B78" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="C78" s="13"/>
-      <c r="D78" s="11"/>
+      <c r="D78" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="E78" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F78" s="20"/>
+        <v>90</v>
+      </c>
+      <c r="F78" s="20" t="s">
+        <v>156</v>
+      </c>
       <c r="G78" s="14"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="8"/>
-      <c r="B79" s="9"/>
+      <c r="B79" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="C79" s="13"/>
-      <c r="D79" s="11"/>
+      <c r="D79" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="E79" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F79" s="20"/>
+        <v>95</v>
+      </c>
+      <c r="F79" s="20" t="s">
+        <v>157</v>
+      </c>
       <c r="G79" s="14"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="8"/>
-      <c r="B80" s="9" t="s">
-        <v>103</v>
-      </c>
+      <c r="B80" s="9"/>
       <c r="C80" s="13"/>
       <c r="D80" s="11" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="F80" s="20" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="G80" s="14"/>
     </row>
@@ -4232,10 +4664,10 @@
         <v>80</v>
       </c>
       <c r="E81" s="10" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F81" s="20" t="s">
-        <v>111</v>
+        <v>158</v>
       </c>
       <c r="G81" s="14"/>
     </row>
@@ -4245,7 +4677,7 @@
       <c r="C82" s="13"/>
       <c r="D82" s="11"/>
       <c r="E82" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F82" s="20"/>
       <c r="G82" s="14"/>
@@ -4256,278 +4688,276 @@
       <c r="C83" s="13"/>
       <c r="D83" s="11"/>
       <c r="E83" s="10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F83" s="20"/>
       <c r="G83" s="14"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="8"/>
-      <c r="B84" s="9"/>
+      <c r="B84" s="9" t="s">
+        <v>103</v>
+      </c>
       <c r="C84" s="13"/>
-      <c r="D84" s="11"/>
+      <c r="D84" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="E84" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="F84" s="20"/>
+        <v>96</v>
+      </c>
+      <c r="F84" s="20" t="s">
+        <v>159</v>
+      </c>
       <c r="G84" s="14"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="8"/>
-      <c r="B85" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C85" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="D85" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E85" s="12" t="s">
-        <v>91</v>
+      <c r="B85" s="9"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>100</v>
       </c>
       <c r="F85" s="20" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
       <c r="G85" s="14"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="8"/>
-      <c r="B86" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C86" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="D86" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E86" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F86" s="20" t="s">
-        <v>162</v>
-      </c>
+      <c r="B86" s="9"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="11"/>
+      <c r="E86" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F86" s="20"/>
       <c r="G86" s="14"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="8"/>
-      <c r="B87" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C87" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="D87" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="B87" s="9"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="11"/>
       <c r="E87" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="F87" s="20" t="s">
-        <v>145</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="F87" s="20"/>
       <c r="G87" s="14"/>
     </row>
-    <row r="88" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A88" s="26"/>
-      <c r="B88" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C88" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="D88" s="35"/>
-      <c r="E88" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="F88" s="36"/>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" s="8"/>
+      <c r="B88" s="9"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="11"/>
+      <c r="E88" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F88" s="20"/>
       <c r="G88" s="14"/>
     </row>
-    <row r="89" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A89" s="26"/>
-      <c r="B89" s="10"/>
-      <c r="C89" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D89" s="11"/>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A89" s="8"/>
+      <c r="B89" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C89" s="13"/>
+      <c r="D89" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="E89" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="F89" s="20"/>
+        <v>97</v>
+      </c>
+      <c r="F89" s="20" t="s">
+        <v>160</v>
+      </c>
       <c r="G89" s="14"/>
     </row>
-    <row r="90" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A90" s="26"/>
-      <c r="B90" s="10"/>
-      <c r="C90" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D90" s="11"/>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" s="8"/>
+      <c r="B90" s="9"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="11" t="s">
+        <v>80</v>
+      </c>
       <c r="E90" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="F90" s="20"/>
+        <v>109</v>
+      </c>
+      <c r="F90" s="20" t="s">
+        <v>111</v>
+      </c>
       <c r="G90" s="14"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A91" s="26"/>
-      <c r="B91" s="10"/>
-      <c r="C91" s="13" t="s">
-        <v>112</v>
-      </c>
+      <c r="A91" s="8"/>
+      <c r="B91" s="9"/>
+      <c r="C91" s="13"/>
       <c r="D91" s="11"/>
       <c r="E91" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="F91" s="21"/>
+        <v>102</v>
+      </c>
+      <c r="F91" s="20"/>
       <c r="G91" s="14"/>
     </row>
-    <row r="92" spans="1:7" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A92" s="26"/>
-      <c r="B92" s="10"/>
-      <c r="C92" s="13" t="s">
-        <v>113</v>
-      </c>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92" s="8"/>
+      <c r="B92" s="9"/>
+      <c r="C92" s="13"/>
       <c r="D92" s="11"/>
-      <c r="E92" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="F92" s="21" t="s">
-        <v>115</v>
-      </c>
+      <c r="E92" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="F92" s="20"/>
       <c r="G92" s="14"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A93" s="26"/>
-      <c r="B93" s="10"/>
-      <c r="C93" s="13" t="s">
-        <v>113</v>
-      </c>
+      <c r="A93" s="8"/>
+      <c r="B93" s="9"/>
+      <c r="C93" s="13"/>
       <c r="D93" s="11"/>
-      <c r="E93" t="s">
-        <v>55</v>
-      </c>
-      <c r="F93" s="21"/>
+      <c r="E93" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="F93" s="20"/>
       <c r="G93" s="14"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A94" s="26"/>
-      <c r="B94" s="10"/>
-      <c r="C94" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D94" s="11"/>
-      <c r="E94" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="F94" s="21"/>
+      <c r="A94" s="8"/>
+      <c r="B94" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D94" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E94" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F94" s="20" t="s">
+        <v>161</v>
+      </c>
       <c r="G94" s="14"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A95" s="26"/>
-      <c r="B95" s="10"/>
-      <c r="C95" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D95" s="11"/>
-      <c r="E95" s="10" t="s">
+      <c r="A95" s="8"/>
+      <c r="B95" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C95" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D95" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E95" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F95" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="G95" s="14"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A96" s="8"/>
+      <c r="B96" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C96" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="F95" s="21"/>
-      <c r="G95" s="14"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A96" s="26"/>
-      <c r="B96" s="10"/>
-      <c r="C96" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D96" s="11"/>
+      <c r="D96" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="E96" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F96" s="21"/>
+      <c r="F96" s="20" t="s">
+        <v>145</v>
+      </c>
       <c r="G96" s="14"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" s="26"/>
-      <c r="B97" s="10"/>
-      <c r="C97" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D97" s="11"/>
-      <c r="E97" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="F97" s="21"/>
+      <c r="B97" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C97" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D97" s="35"/>
+      <c r="E97" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="F97" s="36"/>
       <c r="G97" s="14"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" s="26"/>
       <c r="B98" s="10"/>
       <c r="C98" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D98" s="11"/>
       <c r="E98" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F98" s="21"/>
+      <c r="F98" s="20"/>
       <c r="G98" s="14"/>
     </row>
-    <row r="99" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" s="26"/>
       <c r="B99" s="10"/>
-      <c r="C99" s="4" t="s">
-        <v>116</v>
+      <c r="C99" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="D99" s="11"/>
-      <c r="E99" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="F99" s="21"/>
+      <c r="E99" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F99" s="20"/>
       <c r="G99" s="14"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" s="26"/>
       <c r="B100" s="10"/>
-      <c r="C100" s="30" t="s">
-        <v>117</v>
+      <c r="C100" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="D100" s="11"/>
       <c r="E100" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F100" s="21" t="s">
-        <v>118</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="F100" s="21"/>
       <c r="G100" s="14"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="28.5" x14ac:dyDescent="0.35">
       <c r="A101" s="26"/>
       <c r="B101" s="10"/>
-      <c r="C101" s="30" t="s">
-        <v>117</v>
+      <c r="C101" s="13" t="s">
+        <v>113</v>
       </c>
       <c r="D101" s="11"/>
-      <c r="E101" s="10" t="s">
-        <v>20</v>
+      <c r="E101" s="27" t="s">
+        <v>114</v>
       </c>
       <c r="F101" s="21" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G101" s="14"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" s="26"/>
       <c r="B102" s="10"/>
-      <c r="C102" s="30" t="s">
-        <v>117</v>
+      <c r="C102" s="13" t="s">
+        <v>113</v>
       </c>
       <c r="D102" s="11"/>
-      <c r="E102" s="10" t="s">
-        <v>70</v>
+      <c r="E102" t="s">
+        <v>55</v>
       </c>
       <c r="F102" s="21"/>
       <c r="G102" s="14"/>
@@ -4535,8 +4965,8 @@
     <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" s="26"/>
       <c r="B103" s="10"/>
-      <c r="C103" s="13" t="s">
-        <v>70</v>
+      <c r="C103" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D103" s="11"/>
       <c r="E103" s="27" t="s">
@@ -4545,15 +4975,15 @@
       <c r="F103" s="21"/>
       <c r="G103" s="14"/>
     </row>
-    <row r="104" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" s="26"/>
       <c r="B104" s="10"/>
-      <c r="C104" s="4" t="s">
-        <v>119</v>
+      <c r="C104" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D104" s="11"/>
-      <c r="E104" s="27" t="s">
-        <v>114</v>
+      <c r="E104" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="F104" s="21"/>
       <c r="G104" s="14"/>
@@ -4561,12 +4991,12 @@
     <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" s="26"/>
       <c r="B105" s="10"/>
-      <c r="C105" s="13" t="s">
-        <v>120</v>
+      <c r="C105" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D105" s="11"/>
       <c r="E105" s="10" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="F105" s="21"/>
       <c r="G105" s="14"/>
@@ -4575,11 +5005,11 @@
       <c r="A106" s="26"/>
       <c r="B106" s="10"/>
       <c r="C106" s="13" t="s">
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="D106" s="11"/>
-      <c r="E106" s="10" t="s">
-        <v>20</v>
+      <c r="E106" s="27" t="s">
+        <v>114</v>
       </c>
       <c r="F106" s="21"/>
       <c r="G106" s="14"/>
@@ -4588,20 +5018,20 @@
       <c r="A107" s="26"/>
       <c r="B107" s="10"/>
       <c r="C107" s="13" t="s">
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="D107" s="11"/>
       <c r="E107" s="10" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="F107" s="21"/>
       <c r="G107" s="14"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A108" s="26"/>
       <c r="B108" s="10"/>
-      <c r="C108" s="13" t="s">
-        <v>76</v>
+      <c r="C108" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="D108" s="11"/>
       <c r="E108" s="27" t="s">
@@ -4610,94 +5040,94 @@
       <c r="F108" s="21"/>
       <c r="G108" s="14"/>
     </row>
-    <row r="109" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" s="26"/>
-      <c r="B109" s="26"/>
-      <c r="C109" s="4" t="s">
-        <v>122</v>
+      <c r="B109" s="10"/>
+      <c r="C109" s="30" t="s">
+        <v>117</v>
       </c>
       <c r="D109" s="11"/>
       <c r="E109" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F109" s="23" t="s">
-        <v>83</v>
+      <c r="F109" s="21" t="s">
+        <v>118</v>
       </c>
       <c r="G109" s="14"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110" s="26"/>
-      <c r="B110" s="26"/>
-      <c r="C110" s="13" t="s">
-        <v>121</v>
+      <c r="B110" s="10"/>
+      <c r="C110" s="30" t="s">
+        <v>117</v>
       </c>
       <c r="D110" s="11"/>
       <c r="E110" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F110" s="21"/>
+      <c r="F110" s="21" t="s">
+        <v>118</v>
+      </c>
       <c r="G110" s="14"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" s="26"/>
-      <c r="B111" s="26"/>
-      <c r="C111" s="13" t="s">
-        <v>121</v>
+      <c r="B111" s="10"/>
+      <c r="C111" s="30" t="s">
+        <v>117</v>
       </c>
       <c r="D111" s="11"/>
       <c r="E111" s="10" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="F111" s="21"/>
       <c r="G111" s="14"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" s="26"/>
-      <c r="B112" s="26"/>
+      <c r="B112" s="10"/>
       <c r="C112" s="13" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="D112" s="11"/>
-      <c r="E112" s="10" t="s">
-        <v>136</v>
+      <c r="E112" s="27" t="s">
+        <v>114</v>
       </c>
       <c r="F112" s="21"/>
       <c r="G112" s="14"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A113" s="26"/>
-      <c r="B113" s="26"/>
-      <c r="C113" s="13" t="s">
-        <v>59</v>
+      <c r="B113" s="10"/>
+      <c r="C113" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="D113" s="11"/>
-      <c r="E113" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="F113" s="21" t="s">
-        <v>138</v>
-      </c>
+      <c r="E113" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="F113" s="21"/>
       <c r="G113" s="14"/>
     </row>
-    <row r="114" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" s="26"/>
-      <c r="B114" s="26"/>
-      <c r="C114" s="15" t="s">
-        <v>123</v>
+      <c r="B114" s="10"/>
+      <c r="C114" s="13" t="s">
+        <v>120</v>
       </c>
       <c r="D114" s="11"/>
       <c r="E114" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F114" s="21" t="s">
-        <v>83</v>
-      </c>
+      <c r="F114" s="21"/>
       <c r="G114" s="14"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" s="26"/>
-      <c r="B115" s="26"/>
-      <c r="C115" s="15"/>
+      <c r="B115" s="10"/>
+      <c r="C115" s="13" t="s">
+        <v>120</v>
+      </c>
       <c r="D115" s="11"/>
       <c r="E115" s="10" t="s">
         <v>20</v>
@@ -4707,61 +5137,67 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" s="26"/>
-      <c r="B116" s="26"/>
-      <c r="C116" s="15"/>
+      <c r="B116" s="10"/>
+      <c r="C116" s="13" t="s">
+        <v>120</v>
+      </c>
       <c r="D116" s="11"/>
       <c r="E116" s="10" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="F116" s="21"/>
       <c r="G116" s="14"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" s="26"/>
-      <c r="B117" s="26"/>
-      <c r="C117" s="15"/>
+      <c r="B117" s="10"/>
+      <c r="C117" s="13" t="s">
+        <v>76</v>
+      </c>
       <c r="D117" s="11"/>
-      <c r="E117" s="10" t="s">
-        <v>81</v>
+      <c r="E117" s="27" t="s">
+        <v>114</v>
       </c>
       <c r="F117" s="21"/>
       <c r="G117" s="14"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A118" s="26"/>
       <c r="B118" s="26"/>
-      <c r="C118" s="13" t="s">
-        <v>60</v>
+      <c r="C118" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="D118" s="11"/>
-      <c r="E118" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="F118" s="21"/>
+      <c r="E118" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F118" s="23" t="s">
+        <v>83</v>
+      </c>
       <c r="G118" s="14"/>
     </row>
-    <row r="119" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" s="26"/>
       <c r="B119" s="26"/>
-      <c r="C119" s="15" t="s">
-        <v>124</v>
+      <c r="C119" s="13" t="s">
+        <v>121</v>
       </c>
       <c r="D119" s="11"/>
       <c r="E119" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F119" s="21" t="s">
-        <v>83</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F119" s="21"/>
       <c r="G119" s="14"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" s="26"/>
       <c r="B120" s="26"/>
-      <c r="C120" s="15"/>
+      <c r="C120" s="13" t="s">
+        <v>121</v>
+      </c>
       <c r="D120" s="11"/>
       <c r="E120" s="10" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="F120" s="21"/>
       <c r="G120" s="14"/>
@@ -4769,10 +5205,12 @@
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" s="26"/>
       <c r="B121" s="26"/>
-      <c r="C121" s="15"/>
+      <c r="C121" s="13" t="s">
+        <v>121</v>
+      </c>
       <c r="D121" s="11"/>
       <c r="E121" s="10" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="F121" s="21"/>
       <c r="G121" s="14"/>
@@ -4780,177 +5218,177 @@
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A122" s="26"/>
       <c r="B122" s="26"/>
-      <c r="C122" s="15"/>
+      <c r="C122" s="13" t="s">
+        <v>59</v>
+      </c>
       <c r="D122" s="11"/>
-      <c r="E122" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F122" s="21"/>
+      <c r="E122" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="F122" s="21" t="s">
+        <v>138</v>
+      </c>
       <c r="G122" s="14"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A123" s="26"/>
       <c r="B123" s="26"/>
-      <c r="C123" s="13" t="s">
-        <v>61</v>
+      <c r="C123" s="15" t="s">
+        <v>123</v>
       </c>
       <c r="D123" s="11"/>
-      <c r="E123" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="F123" s="21"/>
+      <c r="E123" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F123" s="21" t="s">
+        <v>83</v>
+      </c>
       <c r="G123" s="14"/>
     </row>
-    <row r="124" spans="1:7" s="5" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124" s="26"/>
-      <c r="B124" s="9"/>
-      <c r="C124" s="15" t="s">
-        <v>125</v>
-      </c>
+      <c r="B124" s="26"/>
+      <c r="C124" s="15"/>
       <c r="D124" s="11"/>
       <c r="E124" s="10" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="F124" s="21"/>
       <c r="G124" s="14"/>
     </row>
-    <row r="125" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A125" s="26"/>
-      <c r="B125" s="9"/>
-      <c r="C125" s="31" t="s">
-        <v>139</v>
-      </c>
+      <c r="B125" s="26"/>
+      <c r="C125" s="15"/>
       <c r="D125" s="11"/>
       <c r="E125" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F125" s="21" t="s">
-        <v>77</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F125" s="21"/>
       <c r="G125" s="14"/>
     </row>
-    <row r="126" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A126" s="26"/>
-      <c r="B126" s="9"/>
-      <c r="C126" s="31" t="s">
-        <v>139</v>
-      </c>
+      <c r="B126" s="26"/>
+      <c r="C126" s="15"/>
       <c r="D126" s="11"/>
       <c r="E126" s="10" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="F126" s="21"/>
       <c r="G126" s="14"/>
     </row>
-    <row r="127" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" s="26"/>
-      <c r="B127" s="9"/>
-      <c r="C127" s="31" t="s">
-        <v>139</v>
+      <c r="B127" s="26"/>
+      <c r="C127" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="D127" s="11"/>
-      <c r="E127" s="10" t="s">
-        <v>84</v>
+      <c r="E127" s="32" t="s">
+        <v>137</v>
       </c>
       <c r="F127" s="21"/>
       <c r="G127" s="14"/>
     </row>
-    <row r="128" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A128" s="26"/>
-      <c r="B128" s="9"/>
-      <c r="C128" s="13" t="s">
-        <v>59</v>
+      <c r="B128" s="26"/>
+      <c r="C128" s="15" t="s">
+        <v>124</v>
       </c>
       <c r="D128" s="11"/>
-      <c r="E128" s="32" t="s">
-        <v>137</v>
+      <c r="E128" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="F128" s="21" t="s">
-        <v>138</v>
+        <v>83</v>
       </c>
       <c r="G128" s="14"/>
     </row>
-    <row r="129" spans="1:7" s="5" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129" s="26"/>
-      <c r="B129" s="9"/>
-      <c r="C129" s="15" t="s">
-        <v>126</v>
-      </c>
+      <c r="B129" s="26"/>
+      <c r="C129" s="15"/>
       <c r="D129" s="11"/>
       <c r="E129" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F129" s="21" t="s">
-        <v>78</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F129" s="21"/>
       <c r="G129" s="14"/>
     </row>
-    <row r="130" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A130" s="26"/>
-      <c r="B130" s="9"/>
-      <c r="C130" s="29"/>
+      <c r="B130" s="26"/>
+      <c r="C130" s="15"/>
       <c r="D130" s="11"/>
       <c r="E130" s="10" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="F130" s="21"/>
       <c r="G130" s="14"/>
     </row>
-    <row r="131" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131" s="26"/>
-      <c r="B131" s="9"/>
-      <c r="C131" s="29"/>
+      <c r="B131" s="26"/>
+      <c r="C131" s="15"/>
       <c r="D131" s="11"/>
       <c r="E131" s="10" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="F131" s="21"/>
       <c r="G131" s="14"/>
     </row>
-    <row r="132" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132" s="26"/>
-      <c r="B132" s="9"/>
-      <c r="C132" s="28"/>
+      <c r="B132" s="26"/>
+      <c r="C132" s="13" t="s">
+        <v>61</v>
+      </c>
       <c r="D132" s="11"/>
-      <c r="E132" s="10" t="s">
-        <v>85</v>
+      <c r="E132" s="32" t="s">
+        <v>137</v>
       </c>
       <c r="F132" s="21"/>
       <c r="G132" s="14"/>
     </row>
-    <row r="133" spans="1:7" s="5" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A133" s="26"/>
       <c r="B133" s="9"/>
       <c r="C133" s="15" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="D133" s="11"/>
       <c r="E133" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F133" s="21" t="s">
-        <v>78</v>
-      </c>
+      <c r="F133" s="21"/>
       <c r="G133" s="14"/>
     </row>
     <row r="134" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A134" s="26"/>
       <c r="B134" s="9"/>
-      <c r="C134" s="29"/>
+      <c r="C134" s="31" t="s">
+        <v>139</v>
+      </c>
       <c r="D134" s="11"/>
       <c r="E134" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F134" s="21"/>
+      <c r="F134" s="21" t="s">
+        <v>77</v>
+      </c>
       <c r="G134" s="14"/>
     </row>
     <row r="135" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A135" s="26"/>
       <c r="B135" s="9"/>
-      <c r="C135" s="29"/>
+      <c r="C135" s="31" t="s">
+        <v>139</v>
+      </c>
       <c r="D135" s="11"/>
-      <c r="E135" s="9" t="s">
-        <v>61</v>
+      <c r="E135" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="F135" s="21"/>
       <c r="G135" s="14"/>
@@ -4958,10 +5396,12 @@
     <row r="136" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A136" s="26"/>
       <c r="B136" s="9"/>
-      <c r="C136" s="29"/>
+      <c r="C136" s="31" t="s">
+        <v>139</v>
+      </c>
       <c r="D136" s="11"/>
-      <c r="E136" s="9" t="s">
-        <v>58</v>
+      <c r="E136" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="F136" s="21"/>
       <c r="G136" s="14"/>
@@ -4969,221 +5409,215 @@
     <row r="137" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A137" s="26"/>
       <c r="B137" s="9"/>
-      <c r="C137" s="9" t="s">
-        <v>61</v>
+      <c r="C137" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="D137" s="11"/>
       <c r="E137" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="F137" s="21"/>
+      <c r="F137" s="21" t="s">
+        <v>138</v>
+      </c>
       <c r="G137" s="14"/>
     </row>
-    <row r="138" spans="1:7" s="5" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A138" s="26"/>
       <c r="B138" s="9"/>
       <c r="C138" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D138" s="11"/>
       <c r="E138" s="10" t="s">
         <v>57</v>
       </c>
       <c r="F138" s="21" t="s">
-        <v>129</v>
+        <v>78</v>
       </c>
       <c r="G138" s="14"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A139" s="26"/>
       <c r="B139" s="9"/>
-      <c r="C139" s="13" t="s">
-        <v>128</v>
-      </c>
+      <c r="C139" s="29"/>
       <c r="D139" s="11"/>
       <c r="E139" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F139" s="22"/>
+      <c r="F139" s="21"/>
       <c r="G139" s="14"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A140" s="26"/>
       <c r="B140" s="9"/>
-      <c r="C140" s="13" t="s">
-        <v>128</v>
-      </c>
+      <c r="C140" s="29"/>
       <c r="D140" s="11"/>
-      <c r="E140" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G140" s="13"/>
-    </row>
-    <row r="141" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E140" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F140" s="21"/>
+      <c r="G140" s="14"/>
+    </row>
+    <row r="141" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A141" s="26"/>
       <c r="B141" s="9"/>
-      <c r="C141" s="15" t="s">
-        <v>130</v>
-      </c>
+      <c r="C141" s="28"/>
       <c r="D141" s="11"/>
       <c r="E141" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F141" s="22"/>
+        <v>85</v>
+      </c>
+      <c r="F141" s="21"/>
       <c r="G141" s="14"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A142" s="26"/>
       <c r="B142" s="9"/>
-      <c r="C142" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="D142" s="9"/>
+      <c r="C142" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="D142" s="11"/>
       <c r="E142" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F142" s="22"/>
+        <v>57</v>
+      </c>
+      <c r="F142" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="G142" s="14"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A143" s="26"/>
       <c r="B143" s="9"/>
-      <c r="C143" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="D143" s="9"/>
-      <c r="E143" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F143" s="22"/>
+      <c r="C143" s="29"/>
+      <c r="D143" s="11"/>
+      <c r="E143" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F143" s="21"/>
       <c r="G143" s="14"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A144" s="26"/>
       <c r="B144" s="9"/>
-      <c r="C144" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="D144" s="9"/>
+      <c r="C144" s="29"/>
+      <c r="D144" s="11"/>
       <c r="E144" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F144" s="22"/>
+        <v>61</v>
+      </c>
+      <c r="F144" s="21"/>
       <c r="G144" s="14"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A145" s="26"/>
       <c r="B145" s="9"/>
-      <c r="C145" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D145" s="9"/>
-      <c r="E145" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="F145" s="22"/>
+      <c r="C145" s="29"/>
+      <c r="D145" s="11"/>
+      <c r="E145" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F145" s="21"/>
       <c r="G145" s="14"/>
     </row>
-    <row r="146" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A146" s="26"/>
       <c r="B146" s="9"/>
-      <c r="C146" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="D146" s="9"/>
-      <c r="E146" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F146" s="22"/>
+      <c r="C146" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D146" s="11"/>
+      <c r="E146" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="F146" s="21"/>
       <c r="G146" s="14"/>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:7" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A147" s="26"/>
       <c r="B147" s="9"/>
-      <c r="C147" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D147" s="9"/>
+      <c r="C147" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="D147" s="11"/>
       <c r="E147" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F147" s="22"/>
-      <c r="G147" s="16"/>
+        <v>57</v>
+      </c>
+      <c r="F147" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="G147" s="14"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A148" s="26"/>
       <c r="B148" s="9"/>
-      <c r="C148" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D148" s="9"/>
-      <c r="E148" s="9" t="s">
-        <v>60</v>
+      <c r="C148" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D148" s="11"/>
+      <c r="E148" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="F148" s="22"/>
-      <c r="G148" s="16"/>
+      <c r="G148" s="14"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A149" s="26"/>
       <c r="B149" s="9"/>
-      <c r="C149" s="14" t="s">
-        <v>133</v>
+      <c r="C149" s="13" t="s">
+        <v>128</v>
       </c>
       <c r="D149" s="11"/>
       <c r="E149" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F149" s="22"/>
-      <c r="G149" s="16"/>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+      <c r="G149" s="13"/>
+    </row>
+    <row r="150" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="26"/>
       <c r="B150" s="9"/>
-      <c r="C150" s="14" t="s">
-        <v>73</v>
+      <c r="C150" s="15" t="s">
+        <v>130</v>
       </c>
       <c r="D150" s="11"/>
-      <c r="E150" s="32" t="s">
-        <v>137</v>
+      <c r="E150" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="F150" s="22"/>
-      <c r="G150" s="16"/>
-    </row>
-    <row r="151" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="G150" s="14"/>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A151" s="26"/>
       <c r="B151" s="9"/>
-      <c r="C151" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="D151" s="11"/>
+      <c r="C151" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="D151" s="9"/>
       <c r="E151" s="10" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="F151" s="22"/>
-      <c r="G151" s="16"/>
+      <c r="G151" s="14"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A152" s="26"/>
       <c r="B152" s="9"/>
-      <c r="C152" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D152" s="11"/>
-      <c r="E152" s="10" t="s">
-        <v>20</v>
+      <c r="C152" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="D152" s="9"/>
+      <c r="E152" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="F152" s="22"/>
-      <c r="G152" s="16"/>
+      <c r="G152" s="14"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A153" s="26"/>
       <c r="B153" s="9"/>
-      <c r="C153" s="14" t="s">
-        <v>135</v>
+      <c r="C153" s="31" t="s">
+        <v>131</v>
       </c>
       <c r="D153" s="9"/>
       <c r="E153" s="9" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="F153" s="22"/>
       <c r="G153" s="14"/>
@@ -5192,534 +5626,679 @@
       <c r="A154" s="26"/>
       <c r="B154" s="9"/>
       <c r="C154" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D154" s="9"/>
+      <c r="E154" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="F154" s="22"/>
+      <c r="G154" s="14"/>
+    </row>
+    <row r="155" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A155" s="26"/>
+      <c r="B155" s="9"/>
+      <c r="C155" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D155" s="9"/>
+      <c r="E155" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F155" s="22"/>
+      <c r="G155" s="14"/>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A156" s="26"/>
+      <c r="B156" s="9"/>
+      <c r="C156" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D156" s="9"/>
+      <c r="E156" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F156" s="22"/>
+      <c r="G156" s="16"/>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A157" s="26"/>
+      <c r="B157" s="9"/>
+      <c r="C157" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D157" s="9"/>
+      <c r="E157" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F157" s="22"/>
+      <c r="G157" s="16"/>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A158" s="26"/>
+      <c r="B158" s="9"/>
+      <c r="C158" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D158" s="11"/>
+      <c r="E158" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F158" s="22"/>
+      <c r="G158" s="16"/>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A159" s="26"/>
+      <c r="B159" s="9"/>
+      <c r="C159" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D159" s="11"/>
+      <c r="E159" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="F159" s="22"/>
+      <c r="G159" s="16"/>
+    </row>
+    <row r="160" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A160" s="26"/>
+      <c r="B160" s="9"/>
+      <c r="C160" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="D160" s="11"/>
+      <c r="E160" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F160" s="22"/>
+      <c r="G160" s="16"/>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A161" s="26"/>
+      <c r="B161" s="9"/>
+      <c r="C161" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="D154" s="10"/>
-      <c r="E154" s="9" t="s">
+      <c r="D161" s="11"/>
+      <c r="E161" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F161" s="22"/>
+      <c r="G161" s="16"/>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A162" s="26"/>
+      <c r="B162" s="9"/>
+      <c r="C162" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D162" s="9"/>
+      <c r="E162" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F162" s="22"/>
+      <c r="G162" s="14"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A163" s="26"/>
+      <c r="B163" s="9"/>
+      <c r="C163" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D163" s="10"/>
+      <c r="E163" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F154" s="20"/>
-      <c r="G154" s="16"/>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A155" s="8"/>
-      <c r="B155" s="9"/>
-      <c r="C155" s="14" t="s">
+      <c r="F163" s="20"/>
+      <c r="G163" s="16"/>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A164" s="8"/>
+      <c r="B164" s="9"/>
+      <c r="C164" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D155" s="10"/>
-      <c r="E155" s="32" t="s">
+      <c r="D164" s="10"/>
+      <c r="E164" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="F155" s="20"/>
-      <c r="G155" s="16"/>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A156" s="8"/>
-      <c r="B156" s="9" t="s">
+      <c r="F164" s="20"/>
+      <c r="G164" s="16"/>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A165" s="8"/>
+      <c r="B165" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C156" s="13"/>
-      <c r="D156" s="11"/>
-      <c r="E156" s="12" t="s">
+      <c r="C165" s="13"/>
+      <c r="D165" s="11"/>
+      <c r="E165" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="F156" s="20" t="s">
+      <c r="F165" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G156" s="14"/>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A157" s="8"/>
-      <c r="B157" s="9" t="s">
+      <c r="G165" s="14"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A166" s="8"/>
+      <c r="B166" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C157" s="13"/>
-      <c r="D157" s="10"/>
-      <c r="E157" s="12" t="s">
+      <c r="C166" s="13"/>
+      <c r="D166" s="10"/>
+      <c r="E166" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="F157" s="20" t="s">
+      <c r="F166" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G157" s="14"/>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A158">
-        <f>ROUND(COUNTA(A4:A157)/ROWS(A4:A157)*100,0)</f>
-        <v>21</v>
-      </c>
-      <c r="B158" s="25" t="s">
+      <c r="G166" s="14"/>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A167">
+        <f>ROUND(COUNTA(A4:A166)/ROWS(A4:A166)*100,0)</f>
+        <v>18</v>
+      </c>
+      <c r="B167" s="25" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A159" s="8"/>
-      <c r="F159" s="22"/>
-      <c r="G159" s="14"/>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C160" s="7"/>
-      <c r="D160" s="5"/>
-      <c r="E160" s="5"/>
-      <c r="F160" s="24"/>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A161" t="s">
-        <v>86</v>
-      </c>
-      <c r="C161" s="7"/>
-      <c r="D161" s="5"/>
-      <c r="E161" s="5"/>
-      <c r="F161" s="24"/>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B162" t="s">
-        <v>87</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E162" t="s">
-        <v>88</v>
-      </c>
-      <c r="F162" s="24"/>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F163" s="24"/>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C164" s="7"/>
-      <c r="D164" s="5"/>
-      <c r="E164" s="5"/>
-      <c r="F164" s="24"/>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C165" s="7"/>
-      <c r="D165" s="5"/>
-      <c r="E165" s="5"/>
-      <c r="F165" s="24"/>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C166" s="7"/>
-      <c r="D166" s="5"/>
-      <c r="E166" s="5"/>
-      <c r="F166" s="24"/>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C167" s="7"/>
-      <c r="D167" s="5"/>
-      <c r="E167" s="5"/>
-      <c r="F167" s="24"/>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C168" s="7"/>
-      <c r="D168" s="5"/>
-      <c r="E168" s="5"/>
-      <c r="F168" s="24"/>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A168" s="8"/>
+      <c r="F168" s="22"/>
+      <c r="G168" s="14"/>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C169" s="7"/>
       <c r="D169" s="5"/>
       <c r="E169" s="5"/>
       <c r="F169" s="24"/>
     </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>86</v>
+      </c>
+      <c r="C170" s="7"/>
+      <c r="D170" s="5"/>
+      <c r="E170" s="5"/>
+      <c r="F170" s="24"/>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B171" t="s">
+        <v>87</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E171" t="s">
+        <v>88</v>
+      </c>
+      <c r="F171" s="24"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F172" s="24"/>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C173" s="7"/>
+      <c r="D173" s="5"/>
+      <c r="E173" s="5"/>
+      <c r="F173" s="24"/>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C174" s="7"/>
+      <c r="D174" s="5"/>
+      <c r="E174" s="5"/>
+      <c r="F174" s="24"/>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C175" s="7"/>
+      <c r="D175" s="5"/>
+      <c r="E175" s="5"/>
+      <c r="F175" s="24"/>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C176" s="7"/>
+      <c r="D176" s="5"/>
+      <c r="E176" s="5"/>
+      <c r="F176" s="24"/>
+    </row>
+    <row r="177" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C177" s="7"/>
+      <c r="D177" s="5"/>
+      <c r="E177" s="5"/>
+      <c r="F177" s="24"/>
+    </row>
+    <row r="178" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C178" s="7"/>
+      <c r="D178" s="5"/>
+      <c r="E178" s="5"/>
+      <c r="F178" s="24"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A159 A88 B109:B123 A13:A14 A8:A9">
-    <cfRule type="notContainsBlanks" dxfId="77" priority="338">
+  <conditionalFormatting sqref="A168 A97 B118:B132 A13:A14 A8">
+    <cfRule type="notContainsBlanks" dxfId="90" priority="351">
       <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37:A56">
-    <cfRule type="notContainsBlanks" dxfId="76" priority="128">
+  <conditionalFormatting sqref="A37:A65">
+    <cfRule type="notContainsBlanks" dxfId="89" priority="141">
       <formula>LEN(TRIM(A37))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A94">
+    <cfRule type="notContainsBlanks" dxfId="87" priority="136">
+      <formula>LEN(TRIM(A94))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A79">
+    <cfRule type="notContainsBlanks" dxfId="86" priority="97">
+      <formula>LEN(TRIM(A79))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68">
+    <cfRule type="notContainsBlanks" dxfId="85" priority="140">
+      <formula>LEN(TRIM(A68))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71:A73">
+    <cfRule type="notContainsBlanks" dxfId="84" priority="139">
+      <formula>LEN(TRIM(A71))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A74:A76">
+    <cfRule type="notContainsBlanks" dxfId="83" priority="138">
+      <formula>LEN(TRIM(A74))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A165:A166">
+    <cfRule type="notContainsBlanks" dxfId="82" priority="133">
+      <formula>LEN(TRIM(A165))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67">
+    <cfRule type="notContainsBlanks" dxfId="81" priority="102">
+      <formula>LEN(TRIM(A67))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66">
+    <cfRule type="notContainsBlanks" dxfId="80" priority="103">
+      <formula>LEN(TRIM(A66))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A80">
+    <cfRule type="notContainsBlanks" dxfId="79" priority="96">
+      <formula>LEN(TRIM(A80))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82">
+    <cfRule type="notContainsBlanks" dxfId="78" priority="94">
+      <formula>LEN(TRIM(A82))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A83">
+    <cfRule type="notContainsBlanks" dxfId="77" priority="93">
+      <formula>LEN(TRIM(A83))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A81">
+    <cfRule type="notContainsBlanks" dxfId="76" priority="95">
+      <formula>LEN(TRIM(A81))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A84">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="92">
+      <formula>LEN(TRIM(A84))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70">
+    <cfRule type="notContainsBlanks" dxfId="74" priority="100">
+      <formula>LEN(TRIM(A70))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A78">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="98">
+      <formula>LEN(TRIM(A78))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="notContainsBlanks" dxfId="72" priority="101">
+      <formula>LEN(TRIM(A69))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A86">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="90">
+      <formula>LEN(TRIM(A86))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A77">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="99">
+      <formula>LEN(TRIM(A77))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="notContainsBlanks" dxfId="69" priority="86">
+      <formula>LEN(TRIM(A90))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A85">
+    <cfRule type="notContainsBlanks" dxfId="68" priority="91">
+      <formula>LEN(TRIM(A85))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A89">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="88">
+      <formula>LEN(TRIM(A89))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="notContainsBlanks" dxfId="66" priority="87">
+      <formula>LEN(TRIM(A91))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A95">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="83">
+      <formula>LEN(TRIM(A95))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A100">
+    <cfRule type="notContainsBlanks" dxfId="64" priority="76">
+      <formula>LEN(TRIM(A100))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A103">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="71">
+      <formula>LEN(TRIM(A103))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A98">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="75">
+      <formula>LEN(TRIM(A98))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A99">
+    <cfRule type="notContainsBlanks" dxfId="61" priority="74">
+      <formula>LEN(TRIM(A99))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A104">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="70">
+      <formula>LEN(TRIM(A104))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A105">
+    <cfRule type="notContainsBlanks" dxfId="59" priority="69">
+      <formula>LEN(TRIM(A105))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A101">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="73">
+      <formula>LEN(TRIM(A101))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A102">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="72">
+      <formula>LEN(TRIM(A102))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A106">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="68">
+      <formula>LEN(TRIM(A106))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A107">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="67">
+      <formula>LEN(TRIM(A107))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A108">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="66">
+      <formula>LEN(TRIM(A108))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A109">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="65">
+      <formula>LEN(TRIM(A109))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A110">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="64">
+      <formula>LEN(TRIM(A110))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A111">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="63">
+      <formula>LEN(TRIM(A111))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A112">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="62">
+      <formula>LEN(TRIM(A112))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A113">
+    <cfRule type="notContainsBlanks" dxfId="49" priority="61">
+      <formula>LEN(TRIM(A113))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A114">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="60">
+      <formula>LEN(TRIM(A114))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A115">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="59">
+      <formula>LEN(TRIM(A115))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A116">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="58">
+      <formula>LEN(TRIM(A116))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A117">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="57">
+      <formula>LEN(TRIM(A117))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A118:A122">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="55">
+      <formula>LEN(TRIM(A118))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A123:A127">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="54">
+      <formula>LEN(TRIM(A123))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A128:A132">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="53">
+      <formula>LEN(TRIM(A128))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A133:A137">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="52">
+      <formula>LEN(TRIM(A133))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A138:A141">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="51">
+      <formula>LEN(TRIM(A138))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A147:A149">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="50">
+      <formula>LEN(TRIM(A147))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A150:A154">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="49">
+      <formula>LEN(TRIM(A150))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A155:A159">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="48">
+      <formula>LEN(TRIM(A155))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A164">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="47">
+      <formula>LEN(TRIM(A164))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A160:A163">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="46">
+      <formula>LEN(TRIM(A160))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A142:A146">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="45">
+      <formula>LEN(TRIM(A142))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="40">
+      <formula>LEN(TRIM(A87))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="39">
+      <formula>LEN(TRIM(A88))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A92">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="38">
+      <formula>LEN(TRIM(A92))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A93">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="37">
+      <formula>LEN(TRIM(A93))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A96">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="36">
+      <formula>LEN(TRIM(A96))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="35">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="22">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="29">
+      <formula>LEN(TRIM(A12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="28">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="27">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16:A19">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="26">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="24">
+      <formula>LEN(TRIM(A22))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="23">
+      <formula>LEN(TRIM(A28))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23:A27">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="21">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="19">
+      <formula>LEN(TRIM(A36))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="12">
+      <formula>LEN(TRIM(A5))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="notContainsBlanks" dxfId="75" priority="178">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="13">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A85">
-    <cfRule type="notContainsBlanks" dxfId="74" priority="123">
-      <formula>LEN(TRIM(A85))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70">
-    <cfRule type="notContainsBlanks" dxfId="73" priority="84">
-      <formula>LEN(TRIM(A70))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59">
-    <cfRule type="notContainsBlanks" dxfId="72" priority="127">
-      <formula>LEN(TRIM(A59))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62:A64">
-    <cfRule type="notContainsBlanks" dxfId="71" priority="126">
-      <formula>LEN(TRIM(A62))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65:A67">
-    <cfRule type="notContainsBlanks" dxfId="70" priority="125">
-      <formula>LEN(TRIM(A65))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A156:A157">
-    <cfRule type="notContainsBlanks" dxfId="69" priority="120">
-      <formula>LEN(TRIM(A156))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A58">
-    <cfRule type="notContainsBlanks" dxfId="68" priority="89">
-      <formula>LEN(TRIM(A58))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A57">
-    <cfRule type="notContainsBlanks" dxfId="67" priority="90">
-      <formula>LEN(TRIM(A57))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71">
-    <cfRule type="notContainsBlanks" dxfId="66" priority="83">
-      <formula>LEN(TRIM(A71))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A73">
-    <cfRule type="notContainsBlanks" dxfId="65" priority="81">
-      <formula>LEN(TRIM(A73))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A74">
-    <cfRule type="notContainsBlanks" dxfId="64" priority="80">
-      <formula>LEN(TRIM(A74))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
-    <cfRule type="notContainsBlanks" dxfId="63" priority="82">
-      <formula>LEN(TRIM(A72))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A75">
-    <cfRule type="notContainsBlanks" dxfId="62" priority="79">
-      <formula>LEN(TRIM(A75))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61">
-    <cfRule type="notContainsBlanks" dxfId="61" priority="87">
-      <formula>LEN(TRIM(A61))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
-    <cfRule type="notContainsBlanks" dxfId="60" priority="85">
-      <formula>LEN(TRIM(A69))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60">
-    <cfRule type="notContainsBlanks" dxfId="59" priority="88">
-      <formula>LEN(TRIM(A60))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A77">
-    <cfRule type="notContainsBlanks" dxfId="58" priority="77">
-      <formula>LEN(TRIM(A77))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68">
-    <cfRule type="notContainsBlanks" dxfId="57" priority="86">
-      <formula>LEN(TRIM(A68))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A81">
-    <cfRule type="notContainsBlanks" dxfId="56" priority="73">
-      <formula>LEN(TRIM(A81))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A76">
-    <cfRule type="notContainsBlanks" dxfId="55" priority="78">
-      <formula>LEN(TRIM(A76))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A80">
-    <cfRule type="notContainsBlanks" dxfId="54" priority="75">
-      <formula>LEN(TRIM(A80))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A82">
-    <cfRule type="notContainsBlanks" dxfId="53" priority="74">
-      <formula>LEN(TRIM(A82))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A86">
-    <cfRule type="notContainsBlanks" dxfId="52" priority="70">
-      <formula>LEN(TRIM(A86))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A91">
-    <cfRule type="notContainsBlanks" dxfId="51" priority="63">
-      <formula>LEN(TRIM(A91))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A94">
-    <cfRule type="notContainsBlanks" dxfId="50" priority="58">
-      <formula>LEN(TRIM(A94))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A89">
-    <cfRule type="notContainsBlanks" dxfId="49" priority="62">
-      <formula>LEN(TRIM(A89))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A90">
-    <cfRule type="notContainsBlanks" dxfId="48" priority="61">
-      <formula>LEN(TRIM(A90))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A95">
-    <cfRule type="notContainsBlanks" dxfId="47" priority="57">
-      <formula>LEN(TRIM(A95))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A96">
-    <cfRule type="notContainsBlanks" dxfId="46" priority="56">
-      <formula>LEN(TRIM(A96))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A92">
-    <cfRule type="notContainsBlanks" dxfId="45" priority="60">
-      <formula>LEN(TRIM(A92))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A93">
-    <cfRule type="notContainsBlanks" dxfId="44" priority="59">
-      <formula>LEN(TRIM(A93))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A97">
-    <cfRule type="notContainsBlanks" dxfId="43" priority="55">
-      <formula>LEN(TRIM(A97))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A98">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="54">
-      <formula>LEN(TRIM(A98))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A99">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="53">
-      <formula>LEN(TRIM(A99))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A100">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="52">
-      <formula>LEN(TRIM(A100))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A101">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="51">
-      <formula>LEN(TRIM(A101))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A102">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="50">
-      <formula>LEN(TRIM(A102))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A103">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="49">
-      <formula>LEN(TRIM(A103))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A104">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="48">
-      <formula>LEN(TRIM(A104))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A105">
-    <cfRule type="notContainsBlanks" dxfId="35" priority="47">
-      <formula>LEN(TRIM(A105))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A106">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="46">
-      <formula>LEN(TRIM(A106))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A107">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="45">
-      <formula>LEN(TRIM(A107))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A108">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="44">
-      <formula>LEN(TRIM(A108))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A109:A113">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="42">
-      <formula>LEN(TRIM(A109))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A114:A118">
-    <cfRule type="notContainsBlanks" dxfId="30" priority="41">
-      <formula>LEN(TRIM(A114))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A119:A123">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="40">
-      <formula>LEN(TRIM(A119))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A124:A128">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="39">
-      <formula>LEN(TRIM(A124))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A129:A132">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="38">
-      <formula>LEN(TRIM(A129))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A138:A140">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="37">
-      <formula>LEN(TRIM(A138))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A141:A145">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="36">
-      <formula>LEN(TRIM(A141))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A146:A150">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="35">
-      <formula>LEN(TRIM(A146))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A155">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="34">
-      <formula>LEN(TRIM(A155))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A151:A154">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="33">
-      <formula>LEN(TRIM(A151))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A133:A137">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="32">
-      <formula>LEN(TRIM(A133))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A78">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="27">
-      <formula>LEN(TRIM(A78))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A79">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="26">
-      <formula>LEN(TRIM(A79))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A83">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="25">
-      <formula>LEN(TRIM(A83))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A84">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="24">
-      <formula>LEN(TRIM(A84))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A87">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="23">
-      <formula>LEN(TRIM(A87))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="22">
-      <formula>LEN(TRIM(A10))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="21">
-      <formula>LEN(TRIM(A5))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
       <formula>LEN(TRIM(A6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="19">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
       <formula>LEN(TRIM(A7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="16">
-      <formula>LEN(TRIM(A12))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="15">
-      <formula>LEN(TRIM(A11))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="14">
-      <formula>LEN(TRIM(A20))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15:A19">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="13">
+  <conditionalFormatting sqref="A9">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
       <formula>LEN(TRIM(A21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="11">
-      <formula>LEN(TRIM(A22))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="10">
-      <formula>LEN(TRIM(A28))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="9">
-      <formula>LEN(TRIM(A32))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23:A27">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="8">
-      <formula>LEN(TRIM(A23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="6">
-      <formula>LEN(TRIM(A36))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29:A31">
+  <conditionalFormatting sqref="A29">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(A29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(A33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(A31))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(A29))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33:A35">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="E39" location="person_1!C44" display="rdf:type cdiscpilot01:VisitScreening1Activity_{#usubjid}"/>
-  </hyperlinks>
+      <formula>LEN(TRIM(A35))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
WIP for DM triples import
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -47,6 +47,30 @@
           </rPr>
           <t xml:space="preserve">
 cdiscpilot01:Person_v29eedorsh9a5vr65uc1iob3mvn9blbb</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Williams Tim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ cdiscpilot01:Lifespan_udj4rptja2ij6a5lmb3meemc3mca7ip3_n6l0u58r7lrhic8l4b1e4u7k8182j6fq</t>
         </r>
       </text>
     </comment>
@@ -292,12 +316,84 @@
         </r>
       </text>
     </comment>
+    <comment ref="C38" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Williams Tim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+cdiscpilot01:DemographicDataCollection_v29eedorsh9a5vr65uc1iob3mvn9blbb</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C49" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Williams Tim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+cdiscpilot01:VisitScreening1Activity_v29eedorsh9a5vr65uc1iob3mvn9blbb</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C54" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Williams Tim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+cdiscpilot01:AgeOutcome_k5ql986im5d6cj0eee80312k9scue0h7</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="243">
   <si>
     <t>rdf:type</t>
   </si>
@@ -1428,9 +1524,6 @@
     <t>AO: Change from Date_30</t>
   </si>
   <si>
-    <t xml:space="preserve">cdiscpilot01:AgeOutcome_1 </t>
-  </si>
-  <si>
     <t>cdiscpilot01:InformedConsentAdult_1</t>
   </si>
   <si>
@@ -1480,15 +1573,6 @@
   </si>
   <si>
     <t>cdiscpilot01:UniqueSubjectIdentifier_{#usubjid}</t>
-  </si>
-  <si>
-    <t>coded</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:VisitScreening1Activity_1 ;</t>
-  </si>
-  <si>
-    <t>code:DemographicDataCollection ;</t>
   </si>
   <si>
     <r>
@@ -1565,12 +1649,6 @@
     <t>cdiscpilot01:VisitScreening1Activity_????</t>
   </si>
   <si>
-    <t>From: VisitScreening1Activity_1</t>
-  </si>
-  <si>
-    <t>What should ??? be based on?</t>
-  </si>
-  <si>
     <t>"P {_ROW_} Screening {????} Demographic data collection</t>
   </si>
   <si>
@@ -1617,6 +1695,42 @@
   </si>
   <si>
     <t>study:sex</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:DemographicDataCollection_{#usubjid}</t>
+  </si>
+  <si>
+    <t>code:Sex_F</t>
+  </si>
+  <si>
+    <t>code:Ethnicity_{#ethnic}</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Date_{#dmdtc}</t>
+  </si>
+  <si>
+    <t>code:Race_{#race}</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:VisitScreening1Activity_{#usubjid}</t>
+  </si>
+  <si>
+    <t>study:AgeOutcome</t>
+  </si>
+  <si>
+    <t>{age} {ageu}^^xsd:string;</t>
+  </si>
+  <si>
+    <t>code:hasUnit</t>
+  </si>
+  <si>
+    <t>time:unitYear</t>
+  </si>
+  <si>
+    <t>code:hasValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{age}^^xsd:int </t>
   </si>
 </sst>
 </file>
@@ -1848,7 +1962,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2055,12 +2169,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2277,7 +2385,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2377,26 +2485,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="25" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="25" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2442,42 +2538,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="91">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="86">
     <dxf>
       <fill>
         <patternFill>
@@ -3390,11 +3451,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G178"/>
+  <dimension ref="A1:G175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D44" sqref="D44:D47"/>
+      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3426,7 +3487,7 @@
         <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
@@ -3449,7 +3510,7 @@
         <v>62</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>0</v>
@@ -3470,7 +3531,7 @@
         <v>62</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>75</v>
@@ -3491,7 +3552,7 @@
         <v>62</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>2</v>
@@ -3510,7 +3571,7 @@
         <v>62</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>3</v>
@@ -3538,7 +3599,7 @@
         <v>62</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>4</v>
@@ -3558,7 +3619,7 @@
       <c r="B10" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="28" t="s">
         <v>175</v>
       </c>
       <c r="D10" s="49" t="s">
@@ -3653,7 +3714,7 @@
         <v>62</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>6</v>
@@ -3674,7 +3735,7 @@
         <v>62</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>0</v>
@@ -3769,7 +3830,7 @@
         <v>62</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>8</v>
@@ -3801,7 +3862,7 @@
         <v>62</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>9</v>
@@ -3828,7 +3889,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="G24" s="14"/>
     </row>
@@ -3891,7 +3952,7 @@
         <v>185</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="3" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.35">
@@ -3911,16 +3972,16 @@
         <v>62</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="59" t="s">
-        <v>196</v>
+      <c r="E29" s="54" t="s">
+        <v>195</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G29" s="14"/>
     </row>
@@ -3931,14 +3992,14 @@
       <c r="B30" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="59" t="s">
-        <v>196</v>
+      <c r="C30" s="54" t="s">
+        <v>195</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>0</v>
       </c>
       <c r="E30" s="43" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F30" s="20"/>
       <c r="G30" s="14"/>
@@ -3951,13 +4012,13 @@
         <v>62</v>
       </c>
       <c r="C31" s="43" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D31" t="s">
         <v>75</v>
       </c>
       <c r="E31" s="43" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F31" s="20"/>
       <c r="G31" s="14"/>
@@ -3979,16 +4040,16 @@
         <v>62</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="59" t="s">
-        <v>203</v>
+      <c r="E33" s="54" t="s">
+        <v>202</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G33" s="14"/>
     </row>
@@ -3999,14 +4060,14 @@
       <c r="B34" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="59" t="s">
-        <v>203</v>
+      <c r="C34" s="54" t="s">
+        <v>202</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>0</v>
       </c>
       <c r="E34" s="43" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F34" s="20"/>
       <c r="G34" s="14"/>
@@ -4019,13 +4080,13 @@
         <v>62</v>
       </c>
       <c r="C35" s="43" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E35" s="43" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F35" s="20"/>
       <c r="G35" s="14"/>
@@ -4040,634 +4101,731 @@
       <c r="G36" s="48"/>
     </row>
     <row r="37" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A37" s="8" t="s">
-        <v>204</v>
+      <c r="A37" s="8">
+        <v>43176</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="43" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G37" s="14" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="8"/>
+      <c r="A38" s="8">
+        <v>43176</v>
+      </c>
       <c r="B38" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="43" t="s">
-        <v>207</v>
+      <c r="C38" s="54" t="s">
+        <v>203</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>0</v>
       </c>
       <c r="E38" s="43" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F38" s="20"/>
       <c r="G38" s="14"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="8"/>
+      <c r="A39" s="8">
+        <v>43176</v>
+      </c>
       <c r="B39" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C39" s="43" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E39" s="43" t="s">
-        <v>221</v>
+      <c r="E39" s="51" t="s">
+        <v>218</v>
       </c>
       <c r="F39" s="20"/>
       <c r="G39" s="14"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="58"/>
-      <c r="B40" s="51"/>
-      <c r="C40" s="54"/>
+      <c r="A40" s="8">
+        <v>43176</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="43" t="s">
+        <v>231</v>
+      </c>
       <c r="D40" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E40" s="54" t="s">
+      <c r="E40" s="43" t="s">
+        <v>216</v>
+      </c>
+      <c r="F40" s="20"/>
+      <c r="G40" s="14"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="8">
+        <v>43176</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="43" t="s">
+        <v>231</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E41" s="43" t="s">
+        <v>219</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="G41" s="14"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="8">
+        <v>43176</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="43" t="s">
+        <v>231</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="E42" s="43" t="s">
+        <v>223</v>
+      </c>
+      <c r="F42" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="F40" s="60" t="s">
+      <c r="G42" s="53"/>
+    </row>
+    <row r="43" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" s="8">
+        <v>43176</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="43" t="s">
+        <v>231</v>
+      </c>
+      <c r="D43" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="G40" s="57" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="8"/>
-      <c r="B41" s="51"/>
-      <c r="C41" s="54"/>
-      <c r="D41" s="53" t="s">
+      <c r="E43" s="43" t="s">
+        <v>225</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="G43" s="14"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="8">
+        <v>43176</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="43" t="s">
+        <v>231</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="E44" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="F44" s="20"/>
+      <c r="G44" s="52"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="8">
+        <v>43176</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="43" t="s">
+        <v>231</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="E45" s="43" t="s">
+        <v>234</v>
+      </c>
+      <c r="F45" s="20"/>
+      <c r="G45" s="52"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="8">
+        <v>43176</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="43" t="s">
+        <v>231</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="E46" s="43" t="s">
+        <v>235</v>
+      </c>
+      <c r="F46" s="20"/>
+      <c r="G46" s="52"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="8">
+        <v>43176</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="43" t="s">
+        <v>231</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="E47" s="43" t="s">
+        <v>232</v>
+      </c>
+      <c r="F47" s="20"/>
+      <c r="G47" s="52"/>
+    </row>
+    <row r="48" spans="1:7" s="3" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="44"/>
+      <c r="B48" s="45"/>
+      <c r="C48" s="39"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="48"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="8">
+        <v>43176</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="54" t="s">
+        <v>236</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="43" t="s">
+        <v>209</v>
+      </c>
+      <c r="F49" s="20"/>
+      <c r="G49" s="14"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="8">
+        <v>43176</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" s="43" t="s">
+        <v>208</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="F50" s="20"/>
+      <c r="G50" s="14"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="8">
+        <v>43176</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="43" t="s">
+        <v>208</v>
+      </c>
+      <c r="D51" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E41" s="54" t="s">
-        <v>225</v>
-      </c>
-      <c r="F41" s="55" t="s">
-        <v>226</v>
-      </c>
-      <c r="G41" s="14"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="8"/>
-      <c r="B42" s="51"/>
-      <c r="C42" s="54"/>
-      <c r="D42" s="53" t="s">
-        <v>227</v>
-      </c>
-      <c r="E42" s="54" t="s">
-        <v>229</v>
-      </c>
-      <c r="F42" s="55" t="s">
-        <v>228</v>
-      </c>
-      <c r="G42" s="14"/>
-    </row>
-    <row r="43" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="8"/>
-      <c r="B43" s="51"/>
-      <c r="C43" s="54"/>
-      <c r="D43" s="53" t="s">
-        <v>230</v>
-      </c>
-      <c r="E43" s="54" t="s">
-        <v>231</v>
-      </c>
-      <c r="F43" s="55" t="s">
-        <v>232</v>
-      </c>
-      <c r="G43" s="56"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="8"/>
-      <c r="B44" s="51"/>
-      <c r="C44" s="54"/>
-      <c r="D44" s="53" t="s">
-        <v>233</v>
-      </c>
-      <c r="E44" s="54"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="56"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="8"/>
-      <c r="B45" s="51"/>
-      <c r="C45" s="54"/>
-      <c r="D45" s="53" t="s">
-        <v>234</v>
-      </c>
-      <c r="E45" s="54"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="56"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="8"/>
-      <c r="B46" s="51"/>
-      <c r="C46" s="54"/>
-      <c r="D46" s="53" t="s">
-        <v>235</v>
-      </c>
-      <c r="E46" s="54"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="56"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="8"/>
-      <c r="B47" s="51"/>
-      <c r="C47" s="54"/>
-      <c r="D47" s="53" t="s">
-        <v>236</v>
-      </c>
-      <c r="E47" s="54"/>
-      <c r="F47" s="55"/>
-      <c r="G47" s="56"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="8"/>
-      <c r="B48" s="51"/>
-      <c r="C48" s="54"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="54"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="56"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="8"/>
-      <c r="B49" s="51"/>
-      <c r="C49" s="54"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="54"/>
-      <c r="F49" s="55"/>
-      <c r="G49" s="56"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" s="8"/>
-      <c r="B50" s="51"/>
-      <c r="C50" s="54"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="54"/>
-      <c r="F50" s="55"/>
-      <c r="G50" s="56"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" s="8"/>
-      <c r="B51" s="51"/>
-      <c r="C51" s="54"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="54"/>
-      <c r="F51" s="55"/>
-      <c r="G51" s="56"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="8"/>
-      <c r="B52" s="51"/>
-      <c r="C52" s="54"/>
-      <c r="D52" s="53"/>
-      <c r="E52" s="54"/>
-      <c r="F52" s="55"/>
-      <c r="G52" s="56"/>
+      <c r="E51" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="F51" s="20"/>
+      <c r="G51" s="14"/>
+    </row>
+    <row r="52" spans="1:7" s="3" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="44"/>
+      <c r="B52" s="45"/>
+      <c r="C52" s="39"/>
+      <c r="D52" s="46"/>
+      <c r="E52" s="45"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="48"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="8" t="s">
-        <v>204</v>
+      <c r="A53" s="8">
+        <v>43176</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C53" s="43" t="s">
-        <v>212</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>0</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="D53" s="11"/>
       <c r="E53" s="43" t="s">
-        <v>213</v>
-      </c>
-      <c r="F53" s="20"/>
+        <v>223</v>
+      </c>
+      <c r="F53" s="20" t="s">
+        <v>146</v>
+      </c>
       <c r="G53" s="14"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" s="8" t="s">
-        <v>204</v>
+      <c r="A54" s="8">
+        <v>43176</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="43" t="s">
-        <v>212</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="F54" s="20"/>
+      <c r="C54" s="54" t="s">
+        <v>223</v>
+      </c>
+      <c r="D54" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>237</v>
+      </c>
       <c r="G54" s="14"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A55" s="8" t="s">
-        <v>204</v>
+      <c r="A55" s="8">
+        <v>43176</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C55" s="43" t="s">
-        <v>212</v>
-      </c>
-      <c r="D55" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D55" t="s">
         <v>75</v>
       </c>
-      <c r="E55" s="9" t="s">
-        <v>216</v>
+      <c r="E55" s="43" t="s">
+        <v>238</v>
       </c>
       <c r="F55" s="20"/>
       <c r="G55" s="14"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A56" s="8"/>
-      <c r="B56" s="51"/>
-      <c r="C56" s="52"/>
-      <c r="D56" s="53"/>
-      <c r="E56" s="54"/>
-      <c r="F56" s="55"/>
-      <c r="G56" s="57"/>
+      <c r="A56" s="8">
+        <v>43176</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56" s="43" t="s">
+        <v>223</v>
+      </c>
+      <c r="D56" t="s">
+        <v>239</v>
+      </c>
+      <c r="E56" s="43" t="s">
+        <v>240</v>
+      </c>
+      <c r="F56" s="20"/>
+      <c r="G56" s="14"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A57" s="8"/>
-      <c r="B57" s="51"/>
-      <c r="C57" s="52"/>
-      <c r="D57" s="53"/>
-      <c r="E57" s="54"/>
-      <c r="F57" s="55"/>
+      <c r="A57" s="8">
+        <v>43176</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C57" s="43" t="s">
+        <v>223</v>
+      </c>
+      <c r="D57" t="s">
+        <v>241</v>
+      </c>
+      <c r="E57" s="43" t="s">
+        <v>242</v>
+      </c>
+      <c r="F57" s="20"/>
       <c r="G57" s="14"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="8"/>
-      <c r="B58" s="51"/>
-      <c r="C58" s="52"/>
-      <c r="D58" s="53"/>
-      <c r="E58" s="54"/>
-      <c r="F58" s="55"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="43"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="20"/>
       <c r="G58" s="14"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="8"/>
-      <c r="B59" s="51"/>
-      <c r="C59" s="52"/>
-      <c r="D59" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="E59" s="54" t="s">
-        <v>205</v>
-      </c>
-      <c r="F59" s="55"/>
-      <c r="G59" s="14"/>
+      <c r="B59" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" s="43" t="s">
+        <v>186</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="G59" s="15"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="8"/>
-      <c r="B60" s="51"/>
-      <c r="C60" s="52"/>
-      <c r="D60" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="E60" s="54" t="s">
-        <v>206</v>
-      </c>
-      <c r="F60" s="55"/>
-      <c r="G60" s="14"/>
+      <c r="B60" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C60" s="13"/>
+      <c r="D60" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E60" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="G60" s="15"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="8"/>
-      <c r="B61" s="51"/>
-      <c r="C61" s="52"/>
-      <c r="D61" s="53"/>
-      <c r="E61" s="54"/>
-      <c r="F61" s="55"/>
-      <c r="G61" s="14"/>
+      <c r="B61" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" s="13"/>
+      <c r="D61" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E61" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F61" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="G61" s="15"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="8"/>
-      <c r="B62" s="51"/>
-      <c r="C62" s="52"/>
-      <c r="D62" s="53"/>
-      <c r="E62" s="54"/>
-      <c r="F62" s="55"/>
-      <c r="G62" s="14"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="43"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="15"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="8"/>
-      <c r="B63" s="51"/>
-      <c r="C63" s="52"/>
-      <c r="D63" s="53"/>
-      <c r="E63" s="54"/>
-      <c r="F63" s="55"/>
-      <c r="G63" s="14"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="43"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="15"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="8"/>
-      <c r="B64" s="51"/>
-      <c r="C64" s="52"/>
-      <c r="D64" s="53"/>
-      <c r="E64" s="54"/>
-      <c r="F64" s="55"/>
-      <c r="G64" s="14"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="43"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="15"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="8"/>
-      <c r="G65" s="14"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="43"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="15"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="8"/>
-      <c r="B66" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="B66" s="9"/>
       <c r="C66" s="13"/>
-      <c r="D66" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E66" s="43" t="s">
-        <v>186</v>
-      </c>
-      <c r="F66" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="G66" s="14"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="43"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="15"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="8"/>
-      <c r="B67" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="B67" s="9"/>
       <c r="C67" s="13"/>
-      <c r="D67" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E67" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="F67" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="G67" s="14"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D67" s="11"/>
+      <c r="E67" s="43"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="15"/>
+    </row>
+    <row r="68" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="8"/>
-      <c r="B68" s="9" t="s">
-        <v>62</v>
+      <c r="B68" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D68" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E68" s="43" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F68" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="G68" s="15"/>
+        <v>149</v>
+      </c>
+      <c r="G68" s="14"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="8"/>
-      <c r="B69" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C69" s="13"/>
-      <c r="D69" s="11" t="s">
-        <v>50</v>
+      <c r="B69" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="E69" s="43" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F69" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="G69" s="15"/>
+        <v>150</v>
+      </c>
+      <c r="G69" s="14"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="8"/>
-      <c r="B70" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C70" s="13"/>
-      <c r="D70" s="11" t="s">
-        <v>51</v>
+      <c r="B70" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="E70" s="43" t="s">
-        <v>20</v>
+        <v>190</v>
       </c>
       <c r="F70" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="G70" s="15"/>
+        <v>151</v>
+      </c>
+      <c r="G70" s="14"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="8"/>
-      <c r="B71" s="10" t="s">
-        <v>49</v>
-      </c>
+      <c r="B71" s="10"/>
       <c r="C71" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D71" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E71" s="43" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F71" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="G71" s="14"/>
+        <v>152</v>
+      </c>
+      <c r="G71" s="15"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="8"/>
-      <c r="B72" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C72" s="13" t="s">
-        <v>208</v>
-      </c>
+      <c r="B72" s="9"/>
+      <c r="C72" s="13"/>
       <c r="D72" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E72" s="43" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F72" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="G72" s="14"/>
+        <v>153</v>
+      </c>
+      <c r="G72" s="15"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="8"/>
-      <c r="B73" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C73" s="13" t="s">
-        <v>208</v>
-      </c>
+      <c r="B73" s="9"/>
+      <c r="C73" s="13"/>
       <c r="D73" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E73" s="43" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F73" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="G73" s="14"/>
+        <v>154</v>
+      </c>
+      <c r="G73" s="15"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="8"/>
-      <c r="B74" s="10"/>
+      <c r="B74" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="C74" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D74" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E74" s="43" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="F74" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="G74" s="15"/>
+        <v>155</v>
+      </c>
+      <c r="G74" s="14"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="8"/>
-      <c r="B75" s="9"/>
+      <c r="B75" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="C75" s="13"/>
-      <c r="D75" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E75" s="43" t="s">
-        <v>193</v>
+      <c r="D75" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>90</v>
       </c>
       <c r="F75" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="G75" s="15"/>
+        <v>156</v>
+      </c>
+      <c r="G75" s="14"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="8"/>
-      <c r="B76" s="9"/>
+      <c r="B76" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="C76" s="13"/>
-      <c r="D76" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E76" s="43" t="s">
-        <v>194</v>
+      <c r="D76" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="F76" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="G76" s="15"/>
+        <v>157</v>
+      </c>
+      <c r="G76" s="14"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="8"/>
-      <c r="B77" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C77" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="D77" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77" s="43" t="s">
-        <v>195</v>
+      <c r="B77" s="9"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>105</v>
       </c>
       <c r="F77" s="20" t="s">
-        <v>155</v>
+        <v>111</v>
       </c>
       <c r="G77" s="14"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="8"/>
-      <c r="B78" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="B78" s="9"/>
       <c r="C78" s="13"/>
       <c r="D78" s="11" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="E78" s="10" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="F78" s="20" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G78" s="14"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="8"/>
-      <c r="B79" s="9" t="s">
-        <v>98</v>
-      </c>
+      <c r="B79" s="9"/>
       <c r="C79" s="13"/>
-      <c r="D79" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="D79" s="11"/>
       <c r="E79" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="F79" s="20" t="s">
-        <v>157</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="F79" s="20"/>
       <c r="G79" s="14"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="8"/>
       <c r="B80" s="9"/>
       <c r="C80" s="13"/>
-      <c r="D80" s="11" t="s">
-        <v>80</v>
-      </c>
+      <c r="D80" s="11"/>
       <c r="E80" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F80" s="20" t="s">
-        <v>111</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="F80" s="20"/>
       <c r="G80" s="14"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="8"/>
-      <c r="B81" s="9"/>
+      <c r="B81" s="9" t="s">
+        <v>103</v>
+      </c>
       <c r="C81" s="13"/>
       <c r="D81" s="11" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="E81" s="10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F81" s="20" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G81" s="14"/>
     </row>
@@ -4675,11 +4833,15 @@
       <c r="A82" s="8"/>
       <c r="B82" s="9"/>
       <c r="C82" s="13"/>
-      <c r="D82" s="11"/>
+      <c r="D82" s="11" t="s">
+        <v>80</v>
+      </c>
       <c r="E82" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="F82" s="20"/>
+        <v>100</v>
+      </c>
+      <c r="F82" s="20" t="s">
+        <v>111</v>
+      </c>
       <c r="G82" s="14"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
@@ -4688,63 +4850,63 @@
       <c r="C83" s="13"/>
       <c r="D83" s="11"/>
       <c r="E83" s="10" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F83" s="20"/>
       <c r="G83" s="14"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="8"/>
-      <c r="B84" s="9" t="s">
-        <v>103</v>
-      </c>
+      <c r="B84" s="9"/>
       <c r="C84" s="13"/>
-      <c r="D84" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="D84" s="11"/>
       <c r="E84" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F84" s="20" t="s">
-        <v>159</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="F84" s="20"/>
       <c r="G84" s="14"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="8"/>
       <c r="B85" s="9"/>
       <c r="C85" s="13"/>
-      <c r="D85" s="11" t="s">
-        <v>80</v>
-      </c>
+      <c r="D85" s="11"/>
       <c r="E85" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="F85" s="20" t="s">
-        <v>111</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="F85" s="20"/>
       <c r="G85" s="14"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="8"/>
-      <c r="B86" s="9"/>
+      <c r="B86" s="9" t="s">
+        <v>103</v>
+      </c>
       <c r="C86" s="13"/>
-      <c r="D86" s="11"/>
+      <c r="D86" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="E86" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="F86" s="20"/>
+        <v>97</v>
+      </c>
+      <c r="F86" s="20" t="s">
+        <v>160</v>
+      </c>
       <c r="G86" s="14"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="8"/>
       <c r="B87" s="9"/>
       <c r="C87" s="13"/>
-      <c r="D87" s="11"/>
+      <c r="D87" s="11" t="s">
+        <v>80</v>
+      </c>
       <c r="E87" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F87" s="20"/>
+        <v>109</v>
+      </c>
+      <c r="F87" s="20" t="s">
+        <v>111</v>
+      </c>
       <c r="G87" s="14"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
@@ -4753,211 +4915,207 @@
       <c r="C88" s="13"/>
       <c r="D88" s="11"/>
       <c r="E88" s="10" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F88" s="20"/>
       <c r="G88" s="14"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="8"/>
-      <c r="B89" s="9" t="s">
-        <v>103</v>
-      </c>
+      <c r="B89" s="9"/>
       <c r="C89" s="13"/>
-      <c r="D89" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="D89" s="11"/>
       <c r="E89" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F89" s="20" t="s">
-        <v>160</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="F89" s="20"/>
       <c r="G89" s="14"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="8"/>
       <c r="B90" s="9"/>
       <c r="C90" s="13"/>
-      <c r="D90" s="11" t="s">
-        <v>80</v>
-      </c>
+      <c r="D90" s="11"/>
       <c r="E90" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F90" s="20" t="s">
-        <v>111</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="F90" s="20"/>
       <c r="G90" s="14"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="8"/>
-      <c r="B91" s="9"/>
-      <c r="C91" s="13"/>
-      <c r="D91" s="11"/>
-      <c r="E91" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="F91" s="20"/>
+      <c r="B91" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="D91" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E91" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F91" s="20" t="s">
+        <v>161</v>
+      </c>
       <c r="G91" s="14"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="8"/>
-      <c r="B92" s="9"/>
-      <c r="C92" s="13"/>
-      <c r="D92" s="11"/>
-      <c r="E92" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="F92" s="20"/>
+      <c r="B92" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C92" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E92" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F92" s="20" t="s">
+        <v>162</v>
+      </c>
       <c r="G92" s="14"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="8"/>
-      <c r="B93" s="9"/>
-      <c r="C93" s="13"/>
-      <c r="D93" s="11"/>
+      <c r="B93" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C93" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D93" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="E93" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="F93" s="20"/>
+        <v>89</v>
+      </c>
+      <c r="F93" s="20" t="s">
+        <v>145</v>
+      </c>
       <c r="G93" s="14"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A94" s="8"/>
-      <c r="B94" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C94" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="D94" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E94" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F94" s="20" t="s">
-        <v>161</v>
-      </c>
+      <c r="A94" s="26"/>
+      <c r="B94" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C94" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D94" s="35"/>
+      <c r="E94" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="F94" s="36"/>
       <c r="G94" s="14"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A95" s="8"/>
-      <c r="B95" s="10" t="s">
-        <v>67</v>
-      </c>
+      <c r="A95" s="26"/>
+      <c r="B95" s="10"/>
       <c r="C95" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="D95" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E95" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F95" s="20" t="s">
-        <v>162</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D95" s="11"/>
+      <c r="E95" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F95" s="20"/>
       <c r="G95" s="14"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A96" s="8"/>
-      <c r="B96" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C96" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="D96" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="A96" s="26"/>
+      <c r="B96" s="10"/>
+      <c r="C96" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D96" s="11"/>
       <c r="E96" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="F96" s="20" t="s">
-        <v>145</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="F96" s="20"/>
       <c r="G96" s="14"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" s="26"/>
-      <c r="B97" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C97" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="D97" s="35"/>
-      <c r="E97" s="33" t="s">
+      <c r="B97" s="10"/>
+      <c r="C97" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="F97" s="36"/>
+      <c r="D97" s="11"/>
+      <c r="E97" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F97" s="21"/>
       <c r="G97" s="14"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" ht="28.5" x14ac:dyDescent="0.35">
       <c r="A98" s="26"/>
       <c r="B98" s="10"/>
       <c r="C98" s="13" t="s">
-        <v>54</v>
+        <v>113</v>
       </c>
       <c r="D98" s="11"/>
-      <c r="E98" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="F98" s="20"/>
+      <c r="E98" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="F98" s="21" t="s">
+        <v>115</v>
+      </c>
       <c r="G98" s="14"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" s="26"/>
       <c r="B99" s="10"/>
       <c r="C99" s="13" t="s">
-        <v>54</v>
+        <v>113</v>
       </c>
       <c r="D99" s="11"/>
-      <c r="E99" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="F99" s="20"/>
+      <c r="E99" t="s">
+        <v>55</v>
+      </c>
+      <c r="F99" s="21"/>
       <c r="G99" s="14"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" s="26"/>
       <c r="B100" s="10"/>
-      <c r="C100" s="13" t="s">
-        <v>112</v>
+      <c r="C100" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D100" s="11"/>
-      <c r="E100" s="10" t="s">
-        <v>89</v>
+      <c r="E100" s="27" t="s">
+        <v>114</v>
       </c>
       <c r="F100" s="21"/>
       <c r="G100" s="14"/>
     </row>
-    <row r="101" spans="1:7" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101" s="26"/>
       <c r="B101" s="10"/>
-      <c r="C101" s="13" t="s">
-        <v>113</v>
+      <c r="C101" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D101" s="11"/>
-      <c r="E101" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="F101" s="21" t="s">
-        <v>115</v>
-      </c>
+      <c r="E101" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F101" s="21"/>
       <c r="G101" s="14"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" s="26"/>
       <c r="B102" s="10"/>
-      <c r="C102" s="13" t="s">
-        <v>113</v>
+      <c r="C102" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D102" s="11"/>
-      <c r="E102" t="s">
-        <v>55</v>
+      <c r="E102" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="F102" s="21"/>
       <c r="G102" s="14"/>
@@ -4965,8 +5123,8 @@
     <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" s="26"/>
       <c r="B103" s="10"/>
-      <c r="C103" s="2" t="s">
-        <v>55</v>
+      <c r="C103" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="D103" s="11"/>
       <c r="E103" s="27" t="s">
@@ -4978,25 +5136,25 @@
     <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" s="26"/>
       <c r="B104" s="10"/>
-      <c r="C104" s="2" t="s">
-        <v>55</v>
+      <c r="C104" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="D104" s="11"/>
       <c r="E104" s="10" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="F104" s="21"/>
       <c r="G104" s="14"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A105" s="26"/>
       <c r="B105" s="10"/>
-      <c r="C105" s="2" t="s">
-        <v>55</v>
+      <c r="C105" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="D105" s="11"/>
-      <c r="E105" s="10" t="s">
-        <v>89</v>
+      <c r="E105" s="27" t="s">
+        <v>114</v>
       </c>
       <c r="F105" s="21"/>
       <c r="G105" s="14"/>
@@ -5004,38 +5162,42 @@
     <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" s="26"/>
       <c r="B106" s="10"/>
-      <c r="C106" s="13" t="s">
+      <c r="C106" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="D106" s="11"/>
+      <c r="E106" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D106" s="11"/>
-      <c r="E106" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="F106" s="21"/>
+      <c r="F106" s="21" t="s">
+        <v>118</v>
+      </c>
       <c r="G106" s="14"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" s="26"/>
       <c r="B107" s="10"/>
-      <c r="C107" s="13" t="s">
-        <v>57</v>
+      <c r="C107" s="30" t="s">
+        <v>117</v>
       </c>
       <c r="D107" s="11"/>
       <c r="E107" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="F107" s="21"/>
+        <v>20</v>
+      </c>
+      <c r="F107" s="21" t="s">
+        <v>118</v>
+      </c>
       <c r="G107" s="14"/>
     </row>
-    <row r="108" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108" s="26"/>
       <c r="B108" s="10"/>
-      <c r="C108" s="4" t="s">
-        <v>116</v>
+      <c r="C108" s="30" t="s">
+        <v>117</v>
       </c>
       <c r="D108" s="11"/>
-      <c r="E108" s="27" t="s">
-        <v>114</v>
+      <c r="E108" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="F108" s="21"/>
       <c r="G108" s="14"/>
@@ -5043,42 +5205,38 @@
     <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" s="26"/>
       <c r="B109" s="10"/>
-      <c r="C109" s="30" t="s">
-        <v>117</v>
+      <c r="C109" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="D109" s="11"/>
-      <c r="E109" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F109" s="21" t="s">
-        <v>118</v>
-      </c>
+      <c r="E109" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="F109" s="21"/>
       <c r="G109" s="14"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A110" s="26"/>
       <c r="B110" s="10"/>
-      <c r="C110" s="30" t="s">
-        <v>117</v>
+      <c r="C110" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="D110" s="11"/>
-      <c r="E110" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F110" s="21" t="s">
-        <v>118</v>
-      </c>
+      <c r="E110" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="F110" s="21"/>
       <c r="G110" s="14"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" s="26"/>
       <c r="B111" s="10"/>
-      <c r="C111" s="30" t="s">
-        <v>117</v>
+      <c r="C111" s="13" t="s">
+        <v>120</v>
       </c>
       <c r="D111" s="11"/>
       <c r="E111" s="10" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="F111" s="21"/>
       <c r="G111" s="14"/>
@@ -5087,24 +5245,24 @@
       <c r="A112" s="26"/>
       <c r="B112" s="10"/>
       <c r="C112" s="13" t="s">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="D112" s="11"/>
-      <c r="E112" s="27" t="s">
-        <v>114</v>
+      <c r="E112" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="F112" s="21"/>
       <c r="G112" s="14"/>
     </row>
-    <row r="113" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" s="26"/>
       <c r="B113" s="10"/>
-      <c r="C113" s="4" t="s">
-        <v>119</v>
+      <c r="C113" s="13" t="s">
+        <v>120</v>
       </c>
       <c r="D113" s="11"/>
-      <c r="E113" s="27" t="s">
-        <v>114</v>
+      <c r="E113" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="F113" s="21"/>
       <c r="G113" s="14"/>
@@ -5113,104 +5271,106 @@
       <c r="A114" s="26"/>
       <c r="B114" s="10"/>
       <c r="C114" s="13" t="s">
-        <v>120</v>
+        <v>76</v>
       </c>
       <c r="D114" s="11"/>
-      <c r="E114" s="10" t="s">
-        <v>57</v>
+      <c r="E114" s="27" t="s">
+        <v>114</v>
       </c>
       <c r="F114" s="21"/>
       <c r="G114" s="14"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A115" s="26"/>
-      <c r="B115" s="10"/>
-      <c r="C115" s="13" t="s">
-        <v>120</v>
+      <c r="B115" s="26"/>
+      <c r="C115" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="D115" s="11"/>
       <c r="E115" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F115" s="21"/>
+        <v>57</v>
+      </c>
+      <c r="F115" s="23" t="s">
+        <v>83</v>
+      </c>
       <c r="G115" s="14"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" s="26"/>
-      <c r="B116" s="10"/>
+      <c r="B116" s="26"/>
       <c r="C116" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D116" s="11"/>
       <c r="E116" s="10" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="F116" s="21"/>
       <c r="G116" s="14"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" s="26"/>
-      <c r="B117" s="10"/>
+      <c r="B117" s="26"/>
       <c r="C117" s="13" t="s">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="D117" s="11"/>
-      <c r="E117" s="27" t="s">
-        <v>114</v>
+      <c r="E117" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="F117" s="21"/>
       <c r="G117" s="14"/>
     </row>
-    <row r="118" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118" s="26"/>
       <c r="B118" s="26"/>
-      <c r="C118" s="4" t="s">
-        <v>122</v>
+      <c r="C118" s="13" t="s">
+        <v>121</v>
       </c>
       <c r="D118" s="11"/>
       <c r="E118" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F118" s="23" t="s">
-        <v>83</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="F118" s="21"/>
       <c r="G118" s="14"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" s="26"/>
       <c r="B119" s="26"/>
       <c r="C119" s="13" t="s">
-        <v>121</v>
+        <v>59</v>
       </c>
       <c r="D119" s="11"/>
-      <c r="E119" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F119" s="21"/>
+      <c r="E119" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="F119" s="21" t="s">
+        <v>138</v>
+      </c>
       <c r="G119" s="14"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A120" s="26"/>
       <c r="B120" s="26"/>
-      <c r="C120" s="13" t="s">
-        <v>121</v>
+      <c r="C120" s="15" t="s">
+        <v>123</v>
       </c>
       <c r="D120" s="11"/>
       <c r="E120" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F120" s="21"/>
+        <v>57</v>
+      </c>
+      <c r="F120" s="21" t="s">
+        <v>83</v>
+      </c>
       <c r="G120" s="14"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" s="26"/>
       <c r="B121" s="26"/>
-      <c r="C121" s="13" t="s">
-        <v>121</v>
-      </c>
+      <c r="C121" s="15"/>
       <c r="D121" s="11"/>
       <c r="E121" s="10" t="s">
-        <v>136</v>
+        <v>20</v>
       </c>
       <c r="F121" s="21"/>
       <c r="G121" s="14"/>
@@ -5218,53 +5378,51 @@
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A122" s="26"/>
       <c r="B122" s="26"/>
-      <c r="C122" s="13" t="s">
-        <v>59</v>
-      </c>
+      <c r="C122" s="15"/>
       <c r="D122" s="11"/>
-      <c r="E122" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="F122" s="21" t="s">
-        <v>138</v>
-      </c>
+      <c r="E122" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F122" s="21"/>
       <c r="G122" s="14"/>
     </row>
-    <row r="123" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123" s="26"/>
       <c r="B123" s="26"/>
-      <c r="C123" s="15" t="s">
-        <v>123</v>
-      </c>
+      <c r="C123" s="15"/>
       <c r="D123" s="11"/>
       <c r="E123" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F123" s="21" t="s">
-        <v>83</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="F123" s="21"/>
       <c r="G123" s="14"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124" s="26"/>
       <c r="B124" s="26"/>
-      <c r="C124" s="15"/>
+      <c r="C124" s="13" t="s">
+        <v>60</v>
+      </c>
       <c r="D124" s="11"/>
-      <c r="E124" s="10" t="s">
-        <v>20</v>
+      <c r="E124" s="32" t="s">
+        <v>137</v>
       </c>
       <c r="F124" s="21"/>
       <c r="G124" s="14"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A125" s="26"/>
       <c r="B125" s="26"/>
-      <c r="C125" s="15"/>
+      <c r="C125" s="15" t="s">
+        <v>124</v>
+      </c>
       <c r="D125" s="11"/>
       <c r="E125" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F125" s="21"/>
+        <v>57</v>
+      </c>
+      <c r="F125" s="21" t="s">
+        <v>83</v>
+      </c>
       <c r="G125" s="14"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
@@ -5273,7 +5431,7 @@
       <c r="C126" s="15"/>
       <c r="D126" s="11"/>
       <c r="E126" s="10" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="F126" s="21"/>
       <c r="G126" s="14"/>
@@ -5281,86 +5439,88 @@
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" s="26"/>
       <c r="B127" s="26"/>
-      <c r="C127" s="13" t="s">
-        <v>60</v>
-      </c>
+      <c r="C127" s="15"/>
       <c r="D127" s="11"/>
-      <c r="E127" s="32" t="s">
-        <v>137</v>
+      <c r="E127" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="F127" s="21"/>
       <c r="G127" s="14"/>
     </row>
-    <row r="128" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" s="26"/>
       <c r="B128" s="26"/>
-      <c r="C128" s="15" t="s">
-        <v>124</v>
-      </c>
+      <c r="C128" s="15"/>
       <c r="D128" s="11"/>
       <c r="E128" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F128" s="21" t="s">
-        <v>83</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F128" s="21"/>
       <c r="G128" s="14"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129" s="26"/>
       <c r="B129" s="26"/>
-      <c r="C129" s="15"/>
+      <c r="C129" s="13" t="s">
+        <v>61</v>
+      </c>
       <c r="D129" s="11"/>
-      <c r="E129" s="10" t="s">
-        <v>20</v>
+      <c r="E129" s="32" t="s">
+        <v>137</v>
       </c>
       <c r="F129" s="21"/>
       <c r="G129" s="14"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A130" s="26"/>
-      <c r="B130" s="26"/>
-      <c r="C130" s="15"/>
+      <c r="B130" s="9"/>
+      <c r="C130" s="15" t="s">
+        <v>125</v>
+      </c>
       <c r="D130" s="11"/>
       <c r="E130" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F130" s="21"/>
       <c r="G130" s="14"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A131" s="26"/>
-      <c r="B131" s="26"/>
-      <c r="C131" s="15"/>
+      <c r="B131" s="9"/>
+      <c r="C131" s="31" t="s">
+        <v>139</v>
+      </c>
       <c r="D131" s="11"/>
       <c r="E131" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F131" s="21"/>
+        <v>20</v>
+      </c>
+      <c r="F131" s="21" t="s">
+        <v>77</v>
+      </c>
       <c r="G131" s="14"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A132" s="26"/>
-      <c r="B132" s="26"/>
-      <c r="C132" s="13" t="s">
-        <v>61</v>
+      <c r="B132" s="9"/>
+      <c r="C132" s="31" t="s">
+        <v>139</v>
       </c>
       <c r="D132" s="11"/>
-      <c r="E132" s="32" t="s">
-        <v>137</v>
+      <c r="E132" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="F132" s="21"/>
       <c r="G132" s="14"/>
     </row>
-    <row r="133" spans="1:7" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A133" s="26"/>
       <c r="B133" s="9"/>
-      <c r="C133" s="15" t="s">
-        <v>125</v>
+      <c r="C133" s="31" t="s">
+        <v>139</v>
       </c>
       <c r="D133" s="11"/>
       <c r="E133" s="10" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="F133" s="21"/>
       <c r="G133" s="14"/>
@@ -5368,40 +5528,40 @@
     <row r="134" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A134" s="26"/>
       <c r="B134" s="9"/>
-      <c r="C134" s="31" t="s">
-        <v>139</v>
+      <c r="C134" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="D134" s="11"/>
-      <c r="E134" s="10" t="s">
-        <v>20</v>
+      <c r="E134" s="32" t="s">
+        <v>137</v>
       </c>
       <c r="F134" s="21" t="s">
-        <v>77</v>
+        <v>138</v>
       </c>
       <c r="G134" s="14"/>
     </row>
-    <row r="135" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A135" s="26"/>
       <c r="B135" s="9"/>
-      <c r="C135" s="31" t="s">
-        <v>139</v>
+      <c r="C135" s="15" t="s">
+        <v>126</v>
       </c>
       <c r="D135" s="11"/>
       <c r="E135" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F135" s="21"/>
+        <v>57</v>
+      </c>
+      <c r="F135" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="G135" s="14"/>
     </row>
     <row r="136" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A136" s="26"/>
       <c r="B136" s="9"/>
-      <c r="C136" s="31" t="s">
-        <v>139</v>
-      </c>
+      <c r="C136" s="29"/>
       <c r="D136" s="11"/>
       <c r="E136" s="10" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="F136" s="21"/>
       <c r="G136" s="14"/>
@@ -5409,42 +5569,38 @@
     <row r="137" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A137" s="26"/>
       <c r="B137" s="9"/>
-      <c r="C137" s="13" t="s">
-        <v>59</v>
-      </c>
+      <c r="C137" s="29"/>
       <c r="D137" s="11"/>
-      <c r="E137" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="F137" s="21" t="s">
-        <v>138</v>
-      </c>
+      <c r="E137" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F137" s="21"/>
       <c r="G137" s="14"/>
     </row>
-    <row r="138" spans="1:7" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A138" s="26"/>
       <c r="B138" s="9"/>
-      <c r="C138" s="15" t="s">
-        <v>126</v>
-      </c>
+      <c r="C138" s="28"/>
       <c r="D138" s="11"/>
       <c r="E138" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F138" s="21" t="s">
-        <v>78</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="F138" s="21"/>
       <c r="G138" s="14"/>
     </row>
-    <row r="139" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A139" s="26"/>
       <c r="B139" s="9"/>
-      <c r="C139" s="29"/>
+      <c r="C139" s="15" t="s">
+        <v>140</v>
+      </c>
       <c r="D139" s="11"/>
       <c r="E139" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F139" s="21"/>
+        <v>57</v>
+      </c>
+      <c r="F139" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="G139" s="14"/>
     </row>
     <row r="140" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -5453,7 +5609,7 @@
       <c r="C140" s="29"/>
       <c r="D140" s="11"/>
       <c r="E140" s="10" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="F140" s="21"/>
       <c r="G140" s="14"/>
@@ -5461,97 +5617,98 @@
     <row r="141" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A141" s="26"/>
       <c r="B141" s="9"/>
-      <c r="C141" s="28"/>
+      <c r="C141" s="29"/>
       <c r="D141" s="11"/>
-      <c r="E141" s="10" t="s">
-        <v>85</v>
+      <c r="E141" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="F141" s="21"/>
       <c r="G141" s="14"/>
     </row>
-    <row r="142" spans="1:7" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A142" s="26"/>
       <c r="B142" s="9"/>
-      <c r="C142" s="15" t="s">
-        <v>140</v>
-      </c>
+      <c r="C142" s="29"/>
       <c r="D142" s="11"/>
-      <c r="E142" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F142" s="21" t="s">
-        <v>78</v>
-      </c>
+      <c r="E142" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F142" s="21"/>
       <c r="G142" s="14"/>
     </row>
     <row r="143" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A143" s="26"/>
       <c r="B143" s="9"/>
-      <c r="C143" s="29"/>
+      <c r="C143" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="D143" s="11"/>
-      <c r="E143" s="10" t="s">
-        <v>20</v>
+      <c r="E143" s="32" t="s">
+        <v>137</v>
       </c>
       <c r="F143" s="21"/>
       <c r="G143" s="14"/>
     </row>
-    <row r="144" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:7" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A144" s="26"/>
       <c r="B144" s="9"/>
-      <c r="C144" s="29"/>
+      <c r="C144" s="15" t="s">
+        <v>127</v>
+      </c>
       <c r="D144" s="11"/>
-      <c r="E144" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F144" s="21"/>
+      <c r="E144" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F144" s="21" t="s">
+        <v>129</v>
+      </c>
       <c r="G144" s="14"/>
     </row>
-    <row r="145" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A145" s="26"/>
       <c r="B145" s="9"/>
-      <c r="C145" s="29"/>
+      <c r="C145" s="13" t="s">
+        <v>128</v>
+      </c>
       <c r="D145" s="11"/>
-      <c r="E145" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F145" s="21"/>
+      <c r="E145" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F145" s="22"/>
       <c r="G145" s="14"/>
     </row>
-    <row r="146" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A146" s="26"/>
       <c r="B146" s="9"/>
-      <c r="C146" s="9" t="s">
-        <v>61</v>
+      <c r="C146" s="13" t="s">
+        <v>128</v>
       </c>
       <c r="D146" s="11"/>
-      <c r="E146" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="F146" s="21"/>
-      <c r="G146" s="14"/>
-    </row>
-    <row r="147" spans="1:7" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E146" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G146" s="13"/>
+    </row>
+    <row r="147" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" s="26"/>
       <c r="B147" s="9"/>
       <c r="C147" s="15" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D147" s="11"/>
       <c r="E147" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F147" s="21" t="s">
-        <v>129</v>
-      </c>
+      <c r="F147" s="22"/>
       <c r="G147" s="14"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A148" s="26"/>
       <c r="B148" s="9"/>
-      <c r="C148" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D148" s="11"/>
+      <c r="C148" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="D148" s="9"/>
       <c r="E148" s="10" t="s">
         <v>20</v>
       </c>
@@ -5561,24 +5718,25 @@
     <row r="149" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A149" s="26"/>
       <c r="B149" s="9"/>
-      <c r="C149" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D149" s="11"/>
+      <c r="C149" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="D149" s="9"/>
       <c r="E149" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G149" s="13"/>
-    </row>
-    <row r="150" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+      <c r="F149" s="22"/>
+      <c r="G149" s="14"/>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A150" s="26"/>
       <c r="B150" s="9"/>
-      <c r="C150" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="D150" s="11"/>
-      <c r="E150" s="10" t="s">
-        <v>57</v>
+      <c r="C150" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="D150" s="9"/>
+      <c r="E150" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="F150" s="22"/>
       <c r="G150" s="14"/>
@@ -5586,25 +5744,25 @@
     <row r="151" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A151" s="26"/>
       <c r="B151" s="9"/>
-      <c r="C151" s="31" t="s">
-        <v>131</v>
+      <c r="C151" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="D151" s="9"/>
-      <c r="E151" s="10" t="s">
-        <v>20</v>
+      <c r="E151" s="32" t="s">
+        <v>137</v>
       </c>
       <c r="F151" s="22"/>
       <c r="G151" s="14"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A152" s="26"/>
       <c r="B152" s="9"/>
-      <c r="C152" s="31" t="s">
-        <v>131</v>
+      <c r="C152" s="15" t="s">
+        <v>132</v>
       </c>
       <c r="D152" s="9"/>
-      <c r="E152" s="9" t="s">
-        <v>59</v>
+      <c r="E152" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="F152" s="22"/>
       <c r="G152" s="14"/>
@@ -5612,64 +5770,64 @@
     <row r="153" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A153" s="26"/>
       <c r="B153" s="9"/>
-      <c r="C153" s="31" t="s">
-        <v>131</v>
+      <c r="C153" s="14" t="s">
+        <v>133</v>
       </c>
       <c r="D153" s="9"/>
-      <c r="E153" s="9" t="s">
-        <v>72</v>
+      <c r="E153" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="F153" s="22"/>
-      <c r="G153" s="14"/>
+      <c r="G153" s="16"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A154" s="26"/>
       <c r="B154" s="9"/>
       <c r="C154" s="14" t="s">
-        <v>72</v>
+        <v>133</v>
       </c>
       <c r="D154" s="9"/>
-      <c r="E154" s="32" t="s">
-        <v>137</v>
+      <c r="E154" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="F154" s="22"/>
-      <c r="G154" s="14"/>
-    </row>
-    <row r="155" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G154" s="16"/>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A155" s="26"/>
       <c r="B155" s="9"/>
-      <c r="C155" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="D155" s="9"/>
-      <c r="E155" s="10" t="s">
-        <v>57</v>
+      <c r="C155" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D155" s="11"/>
+      <c r="E155" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="F155" s="22"/>
-      <c r="G155" s="14"/>
+      <c r="G155" s="16"/>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A156" s="26"/>
       <c r="B156" s="9"/>
       <c r="C156" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D156" s="9"/>
-      <c r="E156" s="10" t="s">
-        <v>20</v>
+        <v>73</v>
+      </c>
+      <c r="D156" s="11"/>
+      <c r="E156" s="32" t="s">
+        <v>137</v>
       </c>
       <c r="F156" s="22"/>
       <c r="G156" s="16"/>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A157" s="26"/>
       <c r="B157" s="9"/>
-      <c r="C157" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D157" s="9"/>
-      <c r="E157" s="9" t="s">
-        <v>60</v>
+      <c r="C157" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="D157" s="11"/>
+      <c r="E157" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="F157" s="22"/>
       <c r="G157" s="16"/>
@@ -5678,11 +5836,11 @@
       <c r="A158" s="26"/>
       <c r="B158" s="9"/>
       <c r="C158" s="14" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D158" s="11"/>
-      <c r="E158" s="9" t="s">
-        <v>73</v>
+      <c r="E158" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="F158" s="22"/>
       <c r="G158" s="16"/>
@@ -5691,152 +5849,131 @@
       <c r="A159" s="26"/>
       <c r="B159" s="9"/>
       <c r="C159" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D159" s="11"/>
-      <c r="E159" s="32" t="s">
-        <v>137</v>
+        <v>135</v>
+      </c>
+      <c r="D159" s="9"/>
+      <c r="E159" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="F159" s="22"/>
-      <c r="G159" s="16"/>
-    </row>
-    <row r="160" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G159" s="14"/>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A160" s="26"/>
       <c r="B160" s="9"/>
-      <c r="C160" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="D160" s="11"/>
-      <c r="E160" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F160" s="22"/>
+      <c r="C160" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D160" s="10"/>
+      <c r="E160" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F160" s="20"/>
       <c r="G160" s="16"/>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A161" s="26"/>
+      <c r="A161" s="8"/>
       <c r="B161" s="9"/>
       <c r="C161" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D161" s="11"/>
-      <c r="E161" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F161" s="22"/>
+        <v>74</v>
+      </c>
+      <c r="D161" s="10"/>
+      <c r="E161" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="F161" s="20"/>
       <c r="G161" s="16"/>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A162" s="26"/>
-      <c r="B162" s="9"/>
-      <c r="C162" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D162" s="9"/>
-      <c r="E162" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F162" s="22"/>
+      <c r="A162" s="8"/>
+      <c r="B162" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C162" s="13"/>
+      <c r="D162" s="11"/>
+      <c r="E162" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F162" s="20" t="s">
+        <v>111</v>
+      </c>
       <c r="G162" s="14"/>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A163" s="26"/>
-      <c r="B163" s="9"/>
-      <c r="C163" s="14" t="s">
-        <v>135</v>
-      </c>
+      <c r="A163" s="8"/>
+      <c r="B163" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C163" s="13"/>
       <c r="D163" s="10"/>
-      <c r="E163" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F163" s="20"/>
-      <c r="G163" s="16"/>
+      <c r="E163" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F163" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="G163" s="14"/>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A164" s="8"/>
-      <c r="B164" s="9"/>
-      <c r="C164" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D164" s="10"/>
-      <c r="E164" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="F164" s="20"/>
-      <c r="G164" s="16"/>
+      <c r="A164">
+        <f>ROUND(COUNTA(A4:A163)/ROWS(A4:A163)*100,0)</f>
+        <v>28</v>
+      </c>
+      <c r="B164" s="25" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A165" s="8"/>
-      <c r="B165" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C165" s="13"/>
-      <c r="D165" s="11"/>
-      <c r="E165" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="F165" s="20" t="s">
-        <v>111</v>
-      </c>
+      <c r="F165" s="22"/>
       <c r="G165" s="14"/>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A166" s="8"/>
-      <c r="B166" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C166" s="13"/>
-      <c r="D166" s="10"/>
-      <c r="E166" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="F166" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="G166" s="14"/>
+      <c r="C166" s="7"/>
+      <c r="D166" s="5"/>
+      <c r="E166" s="5"/>
+      <c r="F166" s="24"/>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A167">
-        <f>ROUND(COUNTA(A4:A166)/ROWS(A4:A166)*100,0)</f>
-        <v>18</v>
-      </c>
-      <c r="B167" s="25" t="s">
-        <v>141</v>
-      </c>
+      <c r="A167" t="s">
+        <v>86</v>
+      </c>
+      <c r="C167" s="7"/>
+      <c r="D167" s="5"/>
+      <c r="E167" s="5"/>
+      <c r="F167" s="24"/>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A168" s="8"/>
-      <c r="F168" s="22"/>
-      <c r="G168" s="14"/>
+      <c r="B168" t="s">
+        <v>87</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E168" t="s">
+        <v>88</v>
+      </c>
+      <c r="F168" s="24"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C169" s="7"/>
-      <c r="D169" s="5"/>
-      <c r="E169" s="5"/>
       <c r="F169" s="24"/>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A170" t="s">
-        <v>86</v>
-      </c>
       <c r="C170" s="7"/>
       <c r="D170" s="5"/>
       <c r="E170" s="5"/>
       <c r="F170" s="24"/>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B171" t="s">
-        <v>87</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E171" t="s">
-        <v>88</v>
-      </c>
+      <c r="C171" s="7"/>
+      <c r="D171" s="5"/>
+      <c r="E171" s="5"/>
       <c r="F171" s="24"/>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C172" s="7"/>
+      <c r="D172" s="5"/>
+      <c r="E172" s="5"/>
       <c r="F172" s="24"/>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.35">
@@ -5857,103 +5994,60 @@
       <c r="E175" s="5"/>
       <c r="F175" s="24"/>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C176" s="7"/>
-      <c r="D176" s="5"/>
-      <c r="E176" s="5"/>
-      <c r="F176" s="24"/>
-    </row>
-    <row r="177" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C177" s="7"/>
-      <c r="D177" s="5"/>
-      <c r="E177" s="5"/>
-      <c r="F177" s="24"/>
-    </row>
-    <row r="178" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C178" s="7"/>
-      <c r="D178" s="5"/>
-      <c r="E178" s="5"/>
-      <c r="F178" s="24"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A168 A97 B118:B132 A13:A14 A8">
-    <cfRule type="notContainsBlanks" dxfId="90" priority="351">
+  <conditionalFormatting sqref="A165 A94 B115:B129 A13:A14 A8 A37:A47 A49:A51">
+    <cfRule type="notContainsBlanks" dxfId="85" priority="354">
       <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37:A65">
-    <cfRule type="notContainsBlanks" dxfId="89" priority="141">
-      <formula>LEN(TRIM(A37))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A94">
-    <cfRule type="notContainsBlanks" dxfId="87" priority="136">
-      <formula>LEN(TRIM(A94))&gt;0</formula>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="notContainsBlanks" dxfId="84" priority="139">
+      <formula>LEN(TRIM(A91))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A76">
+    <cfRule type="notContainsBlanks" dxfId="83" priority="100">
+      <formula>LEN(TRIM(A76))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="notContainsBlanks" dxfId="82" priority="143">
+      <formula>LEN(TRIM(A59))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68:A70">
+    <cfRule type="notContainsBlanks" dxfId="81" priority="142">
+      <formula>LEN(TRIM(A68))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71:A73">
+    <cfRule type="notContainsBlanks" dxfId="80" priority="141">
+      <formula>LEN(TRIM(A71))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A162:A163">
+    <cfRule type="notContainsBlanks" dxfId="79" priority="136">
+      <formula>LEN(TRIM(A162))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58">
+    <cfRule type="notContainsBlanks" dxfId="78" priority="105">
+      <formula>LEN(TRIM(A58))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A77">
+    <cfRule type="notContainsBlanks" dxfId="76" priority="99">
+      <formula>LEN(TRIM(A77))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A79">
-    <cfRule type="notContainsBlanks" dxfId="86" priority="97">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="97">
       <formula>LEN(TRIM(A79))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A68">
-    <cfRule type="notContainsBlanks" dxfId="85" priority="140">
-      <formula>LEN(TRIM(A68))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71:A73">
-    <cfRule type="notContainsBlanks" dxfId="84" priority="139">
-      <formula>LEN(TRIM(A71))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A74:A76">
-    <cfRule type="notContainsBlanks" dxfId="83" priority="138">
-      <formula>LEN(TRIM(A74))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A165:A166">
-    <cfRule type="notContainsBlanks" dxfId="82" priority="133">
-      <formula>LEN(TRIM(A165))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67">
-    <cfRule type="notContainsBlanks" dxfId="81" priority="102">
-      <formula>LEN(TRIM(A67))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A66">
-    <cfRule type="notContainsBlanks" dxfId="80" priority="103">
-      <formula>LEN(TRIM(A66))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A80">
-    <cfRule type="notContainsBlanks" dxfId="79" priority="96">
+    <cfRule type="notContainsBlanks" dxfId="74" priority="96">
       <formula>LEN(TRIM(A80))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A82">
-    <cfRule type="notContainsBlanks" dxfId="78" priority="94">
-      <formula>LEN(TRIM(A82))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A83">
-    <cfRule type="notContainsBlanks" dxfId="77" priority="93">
-      <formula>LEN(TRIM(A83))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A81">
-    <cfRule type="notContainsBlanks" dxfId="76" priority="95">
-      <formula>LEN(TRIM(A81))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A84">
-    <cfRule type="notContainsBlanks" dxfId="75" priority="92">
-      <formula>LEN(TRIM(A84))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70">
-    <cfRule type="notContainsBlanks" dxfId="74" priority="100">
-      <formula>LEN(TRIM(A70))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78">
@@ -5961,339 +6055,369 @@
       <formula>LEN(TRIM(A78))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
-    <cfRule type="notContainsBlanks" dxfId="72" priority="101">
-      <formula>LEN(TRIM(A69))&gt;0</formula>
+  <conditionalFormatting sqref="A81">
+    <cfRule type="notContainsBlanks" dxfId="72" priority="95">
+      <formula>LEN(TRIM(A81))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:A67">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="103">
+      <formula>LEN(TRIM(A61))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A75">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="101">
+      <formula>LEN(TRIM(A75))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60">
+    <cfRule type="notContainsBlanks" dxfId="69" priority="104">
+      <formula>LEN(TRIM(A60))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A83">
+    <cfRule type="notContainsBlanks" dxfId="68" priority="93">
+      <formula>LEN(TRIM(A83))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A74">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="102">
+      <formula>LEN(TRIM(A74))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="notContainsBlanks" dxfId="66" priority="89">
+      <formula>LEN(TRIM(A87))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="94">
+      <formula>LEN(TRIM(A82))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86">
-    <cfRule type="notContainsBlanks" dxfId="71" priority="90">
+    <cfRule type="notContainsBlanks" dxfId="64" priority="91">
       <formula>LEN(TRIM(A86))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A77">
-    <cfRule type="notContainsBlanks" dxfId="70" priority="99">
-      <formula>LEN(TRIM(A77))&gt;0</formula>
+  <conditionalFormatting sqref="A88">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="90">
+      <formula>LEN(TRIM(A88))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A92">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="86">
+      <formula>LEN(TRIM(A92))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A97">
+    <cfRule type="notContainsBlanks" dxfId="61" priority="79">
+      <formula>LEN(TRIM(A97))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A100">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="74">
+      <formula>LEN(TRIM(A100))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A95">
+    <cfRule type="notContainsBlanks" dxfId="59" priority="78">
+      <formula>LEN(TRIM(A95))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A96">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="77">
+      <formula>LEN(TRIM(A96))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A101">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="73">
+      <formula>LEN(TRIM(A101))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A102">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="72">
+      <formula>LEN(TRIM(A102))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A98">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="76">
+      <formula>LEN(TRIM(A98))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A99">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="75">
+      <formula>LEN(TRIM(A99))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A103">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="71">
+      <formula>LEN(TRIM(A103))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A104">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="70">
+      <formula>LEN(TRIM(A104))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A105">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="69">
+      <formula>LEN(TRIM(A105))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A106">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="68">
+      <formula>LEN(TRIM(A106))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A107">
+    <cfRule type="notContainsBlanks" dxfId="49" priority="67">
+      <formula>LEN(TRIM(A107))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A108">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="66">
+      <formula>LEN(TRIM(A108))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A109">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="65">
+      <formula>LEN(TRIM(A109))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A110">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="64">
+      <formula>LEN(TRIM(A110))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A111">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="63">
+      <formula>LEN(TRIM(A111))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A112">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="62">
+      <formula>LEN(TRIM(A112))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A113">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="61">
+      <formula>LEN(TRIM(A113))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A114">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="60">
+      <formula>LEN(TRIM(A114))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A115:A119">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="58">
+      <formula>LEN(TRIM(A115))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A120:A124">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="57">
+      <formula>LEN(TRIM(A120))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A125:A129">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="56">
+      <formula>LEN(TRIM(A125))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A130:A134">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="55">
+      <formula>LEN(TRIM(A130))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A135:A138">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="54">
+      <formula>LEN(TRIM(A135))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A144:A146">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="53">
+      <formula>LEN(TRIM(A144))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A147:A151">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="52">
+      <formula>LEN(TRIM(A147))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A152:A156">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="51">
+      <formula>LEN(TRIM(A152))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A161">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="50">
+      <formula>LEN(TRIM(A161))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A157:A160">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="49">
+      <formula>LEN(TRIM(A157))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A139:A143">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="48">
+      <formula>LEN(TRIM(A139))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A84">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="43">
+      <formula>LEN(TRIM(A84))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A85">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="42">
+      <formula>LEN(TRIM(A85))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A89">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="41">
+      <formula>LEN(TRIM(A89))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90">
-    <cfRule type="notContainsBlanks" dxfId="69" priority="86">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="40">
       <formula>LEN(TRIM(A90))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A85">
-    <cfRule type="notContainsBlanks" dxfId="68" priority="91">
-      <formula>LEN(TRIM(A85))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A89">
-    <cfRule type="notContainsBlanks" dxfId="67" priority="88">
-      <formula>LEN(TRIM(A89))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A91">
-    <cfRule type="notContainsBlanks" dxfId="66" priority="87">
-      <formula>LEN(TRIM(A91))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A95">
-    <cfRule type="notContainsBlanks" dxfId="65" priority="83">
-      <formula>LEN(TRIM(A95))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A100">
-    <cfRule type="notContainsBlanks" dxfId="64" priority="76">
-      <formula>LEN(TRIM(A100))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A103">
-    <cfRule type="notContainsBlanks" dxfId="63" priority="71">
-      <formula>LEN(TRIM(A103))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A98">
-    <cfRule type="notContainsBlanks" dxfId="62" priority="75">
-      <formula>LEN(TRIM(A98))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A99">
-    <cfRule type="notContainsBlanks" dxfId="61" priority="74">
-      <formula>LEN(TRIM(A99))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A104">
-    <cfRule type="notContainsBlanks" dxfId="60" priority="70">
-      <formula>LEN(TRIM(A104))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A105">
-    <cfRule type="notContainsBlanks" dxfId="59" priority="69">
-      <formula>LEN(TRIM(A105))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A101">
-    <cfRule type="notContainsBlanks" dxfId="58" priority="73">
-      <formula>LEN(TRIM(A101))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A102">
-    <cfRule type="notContainsBlanks" dxfId="57" priority="72">
-      <formula>LEN(TRIM(A102))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A106">
-    <cfRule type="notContainsBlanks" dxfId="56" priority="68">
-      <formula>LEN(TRIM(A106))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A107">
-    <cfRule type="notContainsBlanks" dxfId="55" priority="67">
-      <formula>LEN(TRIM(A107))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A108">
-    <cfRule type="notContainsBlanks" dxfId="54" priority="66">
-      <formula>LEN(TRIM(A108))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A109">
-    <cfRule type="notContainsBlanks" dxfId="53" priority="65">
-      <formula>LEN(TRIM(A109))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A110">
-    <cfRule type="notContainsBlanks" dxfId="52" priority="64">
-      <formula>LEN(TRIM(A110))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A111">
-    <cfRule type="notContainsBlanks" dxfId="51" priority="63">
-      <formula>LEN(TRIM(A111))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A112">
-    <cfRule type="notContainsBlanks" dxfId="50" priority="62">
-      <formula>LEN(TRIM(A112))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A113">
-    <cfRule type="notContainsBlanks" dxfId="49" priority="61">
-      <formula>LEN(TRIM(A113))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A114">
-    <cfRule type="notContainsBlanks" dxfId="48" priority="60">
-      <formula>LEN(TRIM(A114))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A115">
-    <cfRule type="notContainsBlanks" dxfId="47" priority="59">
-      <formula>LEN(TRIM(A115))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A116">
-    <cfRule type="notContainsBlanks" dxfId="46" priority="58">
-      <formula>LEN(TRIM(A116))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A117">
-    <cfRule type="notContainsBlanks" dxfId="45" priority="57">
-      <formula>LEN(TRIM(A117))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A118:A122">
-    <cfRule type="notContainsBlanks" dxfId="44" priority="55">
-      <formula>LEN(TRIM(A118))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A123:A127">
-    <cfRule type="notContainsBlanks" dxfId="43" priority="54">
-      <formula>LEN(TRIM(A123))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A128:A132">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="53">
-      <formula>LEN(TRIM(A128))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A133:A137">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="52">
-      <formula>LEN(TRIM(A133))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A138:A141">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="51">
-      <formula>LEN(TRIM(A138))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A147:A149">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="50">
-      <formula>LEN(TRIM(A147))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A150:A154">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="49">
-      <formula>LEN(TRIM(A150))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A155:A159">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="48">
-      <formula>LEN(TRIM(A155))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A164">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="47">
-      <formula>LEN(TRIM(A164))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A160:A163">
-    <cfRule type="notContainsBlanks" dxfId="35" priority="46">
-      <formula>LEN(TRIM(A160))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A142:A146">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="45">
-      <formula>LEN(TRIM(A142))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A87">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="40">
-      <formula>LEN(TRIM(A87))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A88">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="39">
-      <formula>LEN(TRIM(A88))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A92">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="38">
-      <formula>LEN(TRIM(A92))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A93">
-    <cfRule type="notContainsBlanks" dxfId="30" priority="37">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="39">
       <formula>LEN(TRIM(A93))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A96">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="36">
-      <formula>LEN(TRIM(A96))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="35">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="38">
       <formula>LEN(TRIM(A10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="22">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="25">
       <formula>LEN(TRIM(A32))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="29">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="32">
       <formula>LEN(TRIM(A12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="28">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="31">
       <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="27">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="30">
       <formula>LEN(TRIM(A20))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:A19">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="26">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="29">
       <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="24">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="27">
       <formula>LEN(TRIM(A22))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="23">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="26">
       <formula>LEN(TRIM(A28))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A27">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="24">
       <formula>LEN(TRIM(A23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="19">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="22">
       <formula>LEN(TRIM(A36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="15">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="16">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
+      <formula>LEN(TRIM(A6))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
+      <formula>LEN(TRIM(A7))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
     <cfRule type="notContainsBlanks" dxfId="10" priority="11">
-      <formula>LEN(TRIM(A6))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
+      <formula>LEN(TRIM(A15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
     <cfRule type="notContainsBlanks" dxfId="9" priority="10">
-      <formula>LEN(TRIM(A7))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
+      <formula>LEN(TRIM(A21))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29">
     <cfRule type="notContainsBlanks" dxfId="8" priority="9">
-      <formula>LEN(TRIM(A9))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
+      <formula>LEN(TRIM(A29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
     <cfRule type="notContainsBlanks" dxfId="7" priority="8">
-      <formula>LEN(TRIM(A15))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
+      <formula>LEN(TRIM(A33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
     <cfRule type="notContainsBlanks" dxfId="6" priority="7">
-      <formula>LEN(TRIM(A21))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31">
     <cfRule type="notContainsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(A29))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
+      <formula>LEN(TRIM(A31))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
     <cfRule type="notContainsBlanks" dxfId="4" priority="5">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
     <cfRule type="notContainsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(A30))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
+      <formula>LEN(TRIM(A35))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48">
     <cfRule type="notContainsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(A31))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
+      <formula>LEN(TRIM(A48))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(A34))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35">
+      <formula>LEN(TRIM(A52))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A53:A57">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A35))&gt;0</formula>
+      <formula>LEN(TRIM(A53))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
WIP for VS and documenting the SMS approach
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="person_1" sheetId="1" r:id="rId1"/>
-    <sheet name="Issues" sheetId="2" r:id="rId2"/>
+    <sheet name="remapping" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -21,42 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="110">
-  <si>
-    <t>cdiscpilot01:Interval_LS1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Interval_RI1</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="122">
   <si>
     <t>Item</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Missing</t>
-  </si>
-  <si>
-    <t>study:StudyParticipationBegin</t>
-  </si>
-  <si>
-    <t>Issue</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Date_19</t>
-  </si>
-  <si>
-    <t>Interval label differs</t>
-  </si>
-  <si>
-    <t>difference</t>
   </si>
   <si>
     <t>Notes</t>
@@ -433,12 +400,81 @@
       <t>Assessed only for Person_1</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">cdiscpilot01:Visit_1e1uak4vs9dpl4d263rl3b9a1pongqrl_01-701-1015 </t>
+  </si>
+  <si>
+    <t>LATER!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:AssumeBodyPositionStanding_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:AssumeBodyPositionSupine_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">       cdiscpilot01:AssumeBodyPositionStanding_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25206_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25208_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25298_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25298_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25298_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25299_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25299_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25299_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25347_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C49676_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C49676_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C49676_3</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Systolic Blood Pressure</t>
+  </si>
+  <si>
+    <t>Diastolic Blood Pressure</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Pulse Rate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -602,6 +638,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -791,7 +834,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -982,7 +1025,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1037,10 +1080,23 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1411,11 +1467,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1431,30 +1487,30 @@
   <sheetData>
     <row r="1" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D1" s="23" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -1462,38 +1518,38 @@
         <v>43173</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C3" s="19">
         <v>1</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="16"/>
       <c r="B4" s="17" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C4" s="19">
         <v>1</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>53</v>
+        <v>41</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>42</v>
       </c>
       <c r="G4" s="18"/>
     </row>
@@ -1502,19 +1558,19 @@
         <v>43180</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C5" s="19">
         <v>1</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G5" s="18"/>
     </row>
@@ -1523,16 +1579,16 @@
         <v>43180</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C6" s="20">
         <v>2</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="F6"/>
       <c r="G6" s="18"/>
@@ -1542,19 +1598,19 @@
         <v>43180</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="G7"/>
     </row>
@@ -1563,16 +1619,16 @@
         <v>43180</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C8" s="20">
         <v>2</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F8"/>
       <c r="G8" s="18"/>
@@ -1582,16 +1638,16 @@
         <v>43181</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C9" s="20">
         <v>1</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="F9"/>
       <c r="G9" s="18"/>
@@ -1601,16 +1657,16 @@
         <v>43181</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C10" s="20">
         <v>2</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="F10"/>
       <c r="G10" s="18"/>
@@ -1620,16 +1676,16 @@
         <v>43181</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C11" s="20">
         <v>3</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F11"/>
       <c r="G11" s="18"/>
@@ -1639,19 +1695,19 @@
         <v>43181</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C12" s="20">
         <v>1</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F12" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="G12" s="18"/>
     </row>
@@ -1660,14 +1716,14 @@
         <v>43181</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="24" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F13"/>
       <c r="G13" s="18"/>
@@ -1677,14 +1733,14 @@
         <v>43181</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="24" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F14"/>
       <c r="G14" s="18"/>
@@ -1694,16 +1750,16 @@
         <v>43180</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C15" s="20">
         <v>1</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="F15"/>
       <c r="G15" s="18"/>
@@ -1713,16 +1769,16 @@
         <v>43180</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C16" s="20">
         <v>1</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="F16"/>
       <c r="G16" s="18"/>
@@ -1732,16 +1788,16 @@
         <v>43180</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C17" s="20">
         <v>1</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="F17"/>
       <c r="G17" s="18"/>
@@ -1751,16 +1807,16 @@
         <v>43180</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C18" s="20">
         <v>1</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="F18"/>
       <c r="G18" s="18"/>
@@ -1770,16 +1826,16 @@
         <v>43180</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C19" s="20">
         <v>1</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F19"/>
       <c r="G19" s="18"/>
@@ -1789,16 +1845,16 @@
         <v>43180</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C20" s="20">
         <v>1</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="F20"/>
       <c r="G20" s="18"/>
@@ -1808,16 +1864,16 @@
         <v>43180</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C21" s="20">
         <v>1</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F21"/>
       <c r="G21" s="18"/>
@@ -1827,16 +1883,16 @@
         <v>43180</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C22" s="20">
         <v>1</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="F22"/>
       <c r="G22" s="18"/>
@@ -1846,16 +1902,16 @@
         <v>43180</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C23" s="19">
         <v>2</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F23"/>
       <c r="G23" s="18"/>
@@ -1865,16 +1921,16 @@
         <v>43180</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C24" s="19">
         <v>2</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F24"/>
       <c r="G24" s="18"/>
@@ -1884,16 +1940,16 @@
         <v>43180</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C25" s="20">
         <v>1</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="F25"/>
       <c r="G25"/>
@@ -1903,16 +1959,16 @@
         <v>43180</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C26" s="20">
         <v>2</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F26"/>
       <c r="G26" s="18"/>
@@ -1922,16 +1978,16 @@
         <v>43180</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C27" s="20">
         <v>2</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F27"/>
       <c r="G27" s="18"/>
@@ -1941,14 +1997,14 @@
         <v>43180</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="23" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="F28"/>
       <c r="G28" s="18"/>
@@ -1958,59 +2014,59 @@
         <v>43180</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C29" s="19"/>
       <c r="D29" s="23" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F29"/>
       <c r="G29" s="18"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="16"/>
-      <c r="B30" s="17" t="s">
-        <v>106</v>
-      </c>
+      <c r="A30" s="16">
+        <v>43181</v>
+      </c>
+      <c r="B30" s="17"/>
       <c r="C30" s="19"/>
       <c r="D30" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" s="26" t="s">
-        <v>101</v>
+        <v>91</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="F30"/>
       <c r="G30" s="18"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="16"/>
-      <c r="B31" s="17" t="s">
-        <v>106</v>
-      </c>
+      <c r="A31" s="16">
+        <v>43181</v>
+      </c>
+      <c r="B31" s="17"/>
       <c r="C31" s="19"/>
       <c r="D31" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" s="26" t="s">
-        <v>101</v>
+        <v>92</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>92</v>
       </c>
       <c r="F31"/>
       <c r="G31" s="18"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="16"/>
-      <c r="B32" s="17" t="s">
-        <v>106</v>
-      </c>
+      <c r="A32" s="16">
+        <v>43181</v>
+      </c>
+      <c r="B32" s="17"/>
       <c r="C32" s="19"/>
       <c r="D32" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="E32" s="26" t="s">
-        <v>101</v>
+        <v>93</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>93</v>
       </c>
       <c r="F32"/>
       <c r="G32" s="18"/>
@@ -2018,116 +2074,193 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="16"/>
       <c r="B33" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="C33" s="19"/>
+        <v>95</v>
+      </c>
+      <c r="C33" s="19">
+        <v>1</v>
+      </c>
       <c r="D33" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="E33" s="26" t="s">
-        <v>101</v>
+        <v>26</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>99</v>
       </c>
       <c r="F33"/>
       <c r="G33" s="18"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="16">
-        <v>43181</v>
-      </c>
+      <c r="A34" s="16"/>
       <c r="B34" s="17"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="E34" s="23" t="s">
-        <v>102</v>
-      </c>
+      <c r="C34" s="19">
+        <v>2</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" s="7"/>
       <c r="F34"/>
       <c r="G34" s="18"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="16">
-        <v>43181</v>
-      </c>
+      <c r="A35" s="16"/>
       <c r="B35" s="17"/>
       <c r="C35" s="19"/>
-      <c r="D35" s="23" t="s">
+      <c r="D35" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="E35" s="23" t="s">
-        <v>103</v>
-      </c>
+      <c r="E35" s="7"/>
       <c r="F35"/>
       <c r="G35" s="18"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="16">
-        <v>43181</v>
-      </c>
+      <c r="A36" s="16"/>
       <c r="B36" s="17"/>
       <c r="C36" s="19"/>
-      <c r="D36" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="E36" s="23" t="s">
-        <v>104</v>
-      </c>
+      <c r="D36" s="34"/>
+      <c r="E36" s="7"/>
       <c r="F36"/>
       <c r="G36" s="18"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <f>ROUND(COUNTA(A3:A36)/ROWS(A3:A36)*100,0)</f>
-        <v>85</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" s="20"/>
+      <c r="A37" s="16"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="7"/>
       <c r="F37"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="8"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="10"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="19">
+        <v>2</v>
+      </c>
+      <c r="D38" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38"/>
+      <c r="G38" s="18"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D39" s="25"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="19"/>
       <c r="E39" s="7"/>
-      <c r="F39" s="14"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D40" s="25"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="14"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D41" s="25"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="14"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D42" s="25"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="14"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D43" s="25"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="14"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D44" s="25"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="14"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D45" s="25"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="14"/>
+      <c r="F39"/>
+      <c r="G39" s="18"/>
+    </row>
+    <row r="40" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="27"/>
+      <c r="B40" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="29"/>
+      <c r="D40" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="31"/>
+      <c r="F40" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G40" s="33"/>
+    </row>
+    <row r="41" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="27"/>
+      <c r="B41" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="29"/>
+      <c r="D41" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G41" s="33"/>
+    </row>
+    <row r="42" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="27"/>
+      <c r="B42" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="29"/>
+      <c r="D42" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F42" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G42" s="33"/>
+    </row>
+    <row r="43" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D43" s="30"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G43" s="31"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <f>ROUND(COUNTA(A3:A42)/ROWS(A3:A42)*100,0)</f>
+        <v>73</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" s="20"/>
+      <c r="F46"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="8"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D48" s="25"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="14"/>
+    </row>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D49" s="25"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="14"/>
+    </row>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D50" s="25"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="14"/>
+    </row>
+    <row r="51" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D51" s="25"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="14"/>
+    </row>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D52" s="25"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="14"/>
+    </row>
+    <row r="53" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D53" s="25"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="14"/>
+    </row>
+    <row r="54" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D54" s="25"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="14"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A38 A8:A36">
+  <conditionalFormatting sqref="A47 A8:A42">
     <cfRule type="notContainsBlanks" dxfId="1" priority="355">
       <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>
@@ -2144,70 +2277,142 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A2:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" customWidth="1"/>
     <col min="4" max="4" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2233,106 +2438,106 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -2341,40 +2546,40 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3">
         <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D16">
         <v>57</v>
@@ -2382,13 +2587,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B17" s="3">
         <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D17">
         <v>64</v>
@@ -2396,13 +2601,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B18" s="4">
         <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D18">
         <v>83</v>
@@ -2412,37 +2617,37 @@
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D19">
         <v>129</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D20">
         <v>131</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D21">
         <v>147</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
nothing to see here.
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="person_1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="128">
   <si>
     <t>Item</t>
   </si>
@@ -469,12 +469,30 @@
   <si>
     <t>Pulse Rate</t>
   </si>
+  <si>
+    <t>C71148.C62166</t>
+  </si>
+  <si>
+    <t>STANDING</t>
+  </si>
+  <si>
+    <t>The outcome of standing</t>
+  </si>
+  <si>
+    <t>ADDTIONAL VALIDATION</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Lifespan_pt2m6avt4r1v33ksdu1m4ggqjgec0q9f_m9eproucjuhbto78r3ij902mqsklh6so</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Lifespan_2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -644,6 +662,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="35">
@@ -1025,7 +1049,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1097,6 +1121,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1467,11 +1492,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1745,79 +1770,45 @@
       <c r="F14"/>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="20">
-        <v>1</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>68</v>
+    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>126</v>
       </c>
       <c r="F15"/>
       <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="20">
-        <v>1</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="A16" s="22"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="21"/>
       <c r="F16"/>
       <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="20">
-        <v>1</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>70</v>
-      </c>
+      <c r="A17" s="22"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="21"/>
       <c r="F17"/>
       <c r="G17" s="18"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="20">
-        <v>1</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="A18" s="22"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="21"/>
       <c r="F18"/>
       <c r="G18" s="18"/>
     </row>
@@ -1832,10 +1823,10 @@
         <v>1</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F19"/>
       <c r="G19" s="18"/>
@@ -1851,10 +1842,10 @@
         <v>1</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F20"/>
       <c r="G20" s="18"/>
@@ -1870,15 +1861,15 @@
         <v>1</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F21"/>
       <c r="G21" s="18"/>
     </row>
-    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="16">
         <v>43180</v>
       </c>
@@ -1889,10 +1880,10 @@
         <v>1</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F22"/>
       <c r="G22" s="18"/>
@@ -1904,14 +1895,14 @@
       <c r="B23" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="19">
-        <v>2</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>81</v>
+      <c r="C23" s="20">
+        <v>1</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="F23"/>
       <c r="G23" s="18"/>
@@ -1923,19 +1914,19 @@
       <c r="B24" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="19">
-        <v>2</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>82</v>
+      <c r="C24" s="20">
+        <v>1</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="F24"/>
       <c r="G24" s="18"/>
     </row>
-    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="16">
         <v>43180</v>
       </c>
@@ -1946,15 +1937,15 @@
         <v>1</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F25"/>
-      <c r="G25"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G25" s="18"/>
+    </row>
+    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="16">
         <v>43180</v>
       </c>
@@ -1962,13 +1953,13 @@
         <v>27</v>
       </c>
       <c r="C26" s="20">
-        <v>2</v>
-      </c>
-      <c r="D26" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>59</v>
+        <v>1</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="F26"/>
       <c r="G26" s="18"/>
@@ -1980,14 +1971,14 @@
       <c r="B27" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="20">
+      <c r="C27" s="19">
         <v>2</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F27"/>
       <c r="G27" s="18"/>
@@ -1999,134 +1990,168 @@
       <c r="B28" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>75</v>
+      <c r="C28" s="19">
+        <v>2</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>82</v>
       </c>
       <c r="F28"/>
       <c r="G28" s="18"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="16">
         <v>43180</v>
       </c>
       <c r="B29" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="19"/>
+      <c r="C29" s="20">
+        <v>1</v>
+      </c>
       <c r="D29" s="23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F29"/>
-      <c r="G29" s="18"/>
+      <c r="G29"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="16">
-        <v>43181</v>
-      </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E30" s="23" t="s">
-        <v>91</v>
+        <v>43180</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="20">
+        <v>2</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>59</v>
       </c>
       <c r="F30"/>
       <c r="G30" s="18"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="16">
-        <v>43181</v>
-      </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>92</v>
+        <v>43180</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="20">
+        <v>2</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>89</v>
       </c>
       <c r="F31"/>
       <c r="G31" s="18"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="16">
-        <v>43181</v>
-      </c>
-      <c r="B32" s="17"/>
+        <v>43180</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>27</v>
+      </c>
       <c r="C32" s="19"/>
       <c r="D32" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E32" s="23" t="s">
-        <v>93</v>
+        <v>49</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="F32"/>
       <c r="G32" s="18"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="16"/>
+      <c r="A33" s="16">
+        <v>43180</v>
+      </c>
       <c r="B33" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C33" s="19">
-        <v>1</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C33" s="19"/>
       <c r="D33" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>99</v>
+        <v>50</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="F33"/>
       <c r="G33" s="18"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="16"/>
+      <c r="A34" s="16">
+        <v>43181</v>
+      </c>
       <c r="B34" s="17"/>
-      <c r="C34" s="19">
-        <v>2</v>
-      </c>
-      <c r="D34" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E34" s="7"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>91</v>
+      </c>
       <c r="F34"/>
       <c r="G34" s="18"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="16"/>
+      <c r="A35" s="16">
+        <v>43181</v>
+      </c>
       <c r="B35" s="17"/>
       <c r="C35" s="19"/>
-      <c r="D35" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="E35" s="7"/>
+      <c r="D35" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>92</v>
+      </c>
       <c r="F35"/>
       <c r="G35" s="18"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="16"/>
+      <c r="A36" s="16">
+        <v>43181</v>
+      </c>
       <c r="B36" s="17"/>
       <c r="C36" s="19"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="7"/>
+      <c r="D36" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>93</v>
+      </c>
       <c r="F36"/>
       <c r="G36" s="18"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="16"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="7"/>
+      <c r="B37" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="19">
+        <v>1</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>99</v>
+      </c>
       <c r="F37"/>
       <c r="G37" s="18"/>
     </row>
@@ -2137,7 +2162,7 @@
         <v>2</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38"/>
@@ -2147,120 +2172,162 @@
       <c r="A39" s="16"/>
       <c r="B39" s="17"/>
       <c r="C39" s="19"/>
+      <c r="D39" s="34" t="s">
+        <v>103</v>
+      </c>
       <c r="E39" s="7"/>
       <c r="F39"/>
       <c r="G39" s="18"/>
     </row>
-    <row r="40" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="27"/>
-      <c r="B40" s="28" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="16"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="7"/>
+      <c r="F40"/>
+      <c r="G40" s="18"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="16"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="7"/>
+      <c r="F41"/>
+      <c r="G41" s="18"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="16"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="19">
+        <v>2</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="F42"/>
+      <c r="G42" s="18"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="16"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="19"/>
+      <c r="E43" s="7"/>
+      <c r="F43"/>
+      <c r="G43" s="18"/>
+    </row>
+    <row r="44" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="27"/>
+      <c r="B44" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="C40" s="29"/>
-      <c r="D40" s="30" t="s">
+      <c r="C44" s="29"/>
+      <c r="D44" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="E40" s="31"/>
-      <c r="F40" s="32" t="s">
+      <c r="E44" s="31"/>
+      <c r="F44" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="G40" s="33"/>
-    </row>
-    <row r="41" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="27"/>
-      <c r="B41" s="28" t="s">
+      <c r="G44" s="33"/>
+    </row>
+    <row r="45" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="27"/>
+      <c r="B45" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="C41" s="29"/>
-      <c r="D41" s="30" t="s">
+      <c r="C45" s="29"/>
+      <c r="D45" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="E41" s="31" t="s">
+      <c r="E45" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="F41" s="32" t="s">
+      <c r="F45" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="G41" s="33"/>
-    </row>
-    <row r="42" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="27"/>
-      <c r="B42" s="28" t="s">
+      <c r="G45" s="33"/>
+    </row>
+    <row r="46" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="27"/>
+      <c r="B46" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="C42" s="29"/>
-      <c r="D42" s="30" t="s">
+      <c r="C46" s="29"/>
+      <c r="D46" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="31" t="s">
+      <c r="E46" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="F42" s="32" t="s">
+      <c r="F46" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="G42" s="33"/>
-    </row>
-    <row r="43" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D43" s="30"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="32" t="s">
+      <c r="G46" s="33"/>
+    </row>
+    <row r="47" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D47" s="30"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="G43" s="31"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46">
-        <f>ROUND(COUNTA(A3:A42)/ROWS(A3:A42)*100,0)</f>
-        <v>73</v>
-      </c>
-      <c r="B46" s="15" t="s">
+      <c r="G47" s="31"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <f>ROUND(COUNTA(A3:A46)/ROWS(A3:A46)*100,0)</f>
+        <v>68</v>
+      </c>
+      <c r="B50" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C46" s="20"/>
-      <c r="F46"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="8"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="10"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D48" s="25"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="14"/>
-    </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D49" s="25"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="14"/>
-    </row>
-    <row r="50" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D50" s="25"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="14"/>
-    </row>
-    <row r="51" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D51" s="25"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="14"/>
-    </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="C50" s="20"/>
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="8"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="10"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D52" s="25"/>
       <c r="E52" s="7"/>
       <c r="F52" s="14"/>
     </row>
-    <row r="53" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D53" s="25"/>
       <c r="E53" s="7"/>
       <c r="F53" s="14"/>
     </row>
-    <row r="54" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D54" s="25"/>
       <c r="E54" s="7"/>
       <c r="F54" s="14"/>
     </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D55" s="25"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="14"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D56" s="25"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="14"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D57" s="25"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="14"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D58" s="25"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="14"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A47 A8:A42">
+  <conditionalFormatting sqref="A51 A8:A46">
     <cfRule type="notContainsBlanks" dxfId="1" priority="355">
       <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>
@@ -2277,10 +2344,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C13"/>
+  <dimension ref="A2:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2291,7 +2358,7 @@
     <col min="4" max="4" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>104</v>
       </c>
@@ -2300,7 +2367,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -2308,7 +2375,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -2319,7 +2386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>107</v>
       </c>
@@ -2330,7 +2397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>108</v>
       </c>
@@ -2341,7 +2408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>109</v>
       </c>
@@ -2352,7 +2419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>110</v>
       </c>
@@ -2363,7 +2430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>111</v>
       </c>
@@ -2374,7 +2441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -2382,7 +2449,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -2393,7 +2460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>114</v>
       </c>
@@ -2404,7 +2471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>115</v>
       </c>
@@ -2413,6 +2480,17 @@
       </c>
       <c r="C13">
         <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP DM and VS conversion
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="person_1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="144">
   <si>
     <t>Item</t>
   </si>
@@ -486,6 +486,54 @@
   </si>
   <si>
     <t>cdiscpilot01:Lifespan_2</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>SDTM remapping</t>
+  </si>
+  <si>
+    <t>Ethnicity</t>
+  </si>
+  <si>
+    <t>Derivation</t>
+  </si>
+  <si>
+    <t>study:ethnicity &lt;http://rdf.cdisc.org/sdtmterm#C66790.C17459&gt; ;</t>
+  </si>
+  <si>
+    <t>study:race &lt;http://rdf.cdisc.org/sdtmterm#C74457.C41261&gt; ;</t>
+  </si>
+  <si>
+    <t>study:sex &lt;http://rdf.cdisc.org/sdtmterm#C66731.C16576&gt; ;</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>study:sex   code:Sex_F;</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">study:race code:Race_8393uepqv42l9mmuen518i9178bnc8sv </t>
+  </si>
+  <si>
+    <t xml:space="preserve">study:ethnicity code:Enthnicity_gnja37oohiiipittns2ro9rma4k5q8i5 </t>
+  </si>
+  <si>
+    <t>hash of "WHITE"</t>
+  </si>
+  <si>
+    <t>hash of "HISPANIC OR LATINO"</t>
+  </si>
+  <si>
+    <t>No hash value!</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1097,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1122,6 +1170,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1494,9 +1543,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1601,7 +1650,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="16">
-        <v>43180</v>
+        <v>43188</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>27</v>
@@ -2344,17 +2393,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D16"/>
+  <dimension ref="A2:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" customWidth="1"/>
+    <col min="2" max="2" width="61" customWidth="1"/>
+    <col min="3" max="3" width="57.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2491,6 +2540,67 @@
       </c>
       <c r="D16" t="s">
         <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B21" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comparison Shiny App working. Next: Add display of just the differences in an additional row of the UI
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="person_1" sheetId="1" r:id="rId1"/>
@@ -718,7 +718,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -907,6 +907,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1097,7 +1103,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1171,6 +1177,7 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1543,9 +1550,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1609,7 +1616,7 @@
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="16"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="17" t="s">
         <v>94</v>
       </c>
@@ -2395,8 +2402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
SMS mapping of VS. Template for US Connect paper
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945"/>
   </bookViews>
   <sheets>
     <sheet name="person_1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="154">
   <si>
     <t>Item</t>
   </si>
@@ -102,9 +102,6 @@
 Passed QC</t>
   </si>
   <si>
-    <t>cdiscpilot01:VisitScreening1_1</t>
-  </si>
-  <si>
     <t>DM</t>
   </si>
   <si>
@@ -192,18 +189,12 @@
     <t xml:space="preserve">    cdiscpilot01:VisitScreening1Activity_1</t>
   </si>
   <si>
-    <t xml:space="preserve">    cdiscpilot01:AgeOutcome_k5ql986im5d6cj0eee80312k9scue0h7</t>
-  </si>
-  <si>
     <t>cdiscpilot01:DemographicDataCollection_01-701-1015</t>
   </si>
   <si>
     <t xml:space="preserve">     cdiscpilot01:Date_19</t>
   </si>
   <si>
-    <t xml:space="preserve">    cdiscpilot01:Date_n6l0u58r7lrhic8l4b1e4u7k8182j6fq </t>
-  </si>
-  <si>
     <t xml:space="preserve">    cdiscpilot01:VisitScreening1Activity_01-701-1015 </t>
   </si>
   <si>
@@ -246,18 +237,12 @@
     <t xml:space="preserve">cdiscpilot01:PopFlagSAFETY_01-701-1015 </t>
   </si>
   <si>
-    <t>cdiscpilot01:StudyParticipationInterval_n6l0u58r7lrhic8l4b1e4u7k8182j6fq_k78l4og87v61q51vabbketftn59735lb</t>
-  </si>
-  <si>
     <t xml:space="preserve">cdiscpilot01::SubjectIdentifier_1015 </t>
   </si>
   <si>
     <t>cdiscpilot01:UniqueSubjectIdentifier_01-701-1015</t>
   </si>
   <si>
-    <t>cdiscpilot01:ReferenceInterval_s6rc8otorv5ukcpag29jggn8m8h5127t_cpkmsvqhc92dn75siimpl3fj20mmtdei</t>
-  </si>
-  <si>
     <t>cdiscpilot01:PopFlagCmpltr24Wk_1</t>
   </si>
   <si>
@@ -267,79 +252,19 @@
     <t xml:space="preserve">    cdiscpilot01:Date_29</t>
   </si>
   <si>
-    <t xml:space="preserve">    cdiscpilot01:Date_s6rc8otorv5ukcpag29jggn8m8h5127t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:Date_cpkmsvqhc92dn75siimpl3fj20mmtdei</t>
-  </si>
-  <si>
     <t xml:space="preserve">       cdiscpilot01:Date_19</t>
   </si>
   <si>
-    <t>cdiscpilot01:Lifespan_udj4rptja2ij6a5lmb3meemc3mca7ip3_n6l0u58r7lrhic8l4b1e4u7k8182j6fq</t>
-  </si>
-  <si>
     <t xml:space="preserve">       cdiscpilot01:Date_6</t>
   </si>
   <si>
-    <t xml:space="preserve">    cdiscpilot01:Date_udj4rptja2ij6a5lmb3meemc3mca7ip3</t>
-  </si>
-  <si>
     <t xml:space="preserve">    cdiscpilot01:Date_19</t>
   </si>
   <si>
     <t xml:space="preserve">    cdiscpilot01:Date_30</t>
   </si>
   <si>
-    <t xml:space="preserve">    cdiscpilot01:Date_k78l4og87v61q51vabbketftn59735lb</t>
-  </si>
-  <si>
     <t>PENDING</t>
-  </si>
-  <si>
-    <r>
-      <t>study:EnrolledSubject</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> [LITERAL]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Person 1  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[LITERAL]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Y </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[LITERAL]</t>
-    </r>
   </si>
   <si>
     <t>DM,EX</t>
@@ -401,21 +326,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">cdiscpilot01:Visit_1e1uak4vs9dpl4d263rl3b9a1pongqrl_01-701-1015 </t>
-  </si>
-  <si>
-    <t>LATER!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:AssumeBodyPositionStanding_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:AssumeBodyPositionSupine_1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">       cdiscpilot01:AssumeBodyPositionStanding_1</t>
-  </si>
-  <si>
     <t xml:space="preserve">  C67153.C25206_1</t>
   </si>
   <si>
@@ -479,15 +389,6 @@
     <t>The outcome of standing</t>
   </si>
   <si>
-    <t>ADDTIONAL VALIDATION</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Lifespan_pt2m6avt4r1v33ksdu1m4ggqjgec0q9f_m9eproucjuhbto78r3ij902mqsklh6so</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Lifespan_2</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -534,13 +435,112 @@
   </si>
   <si>
     <t>No hash value!</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Lifespan_1951-01-02_2013-12-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:Date_2013-12-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:Date_1951-01-02</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:ReferenceInterval_2014-01-02_2014-07-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:Date_2014-01-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:Date_2014-07-02</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:StudyParticipationInterval_2013-12-26_2014-07-02T11%3A45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This query works fine in Stardog but not from the RShiny:
+prefix cdiscpilot01: &lt;https://raw.githubusercontent.com/phuse-org/CTDasRDF/master/data/rdf/cdiscpilot01.ttl#&gt;
+SELECT *
+WHERE{
+cdiscpilot01:StudyParticipationInterval_2013-12-26_2014-07-02T11%3A45  ?p ?o
+} 
+</t>
+  </si>
+  <si>
+    <t> cdiscpilot01:Date_2013-12-26</t>
+  </si>
+  <si>
+    <t> cdiscpilot01:Date_2014-07-02T11%3A45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:CumulativeProductAdministrationInterval_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:DrugAdministration_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:DrugAdministration_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:DrugAdministration_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:VisitBaselineActivity_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:VisitWk2Activity_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:FixedDoseInterval_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:FixedDoseInterval_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:VisitWk24Activity_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:FixedDoseInterval_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:CumulativeProductAdministrationInterval_01-701-1015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:AgeOutcome_63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       cdiscpilot01:Date_2013-12-26</t>
+  </si>
+  <si>
+    <t>SUPPDM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            cdiscpilot01:Date_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            cdiscpilot01:Date_31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:Date_2014-01-16</t>
+  </si>
+  <si>
+    <t>EX</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:VisitBASELINE_01-701-1015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEVLEOPING BELOW HERE&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:DrugAdministration_01-701-1015_xxxxxx-xxxx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -705,20 +705,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -916,8 +923,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1058,6 +1071,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1103,7 +1129,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1117,18 +1143,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1137,18 +1155,9 @@
     <xf numFmtId="49" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1159,25 +1168,67 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="15" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="15" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="24" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1223,7 +1274,84 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1548,849 +1676,955 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="44.54296875" style="23" customWidth="1"/>
-    <col min="5" max="5" width="68.1796875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="49.81640625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="57.1796875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="22" customWidth="1"/>
+    <col min="4" max="4" width="55.42578125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="68.140625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="49.85546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="57.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="D1" s="23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="24">
+        <v>1</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="34"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="19"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="27">
+        <v>1</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="24">
+        <v>2</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="24">
+        <v>2</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F9"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A10" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="24">
+        <v>1</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="F11" s="19"/>
+      <c r="G11" s="11"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="F12" s="19"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="19"/>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="19"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+      <c r="B15" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="24">
+        <v>1</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="24">
+        <v>2</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="F16" s="19"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
+      <c r="B17" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="25">
+        <v>2</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="26"/>
+      <c r="B18" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="25">
+        <v>3</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
+      <c r="B19" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="25">
+        <v>3</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="25">
+        <v>2</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F20" s="19"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="26"/>
+      <c r="B21" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="25">
+        <v>3</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="25">
+        <v>3</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="25">
+        <v>2</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F23" s="19"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="26"/>
+      <c r="B24" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="24">
+        <v>3</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" s="19"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="26"/>
+      <c r="B25" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="24">
+        <v>3</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="F25" s="19"/>
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="24">
+        <v>1</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="24">
+        <v>2</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="F27"/>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="24">
+        <v>2</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28"/>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="24">
+        <v>2</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="27">
+        <v>1</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="19"/>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="27">
+        <v>2</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="19"/>
+      <c r="G31" s="11"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="27">
+        <v>3</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="26">
+        <v>43196</v>
+      </c>
+      <c r="B33" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" s="24">
+        <v>1</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="11"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="26">
+        <v>43196</v>
+      </c>
+      <c r="B34" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" s="27">
+        <v>1</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G34" s="11"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="26">
+        <v>43196</v>
+      </c>
+      <c r="B35" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C35" s="27">
+        <v>1</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="26">
+        <v>43196</v>
+      </c>
+      <c r="B36" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C36" s="27">
+        <v>1</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="26">
+        <v>43196</v>
+      </c>
+      <c r="B37" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C37" s="27">
+        <v>1</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F37"/>
+      <c r="G37" s="11"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="26">
+        <v>43196</v>
+      </c>
+      <c r="B38" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C38" s="27">
+        <v>1</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38"/>
+      <c r="G38" s="11"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="23">
+        <v>43195</v>
+      </c>
+      <c r="B39" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="22">
+        <v>1</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F39"/>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="23"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="F40" t="s">
+        <v>64</v>
+      </c>
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="23"/>
+      <c r="B41" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" s="29">
+        <v>1</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="23">
+        <v>43196</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C42" s="29">
+        <v>2</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="23"/>
+      <c r="B43" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C43" s="29">
+        <v>2</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="23"/>
+      <c r="B44" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C44" s="29">
+        <v>3</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E44" s="16"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="23"/>
+      <c r="B45" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C45" s="29">
+        <v>3</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="E45" s="16"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="23"/>
+      <c r="B46" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C46" s="29">
+        <v>4</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="23"/>
+      <c r="B47" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C47" s="29">
+        <v>4</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="23"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="23"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="23"/>
+      <c r="B50" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="29"/>
+      <c r="D50" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="23"/>
+      <c r="B51" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51" s="29"/>
+      <c r="D51" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="23">
+        <f>ROUND(COUNTA(A3:A51)/ROWS(A3:A51)*100,0)</f>
+        <v>57</v>
+      </c>
+      <c r="B52" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="16">
-        <v>43173</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="19">
-        <v>1</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="37"/>
-      <c r="B4" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="19">
-        <v>1</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" s="18"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="19">
-        <v>1</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="18"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="16">
-        <v>43188</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="20">
-        <v>2</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6"/>
-      <c r="G6" s="18"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="20">
-        <v>2</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8"/>
-      <c r="G8" s="18"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="22">
-        <v>43181</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="20">
-        <v>1</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9"/>
-      <c r="G9" s="18"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="22">
-        <v>43181</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="20">
-        <v>2</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10"/>
-      <c r="G10" s="18"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="22">
-        <v>43181</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="20">
-        <v>3</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11"/>
-      <c r="G11" s="18"/>
-    </row>
-    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="22">
-        <v>43181</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="20">
-        <v>1</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="18"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="22">
-        <v>43181</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13"/>
-      <c r="G13" s="18"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="22">
-        <v>43181</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="F14"/>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="F15"/>
-      <c r="G15" s="18"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="22"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="21"/>
-      <c r="F16"/>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="22"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="21"/>
-      <c r="F17"/>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="22"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="21"/>
-      <c r="F18"/>
-      <c r="G18" s="18"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="20">
-        <v>1</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F19"/>
-      <c r="G19" s="18"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="20">
-        <v>1</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20"/>
-      <c r="G20" s="18"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="20">
-        <v>1</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21"/>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="20">
-        <v>1</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22"/>
-      <c r="G22" s="18"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="20">
-        <v>1</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23"/>
-      <c r="G23" s="18"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="20">
-        <v>1</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24"/>
-      <c r="G24" s="18"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="20">
-        <v>1</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25"/>
-      <c r="G25" s="18"/>
-    </row>
-    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="20">
-        <v>1</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26"/>
-      <c r="G26" s="18"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="19">
-        <v>2</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27"/>
-      <c r="G27" s="18"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="19">
-        <v>2</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E28" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="F28"/>
-      <c r="G28" s="18"/>
-    </row>
-    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="20">
-        <v>1</v>
-      </c>
-      <c r="D29" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F29"/>
-      <c r="G29"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="20">
-        <v>2</v>
-      </c>
-      <c r="D30" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30"/>
-      <c r="G30" s="18"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="20">
-        <v>2</v>
-      </c>
-      <c r="D31" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="E31" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="F31"/>
-      <c r="G31" s="18"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F32"/>
-      <c r="G32" s="18"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="16">
-        <v>43180</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F33"/>
-      <c r="G33" s="18"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="16">
-        <v>43181</v>
-      </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E34" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="F34"/>
-      <c r="G34" s="18"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="16">
-        <v>43181</v>
-      </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="E35" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="F35"/>
-      <c r="G35" s="18"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="16">
-        <v>43181</v>
-      </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E36" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="F36"/>
-      <c r="G36" s="18"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="16"/>
-      <c r="B37" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C37" s="19">
-        <v>1</v>
-      </c>
-      <c r="D37" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F37"/>
-      <c r="G37" s="18"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="16"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="19">
-        <v>2</v>
-      </c>
-      <c r="D38" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E38" s="7"/>
-      <c r="F38"/>
-      <c r="G38" s="18"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="16"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="E39" s="7"/>
-      <c r="F39"/>
-      <c r="G39" s="18"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="16"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="7"/>
-      <c r="F40"/>
-      <c r="G40" s="18"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="16"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="7"/>
-      <c r="F41"/>
-      <c r="G41" s="18"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="16"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="19">
-        <v>2</v>
-      </c>
-      <c r="D42" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E42" s="7"/>
-      <c r="F42"/>
-      <c r="G42" s="18"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="16"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="19"/>
-      <c r="E43" s="7"/>
-      <c r="F43"/>
-      <c r="G43" s="18"/>
-    </row>
-    <row r="44" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="27"/>
-      <c r="B44" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="C44" s="29"/>
-      <c r="D44" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="E44" s="31"/>
-      <c r="F44" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="G44" s="33"/>
-    </row>
-    <row r="45" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="27"/>
-      <c r="B45" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="29"/>
-      <c r="D45" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="E45" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="F45" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="G45" s="33"/>
-    </row>
-    <row r="46" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="27"/>
-      <c r="B46" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="C46" s="29"/>
-      <c r="D46" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E46" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="F46" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="G46" s="33"/>
-    </row>
-    <row r="47" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D47" s="30"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="G47" s="31"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50">
-        <f>ROUND(COUNTA(A3:A46)/ROWS(A3:A46)*100,0)</f>
-        <v>68</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C50" s="20"/>
-      <c r="F50"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" s="8"/>
-      <c r="F51" s="13"/>
-      <c r="G51" s="10"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D52" s="25"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="14"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D53" s="25"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="14"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D54" s="25"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="14"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D55" s="25"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="14"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D56" s="25"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="14"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D57" s="25"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="14"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D58" s="25"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="14"/>
+      <c r="C52" s="27"/>
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="31"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="7"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="10"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="10"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="10"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="10"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="10"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="10"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="10"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A51 A8:A46">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="355">
+  <conditionalFormatting sqref="A53 A15 A26:A31 A33:A38">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="366">
+      <formula>LEN(TRIM(A15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:A6">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
+      <formula>LEN(TRIM(A3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
+      <formula>LEN(TRIM(A7))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
       <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A7">
+  <conditionalFormatting sqref="A9">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12:A14">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(A12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17:A25">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(A39))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:A52">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A3))&gt;0</formula>
+      <formula>LEN(TRIM(A40))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2406,208 +2640,208 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61" customWidth="1"/>
-    <col min="3" max="3" width="57.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.54296875" customWidth="1"/>
+    <col min="3" max="3" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="35" t="s">
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" t="s">
         <v>122</v>
-      </c>
-      <c r="B16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D16" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="36" t="s">
-        <v>132</v>
-      </c>
-      <c r="D20" s="36" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>129</v>
-      </c>
-      <c r="B21" t="s">
-        <v>134</v>
-      </c>
-      <c r="C21" t="s">
-        <v>139</v>
-      </c>
-      <c r="D21" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>131</v>
-      </c>
-      <c r="B22" t="s">
-        <v>133</v>
-      </c>
-      <c r="C22" t="s">
-        <v>140</v>
-      </c>
-      <c r="D22" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>136</v>
-      </c>
-      <c r="B23" t="s">
-        <v>135</v>
-      </c>
-      <c r="C23" t="s">
-        <v>137</v>
-      </c>
-      <c r="D23" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2624,14 +2858,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -2639,7 +2873,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2647,7 +2881,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2655,7 +2889,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -2663,7 +2897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2671,7 +2905,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2679,7 +2913,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -2693,7 +2927,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2707,7 +2941,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2721,7 +2955,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2735,16 +2969,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -2752,7 +2986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -2766,7 +3000,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2780,7 +3014,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2794,7 +3028,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2808,7 +3042,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
@@ -2821,7 +3055,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
@@ -2834,7 +3068,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>24</v>
       </c>
@@ -2845,11 +3079,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="3"/>
     </row>

</xml_diff>

<commit_message>
added graph metadata source, TTL, R timestamp.
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="173">
   <si>
     <t>Item</t>
   </si>
@@ -588,6 +588,9 @@
   </si>
   <si>
     <t xml:space="preserve">            cdiscpilot01:Date_29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:Date_2014-01-17</t>
   </si>
 </sst>
 </file>
@@ -1729,8 +1732,8 @@
   <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D62" sqref="D62"/>
+      <pane ySplit="3" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1744,12 +1747,12 @@
     <col min="7" max="7" width="57.125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="D1" s="12" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>25</v>
       </c>
@@ -1895,7 +1898,7 @@
       <c r="F9"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="23">
         <v>43195</v>
       </c>
@@ -1974,7 +1977,7 @@
       <c r="F14" s="19"/>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
       <c r="B15" s="25" t="s">
         <v>79</v>
@@ -2580,7 +2583,9 @@
       <c r="D51" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="E51" s="20"/>
+      <c r="E51" s="13" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="23"/>

</xml_diff>

<commit_message>
DM proofing and dev.  Commit prior to merge.
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="165">
   <si>
     <t>Item</t>
   </si>
@@ -114,66 +114,15 @@
     <t>%reviewed</t>
   </si>
   <si>
-    <t>cdiscpilot01:InformedConsentAdult_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:PopFlagCmpltr16Wk_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:PopFlagCmpltr8Wk_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:PopFlagEff_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:PopFlagItt_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:PopFlagSaf_1</t>
-  </si>
-  <si>
     <t>Except for :VS: VisitBaseline_, VisitScreening, VisitWk24_, VisitWk2</t>
   </si>
   <si>
-    <t>cdiscpilot01:Person_1</t>
-  </si>
-  <si>
     <t>cdiscpilot01:Person_01-701-1015</t>
   </si>
   <si>
-    <t>cdiscpilot01:CumulativeProductAdministration_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:CumulativeProductAdministration_01-701-1015</t>
-  </si>
-  <si>
-    <t>Incomplete. Depends on EX domain</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:DemographicDataCollection_1</t>
-  </si>
-  <si>
     <t>Level</t>
   </si>
   <si>
-    <t>cdiscpilot01:Lifespan_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:RandomizationBAL3_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:ReferenceInterval_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:StudyParticipationInterval_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:SubjectIdentifier_1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:UniqueSubjectIdentifier_1</t>
-  </si>
-  <si>
     <t>cdiscpilot01:VisitBaseline_1</t>
   </si>
   <si>
@@ -183,36 +132,15 @@
     <t>cdiscpilot01:VisitWk2_1</t>
   </si>
   <si>
-    <t xml:space="preserve">    cdiscpilot01:AgeOutcome_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:VisitScreening1Activity_1</t>
-  </si>
-  <si>
     <t>cdiscpilot01:DemographicDataCollection_01-701-1015</t>
   </si>
   <si>
-    <t xml:space="preserve">     cdiscpilot01:Date_19</t>
-  </si>
-  <si>
     <t xml:space="preserve">    cdiscpilot01:VisitScreening1Activity_01-701-1015 </t>
   </si>
   <si>
-    <t>incomplete comparision but passed</t>
-  </si>
-  <si>
-    <t>SDTM terms are being corrected in Source TTL</t>
-  </si>
-  <si>
     <t xml:space="preserve">cdiscpilot01:InformedConsentAdult_01-701-1015 </t>
   </si>
   <si>
-    <t xml:space="preserve">    cdiscpilot01:InformedConsentInterval_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:InformedConsentInterval_01-701-1015 </t>
-  </si>
-  <si>
     <t>cdiscpilot01:RandomizationBAL3_01-701-1015</t>
   </si>
   <si>
@@ -234,33 +162,9 @@
     <t xml:space="preserve">cdiscpilot01:PopFlagSAFETY_01-701-1015 </t>
   </si>
   <si>
-    <t xml:space="preserve">cdiscpilot01::SubjectIdentifier_1015 </t>
-  </si>
-  <si>
     <t>cdiscpilot01:UniqueSubjectIdentifier_01-701-1015</t>
   </si>
   <si>
-    <t>cdiscpilot01:PopFlagCmpltr24Wk_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:Date_20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:Date_29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       cdiscpilot01:Date_19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       cdiscpilot01:Date_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:Date_19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:Date_30</t>
-  </si>
-  <si>
     <t>DM,EX</t>
   </si>
   <si>
@@ -271,6 +175,377 @@
   </si>
   <si>
     <t>Derived Subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25206_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25208_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25298_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25298_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25298_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25299_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25299_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25299_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C25347_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C49676_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C49676_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C67153.C49676_3</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Systolic Blood Pressure</t>
+  </si>
+  <si>
+    <t>Diastolic Blood Pressure</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Pulse Rate</t>
+  </si>
+  <si>
+    <t>C71148.C62166</t>
+  </si>
+  <si>
+    <t>STANDING</t>
+  </si>
+  <si>
+    <t>The outcome of standing</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>SDTM remapping</t>
+  </si>
+  <si>
+    <t>Ethnicity</t>
+  </si>
+  <si>
+    <t>Derivation</t>
+  </si>
+  <si>
+    <t>study:ethnicity &lt;http://rdf.cdisc.org/sdtmterm#C66790.C17459&gt; ;</t>
+  </si>
+  <si>
+    <t>study:race &lt;http://rdf.cdisc.org/sdtmterm#C74457.C41261&gt; ;</t>
+  </si>
+  <si>
+    <t>study:sex &lt;http://rdf.cdisc.org/sdtmterm#C66731.C16576&gt; ;</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>study:sex   code:Sex_F;</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">study:race code:Race_8393uepqv42l9mmuen518i9178bnc8sv </t>
+  </si>
+  <si>
+    <t xml:space="preserve">study:ethnicity code:Enthnicity_gnja37oohiiipittns2ro9rma4k5q8i5 </t>
+  </si>
+  <si>
+    <t>hash of "WHITE"</t>
+  </si>
+  <si>
+    <t>hash of "HISPANIC OR LATINO"</t>
+  </si>
+  <si>
+    <t>No hash value!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:Date_2013-12-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:Date_1951-01-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:Date_2014-01-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:Date_2014-07-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:VisitBaselineActivity_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:VisitWk2Activity_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:FixedDoseInterval_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:FixedDoseInterval_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:VisitWk24Activity_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:FixedDoseInterval_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:AgeOutcome_63</t>
+  </si>
+  <si>
+    <t>SUPPDM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            cdiscpilot01:Date_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            cdiscpilot01:Date_31</t>
+  </si>
+  <si>
+    <t>EX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:DrugAdministration_01-701-1015_2014-01-02_2014-01-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:Interval_2014-01-02_2014-01-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            cdiscpilot01:Date_2014-01-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            cdiscpilot01:Date_2014-01-16</t>
+  </si>
+  <si>
+    <t>DEV BELOW HERE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:DrugAdministration_01-701-1015_2014-01-17_2014-06-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         cdiscpilot01:FixedDoseInterval_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       cdiscpilot01:FixedDoseInterval_3</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Person_101-701-1015</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_1951-01-02_2013-12-26</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_2014-01-02_2014-07-02</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:Interval_2013-12-26_2014-07-02T11:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cdiscpilot01:SubjectIdentifier_1015 </t>
+  </si>
+  <si>
+    <t>cdiscpilot01:CumulativeDrugAdministration_01-701-1015</t>
+  </si>
+  <si>
+    <t>minor discrep in label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:Date_2014-07-02T11:45</t>
+  </si>
+  <si>
+    <t>Must query from within Studio, not RShiny</t>
+  </si>
+  <si>
+    <t>DM,VS</t>
+  </si>
+  <si>
+    <r>
+      <t>Ontology: study:Cumulative</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Product</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>AdministrationEnd</t>
+    </r>
+  </si>
+  <si>
+    <t>Ontology: is also a study:VisitDate  for patient 1015 Baseline visit</t>
+  </si>
+  <si>
+    <t>AO informed date</t>
+  </si>
+  <si>
+    <t>17APR</t>
+  </si>
+  <si>
+    <t>Ontology pending correction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ontology uses usubjid in IRI, I used date range. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:DrugAdministration_01-701-1015_2014-06-19_2014-07-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:Interval_2014-01-02_2014-07-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cdiscpilot01:Interval_2014-01-02_2014-07-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:Date_2014-01-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:Date_2014-07-02</t>
+  </si>
+  <si>
+    <t>Ontology: Change from study:CumulativeProductAdministrationEnd to CumulativeDrugAdministrationEnd</t>
+  </si>
+  <si>
+    <t>Various for code: custom: , etc.  Sent to AO today.</t>
+  </si>
+  <si>
+    <t>SDTM terms and some label and encoding differences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:Interval_2013-12-26_</t>
+  </si>
+  <si>
+    <t>Label difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      cdiscpilot01:Date_2013-12-26</t>
+  </si>
+  <si>
+    <t>Label and ARM assignment discrepancies</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:VisitBaseline_01-701-1015</t>
+  </si>
+  <si>
+    <t>Ontology: Date is missing the:  study:VisitDate (see above)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       cdiscpilot01:DrugAdministration_01-701-1015_2014-01-02_2014-01-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:VisitBaselineActivity_01-701-1015</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:VisitWk2_01-701-1015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:Date_2014-01-16</t>
+  </si>
+  <si>
+    <t>Note how date is from VS, NOT EX!!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         cdiscpilot01:VisitWk2Activity_01-701-1015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       cdiscpilot01:Interval_2014-01-17_2014-06-18</t>
+  </si>
+  <si>
+    <t>the fixed dose interval</t>
+  </si>
+  <si>
+    <t>SDTM terminology needs recoding!</t>
+  </si>
+  <si>
+    <t>small discrepancy in label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           cdiscpilot01:Date_2014-01-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            cdiscpilot01:Date_2014-06-18</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:VisitWk24_01-701-1015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:Date_2014-06-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cdiscpilot01:VisitWk24Activity_01-701-1015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:VisitWk24Activity_01-701-1015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cdiscpilot01:Interval_2014-06-19_2014-07-02</t>
+  </si>
+  <si>
+    <t>Placebo IRI , SDTM terms</t>
+  </si>
+  <si>
+    <t>label needs fix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            cdiscpilot01:Date_2014-06-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            cdiscpilot01:Date_2014-07-02</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">           </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> cdiscpilot01:Date_2014-07-02</t>
+    </r>
+  </si>
+  <si>
+    <t>Date object change to Drug:  study:CumulativeProductAdministrationEnd</t>
   </si>
   <si>
     <r>
@@ -316,288 +591,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Assessed only for Person_1</t>
+      <t>Assessed only for Person_01-701-1015</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">  C67153.C25206_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  C67153.C25208_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  C67153.C25298_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  C67153.C25298_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  C67153.C25298_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  C67153.C25299_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  C67153.C25299_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  C67153.C25299_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  C67153.C25347_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  C67153.C49676_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  C67153.C49676_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  C67153.C49676_3</t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>Systolic Blood Pressure</t>
-  </si>
-  <si>
-    <t>Diastolic Blood Pressure</t>
-  </si>
-  <si>
-    <t>Height</t>
-  </si>
-  <si>
-    <t>Pulse Rate</t>
-  </si>
-  <si>
-    <t>C71148.C62166</t>
-  </si>
-  <si>
-    <t>STANDING</t>
-  </si>
-  <si>
-    <t>The outcome of standing</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Race</t>
-  </si>
-  <si>
-    <t>SDTM remapping</t>
-  </si>
-  <si>
-    <t>Ethnicity</t>
-  </si>
-  <si>
-    <t>Derivation</t>
-  </si>
-  <si>
-    <t>study:ethnicity &lt;http://rdf.cdisc.org/sdtmterm#C66790.C17459&gt; ;</t>
-  </si>
-  <si>
-    <t>study:race &lt;http://rdf.cdisc.org/sdtmterm#C74457.C41261&gt; ;</t>
-  </si>
-  <si>
-    <t>study:sex &lt;http://rdf.cdisc.org/sdtmterm#C66731.C16576&gt; ;</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>study:sex   code:Sex_F;</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">study:race code:Race_8393uepqv42l9mmuen518i9178bnc8sv </t>
-  </si>
-  <si>
-    <t xml:space="preserve">study:ethnicity code:Enthnicity_gnja37oohiiipittns2ro9rma4k5q8i5 </t>
-  </si>
-  <si>
-    <t>hash of "WHITE"</t>
-  </si>
-  <si>
-    <t>hash of "HISPANIC OR LATINO"</t>
-  </si>
-  <si>
-    <t>No hash value!</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Lifespan_1951-01-02_2013-12-26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:Date_2013-12-26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:Date_1951-01-02</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:ReferenceInterval_2014-01-02_2014-07-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:Date_2014-01-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:Date_2014-07-02</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:StudyParticipationInterval_2013-12-26_2014-07-02T11%3A45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This query works fine in Stardog but not from the RShiny:
-prefix cdiscpilot01: &lt;https://raw.githubusercontent.com/phuse-org/CTDasRDF/master/data/rdf/cdiscpilot01.ttl#&gt;
-SELECT *
-WHERE{
-cdiscpilot01:StudyParticipationInterval_2013-12-26_2014-07-02T11%3A45  ?p ?o
-} 
-</t>
-  </si>
-  <si>
-    <t> cdiscpilot01:Date_2013-12-26</t>
-  </si>
-  <si>
-    <t> cdiscpilot01:Date_2014-07-02T11%3A45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:CumulativeProductAdministrationInterval_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:DrugAdministration_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:DrugAdministration_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:DrugAdministration_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        cdiscpilot01:VisitBaselineActivity_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        cdiscpilot01:VisitWk2Activity_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        cdiscpilot01:FixedDoseInterval_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        cdiscpilot01:FixedDoseInterval_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        cdiscpilot01:VisitWk24Activity_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        cdiscpilot01:FixedDoseInterval_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:CumulativeProductAdministrationInterval_01-701-1015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:AgeOutcome_63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       cdiscpilot01:Date_2013-12-26</t>
-  </si>
-  <si>
-    <t>SUPPDM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            cdiscpilot01:Date_20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            cdiscpilot01:Date_31</t>
-  </si>
-  <si>
-    <t>EX</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:VisitBASELINE_01-701-1015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:DrugAdministration_01-701-1015_2014-01-02_2014-01-16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        cdiscpilot01:VisitBASELINEActivity_01-701-1015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        cdiscpilot01:Interval_2014-01-02_2014-01-16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            cdiscpilot01:Date_2014-01-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            cdiscpilot01:Date_2014-01-16</t>
-  </si>
-  <si>
-    <t>DEV BELOW HERE</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:VisitWEEK24_01-701-1015</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:VisitWEEK2_01-701-1015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:Date_31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:Date_2014-01-17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   cdiscpilot01:DrugAdministration_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:DrugAdministration_01-701-1015_2014-01-17_2014-06-18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            cdiscpilot01:Date_32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         cdiscpilot01:VisitWk2Activity_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         cdiscpilot01:FixedDoseInterval_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            cdiscpilot01:Date_38</t>
-  </si>
-  <si>
-    <t>SEE COMMENTS</t>
-  </si>
-  <si>
-    <t>Make consistent with the triples from EX, above!!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    cdiscpilot01:Date_38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   cdiscpilot01:DrugAdministration_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       cdiscpilot01:FixedDoseInterval_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            cdiscpilot01:Date_33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            cdiscpilot01:Date_29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        cdiscpilot01:Date_2014-01-17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -781,8 +783,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -983,6 +999,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1186,7 +1214,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1286,8 +1314,33 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="14" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1334,7 +1387,98 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="25">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1729,11 +1873,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
+      <pane ySplit="3" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,18 +1885,18 @@
     <col min="1" max="1" width="10" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" style="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="22" customWidth="1"/>
-    <col min="4" max="4" width="55.375" style="12" customWidth="1"/>
-    <col min="5" max="5" width="68.125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="49.875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="57.125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="69.7109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="68.140625" style="12" customWidth="1"/>
+    <col min="6" max="7" width="49.85546875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="57.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D1" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>25</v>
       </c>
@@ -1760,25 +1904,26 @@
         <v>28</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" s="35" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="23">
-        <v>43195</v>
-      </c>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
       <c r="B3" s="32" t="s">
         <v>26</v>
       </c>
@@ -1786,64 +1931,76 @@
         <v>1</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>37</v>
+        <v>111</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="34"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="G3" s="33"/>
+      <c r="H3" s="34"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="23">
-        <v>43195</v>
-      </c>
-      <c r="B4" s="25"/>
+        <v>43207</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>26</v>
+      </c>
       <c r="C4" s="24"/>
       <c r="D4" s="12" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="5" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F4" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="40"/>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23">
-        <v>43195</v>
-      </c>
-      <c r="B5" s="25"/>
+        <v>43207</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>26</v>
+      </c>
       <c r="C5" s="24"/>
       <c r="D5" s="13" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="F5" s="19"/>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="19"/>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="23">
-        <v>43195</v>
-      </c>
-      <c r="B6" s="25"/>
+        <v>43207</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>120</v>
+      </c>
       <c r="C6" s="24"/>
       <c r="D6" s="13" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="F6" s="19"/>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="19"/>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="23">
-        <v>43195</v>
+        <v>43207</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>26</v>
@@ -1852,360 +2009,388 @@
         <v>1</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>46</v>
+        <v>113</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F7"/>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="23">
-        <v>43195</v>
-      </c>
+      <c r="G7"/>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="41"/>
       <c r="B8" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="24">
         <v>2</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="F8"/>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="23">
-        <v>43195</v>
-      </c>
+      <c r="D8" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="20"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="41"/>
       <c r="B9" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="24">
         <v>2</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="F9"/>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="23">
-        <v>43195</v>
-      </c>
+      <c r="D9" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="G9" s="20"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="41"/>
       <c r="B10" s="25"/>
       <c r="C10" s="24">
         <v>1</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>47</v>
+      <c r="D10" s="39" t="s">
+        <v>114</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="23">
-        <v>43195</v>
+        <v>43207</v>
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="24"/>
       <c r="D11" s="13" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="F11" s="19"/>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="19"/>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="23">
-        <v>43195</v>
+        <v>43207</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="24"/>
       <c r="D12" s="13" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="F12" s="19"/>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="19"/>
+      <c r="H12" s="19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="23">
-        <v>43195</v>
+        <v>43207</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="24"/>
       <c r="D13" s="12" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="F13" s="19"/>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="23">
-        <v>43195</v>
-      </c>
+      <c r="G13" s="19"/>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
       <c r="B14" s="25"/>
       <c r="C14" s="24"/>
-      <c r="D14" s="12" t="s">
-        <v>49</v>
+      <c r="D14" s="39" t="s">
+        <v>46</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="F14" s="19"/>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+      <c r="G14" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="42">
+        <v>43207</v>
+      </c>
       <c r="B15" s="25" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="C15" s="24">
         <v>1</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>39</v>
+        <v>116</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="11"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="23">
-        <v>43195</v>
+        <v>126</v>
+      </c>
+      <c r="G15" s="19"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="42">
+        <v>43207</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="C16" s="24">
         <v>2</v>
       </c>
       <c r="D16" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="43"/>
+      <c r="B17" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="G17" s="19"/>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="43"/>
+      <c r="B18" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="11"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="25">
+      <c r="E18" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="G18" s="19"/>
+      <c r="H18" s="11"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="42"/>
+      <c r="B19" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="25">
         <v>2</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="25">
+      <c r="D19" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="42"/>
+      <c r="B20" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="25">
         <v>3</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="11"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="25">
-        <v>3</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="25">
-        <v>2</v>
-      </c>
       <c r="D20" s="13" t="s">
-        <v>133</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E20" s="13"/>
       <c r="F20" s="19"/>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="42"/>
       <c r="B21" s="25" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="C21" s="25">
         <v>3</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>136</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="E21" s="13"/>
       <c r="F21" s="19"/>
-      <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="42"/>
       <c r="B22" s="25" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="C22" s="25">
+        <v>2</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="11"/>
+    </row>
+    <row r="23" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="42"/>
+      <c r="B23" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="25">
         <v>3</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" s="25">
+      <c r="D23" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="11"/>
+    </row>
+    <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="42"/>
+      <c r="B24" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="25">
+        <v>3</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="11"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="42"/>
+      <c r="B25" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="25">
         <v>2</v>
       </c>
-      <c r="D23" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C24" s="24">
+      <c r="D25" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="11"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="42"/>
+      <c r="B26" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="24">
         <v>3</v>
       </c>
-      <c r="D24" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="11"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" s="24">
+      <c r="D26" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="11"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="42"/>
+      <c r="B27" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="24">
         <v>3</v>
       </c>
-      <c r="D25" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="23">
-        <v>43195</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="24">
-        <v>1</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" t="s">
-        <v>59</v>
-      </c>
-      <c r="G26" s="11"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="23">
-        <v>43195</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="24">
-        <v>2</v>
-      </c>
       <c r="D27" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="F27"/>
-      <c r="G27" s="11"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="23">
-        <v>43195</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="11"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
       <c r="B28" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="24">
-        <v>2</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F28"/>
-      <c r="G28" s="11"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="23">
-        <v>43195</v>
+        <v>1</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="G28"/>
+      <c r="H28" s="11"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="42">
+        <v>43207</v>
       </c>
       <c r="B29" s="25" t="s">
         <v>26</v>
@@ -2214,598 +2399,715 @@
         <v>2</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="F29" t="s">
-        <v>58</v>
-      </c>
-      <c r="G29" s="11"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="23">
-        <v>43195</v>
+        <v>98</v>
+      </c>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29" s="11"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="42">
+        <v>43207</v>
       </c>
       <c r="B30" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="27">
-        <v>1</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F30" s="19"/>
-      <c r="G30" s="11"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="23">
-        <v>43195</v>
+      <c r="C30" s="24">
+        <v>2</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30" s="11"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="42">
+        <v>43207</v>
       </c>
       <c r="B31" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="27">
+      <c r="C31" s="24">
         <v>2</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F31" s="19"/>
-      <c r="G31" s="11"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="23">
-        <v>43195</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31" s="11"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="26"/>
       <c r="B32" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C32" s="27">
+        <v>1</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="G32" s="19"/>
+      <c r="H32" s="11"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="42">
+        <v>43207</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="27">
+        <v>2</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="11"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="42">
+        <v>43207</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="27">
         <v>3</v>
       </c>
-      <c r="D32" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="26">
-        <v>43196</v>
-      </c>
-      <c r="B33" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C33" s="24">
+      <c r="D34" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="42">
+        <v>43207</v>
+      </c>
+      <c r="B35" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="24">
         <v>1</v>
       </c>
-      <c r="D33" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G33" s="11"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="26">
-        <v>43196</v>
-      </c>
-      <c r="B34" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C34" s="27">
-        <v>1</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G34" s="11"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="26">
-        <v>43196</v>
-      </c>
-      <c r="B35" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C35" s="27">
-        <v>1</v>
-      </c>
       <c r="D35" s="12" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G35"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="26">
-        <v>43196</v>
+        <v>40</v>
+      </c>
+      <c r="H35" s="11"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="42">
+        <v>43207</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>144</v>
+        <v>99</v>
       </c>
       <c r="C36" s="27">
         <v>1</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="G36" s="11"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="26">
-        <v>43196</v>
+        <v>41</v>
+      </c>
+      <c r="H36" s="11"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="42">
+        <v>43207</v>
       </c>
       <c r="B37" s="38" t="s">
-        <v>144</v>
+        <v>99</v>
       </c>
       <c r="C37" s="27">
         <v>1</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F37"/>
-      <c r="G37" s="11"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="26">
-        <v>43196</v>
+        <v>42</v>
+      </c>
+      <c r="H37"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="42">
+        <v>43207</v>
       </c>
       <c r="B38" s="38" t="s">
-        <v>144</v>
+        <v>99</v>
       </c>
       <c r="C38" s="27">
         <v>1</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="F38"/>
-      <c r="G38" s="11"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="23">
-        <v>43195</v>
+        <v>43</v>
+      </c>
+      <c r="H38" s="11"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="42">
+        <v>43207</v>
       </c>
       <c r="B39" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="27">
+        <v>1</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39" s="11"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="42">
+        <v>43207</v>
+      </c>
+      <c r="B40" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" s="27">
+        <v>1</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40" s="11"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="26"/>
+      <c r="B41" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="22">
+      <c r="C41" s="22">
         <v>1</v>
       </c>
-      <c r="D39" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F39"/>
-      <c r="G39" s="11"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="23">
-        <v>43202</v>
-      </c>
-      <c r="B40" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="C40" s="29">
+      <c r="D41" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F41" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="G41"/>
+      <c r="H41" s="11"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="41"/>
+      <c r="B42" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="29">
         <v>1</v>
       </c>
-      <c r="D40" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E40" s="16" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="23">
-        <v>43196</v>
-      </c>
-      <c r="B41" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="C41" s="29">
+      <c r="D42" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="26"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="29">
         <v>2</v>
       </c>
-      <c r="D41" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="23">
-        <v>43202</v>
-      </c>
-      <c r="B42" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="C42" s="29">
+      <c r="D43" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="42"/>
+      <c r="B44" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="29">
         <v>2</v>
       </c>
-      <c r="D42" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="23">
-        <v>43202</v>
-      </c>
-      <c r="B43" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="C43" s="29">
+      <c r="D44" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="23"/>
+      <c r="B45" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" s="29">
         <v>3</v>
       </c>
-      <c r="D43" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="23">
-        <v>43202</v>
-      </c>
-      <c r="B44" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="C44" s="29">
+      <c r="D45" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="23"/>
+      <c r="B46" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="29">
         <v>3</v>
       </c>
-      <c r="D44" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="23">
-        <v>43202</v>
-      </c>
-      <c r="B45" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="C45" s="29">
+      <c r="D46" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="23"/>
+      <c r="B47" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" s="29">
         <v>4</v>
       </c>
-      <c r="D45" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="23">
-        <v>43202</v>
-      </c>
-      <c r="B46" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="C46" s="29">
-        <v>4</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
-      <c r="B47" s="28"/>
-      <c r="C47" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D47" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="23"/>
       <c r="B48" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="C48" s="29"/>
-      <c r="D48" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>156</v>
+        <v>102</v>
+      </c>
+      <c r="C48" s="29">
+        <v>4</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="23"/>
       <c r="B49" s="28"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>158</v>
-      </c>
+      <c r="C49" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="B50" s="28"/>
+      <c r="A50" s="23"/>
+      <c r="B50" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="C50" s="29"/>
-      <c r="D50" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>166</v>
+      <c r="D50" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="23"/>
+      <c r="A51" s="23">
+        <v>43207</v>
+      </c>
       <c r="B51" s="28"/>
       <c r="C51" s="29"/>
       <c r="D51" s="13" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>172</v>
+        <v>144</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
+      <c r="A52" s="27"/>
       <c r="B52" s="28"/>
       <c r="C52" s="29"/>
-      <c r="D52" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="E52" s="20"/>
+      <c r="D52" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
+      <c r="A53" s="47"/>
       <c r="B53" s="28"/>
       <c r="C53" s="29"/>
       <c r="D53" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="E53" s="20"/>
+        <v>146</v>
+      </c>
+      <c r="E53" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
+      <c r="A54" s="41"/>
       <c r="B54" s="28"/>
       <c r="C54" s="29"/>
-      <c r="D54" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="E54" s="20"/>
+      <c r="D54" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="E54" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
-      <c r="B55" s="28" t="s">
-        <v>80</v>
-      </c>
+      <c r="A55" s="23">
+        <v>43207</v>
+      </c>
+      <c r="B55" s="28"/>
       <c r="C55" s="29"/>
-      <c r="D55" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E55" s="20" t="s">
-        <v>155</v>
+      <c r="D55" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="E55" s="48" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="23"/>
+      <c r="A56" s="23">
+        <v>43207</v>
+      </c>
       <c r="B56" s="28"/>
       <c r="C56" s="29"/>
-      <c r="D56" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="E56" s="20"/>
+      <c r="D56" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="E56" s="48" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="23"/>
+      <c r="A57" s="41"/>
       <c r="B57" s="28"/>
       <c r="C57" s="29"/>
-      <c r="D57" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E57" s="20"/>
+      <c r="D57" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="23"/>
+      <c r="A58" s="23">
+        <v>43207</v>
+      </c>
       <c r="B58" s="28"/>
       <c r="C58" s="29"/>
-      <c r="D58" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="E58" s="20"/>
+      <c r="D58" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="E58" s="48" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
+      <c r="A59" s="47"/>
       <c r="B59" s="28"/>
       <c r="C59" s="29"/>
-      <c r="D59" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="E59" s="20"/>
+      <c r="D59" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="E59" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="23"/>
       <c r="B60" s="28"/>
       <c r="C60" s="29"/>
       <c r="D60" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="E60" s="20"/>
+        <v>155</v>
+      </c>
+      <c r="E60" s="48" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
+      <c r="A61" s="47"/>
       <c r="B61" s="28"/>
       <c r="C61" s="29"/>
-      <c r="D61" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="E61" s="20"/>
+      <c r="D61" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="E61" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="23"/>
+      <c r="A62" s="23">
+        <v>43207</v>
+      </c>
       <c r="B62" s="28"/>
       <c r="C62" s="29"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="20"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="23"/>
+      <c r="D62" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="E62" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="47"/>
       <c r="B63" s="28"/>
       <c r="C63" s="29"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="20"/>
+      <c r="D63" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E63" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="23">
-        <f>ROUND(COUNTA(A3:A55)/ROWS(A3:A55)*100,0)</f>
-        <v>66</v>
-      </c>
-      <c r="B64" s="30" t="s">
+      <c r="A64" s="23"/>
+      <c r="B64" s="28"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="20"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="23"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="20"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="45">
+        <f>(COUNTA(A3:A65)/ROWS(A3:A65)) *100</f>
+        <v>39.682539682539684</v>
+      </c>
+      <c r="B66" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C64" s="27"/>
-      <c r="D64" s="16"/>
-      <c r="F64"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="31"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="7"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="10"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="10"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C66" s="27"/>
+      <c r="D66" s="16"/>
+      <c r="F66"/>
+      <c r="G66"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="31"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="7"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
       <c r="F68" s="10"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G68" s="10"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
       <c r="F69" s="10"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G69" s="10"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
       <c r="F70" s="10"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G70" s="10"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D71" s="14"/>
       <c r="E71" s="14"/>
       <c r="F71" s="10"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G71" s="10"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D72" s="14"/>
       <c r="E72" s="14"/>
       <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="10"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="10"/>
+      <c r="G74" s="10"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A15 A26:A31 A33:A38 A40:A49 A51:A65">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="366">
+  <conditionalFormatting sqref="A15 A42:A51 A28:A33 A53:A67">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="379">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A6">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="25">
       <formula>LEN(TRIM(A3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="11">
+  <conditionalFormatting sqref="A14">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="19">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="21">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19:A27">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="18">
+      <formula>LEN(TRIM(A19))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17:A18">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="17">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="15">
+      <formula>LEN(TRIM(A41))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:A9">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
       <formula>LEN(TRIM(A7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="10">
-      <formula>LEN(TRIM(A8))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="9">
-      <formula>LEN(TRIM(A9))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="8">
-      <formula>LEN(TRIM(A10))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="7">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
       <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12:A14">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
+  <conditionalFormatting sqref="A12">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="10">
       <formula>LEN(TRIM(A12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17:A25">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="5">
-      <formula>LEN(TRIM(A17))&gt;0</formula>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="9">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
       <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="3">
-      <formula>LEN(TRIM(A32))&gt;0</formula>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(A35))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(A36))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(A37))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(A38))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A39))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(A40))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2823,35 +3125,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61" customWidth="1"/>
-    <col min="3" max="3" width="57.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.625" customWidth="1"/>
+    <col min="3" max="3" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2859,10 +3161,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -2870,10 +3172,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -2881,10 +3183,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2892,10 +3194,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -2903,10 +3205,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -2914,18 +3216,18 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2933,10 +3235,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -2944,10 +3246,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -2955,74 +3257,74 @@
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="D21" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="D23" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -3042,8 +3344,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="12.375" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
commit before merge. Still WIP
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="person_1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="166">
   <si>
     <t>Item</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>%reviewed</t>
-  </si>
-  <si>
-    <t>Except for :VS: VisitBaseline_, VisitScreening, VisitWk24_, VisitWk2</t>
   </si>
   <si>
     <t>cdiscpilot01:Person_01-701-1015</t>
@@ -593,6 +590,12 @@
       </rPr>
       <t>Assessed only for Person_01-701-1015</t>
     </r>
+  </si>
+  <si>
+    <t>Object discprepancies sent to AO</t>
+  </si>
+  <si>
+    <t>18APR18</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1217,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1342,6 +1345,10 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1387,49 +1394,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <fill>
         <patternFill>
@@ -1876,27 +1841,27 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D69" sqref="D69"/>
+      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" style="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="22" customWidth="1"/>
-    <col min="4" max="4" width="69.7109375" style="12" customWidth="1"/>
-    <col min="5" max="5" width="68.140625" style="12" customWidth="1"/>
-    <col min="6" max="7" width="49.85546875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="57.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="69.7265625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="68.1796875" style="12" customWidth="1"/>
+    <col min="6" max="7" width="49.81640625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="57.1796875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="D1" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
         <v>25</v>
       </c>
@@ -1904,25 +1869,25 @@
         <v>28</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="35" t="s">
         <v>49</v>
-      </c>
-      <c r="E2" s="35" t="s">
-        <v>50</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>27</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H2" s="35" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="23"/>
       <c r="B3" s="32" t="s">
         <v>26</v>
@@ -1931,18 +1896,20 @@
         <v>1</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="33"/>
+        <v>164</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>165</v>
+      </c>
       <c r="H3" s="34"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="23">
         <v>43207</v>
       </c>
@@ -1950,19 +1917,21 @@
         <v>26</v>
       </c>
       <c r="C4" s="24"/>
-      <c r="D4" s="12" t="s">
-        <v>112</v>
+      <c r="D4" s="49" t="s">
+        <v>111</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="G4" s="40"/>
+        <v>116</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>165</v>
+      </c>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23">
         <v>43207</v>
       </c>
@@ -1971,36 +1940,36 @@
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="23">
         <v>43207</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
       <c r="H6" s="11"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="23">
-        <v>43207</v>
+        <v>43208</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>26</v>
@@ -2009,16 +1978,16 @@
         <v>1</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="41"/>
       <c r="B8" s="25" t="s">
         <v>26</v>
@@ -2027,18 +1996,18 @@
         <v>2</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="41"/>
       <c r="B9" s="25" t="s">
         <v>26</v>
@@ -2047,328 +2016,330 @@
         <v>2</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E9" s="39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="G9" s="20"/>
+        <v>120</v>
+      </c>
+      <c r="G9" s="50">
+        <v>43208</v>
+      </c>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="41"/>
       <c r="B10" s="25"/>
       <c r="C10" s="24">
         <v>1</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="23">
         <v>43207</v>
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="24"/>
       <c r="D11" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
       <c r="H11" s="11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="23">
         <v>43207</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="24"/>
       <c r="D12" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
       <c r="H12" s="19" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="23">
         <v>43207</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="24"/>
       <c r="D13" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
       <c r="H13" s="11"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="41"/>
       <c r="B14" s="25"/>
       <c r="C14" s="24"/>
       <c r="D14" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="42">
         <v>43207</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="24">
         <v>1</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="11"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="42">
         <v>43207</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="24">
         <v>2</v>
       </c>
       <c r="D16" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>128</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>129</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
       <c r="H16" s="11"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="43"/>
       <c r="B17" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="24"/>
       <c r="D17" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G17" s="19"/>
       <c r="H17" s="11"/>
     </row>
-    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="43"/>
       <c r="B18" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" s="19" t="s">
         <v>131</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>132</v>
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="11"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="42"/>
       <c r="B19" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="25">
         <v>2</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H19" s="11"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="42"/>
       <c r="B20" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="25">
         <v>3</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
       <c r="H20" s="11"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="42"/>
       <c r="B21" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="25">
         <v>3</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
       <c r="H21" s="11"/>
     </row>
-    <row r="22" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="42"/>
       <c r="B22" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="25">
         <v>2</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
       <c r="H22" s="11"/>
     </row>
-    <row r="23" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="42"/>
       <c r="B23" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" s="25">
         <v>3</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
       <c r="H23" s="11"/>
     </row>
-    <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="42"/>
       <c r="B24" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="25">
         <v>3</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
       <c r="H24" s="11"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="42"/>
       <c r="B25" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" s="25">
         <v>2</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
       <c r="H25" s="11"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="42"/>
       <c r="B26" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" s="24">
         <v>3</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
       <c r="H26" s="11"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="42"/>
       <c r="B27" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="24">
         <v>3</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
       <c r="H27" s="11"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="26"/>
       <c r="B28" s="25" t="s">
         <v>26</v>
@@ -2377,18 +2348,18 @@
         <v>1</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F28" s="44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G28"/>
       <c r="H28" s="11"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="42">
         <v>43207</v>
       </c>
@@ -2399,16 +2370,16 @@
         <v>2</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F29"/>
       <c r="G29"/>
       <c r="H29" s="11"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="42">
         <v>43207</v>
       </c>
@@ -2419,16 +2390,16 @@
         <v>2</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F30"/>
       <c r="G30"/>
       <c r="H30" s="11"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="42">
         <v>43207</v>
       </c>
@@ -2439,16 +2410,16 @@
         <v>2</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F31"/>
       <c r="G31"/>
       <c r="H31" s="11"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="26"/>
       <c r="B32" s="25" t="s">
         <v>26</v>
@@ -2457,18 +2428,18 @@
         <v>1</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G32" s="19"/>
       <c r="H32" s="11"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="42">
         <v>43207</v>
       </c>
@@ -2479,16 +2450,16 @@
         <v>2</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
       <c r="H33" s="11"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="42">
         <v>43207</v>
       </c>
@@ -2499,125 +2470,125 @@
         <v>3</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="42">
         <v>43207</v>
       </c>
       <c r="B35" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C35" s="24">
         <v>1</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H35" s="11"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="42">
         <v>43207</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C36" s="27">
         <v>1</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H36" s="11"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="42">
         <v>43207</v>
       </c>
       <c r="B37" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C37" s="27">
         <v>1</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H37"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="42">
         <v>43207</v>
       </c>
       <c r="B38" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C38" s="27">
         <v>1</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H38" s="11"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="42">
         <v>43207</v>
       </c>
       <c r="B39" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C39" s="27">
         <v>1</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F39"/>
       <c r="G39"/>
       <c r="H39" s="11"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="42">
         <v>43207</v>
       </c>
       <c r="B40" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C40" s="27">
         <v>1</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F40"/>
       <c r="G40"/>
       <c r="H40" s="11"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="26"/>
       <c r="B41" s="38" t="s">
         <v>26</v>
@@ -2626,334 +2597,340 @@
         <v>1</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F41" s="44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G41"/>
       <c r="H41" s="11"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="41"/>
       <c r="B42" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" s="29">
         <v>1</v>
       </c>
       <c r="D42" s="46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="26"/>
       <c r="B43" s="28"/>
       <c r="C43" s="29">
         <v>2</v>
       </c>
       <c r="D43" s="39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="42"/>
       <c r="B44" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C44" s="29">
         <v>2</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="23"/>
       <c r="B45" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C45" s="29">
         <v>3</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="23"/>
       <c r="B46" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C46" s="29">
         <v>3</v>
       </c>
       <c r="D46" s="39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="23"/>
       <c r="B47" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C47" s="29">
         <v>4</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="23"/>
       <c r="B48" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C48" s="29">
         <v>4</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="23"/>
       <c r="B49" s="28"/>
       <c r="C49" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="23"/>
       <c r="B50" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C50" s="29"/>
       <c r="D50" s="46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E50" s="20" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="23">
         <v>43207</v>
       </c>
       <c r="B51" s="28"/>
       <c r="C51" s="29"/>
       <c r="D51" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="F51" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="E51" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="27"/>
       <c r="B52" s="28"/>
       <c r="C52" s="29"/>
       <c r="D52" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="47"/>
       <c r="B53" s="28"/>
       <c r="C53" s="29"/>
       <c r="D53" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E53" s="48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="41"/>
       <c r="B54" s="28"/>
       <c r="C54" s="29"/>
       <c r="D54" s="39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E54" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F54" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="F54" s="8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="23">
         <v>43207</v>
       </c>
       <c r="B55" s="28"/>
       <c r="C55" s="29"/>
       <c r="D55" s="48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E55" s="48" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="23">
         <v>43207</v>
       </c>
       <c r="B56" s="28"/>
       <c r="C56" s="29"/>
       <c r="D56" s="48" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E56" s="48" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="41"/>
       <c r="B57" s="28"/>
       <c r="C57" s="29"/>
       <c r="D57" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E57" s="20" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="23">
         <v>43207</v>
       </c>
       <c r="B58" s="28"/>
       <c r="C58" s="29"/>
       <c r="D58" s="48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E58" s="48" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="47"/>
       <c r="B59" s="28"/>
       <c r="C59" s="29"/>
       <c r="D59" s="48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E59" s="48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="23"/>
       <c r="B60" s="28"/>
       <c r="C60" s="29"/>
       <c r="D60" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="E60" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="E60" s="48" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="47"/>
       <c r="B61" s="28"/>
       <c r="C61" s="29"/>
       <c r="D61" s="39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E61" s="48" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="23">
         <v>43207</v>
       </c>
       <c r="B62" s="28"/>
       <c r="C62" s="29"/>
       <c r="D62" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="47"/>
       <c r="B63" s="28"/>
       <c r="C63" s="29"/>
       <c r="D63" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E63" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="F63" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="E63" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="F63" s="8" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="23"/>
       <c r="B64" s="28"/>
       <c r="C64" s="29"/>
       <c r="D64" s="16"/>
       <c r="E64" s="20"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="23"/>
       <c r="B65" s="28"/>
       <c r="C65" s="29"/>
       <c r="D65" s="16"/>
       <c r="E65" s="20"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="45">
         <f>(COUNTA(A3:A65)/ROWS(A3:A65)) *100</f>
         <v>39.682539682539684</v>
@@ -2966,49 +2943,49 @@
       <c r="F66"/>
       <c r="G66"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="31"/>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
       <c r="H67" s="7"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
       <c r="F68" s="10"/>
       <c r="G68" s="10"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
       <c r="F69" s="10"/>
       <c r="G69" s="10"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
       <c r="F70" s="10"/>
       <c r="G70" s="10"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D71" s="14"/>
       <c r="E71" s="14"/>
       <c r="F71" s="10"/>
       <c r="G71" s="10"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D72" s="14"/>
       <c r="E72" s="14"/>
       <c r="F72" s="10"/>
       <c r="G72" s="10"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D73" s="14"/>
       <c r="E73" s="14"/>
       <c r="F73" s="10"/>
       <c r="G73" s="10"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D74" s="14"/>
       <c r="E74" s="14"/>
       <c r="F74" s="10"/>
@@ -3016,57 +2993,57 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A15 A42:A51 A28:A33 A53:A67">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="379">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="379">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A6">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="25">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="25">
       <formula>LEN(TRIM(A3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="19">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="19">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="21">
       <formula>LEN(TRIM(A10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:A27">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="18">
       <formula>LEN(TRIM(A19))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:A18">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="17">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="17">
       <formula>LEN(TRIM(A17))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="15">
       <formula>LEN(TRIM(A41))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A9">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="13">
       <formula>LEN(TRIM(A7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="12">
       <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
       <formula>LEN(TRIM(A12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3123,208 +3100,208 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61" customWidth="1"/>
-    <col min="3" max="3" width="57.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="57.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>51</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>52</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>65</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>59</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" t="s">
-        <v>68</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
         <v>69</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>70</v>
       </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="18" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>72</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
         <v>78</v>
       </c>
-      <c r="C21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>80</v>
-      </c>
-      <c r="B23" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -3341,14 +3318,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -3356,7 +3333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3364,7 +3341,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -3372,7 +3349,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -3380,7 +3357,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3388,7 +3365,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3396,7 +3373,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -3410,7 +3387,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3424,7 +3401,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3438,7 +3415,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3452,16 +3429,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -3469,7 +3446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -3483,7 +3460,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -3497,7 +3474,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -3511,7 +3488,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3525,7 +3502,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
@@ -3538,7 +3515,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
@@ -3551,7 +3528,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>24</v>
       </c>
@@ -3562,11 +3539,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="3"/>
     </row>

</xml_diff>

<commit_message>
additional updates. Awaiting discussion on next steps for VS
</commit_message>
<xml_diff>
--- a/r/validation/TripleQCCheckList.xlsx
+++ b/r/validation/TripleQCCheckList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="person_1" sheetId="1" r:id="rId1"/>
@@ -21,81 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="152">
-  <si>
-    <t>Item</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="145">
   <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Ont</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Interval_RI1  rdfs:label  Interval 10</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Interval_RI1  time:hasEnd  cdiscpilot01:Date_29</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Interval_LS1  rdfs:label  Interval 4</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Interval_RI1  rdfs:label  Reference Interval 1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Interval_RI1  time:hasEnd  cdiscpilot01:Date_30</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Interval_LS1  rdfs:label  Lifespan Interval 1</t>
-  </si>
-  <si>
-    <t>cdiscpilot01:Interval_LS1  rdfs:label  Study Participation Interval 1</t>
-  </si>
-  <si>
     <t>Ontology</t>
-  </si>
-  <si>
-    <t>DBP_1</t>
-  </si>
-  <si>
-    <t>links to</t>
-  </si>
-  <si>
-    <t>bpoutcome_2</t>
-  </si>
-  <si>
-    <t>bpoutcome_3</t>
-  </si>
-  <si>
-    <t>bpoutcome_1</t>
-  </si>
-  <si>
-    <t>DBP_2</t>
-  </si>
-  <si>
-    <t>DBP_3</t>
-  </si>
-  <si>
-    <t>Then in the custom terminlogy:</t>
-  </si>
-  <si>
-    <t>links to value:</t>
-  </si>
-  <si>
-    <t>(systolic)</t>
-  </si>
-  <si>
-    <t>bpoutcome_4</t>
-  </si>
-  <si>
-    <t>bpoutcome_5</t>
-  </si>
-  <si>
-    <t>bpoutcome_6</t>
   </si>
   <si>
     <t>DM</t>
@@ -523,6 +454,54 @@
   </si>
   <si>
     <t>prefLabel difference Person 1</t>
+  </si>
+  <si>
+    <t>ADDITIONAL PATIENTS</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:DemographicDataCollection_01-701-1023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  study:hasSubActivity cdiscpilot01:DrugAdministration_01-701-1023_2012-08-05_2012-08-27 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  study:hasSubActivity cdiscpilot01:DrugAdministration_01-701-1023_2012-08-28_2012-09-01 ;</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:DrugAdministration_01-701-1023_2012-08-05_2012-08-27</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:DrugAdministration_01-701-1023_2012-08-28_2012-09-01</t>
+  </si>
+  <si>
+    <t>Drug Admin</t>
+  </si>
+  <si>
+    <t>01-701-1023</t>
+  </si>
+  <si>
+    <t>01-701-1028</t>
+  </si>
+  <si>
+    <t>01-701-1015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  study:hasSubActivity cdiscpilot01:DrugAdministration_01-701-1015_2014-01-02_2014-01-16 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  study:hasSubActivity cdiscpilot01:DrugAdministration_01-701-1015_2014-01-17_2014-06-18 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  study:hasSubActivity cdiscpilot01:DrugAdministration_01-701-1015_2014-06-19_2014-07-02 ;</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:DrugAdministration_01-701-1015_2014-01-02_2014-01-16</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:DrugAdministration_01-701-1015_2014-01-17_2014-06-18</t>
+  </si>
+  <si>
+    <t>cdiscpilot01:DrugAdministration_01-701-1015_2014-06-19_2014-07-02</t>
   </si>
 </sst>
 </file>
@@ -1677,11 +1656,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C66" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A89" sqref="A89"/>
+      <selection pane="bottomRight" activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,36 +1677,36 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="E1" s="12" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>144</v>
+        <v>121</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="I2" s="32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1735,19 +1714,19 @@
         <v>43219</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D3" s="23">
         <v>1</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="G3" s="44"/>
       <c r="H3" s="30"/>
@@ -1758,23 +1737,23 @@
         <v>43219</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="38" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="G4" s="44" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="I4" s="11"/>
     </row>
@@ -1783,17 +1762,17 @@
         <v>43219</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="13" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="G5" s="18"/>
       <c r="H5" s="18"/>
@@ -1804,23 +1783,23 @@
         <v>43220</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="13" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="G6" s="49" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="H6" s="48" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="I6" s="11"/>
     </row>
@@ -1829,19 +1808,19 @@
         <v>43219</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D7" s="25">
         <v>1</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7"/>
@@ -1852,25 +1831,25 @@
         <v>43220</v>
       </c>
       <c r="B8" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="D8" s="23">
         <v>2</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="G8" s="49" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="H8" s="48" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="I8" s="11"/>
     </row>
@@ -1879,19 +1858,19 @@
         <v>43219</v>
       </c>
       <c r="B9" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D9" s="23">
         <v>2</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="G9" s="45"/>
       <c r="H9" s="39"/>
@@ -1902,23 +1881,23 @@
         <v>43219</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="23">
         <v>1</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="I10" s="18"/>
     </row>
@@ -1927,23 +1906,23 @@
         <v>43220</v>
       </c>
       <c r="B11" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="13" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="G11" s="49" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="H11" s="48" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="I11" s="11"/>
     </row>
@@ -1952,15 +1931,15 @@
         <v>43219</v>
       </c>
       <c r="B12" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C12" s="24"/>
       <c r="D12" s="23"/>
       <c r="E12" s="13" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="G12" s="18"/>
       <c r="H12" s="18"/>
@@ -1971,17 +1950,17 @@
         <v>43219</v>
       </c>
       <c r="B13" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="12" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="G13" s="18"/>
       <c r="H13" s="18"/>
@@ -1992,17 +1971,17 @@
         <v>43219</v>
       </c>
       <c r="B14" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="12" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="G14" s="18"/>
       <c r="H14" s="18"/>
@@ -2013,17 +1992,17 @@
         <v>43219</v>
       </c>
       <c r="B15" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="12" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="18"/>
@@ -2034,20 +2013,20 @@
         <v>43220</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="13" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="11"/>
@@ -2057,20 +2036,20 @@
         <v>43220</v>
       </c>
       <c r="B17" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="13" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="G17" s="49" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="H17" s="18"/>
       <c r="I17" s="11"/>
@@ -2080,17 +2059,17 @@
         <v>43220</v>
       </c>
       <c r="B18" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D18" s="23"/>
       <c r="E18" s="13" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
@@ -2101,17 +2080,17 @@
         <v>43220</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D19" s="23"/>
       <c r="E19" s="13" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="G19" s="46"/>
       <c r="H19" s="18"/>
@@ -2122,17 +2101,17 @@
         <v>43220</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D20" s="23"/>
       <c r="E20" s="13" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G20" s="18"/>
       <c r="H20" s="18"/>
@@ -2143,23 +2122,23 @@
         <v>43220</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D21" s="23"/>
       <c r="E21" s="13" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="I21" s="11"/>
     </row>
@@ -2168,17 +2147,17 @@
         <v>43220</v>
       </c>
       <c r="B22" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D22" s="23"/>
       <c r="E22" s="13" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="G22" s="49"/>
       <c r="H22" s="18"/>
@@ -2189,17 +2168,17 @@
         <v>43220</v>
       </c>
       <c r="B23" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="13" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="G23" s="49"/>
       <c r="H23" s="18"/>
@@ -2210,17 +2189,17 @@
         <v>43220</v>
       </c>
       <c r="B24" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D24" s="23"/>
       <c r="E24" s="13" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="G24" s="18"/>
       <c r="H24" s="18"/>
@@ -2231,20 +2210,20 @@
         <v>43220</v>
       </c>
       <c r="B25" s="42" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D25" s="23"/>
       <c r="E25" s="13" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="H25" s="18"/>
       <c r="I25" s="11"/>
@@ -2254,17 +2233,17 @@
         <v>43220</v>
       </c>
       <c r="B26" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D26" s="23"/>
       <c r="E26" s="13" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="G26" s="18"/>
       <c r="H26" s="18"/>
@@ -2275,17 +2254,17 @@
         <v>43220</v>
       </c>
       <c r="B27" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D27" s="23"/>
       <c r="E27" s="13" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="G27" s="18"/>
       <c r="H27" s="18"/>
@@ -2296,17 +2275,17 @@
         <v>43220</v>
       </c>
       <c r="B28" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="13" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="G28" s="18"/>
       <c r="H28" s="18"/>
@@ -2317,17 +2296,17 @@
         <v>43220</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="13" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="G29" s="18"/>
       <c r="H29" s="18"/>
@@ -2338,20 +2317,20 @@
         <v>43220</v>
       </c>
       <c r="B30" s="42" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="13" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="H30" s="18"/>
       <c r="I30" s="11"/>
@@ -2361,14 +2340,14 @@
         <v>43220</v>
       </c>
       <c r="B31" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D31" s="23"/>
       <c r="E31" s="13" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
@@ -2379,14 +2358,14 @@
         <v>43220</v>
       </c>
       <c r="B32" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D32" s="23"/>
       <c r="E32" s="13" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="G32" s="18"/>
       <c r="H32" s="18"/>
@@ -2397,14 +2376,14 @@
         <v>43220</v>
       </c>
       <c r="B33" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D33" s="23"/>
       <c r="E33" s="13" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="G33" s="18"/>
       <c r="H33" s="18"/>
@@ -2415,19 +2394,19 @@
         <v>43220</v>
       </c>
       <c r="B34" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D34" s="23">
         <v>1</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="G34" s="47"/>
       <c r="H34" s="18"/>
@@ -2438,19 +2417,19 @@
         <v>43220</v>
       </c>
       <c r="B35" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D35" s="23">
         <v>2</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
@@ -2461,17 +2440,17 @@
         <v>43220</v>
       </c>
       <c r="B36" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D36" s="23"/>
       <c r="E36" s="13" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="G36" s="45"/>
       <c r="H36" s="18"/>
@@ -2482,17 +2461,17 @@
         <v>43220</v>
       </c>
       <c r="B37" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D37" s="23"/>
       <c r="E37" s="13" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
@@ -2503,19 +2482,19 @@
         <v>43220</v>
       </c>
       <c r="B38" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D38" s="24">
         <v>2</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="G38" s="46"/>
       <c r="H38" s="18"/>
@@ -2526,19 +2505,19 @@
         <v>43220</v>
       </c>
       <c r="B39" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D39" s="24">
         <v>3</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G39" s="18"/>
       <c r="H39" s="18"/>
@@ -2549,22 +2528,22 @@
         <v>43220</v>
       </c>
       <c r="B40" s="42" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D40" s="24">
         <v>3</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="H40" s="18"/>
       <c r="I40" s="11"/>
@@ -2574,17 +2553,17 @@
         <v>43220</v>
       </c>
       <c r="B41" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D41" s="24"/>
       <c r="E41" s="13" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="G41" s="18"/>
       <c r="H41" s="18"/>
@@ -2595,15 +2574,15 @@
         <v>43220</v>
       </c>
       <c r="B42" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C42" s="24"/>
       <c r="D42" s="24"/>
       <c r="E42" s="13" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="G42" s="18"/>
       <c r="H42" s="18"/>
@@ -2614,19 +2593,19 @@
         <v>43220</v>
       </c>
       <c r="B43" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D43" s="24">
         <v>2</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="G43" s="18"/>
       <c r="H43" s="18"/>
@@ -2637,22 +2616,22 @@
         <v>43220</v>
       </c>
       <c r="B44" s="42" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D44" s="24">
         <v>3</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="G44" s="18" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="H44" s="18"/>
       <c r="I44" s="11"/>
@@ -2662,19 +2641,19 @@
         <v>43220</v>
       </c>
       <c r="B45" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D45" s="24">
         <v>3</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="G45" s="18"/>
       <c r="H45" s="18"/>
@@ -2685,15 +2664,15 @@
         <v>43220</v>
       </c>
       <c r="B46" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C46" s="24"/>
       <c r="D46" s="24"/>
       <c r="E46" s="13" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="G46" s="18"/>
       <c r="H46" s="18"/>
@@ -2704,15 +2683,15 @@
         <v>43220</v>
       </c>
       <c r="B47" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C47" s="24"/>
       <c r="D47" s="24"/>
       <c r="E47" s="13" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="G47" s="18"/>
       <c r="H47" s="18"/>
@@ -2723,19 +2702,19 @@
         <v>43220</v>
       </c>
       <c r="B48" s="42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D48" s="24">
         <v>2</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="G48" s="18"/>
       <c r="H48" s="18"/>
@@ -2746,22 +2725,22 @@
         <v>43220</v>
       </c>
       <c r="B49" s="42" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D49" s="23">
         <v>3</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="G49" s="18" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="H49" s="18"/>
       <c r="I49" s="11"/>
@@ -2771,19 +2750,19 @@
         <v>43220</v>
       </c>
       <c r="B50" s="42" t="s">
-        <v>132</v>
+